<commit_message>
Added two methods to load and add an event to the registry. Now I will have to create loaders for the handler maps.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="17895" windowHeight="4995" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="17895" windowHeight="4995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
     <sheet name="Items" sheetId="2" r:id="rId2"/>
     <sheet name="Individuals" sheetId="3" r:id="rId3"/>
+    <sheet name="Events" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -331,6 +332,18 @@
   </si>
   <si>
     <t>dialogID</t>
+  </si>
+  <si>
+    <t>int a</t>
+  </si>
+  <si>
+    <t>int b</t>
+  </si>
+  <si>
+    <t>nextEventID</t>
+  </si>
+  <si>
+    <t>message</t>
   </si>
 </sst>
 </file>
@@ -665,7 +678,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B6" sqref="B6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1684,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2477,4 +2490,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="A3:H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>206</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
The next thing I'm trying to create between dialogs and events is shopping functionality. Basically by adding currency to the game (individuals have gold, items are worth gold) and adding a buyMode to the inventory, the player can talk to a merchant and then see a inventoryView of their wares, and see the cost associated with each item. when they hit enter, they will attempt to buy the item (popping up a dialog box in response to success or failure). So far, I've just added the simple functionality of gold to individuals and items, as well as the buyMode for inventoryView and drawing the price next to each item. The next step is tying it all together.
Also I've corrected some of the tests, adding new random number
generation caused one of the tests to change slightly, but nothing
major.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="17895" windowHeight="4995" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="810" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="119">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -344,6 +344,36 @@
   </si>
   <si>
     <t>message</t>
+  </si>
+  <si>
+    <t>Triggers:</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Harm</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>EventID</t>
+  </si>
+  <si>
+    <t>"Have at you!"</t>
+  </si>
+  <si>
+    <t>Welcome! We've got the lowest prices!</t>
+  </si>
+  <si>
+    <t>What would you like?</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>gold</t>
   </si>
 </sst>
 </file>
@@ -675,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:F6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -816,6 +846,63 @@
         <v>1003</v>
       </c>
     </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>1004</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1005</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>1005</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>1005</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -823,10 +910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN7"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -834,7 +921,7 @@
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:41">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -857,106 +944,109 @@
         <v>37</v>
       </c>
       <c r="H1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>41</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>42</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>45</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>47</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>48</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>49</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>50</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>51</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>52</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>53</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>55</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>56</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>57</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>58</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>59</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>60</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>61</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>63</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>64</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>65</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>66</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>67</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>68</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>69</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:41">
       <c r="A2">
         <v>0</v>
       </c>
@@ -979,26 +1069,26 @@
         <v>15</v>
       </c>
       <c r="H2">
+        <v>25</v>
+      </c>
+      <c r="I2">
         <v>255</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
         <v>255</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>3</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>4</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
       <c r="O2">
         <v>0</v>
       </c>
@@ -1009,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -1024,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2">
         <v>0</v>
@@ -1074,11 +1164,14 @@
       <c r="AM2">
         <v>0</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:41">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1101,31 +1194,31 @@
         <v>19</v>
       </c>
       <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
         <v>255</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
       <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>255</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>20</v>
-      </c>
-      <c r="L3">
-        <v>3</v>
       </c>
       <c r="M3">
         <v>3</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1143,17 +1236,17 @@
         <v>0</v>
       </c>
       <c r="V3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="Y3">
         <v>5</v>
       </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
       <c r="Z3">
         <v>0</v>
       </c>
@@ -1196,11 +1289,14 @@
       <c r="AM3">
         <v>0</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:41">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1223,25 +1319,25 @@
         <v>15</v>
       </c>
       <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
         <v>255</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
       <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>255</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>22</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
       <c r="M4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1250,10 +1346,10 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -1318,11 +1414,14 @@
       <c r="AM4">
         <v>0</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:41">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1345,32 +1444,32 @@
         <v>15</v>
       </c>
       <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="I5">
         <v>255</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
       <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>255</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>24</v>
       </c>
-      <c r="L5">
-        <v>2</v>
-      </c>
       <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
         <v>3</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
       <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>10</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
       <c r="Q5">
         <v>0</v>
       </c>
@@ -1440,11 +1539,14 @@
       <c r="AM5">
         <v>0</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:41">
       <c r="A6">
         <v>200</v>
       </c>
@@ -1467,20 +1569,20 @@
         <v>15</v>
       </c>
       <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6">
         <v>255</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
       <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>255</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>16</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
       <c r="M6">
         <v>0</v>
       </c>
@@ -1497,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -1512,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -1560,13 +1662,16 @@
         <v>0</v>
       </c>
       <c r="AM6">
-        <v>1</v>
-      </c>
-      <c r="AN6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>1</v>
+      </c>
+      <c r="AO6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:41">
       <c r="A7">
         <v>200</v>
       </c>
@@ -1589,20 +1694,20 @@
         <v>15</v>
       </c>
       <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="I7">
         <v>255</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
       <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>255</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>29</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
       <c r="M7">
         <v>0</v>
       </c>
@@ -1646,7 +1751,7 @@
         <v>0</v>
       </c>
       <c r="AA7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB7">
         <v>2</v>
@@ -1658,7 +1763,7 @@
         <v>2</v>
       </c>
       <c r="AE7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF7">
         <v>0</v>
@@ -1682,9 +1787,12 @@
         <v>0</v>
       </c>
       <c r="AM7">
-        <v>1</v>
-      </c>
-      <c r="AN7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>1</v>
+      </c>
+      <c r="AO7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1695,15 +1803,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF8"/>
+  <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1800,8 +1908,11 @@
       <c r="AF1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:32">
+      <c r="AG1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -1898,8 +2009,11 @@
       <c r="AF2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:32">
+      <c r="AG2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
       <c r="A3">
         <v>2006</v>
       </c>
@@ -1996,8 +2110,11 @@
       <c r="AF3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:32">
+      <c r="AG3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
       <c r="A4">
         <v>2007</v>
       </c>
@@ -2094,8 +2211,11 @@
       <c r="AF4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:32">
+      <c r="AG4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
       <c r="A5">
         <v>2008</v>
       </c>
@@ -2192,8 +2312,11 @@
       <c r="AF5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:32">
+      <c r="AG5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
       <c r="A6">
         <v>2009</v>
       </c>
@@ -2290,8 +2413,11 @@
       <c r="AF6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:32">
+      <c r="AG6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -2388,8 +2514,11 @@
       <c r="AF7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:32">
+      <c r="AG7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
       <c r="A8">
         <v>2013</v>
       </c>
@@ -2485,6 +2614,9 @@
       </c>
       <c r="AF8">
         <v>1000</v>
+      </c>
+      <c r="AG8">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2494,19 +2626,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="A3:H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -2531,8 +2666,40 @@
       <c r="H1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2554,8 +2721,14 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>0</v>
+      <c r="H3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K3">
+        <v>206</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ive implemented buyMode, and it works! I encountered a few little problems, including not processing the event on the first dialog message and not updating the inventoryView->playerItems. After that, everything worked as expected!
As an aside, the game would crash when I went to map 2 and it was the
enemy's turn-of course this was because there were no enemies and there
wasn't a empty-check. I added a check in the beginning of
enemyActionMode, and included the proper end/start cycle.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="810" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="118">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -365,9 +365,6 @@
   </si>
   <si>
     <t>Welcome! We've got the lowest prices!</t>
-  </si>
-  <si>
-    <t>What would you like?</t>
   </si>
   <si>
     <t>price</t>
@@ -705,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="A11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -863,44 +860,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>1005</v>
-      </c>
-      <c r="B12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20">
-        <v>1005</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -910,10 +870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO7"/>
+  <dimension ref="A1:AO9"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AO7"/>
+      <selection activeCell="A2" sqref="A2:AO9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -944,7 +904,7 @@
         <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I1" t="s">
         <v>38</v>
@@ -1794,6 +1754,256 @@
       </c>
       <c r="AO7" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41">
+      <c r="A8">
+        <v>207</v>
+      </c>
+      <c r="B8">
+        <v>3023</v>
+      </c>
+      <c r="C8">
+        <v>1102</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>255</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>255</v>
+      </c>
+      <c r="L8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41">
+      <c r="A9">
+        <v>207</v>
+      </c>
+      <c r="B9">
+        <v>3022</v>
+      </c>
+      <c r="C9">
+        <v>1104</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
+      </c>
+      <c r="I9">
+        <v>255</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>255</v>
+      </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1803,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG8"/>
+  <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1909,7 +2119,7 @@
         <v>104</v>
       </c>
       <c r="AG1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:33">
@@ -2617,6 +2827,107 @@
       </c>
       <c r="AG8">
         <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9">
+        <v>2013</v>
+      </c>
+      <c r="B9">
+        <v>207</v>
+      </c>
+      <c r="C9">
+        <v>255</v>
+      </c>
+      <c r="D9">
+        <v>70</v>
+      </c>
+      <c r="E9">
+        <v>255</v>
+      </c>
+      <c r="F9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>15</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>10</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>79</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>3</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>1004</v>
+      </c>
+      <c r="AG9">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2626,10 +2937,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2731,6 +3042,32 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:18">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>207</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed a bug with events; to prevent multiple event triggers, now the check for event logic comes before advanceDialog() -- since the first message is displayed without the advanceDialog() call, the event gets ignored until after the second message is loaded--now it functions properly.
I also added two new fields for events: dialogIDA and dialogIDB. These
will be the bread and butter of Checks - for example, I can create an
event which does a CHR roll to see if the player passes - if they
succeed, then go down dialogIDA path, else dialogIDB. 

After I add dialogs to the global registry, I will begin work on stats
and magic!
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -371,6 +371,12 @@
   </si>
   <si>
     <t>gold</t>
+  </si>
+  <si>
+    <t>dialogIDA</t>
+  </si>
+  <si>
+    <t>dialogIDB</t>
   </si>
 </sst>
 </file>
@@ -704,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="A11:F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2937,10 +2943,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2952,7 +2958,7 @@
     <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -2975,42 +2981,48 @@
         <v>106</v>
       </c>
       <c r="H1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" t="s">
         <v>108</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>109</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>110</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="K2" t="s">
+    <row r="2" spans="1:20">
+      <c r="M2" t="s">
         <v>31</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>113</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>31</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>113</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3032,17 +3044,23 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
         <v>114</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>206</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3065,6 +3083,12 @@
         <v>0</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tentative Commit: Ok, so I revamped the attacking system to be more like DnD, which was a  lot of business logic. Just a summary: I added stat mod to all items, this is because I needed to know how much STR would affect the attack (I actually have to change this to be a float, because I need to be able to do X.5 * STR calculations). min/max dam is actually the dice spread of the attack, not the absolute max/min. A search is done for a currently equipt weapon, if one is found, it uses the weapons min/max spread. otherwise, it defaults to the individuals min/max spread. A separate calculation is done for baseDam (also a new attribute for individuals), it includes the STR/weapon calculations, although not in the getAttributeSum() method. Updated other methods (createIndividual, createItem, etc.) to fit the above changes.
The logic is still far from finished, I wonder if it's too soon to worry
about dual wielding...
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="137">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -265,18 +265,9 @@
     <t>direction</t>
   </si>
   <si>
-    <t>totalHP</t>
-  </si>
-  <si>
     <t>totalActions</t>
   </si>
   <si>
-    <t>totalMana</t>
-  </si>
-  <si>
-    <t>ac</t>
-  </si>
-  <si>
     <t>attack</t>
   </si>
   <si>
@@ -377,6 +368,66 @@
   </si>
   <si>
     <t>dialogIDB</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>DEX</t>
+  </si>
+  <si>
+    <t>CON</t>
+  </si>
+  <si>
+    <t>WILL</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>WIS</t>
+  </si>
+  <si>
+    <t>CHR</t>
+  </si>
+  <si>
+    <t>LUCK</t>
+  </si>
+  <si>
+    <t>baseHP</t>
+  </si>
+  <si>
+    <t>baseMana</t>
+  </si>
+  <si>
+    <t>baseAC</t>
+  </si>
+  <si>
+    <t>baseDam</t>
+  </si>
+  <si>
+    <t>strMod</t>
+  </si>
+  <si>
+    <t>dexMod</t>
+  </si>
+  <si>
+    <t>conMod</t>
+  </si>
+  <si>
+    <t>willMod</t>
+  </si>
+  <si>
+    <t>intMod</t>
+  </si>
+  <si>
+    <t>wisMod</t>
+  </si>
+  <si>
+    <t>chrMod</t>
+  </si>
+  <si>
+    <t>luckMod</t>
   </si>
 </sst>
 </file>
@@ -710,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
@@ -854,7 +905,7 @@
         <v>1004</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -876,18 +927,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO9"/>
+  <dimension ref="A1:AW9"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AO9"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:49">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -910,7 +963,7 @@
         <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I1" t="s">
         <v>38</v>
@@ -931,88 +984,112 @@
         <v>43</v>
       </c>
       <c r="O1" t="s">
+        <v>129</v>
+      </c>
+      <c r="P1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" t="s">
+        <v>133</v>
+      </c>
+      <c r="T1" t="s">
+        <v>134</v>
+      </c>
+      <c r="U1" t="s">
+        <v>135</v>
+      </c>
+      <c r="V1" t="s">
+        <v>136</v>
+      </c>
+      <c r="W1" t="s">
         <v>44</v>
       </c>
-      <c r="P1" t="s">
+      <c r="X1" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Y1" t="s">
         <v>46</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Z1" t="s">
         <v>47</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AA1" t="s">
         <v>48</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AB1" t="s">
         <v>49</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AC1" t="s">
         <v>50</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AD1" t="s">
         <v>51</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AE1" t="s">
         <v>52</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AF1" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AG1" t="s">
         <v>54</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AH1" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AI1" t="s">
         <v>56</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AJ1" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AK1" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AL1" t="s">
         <v>59</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AM1" t="s">
         <v>60</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AN1" t="s">
         <v>61</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AO1" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AP1" t="s">
         <v>63</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AQ1" t="s">
         <v>64</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AR1" t="s">
         <v>65</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AS1" t="s">
         <v>66</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AT1" t="s">
         <v>67</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AU1" t="s">
         <v>68</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AV1" t="s">
         <v>69</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AW1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:49">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1056,7 +1133,7 @@
         <v>4</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1068,19 +1145,19 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <v>0</v>
@@ -1092,19 +1169,19 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF2">
         <v>0</v>
@@ -1133,11 +1210,35 @@
       <c r="AN2">
         <v>0</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:49">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1184,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1205,38 +1306,38 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <v>2</v>
       </c>
       <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>2</v>
+      </c>
+      <c r="AG3">
         <v>5</v>
       </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
       <c r="AH3">
         <v>0</v>
       </c>
@@ -1258,11 +1359,35 @@
       <c r="AN3">
         <v>0</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:49">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1315,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -1339,7 +1464,7 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA4">
         <v>0</v>
@@ -1383,11 +1508,35 @@
       <c r="AN4">
         <v>0</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:49">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1434,32 +1583,32 @@
         <v>0</v>
       </c>
       <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
         <v>10</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
       <c r="Y5">
         <v>0</v>
       </c>
@@ -1508,11 +1657,35 @@
       <c r="AN5">
         <v>0</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:49">
       <c r="A6">
         <v>200</v>
       </c>
@@ -1556,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1568,19 +1741,19 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -1592,19 +1765,19 @@
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF6">
         <v>0</v>
@@ -1631,13 +1804,37 @@
         <v>0</v>
       </c>
       <c r="AN6">
-        <v>1</v>
-      </c>
-      <c r="AO6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>1</v>
+      </c>
+      <c r="AW6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:49">
       <c r="A7">
         <v>200</v>
       </c>
@@ -1720,16 +1917,16 @@
         <v>0</v>
       </c>
       <c r="AB7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF7">
         <v>0</v>
@@ -1744,25 +1941,49 @@
         <v>0</v>
       </c>
       <c r="AJ7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN7">
-        <v>1</v>
-      </c>
-      <c r="AO7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>1</v>
+      </c>
+      <c r="AW7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:49">
       <c r="A8">
         <v>207</v>
       </c>
@@ -1815,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -1839,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA8">
         <v>0</v>
@@ -1883,11 +2104,35 @@
       <c r="AN8">
         <v>0</v>
       </c>
-      <c r="AO8" t="s">
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:49">
       <c r="A9">
         <v>207</v>
       </c>
@@ -1934,32 +2179,32 @@
         <v>0</v>
       </c>
       <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
         <v>10</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
       <c r="Y9">
         <v>0</v>
       </c>
@@ -2008,7 +2253,31 @@
       <c r="AN9">
         <v>0</v>
       </c>
-      <c r="AO9" t="s">
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
+      <c r="AW9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2019,15 +2288,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AP9"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:AG9"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:42">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -2056,79 +2325,106 @@
         <v>43</v>
       </c>
       <c r="J1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S1" t="s">
         <v>82</v>
       </c>
-      <c r="K1" t="s">
+      <c r="T1" t="s">
+        <v>126</v>
+      </c>
+      <c r="U1" t="s">
+        <v>127</v>
+      </c>
+      <c r="V1" t="s">
         <v>83</v>
       </c>
-      <c r="L1" t="s">
+      <c r="W1" t="s">
         <v>84</v>
       </c>
-      <c r="M1" t="s">
+      <c r="X1" t="s">
         <v>85</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Y1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z1" t="s">
         <v>86</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AA1" t="s">
         <v>87</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AC1" t="s">
         <v>89</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AD1" t="s">
         <v>90</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AE1" t="s">
         <v>91</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AF1" t="s">
         <v>92</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AG1" t="s">
         <v>93</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AH1" t="s">
         <v>94</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AI1" t="s">
         <v>95</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AJ1" t="s">
         <v>96</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AK1" t="s">
         <v>97</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AL1" t="s">
         <v>98</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AM1" t="s">
         <v>99</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AN1" t="s">
         <v>100</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AO1" t="s">
         <v>101</v>
       </c>
-      <c r="AD1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>117</v>
+      <c r="AP1" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:42">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -2157,62 +2453,62 @@
         <v>0</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>8</v>
       </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2">
+      <c r="S2">
+        <v>2</v>
+      </c>
+      <c r="T2">
         <v>6</v>
       </c>
-      <c r="M2">
+      <c r="U2">
         <v>8</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
         <v>3</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
         <v>72</v>
       </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
         <v>3</v>
       </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
       <c r="AC2">
         <v>0</v>
       </c>
@@ -2226,10 +2522,37 @@
         <v>0</v>
       </c>
       <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:42">
       <c r="A3">
         <v>2006</v>
       </c>
@@ -2258,62 +2581,62 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3">
         <v>8</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
         <v>3</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s">
         <v>72</v>
       </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
         <v>3</v>
       </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
       <c r="AC3">
         <v>0</v>
       </c>
@@ -2327,10 +2650,37 @@
         <v>0</v>
       </c>
       <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:42">
       <c r="A4">
         <v>2007</v>
       </c>
@@ -2359,62 +2709,62 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
+      <c r="U4">
         <v>8</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
         <v>3</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s">
         <v>72</v>
       </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
         <v>3</v>
       </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
       <c r="AC4">
         <v>0</v>
       </c>
@@ -2428,10 +2778,37 @@
         <v>0</v>
       </c>
       <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:42">
       <c r="A5">
         <v>2008</v>
       </c>
@@ -2460,62 +2837,62 @@
         <v>3</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>2</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5">
         <v>8</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
         <v>3</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
         <v>72</v>
       </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
         <v>3</v>
       </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
       <c r="AC5">
         <v>0</v>
       </c>
@@ -2529,10 +2906,37 @@
         <v>0</v>
       </c>
       <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:42">
       <c r="A6">
         <v>2009</v>
       </c>
@@ -2561,62 +2965,62 @@
         <v>3</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>2</v>
+      </c>
+      <c r="T6">
+        <v>2</v>
+      </c>
+      <c r="U6">
         <v>8</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
         <v>3</v>
       </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s">
         <v>72</v>
       </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
         <v>3</v>
       </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
       <c r="AC6">
         <v>0</v>
       </c>
@@ -2630,10 +3034,37 @@
         <v>0</v>
       </c>
       <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:42">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -2662,62 +3093,62 @@
         <v>15</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7">
         <v>8</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
         <v>3</v>
       </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s">
         <v>72</v>
       </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
         <v>3</v>
       </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
       <c r="AC7">
         <v>0</v>
       </c>
@@ -2731,10 +3162,37 @@
         <v>0</v>
       </c>
       <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:42">
       <c r="A8">
         <v>2013</v>
       </c>
@@ -2763,62 +3221,62 @@
         <v>2</v>
       </c>
       <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
         <v>15</v>
       </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
-      <c r="L8">
+      <c r="S8">
+        <v>2</v>
+      </c>
+      <c r="T8">
         <v>10</v>
       </c>
-      <c r="M8">
+      <c r="U8">
         <v>10</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
         <v>5</v>
       </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="s">
         <v>79</v>
       </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8">
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
         <v>3</v>
       </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
       <c r="AC8">
         <v>0</v>
       </c>
@@ -2829,13 +3287,40 @@
         <v>0</v>
       </c>
       <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
         <v>1000</v>
       </c>
-      <c r="AG8">
+      <c r="AP8">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:42">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -2864,62 +3349,62 @@
         <v>2</v>
       </c>
       <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
         <v>15</v>
       </c>
-      <c r="K9">
-        <v>2</v>
-      </c>
-      <c r="L9">
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9">
         <v>10</v>
       </c>
-      <c r="M9">
+      <c r="U9">
         <v>10</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
         <v>5</v>
       </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="s">
         <v>79</v>
       </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9">
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
         <v>3</v>
       </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9">
-        <v>0</v>
-      </c>
       <c r="AC9">
         <v>0</v>
       </c>
@@ -2930,9 +3415,36 @@
         <v>0</v>
       </c>
       <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
         <v>1004</v>
       </c>
-      <c r="AG9">
+      <c r="AP9">
         <v>100</v>
       </c>
     </row>
@@ -2966,7 +3478,7 @@
         <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
         <v>31</v>
@@ -2975,31 +3487,31 @@
         <v>32</v>
       </c>
       <c r="F1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>106</v>
       </c>
-      <c r="H1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" t="s">
         <v>108</v>
       </c>
-      <c r="L1" t="s">
+      <c r="S1" t="s">
         <v>109</v>
-      </c>
-      <c r="M1" t="s">
-        <v>110</v>
-      </c>
-      <c r="P1" t="s">
-        <v>111</v>
-      </c>
-      <c r="S1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -3007,19 +3519,19 @@
         <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="P2" t="s">
         <v>31</v>
       </c>
       <c r="Q2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S2" t="s">
         <v>31</v>
       </c>
       <c r="T2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -3051,7 +3563,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M3">
         <v>206</v>

</xml_diff>

<commit_message>
More progress - I implemented a new item parameter to keep track of the weapons STR modifier, I also fixed the tests and a bug with creating a simpleDialog.
I did encounter some annoying issues while doing this; atoi() returns a
int, guess what atof() returns? that's right, a double. I was assigning
it to a float, which was creating some bizarre issues when I was passing
it in as a parameter--it would shove all the other parameters 'down one'
so to speak, and strangely it didn't cause everything to crash. C is a
wonderful tool which can do a lot, but has very few guards.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="138">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>luckMod</t>
+  </si>
+  <si>
+    <t>weaponStrMod</t>
   </si>
 </sst>
 </file>
@@ -927,10 +930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW9"/>
+  <dimension ref="A1:AX9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AH12" sqref="AH12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -938,9 +941,10 @@
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:50">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -984,112 +988,115 @@
         <v>43</v>
       </c>
       <c r="O1" t="s">
+        <v>137</v>
+      </c>
+      <c r="P1" t="s">
         <v>129</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>130</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>131</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>132</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>133</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>134</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>135</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>136</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>44</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>47</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>51</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>52</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>53</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>54</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>55</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>56</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>57</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>58</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>59</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>60</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>61</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>62</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>63</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>64</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>65</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>66</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>67</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>68</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>69</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:50">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1169,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2">
         <v>1</v>
@@ -1184,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="AF2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG2">
         <v>0</v>
@@ -1234,11 +1241,14 @@
       <c r="AV2">
         <v>0</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:50">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1309,10 +1319,10 @@
         <v>0</v>
       </c>
       <c r="X3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z3">
         <v>0</v>
@@ -1330,17 +1340,17 @@
         <v>0</v>
       </c>
       <c r="AE3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG3">
+        <v>2</v>
+      </c>
+      <c r="AH3">
         <v>5</v>
       </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
       <c r="AI3">
         <v>0</v>
       </c>
@@ -1383,11 +1393,14 @@
       <c r="AV3">
         <v>0</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:50">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1464,10 +1477,10 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB4">
         <v>0</v>
@@ -1532,11 +1545,14 @@
       <c r="AV4">
         <v>0</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:50">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1607,11 +1623,11 @@
         <v>0</v>
       </c>
       <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
         <v>10</v>
       </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
       <c r="Z5">
         <v>0</v>
       </c>
@@ -1681,11 +1697,14 @@
       <c r="AV5">
         <v>0</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:50">
       <c r="A6">
         <v>200</v>
       </c>
@@ -1765,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <v>1</v>
@@ -1780,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="AF6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6">
         <v>0</v>
@@ -1828,13 +1847,16 @@
         <v>0</v>
       </c>
       <c r="AV6">
-        <v>1</v>
-      </c>
-      <c r="AW6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>1</v>
+      </c>
+      <c r="AX6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:49">
+    <row r="7" spans="1:50">
       <c r="A7">
         <v>200</v>
       </c>
@@ -1941,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="AJ7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK7">
         <v>2</v>
@@ -1953,7 +1975,7 @@
         <v>2</v>
       </c>
       <c r="AN7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO7">
         <v>0</v>
@@ -1977,13 +1999,16 @@
         <v>0</v>
       </c>
       <c r="AV7">
-        <v>1</v>
-      </c>
-      <c r="AW7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>1</v>
+      </c>
+      <c r="AX7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:50">
       <c r="A8">
         <v>207</v>
       </c>
@@ -2060,10 +2085,10 @@
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB8">
         <v>0</v>
@@ -2128,11 +2153,14 @@
       <c r="AV8">
         <v>0</v>
       </c>
-      <c r="AW8" t="s">
+      <c r="AW8">
+        <v>0</v>
+      </c>
+      <c r="AX8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:50">
       <c r="A9">
         <v>207</v>
       </c>
@@ -2203,11 +2231,11 @@
         <v>0</v>
       </c>
       <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
         <v>10</v>
       </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
       <c r="Z9">
         <v>0</v>
       </c>
@@ -2277,7 +2305,10 @@
       <c r="AV9">
         <v>0</v>
       </c>
-      <c r="AW9" t="s">
+      <c r="AW9">
+        <v>0</v>
+      </c>
+      <c r="AX9" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I've implemented a new event: stat checking. It's technically agnostic to any attribute the individual has, so it could be used for anything. It's fairly basic, the event has a number to check against, and a success/fail dialog. The resulting dialog is set to the currentMessage->nextMessage (however the currentMessage must have a null nextMessage value to prevent misuse). I've updated the tests for this as well.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
     <sheet name="Items" sheetId="2" r:id="rId2"/>
     <sheet name="Individuals" sheetId="3" r:id="rId3"/>
     <sheet name="Events" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="213">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -28,9 +29,6 @@
     <t>I agree - I found them in the graveyard to the east.</t>
   </si>
   <si>
-    <t>Hmph. It's better than what you have.</t>
-  </si>
-  <si>
     <t>Yes - they are quite flattering, fit for a wealthy noble</t>
   </si>
   <si>
@@ -352,9 +350,6 @@
     <t>EventID</t>
   </si>
   <si>
-    <t>"Have at you!"</t>
-  </si>
-  <si>
     <t>Welcome! We've got the lowest prices!</t>
   </si>
   <si>
@@ -431,6 +426,237 @@
   </si>
   <si>
     <t>weaponStrMod</t>
+  </si>
+  <si>
+    <t>createItem(npcID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> imageID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RGB(r</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> description</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dexMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> conMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> willMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> intMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wisMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chrMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> luckMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> armorClass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> itemType</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> price</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> minTurns</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> maxTurns</t>
+  </si>
+  <si>
+    <t>lightningDRMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lightiningWeaknessMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> isEquipt);</t>
+  </si>
+  <si>
+    <t>createItem(int npcID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int imageID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COLORREF rgb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int x</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> char type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> char name[32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> char description[256]</t>
+  </si>
+  <si>
+    <t>float weaponStrMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int strMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int dexMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int conMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int willMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int intMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int wisMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int chrMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int luckMod</t>
+  </si>
+  <si>
+    <t>char weaponDamageType</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> char armorClass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> char itemType</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int price</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int totalHealthMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int healthMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int totalManaMod</t>
+  </si>
+  <si>
+    <t>int manaMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int acMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int attackMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int damMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int maxDamMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int minDamMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int minTurns</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int maxTurns</t>
+  </si>
+  <si>
+    <t>int mvmtMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int rangeMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int bluntDRMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int chopDRMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int slashDRMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int pierceDRMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int earthDRMod</t>
+  </si>
+  <si>
+    <t>int fireDRMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int waterDRMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int lightningDRMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int earthWeaknessMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int fireWeaknessMod</t>
+  </si>
+  <si>
+    <t>int waterWeaknessMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int lightiningWeaknessMod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int isEquipt){</t>
+  </si>
+  <si>
+    <t>Dingy?! Are you trying to rile me?</t>
+  </si>
+  <si>
+    <t>Yes! Have at you, poorly dressed mongrel!</t>
+  </si>
+  <si>
+    <t>Have at you!</t>
+  </si>
+  <si>
+    <t>No! I'm mearly trying to infrom you as a friend! (CHR Check)</t>
+  </si>
+  <si>
+    <t>(CHR check)</t>
+  </si>
+  <si>
+    <t>Ah - forgive me for my agression. It takes a stronger man to say the honest thing.</t>
+  </si>
+  <si>
+    <t>Map 2</t>
   </si>
 </sst>
 </file>
@@ -466,8 +692,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,15 +989,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -778,27 +1005,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -866,10 +1093,10 @@
         <v>1003</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>206</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -878,48 +1105,135 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>1001</v>
+        <v>1006</v>
       </c>
       <c r="B7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>4</v>
-      </c>
-      <c r="C7">
-        <v>1002</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>1001</v>
+        <v>1005</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>208</v>
       </c>
       <c r="C8">
-        <v>1003</v>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>1007</v>
+      </c>
+      <c r="B9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
+        <v>1001</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>1001</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>1003</v>
+      </c>
+      <c r="B13" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>1003</v>
+      </c>
+      <c r="B14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C14">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
         <v>1004</v>
       </c>
-      <c r="B11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>1005</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
         <v>3</v>
       </c>
     </row>
@@ -932,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AX9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -946,154 +1260,154 @@
   <sheetData>
     <row r="1" spans="1:50">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>42</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>135</v>
+      </c>
+      <c r="P1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R1" t="s">
+        <v>129</v>
+      </c>
+      <c r="S1" t="s">
+        <v>130</v>
+      </c>
+      <c r="T1" t="s">
+        <v>131</v>
+      </c>
+      <c r="U1" t="s">
+        <v>132</v>
+      </c>
+      <c r="V1" t="s">
+        <v>133</v>
+      </c>
+      <c r="W1" t="s">
+        <v>134</v>
+      </c>
+      <c r="X1" t="s">
         <v>43</v>
       </c>
-      <c r="O1" t="s">
-        <v>137</v>
-      </c>
-      <c r="P1" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>130</v>
-      </c>
-      <c r="R1" t="s">
-        <v>131</v>
-      </c>
-      <c r="S1" t="s">
-        <v>132</v>
-      </c>
-      <c r="T1" t="s">
-        <v>133</v>
-      </c>
-      <c r="U1" t="s">
-        <v>134</v>
-      </c>
-      <c r="V1" t="s">
-        <v>135</v>
-      </c>
-      <c r="W1" t="s">
-        <v>136</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>48</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>49</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>50</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>51</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>52</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>53</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>54</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>55</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>58</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>59</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>60</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>61</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>62</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>63</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>64</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>65</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>66</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>67</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>68</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>69</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:50">
@@ -1107,16 +1421,16 @@
         <v>1100</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
       </c>
       <c r="H2">
         <v>25</v>
@@ -1131,7 +1445,7 @@
         <v>255</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M2">
         <v>3</v>
@@ -1140,7 +1454,7 @@
         <v>4</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1188,7 +1502,7 @@
         <v>1</v>
       </c>
       <c r="AE2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AF2">
         <v>1</v>
@@ -1245,7 +1559,7 @@
         <v>0</v>
       </c>
       <c r="AX2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:50">
@@ -1259,16 +1573,16 @@
         <v>1101</v>
       </c>
       <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -1283,7 +1597,7 @@
         <v>255</v>
       </c>
       <c r="L3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M3">
         <v>3</v>
@@ -1397,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="AX3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:50">
@@ -1411,16 +1725,16 @@
         <v>1102</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
       </c>
       <c r="H4">
         <v>20</v>
@@ -1435,7 +1749,7 @@
         <v>255</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -1549,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="AX4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:50">
@@ -1563,16 +1877,16 @@
         <v>1104</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
       </c>
       <c r="H5">
         <v>15</v>
@@ -1587,7 +1901,7 @@
         <v>255</v>
       </c>
       <c r="L5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M5">
         <v>2</v>
@@ -1701,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="AX5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:50">
@@ -1715,16 +2029,16 @@
         <v>1001</v>
       </c>
       <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
       </c>
       <c r="H6">
         <v>25</v>
@@ -1739,7 +2053,7 @@
         <v>255</v>
       </c>
       <c r="L6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1748,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1796,7 +2110,7 @@
         <v>1</v>
       </c>
       <c r="AE6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AF6">
         <v>1</v>
@@ -1853,7 +2167,7 @@
         <v>1</v>
       </c>
       <c r="AX6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:50">
@@ -1867,16 +2181,16 @@
         <v>1002</v>
       </c>
       <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7">
         <v>50</v>
@@ -1891,7 +2205,7 @@
         <v>255</v>
       </c>
       <c r="L7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -2005,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="AX7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:50">
@@ -2019,16 +2333,16 @@
         <v>1102</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
       </c>
       <c r="H8">
         <v>20</v>
@@ -2043,7 +2357,7 @@
         <v>255</v>
       </c>
       <c r="L8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -2157,7 +2471,7 @@
         <v>0</v>
       </c>
       <c r="AX8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:50">
@@ -2171,16 +2485,16 @@
         <v>1104</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
       </c>
       <c r="H9">
         <v>15</v>
@@ -2195,7 +2509,7 @@
         <v>255</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -2309,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="AX9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2321,138 +2635,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:42">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" t="s">
+        <v>119</v>
+      </c>
+      <c r="O1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>122</v>
+      </c>
+      <c r="R1" t="s">
+        <v>123</v>
+      </c>
+      <c r="S1" t="s">
         <v>81</v>
       </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" t="s">
-        <v>117</v>
-      </c>
-      <c r="K1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" t="s">
-        <v>122</v>
-      </c>
-      <c r="P1" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>124</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>125</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>82</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
+        <v>83</v>
+      </c>
+      <c r="X1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y1" t="s">
         <v>126</v>
       </c>
-      <c r="U1" t="s">
-        <v>127</v>
-      </c>
-      <c r="V1" t="s">
-        <v>83</v>
-      </c>
-      <c r="W1" t="s">
-        <v>84</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>85</v>
       </c>
-      <c r="Y1" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>86</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>87</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>88</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>89</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>90</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>91</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>92</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>93</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>94</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>95</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>96</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>97</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>98</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>99</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>100</v>
       </c>
-      <c r="AO1" t="s">
-        <v>101</v>
-      </c>
       <c r="AP1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:42">
@@ -2472,7 +2786,7 @@
         <v>255</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2532,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="Z2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -2600,7 +2914,7 @@
         <v>255</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -2660,7 +2974,7 @@
         <v>0</v>
       </c>
       <c r="Z3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -2728,7 +3042,7 @@
         <v>255</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2788,7 +3102,7 @@
         <v>0</v>
       </c>
       <c r="Z4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -2856,7 +3170,7 @@
         <v>255</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -2916,7 +3230,7 @@
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -2984,7 +3298,7 @@
         <v>255</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -3044,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA6">
         <v>1</v>
@@ -3112,7 +3426,7 @@
         <v>255</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -3172,7 +3486,7 @@
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA7">
         <v>1</v>
@@ -3240,7 +3554,7 @@
         <v>255</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -3300,7 +3614,7 @@
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA8">
         <v>1</v>
@@ -3368,7 +3682,7 @@
         <v>255</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -3428,7 +3742,7 @@
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA9">
         <v>1</v>
@@ -3486,10 +3800,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3503,66 +3817,96 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I1" t="s">
-        <v>116</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>105</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>106</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>107</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>108</v>
-      </c>
-      <c r="S1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:20">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>206</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -3594,7 +3938,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>111</v>
+        <v>208</v>
       </c>
       <c r="M3">
         <v>206</v>
@@ -3633,6 +3977,345 @@
       </c>
       <c r="J4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>206</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1007</v>
+      </c>
+      <c r="I5">
+        <v>1005</v>
+      </c>
+      <c r="J5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AV2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:48">
+      <c r="A1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M1" t="s">
+        <v>144</v>
+      </c>
+      <c r="N1" t="s">
+        <v>145</v>
+      </c>
+      <c r="O1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>148</v>
+      </c>
+      <c r="R1" t="s">
+        <v>149</v>
+      </c>
+      <c r="S1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" t="s">
+        <v>150</v>
+      </c>
+      <c r="U1" t="s">
+        <v>151</v>
+      </c>
+      <c r="V1" t="s">
+        <v>152</v>
+      </c>
+      <c r="W1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48">
+      <c r="A2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" t="s">
+        <v>168</v>
+      </c>
+      <c r="L2" t="s">
+        <v>169</v>
+      </c>
+      <c r="M2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N2" t="s">
+        <v>171</v>
+      </c>
+      <c r="O2" t="s">
+        <v>172</v>
+      </c>
+      <c r="P2" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>174</v>
+      </c>
+      <c r="R2" t="s">
+        <v>175</v>
+      </c>
+      <c r="S2" t="s">
+        <v>176</v>
+      </c>
+      <c r="T2" t="s">
+        <v>177</v>
+      </c>
+      <c r="U2" t="s">
+        <v>178</v>
+      </c>
+      <c r="V2" t="s">
+        <v>179</v>
+      </c>
+      <c r="W2" t="s">
+        <v>180</v>
+      </c>
+      <c r="X2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>188</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>192</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Back in the saddle! I've been putting this off because I hadn't thought of a good way to design a solution, however I think that I've got a reasonable prototype. I'm committing the structs that will be used: How it works is the individual will make an Ability which is composed of several Effects, and the Effects are made up from a collection of Properties.
For example, there can be two defined Effects (say fireball and burn)
which utilize different properties. Fireball can use Range, DiceDamage,
and targeted, while burn uses DiceDamage and Duration. The User could
make a 'Burning Fireball' ability which has a range of 5 spaces and
damages the target 1d8, while causing 1d4 burn for 1d4 turns.

Mana cost will be calculated for each of the effects, taking into logic
such as 'if there's DiceDamage and Duration effects, mana += DiceDamage
* Duration'.

I've still got plenty more to add, however I want to commit what I have
for now.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="213">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -1244,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX9"/>
+  <dimension ref="A1:AX10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1418,7 +1418,7 @@
         <v>3020</v>
       </c>
       <c r="C2">
-        <v>1100</v>
+        <v>1001</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1570,7 +1570,7 @@
         <v>3021</v>
       </c>
       <c r="C3">
-        <v>1101</v>
+        <v>1002</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -1722,7 +1722,7 @@
         <v>3023</v>
       </c>
       <c r="C4">
-        <v>1102</v>
+        <v>1003</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -1874,7 +1874,7 @@
         <v>3022</v>
       </c>
       <c r="C5">
-        <v>1104</v>
+        <v>1004</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -2026,7 +2026,7 @@
         <v>3020</v>
       </c>
       <c r="C6">
-        <v>1001</v>
+        <v>1005</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -2178,7 +2178,7 @@
         <v>3020</v>
       </c>
       <c r="C7">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="D7" t="s">
         <v>26</v>
@@ -2330,7 +2330,7 @@
         <v>3023</v>
       </c>
       <c r="C8">
-        <v>1102</v>
+        <v>1007</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -2482,7 +2482,7 @@
         <v>3022</v>
       </c>
       <c r="C9">
-        <v>1104</v>
+        <v>1008</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -2624,6 +2624,158 @@
       </c>
       <c r="AX9" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>3020</v>
+      </c>
+      <c r="C10">
+        <v>1009</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>25</v>
+      </c>
+      <c r="I10">
+        <v>255</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>255</v>
+      </c>
+      <c r="L10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>1.5</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10">
+        <v>1</v>
+      </c>
+      <c r="AE10">
+        <v>6</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>0</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3802,8 +3954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="A2:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Committing what I have for now: I'm laying down more of the ground work, specifically how abilities and effects are going to be loaded and exist in the global registry. Basically, the template effects as used by the individual will be placed in the registry, as well as modified effects which will be used for pre-made npc abilities. My next step is to create the template effects by line, and add them to the registry.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
     <sheet name="Items" sheetId="2" r:id="rId2"/>
     <sheet name="Individuals" sheetId="3" r:id="rId3"/>
     <sheet name="Events" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Effects" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="169">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -428,216 +428,6 @@
     <t>weaponStrMod</t>
   </si>
   <si>
-    <t>createItem(npcID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> imageID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RGB(r</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> type</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> name</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> description</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dexMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> conMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> willMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> intMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> wisMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> chrMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> luckMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> armorClass</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> itemType</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> price</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> minTurns</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> maxTurns</t>
-  </si>
-  <si>
-    <t>lightningDRMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lightiningWeaknessMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> isEquipt);</t>
-  </si>
-  <si>
-    <t>createItem(int npcID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int imageID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> COLORREF rgb</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int x</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int y</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> char type</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> char name[32]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> char description[256]</t>
-  </si>
-  <si>
-    <t>float weaponStrMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int strMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int dexMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int conMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int willMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int intMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int wisMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int chrMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int luckMod</t>
-  </si>
-  <si>
-    <t>char weaponDamageType</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> char armorClass</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> char itemType</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int price</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int totalHealthMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int healthMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int totalManaMod</t>
-  </si>
-  <si>
-    <t>int manaMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int acMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int attackMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int damMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int maxDamMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int minDamMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int minTurns</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int maxTurns</t>
-  </si>
-  <si>
-    <t>int mvmtMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int rangeMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int bluntDRMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int chopDRMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int slashDRMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int pierceDRMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int earthDRMod</t>
-  </si>
-  <si>
-    <t>int fireDRMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int waterDRMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int lightningDRMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int earthWeaknessMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int fireWeaknessMod</t>
-  </si>
-  <si>
-    <t>int waterWeaknessMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int lightiningWeaknessMod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> int isEquipt){</t>
-  </si>
-  <si>
     <t>Dingy?! Are you trying to rile me?</t>
   </si>
   <si>
@@ -657,13 +447,91 @@
   </si>
   <si>
     <t>Map 2</t>
+  </si>
+  <si>
+    <t>damageTypeEnabled</t>
+  </si>
+  <si>
+    <t>damageType</t>
+  </si>
+  <si>
+    <t>rangeEnabled</t>
+  </si>
+  <si>
+    <t>targetedEnabled</t>
+  </si>
+  <si>
+    <t>targeted</t>
+  </si>
+  <si>
+    <t>diceDamageEnabled</t>
+  </si>
+  <si>
+    <t>diceDamage</t>
+  </si>
+  <si>
+    <t>diceDamagedurationEnabled</t>
+  </si>
+  <si>
+    <t>diceDamageDuration</t>
+  </si>
+  <si>
+    <t>acEnabled</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>damageModEnabled</t>
+  </si>
+  <si>
+    <t>damageMod</t>
+  </si>
+  <si>
+    <t>bluntDREnabled</t>
+  </si>
+  <si>
+    <t>chopDREnabled</t>
+  </si>
+  <si>
+    <t>pierceDREnabled</t>
+  </si>
+  <si>
+    <t>slashDREnabled</t>
+  </si>
+  <si>
+    <t>Fireball</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>1,0,10,1,20,2,30,3</t>
+  </si>
+  <si>
+    <t>0,-1,1,0</t>
+  </si>
+  <si>
+    <t>4,1,6,2,8,3,10,4,12,5</t>
+  </si>
+  <si>
+    <t>0,0,1,1,2,2,3,3,4,4,5,5,6,6,7,7,8,8,9,9,10,10</t>
+  </si>
+  <si>
+    <t>Burn</t>
+  </si>
+  <si>
+    <t>Duration effect: fire damage over time</t>
+  </si>
+  <si>
+    <t>Targeted effect: a flying ball of fire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,16 +539,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -688,13 +570,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1093,7 +998,7 @@
         <v>1003</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>136</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1113,7 +1018,7 @@
         <v>1006</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1133,7 +1038,7 @@
         <v>1005</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>138</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1153,7 +1058,7 @@
         <v>1007</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>141</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1195,7 +1100,7 @@
         <v>1003</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>137</v>
       </c>
       <c r="C13">
         <v>1005</v>
@@ -1206,7 +1111,7 @@
         <v>1003</v>
       </c>
       <c r="B14" t="s">
-        <v>209</v>
+        <v>139</v>
       </c>
       <c r="C14">
         <v>1006</v>
@@ -1214,7 +1119,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>212</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1246,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AX10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4090,7 +3995,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>208</v>
+        <v>138</v>
       </c>
       <c r="M3">
         <v>206</v>
@@ -4170,307 +4075,296 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AV2"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:48">
-      <c r="A1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J1" t="s">
-        <v>135</v>
-      </c>
-      <c r="K1" t="s">
-        <v>127</v>
-      </c>
-      <c r="L1" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="4" customFormat="1">
+      <c r="A3" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="M1" t="s">
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="N1" t="s">
+      <c r="B4" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="O1" t="s">
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="P1" t="s">
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="B8" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="R1" t="s">
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="S1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="B10" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="U1" t="s">
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="V1" t="s">
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="W1" t="s">
-        <v>43</v>
-      </c>
-      <c r="X1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="AH1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ1" t="s">
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="AR1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU1" t="s">
+      <c r="B16" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:48">
-      <c r="A2" s="1" t="s">
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B21" s="5">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G2" t="s">
-        <v>164</v>
-      </c>
-      <c r="H2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="K2" t="s">
-        <v>168</v>
-      </c>
-      <c r="L2" t="s">
-        <v>169</v>
-      </c>
-      <c r="M2" t="s">
-        <v>170</v>
-      </c>
-      <c r="N2" t="s">
-        <v>171</v>
-      </c>
-      <c r="O2" t="s">
-        <v>172</v>
-      </c>
-      <c r="P2" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>174</v>
-      </c>
-      <c r="R2" t="s">
-        <v>175</v>
-      </c>
-      <c r="S2" t="s">
-        <v>176</v>
-      </c>
-      <c r="T2" t="s">
-        <v>177</v>
-      </c>
-      <c r="U2" t="s">
-        <v>178</v>
-      </c>
-      <c r="V2" t="s">
-        <v>179</v>
-      </c>
-      <c r="W2" t="s">
-        <v>180</v>
-      </c>
-      <c r="X2" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>183</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>186</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>187</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>188</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>189</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>190</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>191</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>192</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>193</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>194</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>195</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>198</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>200</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>201</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>202</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>204</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>205</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I will say this about it, the global registry system's pretty alright to use. I was able to implement 'Effects' very quickly - now I have loading/adding functions for the GR - it's all over but the parsing.
Speaking of which, I added a bunch of fields to the effect struct, and
I've managed to get everything into a semi-colon delimited line. Now I
just gotta open the file and parse it, which hopefully wont be too much
of a chore.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="187">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -525,6 +525,60 @@
   </si>
   <si>
     <t>Targeted effect: a flying ball of fire</t>
+  </si>
+  <si>
+    <t>STREnabled</t>
+  </si>
+  <si>
+    <t>LUCKEnabled</t>
+  </si>
+  <si>
+    <t>CHREnabled</t>
+  </si>
+  <si>
+    <t>WISEnabled</t>
+  </si>
+  <si>
+    <t>INTEnabled</t>
+  </si>
+  <si>
+    <t>WILLEnabled</t>
+  </si>
+  <si>
+    <t>CONEnabled</t>
+  </si>
+  <si>
+    <t>DEXEnabled</t>
+  </si>
+  <si>
+    <t>totalHP</t>
+  </si>
+  <si>
+    <t>totalHPEnabled</t>
+  </si>
+  <si>
+    <t>manaEnabled</t>
+  </si>
+  <si>
+    <t>mana</t>
+  </si>
+  <si>
+    <t>hpEnabled</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>earthDREnabled</t>
+  </si>
+  <si>
+    <t>fireDREnabled</t>
+  </si>
+  <si>
+    <t>waterDREnabled</t>
+  </si>
+  <si>
+    <t>lightningDREnabled</t>
   </si>
 </sst>
 </file>
@@ -4075,10 +4129,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4092,10 +4146,10 @@
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="4">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4">
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4222,18 +4276,18 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="B13" s="5">
         <v>0</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
@@ -4244,21 +4298,21 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>165</v>
+        <v>116</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
       </c>
       <c r="C16" s="5">
         <v>0</v>
@@ -4266,18 +4320,18 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="B17" s="5">
         <v>0</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="B18" s="5">
         <v>0</v>
@@ -4288,18 +4342,18 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="B19" s="5">
         <v>0</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="B20" s="5">
         <v>0</v>
@@ -4310,18 +4364,18 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="B21" s="5">
         <v>0</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="B22" s="5">
         <v>0</v>
@@ -4332,18 +4386,18 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B23" s="5">
         <v>0</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="B24" s="5">
         <v>0</v>
@@ -4354,12 +4408,342 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="5">
+        <v>0</v>
+      </c>
+      <c r="C33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0</v>
+      </c>
+      <c r="C34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0</v>
+      </c>
+      <c r="C37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="5">
+        <v>0</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="5">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0</v>
+      </c>
+      <c r="C42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43" s="5">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="5">
+        <v>0</v>
+      </c>
+      <c r="C44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0</v>
+      </c>
+      <c r="C46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0</v>
+      </c>
+      <c r="C47" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0</v>
+      </c>
+      <c r="C48" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0</v>
+      </c>
+      <c r="C49" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0</v>
+      </c>
+      <c r="C50" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B51" s="5">
+        <v>0</v>
+      </c>
+      <c r="C51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="5">
+        <v>0</v>
+      </c>
+      <c r="C52" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B53" s="5">
+        <v>0</v>
+      </c>
+      <c r="C53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0</v>
+      </c>
+      <c r="C54" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B55" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Well you learn something new every day - today I learned that strtok is a crappy function, because it cannot be performed more than once at a time on different strings. Evidently, it uses a global variable to keep track of which string it's tokenizing, so if you interrupt it with another, it will change that variable and ruin everything.
Today I welcome Charlie Gorden's strtok_r function (one I may re-write
for learning's sake). It takes in a character pointer which stores the
remaining string, and is used everytime strtok_r is called for that
particular string. Quite handy - and it fixes my delema with loading the
Effect (which is now working).
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="214">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -557,12 +557,6 @@
     <t>totalHPEnabled</t>
   </si>
   <si>
-    <t>manaEnabled</t>
-  </si>
-  <si>
-    <t>mana</t>
-  </si>
-  <si>
     <t>hpEnabled</t>
   </si>
   <si>
@@ -579,6 +573,93 @@
   </si>
   <si>
     <t>lightningDREnabled</t>
+  </si>
+  <si>
+    <t>totalMana</t>
+  </si>
+  <si>
+    <t>totalManaEnabled</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>4,4</t>
+  </si>
+  <si>
+    <t>5,5</t>
+  </si>
+  <si>
+    <t>6,6</t>
+  </si>
+  <si>
+    <t>7,7</t>
+  </si>
+  <si>
+    <t>8,8</t>
+  </si>
+  <si>
+    <t>9,9</t>
+  </si>
+  <si>
+    <t>10,10</t>
+  </si>
+  <si>
+    <t>11,11</t>
+  </si>
+  <si>
+    <t>12,12</t>
+  </si>
+  <si>
+    <t>13,13</t>
+  </si>
+  <si>
+    <t>14,14</t>
+  </si>
+  <si>
+    <t>15,15</t>
+  </si>
+  <si>
+    <t>16,16</t>
+  </si>
+  <si>
+    <t>17,17</t>
+  </si>
+  <si>
+    <t>18,18</t>
+  </si>
+  <si>
+    <t>19,19</t>
+  </si>
+  <si>
+    <t>20,20</t>
+  </si>
+  <si>
+    <t>21,21</t>
+  </si>
+  <si>
+    <t>22,22</t>
+  </si>
+  <si>
+    <t>23,23</t>
+  </si>
+  <si>
+    <t>24,24</t>
+  </si>
+  <si>
+    <t>25,25</t>
   </si>
 </sst>
 </file>
@@ -4129,10 +4210,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" activeCellId="1" sqref="C11 B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4142,40 +4223,49 @@
     <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="5">
-        <v>1</v>
+      <c r="B1" s="4">
+        <v>0</v>
       </c>
       <c r="C1" s="5">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1">
+    <row r="3" spans="1:4" s="4" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>144</v>
       </c>
@@ -4185,565 +4275,721 @@
       <c r="C4" s="5" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
         <v>147</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
         <v>169</v>
       </c>
       <c r="B13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B14" s="5">
-        <v>0</v>
+      <c r="B14" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="C14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
         <v>176</v>
       </c>
       <c r="B15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="5">
-        <v>0</v>
+      <c r="B16" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="C16" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>175</v>
       </c>
       <c r="B17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="5">
-        <v>0</v>
+      <c r="B18" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="C18" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
         <v>174</v>
       </c>
       <c r="B19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="5">
-        <v>0</v>
+      <c r="B20" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="C20" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="5">
-        <v>0</v>
+      <c r="B22" s="5" t="s">
+        <v>197</v>
       </c>
       <c r="C22" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
         <v>172</v>
       </c>
       <c r="B23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="5">
-        <v>0</v>
+      <c r="B24" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="C24" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B26" s="5">
-        <v>0</v>
+      <c r="B26" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="C26" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
         <v>170</v>
       </c>
       <c r="B27" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="5">
-        <v>0</v>
+      <c r="B28" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="C28" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
         <v>152</v>
       </c>
       <c r="B29" s="5">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B30" s="5">
-        <v>0</v>
+      <c r="B30" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="C30" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
         <v>154</v>
       </c>
       <c r="B31" s="5">
         <v>1</v>
       </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
         <v>155</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C32" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B33" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B34" s="5">
-        <v>0</v>
+        <v>180</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="C34" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
         <v>178</v>
       </c>
       <c r="B35" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B36" s="5">
-        <v>0</v>
+      <c r="B36" s="5" t="s">
+        <v>204</v>
       </c>
       <c r="C36" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B37" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B38" s="5">
-        <v>0</v>
+        <v>185</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="C38" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
         <v>156</v>
       </c>
       <c r="B39" s="5">
-        <v>0</v>
-      </c>
-      <c r="C39" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="5">
-        <v>0</v>
+      <c r="B40" s="5" t="s">
+        <v>206</v>
       </c>
       <c r="C40" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B41" s="5">
-        <v>0</v>
-      </c>
-      <c r="C41" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="5">
-        <v>0</v>
+      <c r="B42" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="C42" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B43" s="5">
-        <v>0</v>
-      </c>
-      <c r="C43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="5">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B44" s="5">
-        <v>0</v>
+      <c r="B44" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="C44" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
         <v>159</v>
       </c>
       <c r="B45" s="5">
-        <v>0</v>
-      </c>
-      <c r="C45" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="C45" s="5">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="5">
-        <v>0</v>
+      <c r="B46" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="C46" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B47" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="5">
-        <v>0</v>
+      <c r="B48" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="C48" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B49" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="5">
-        <v>0</v>
+      <c r="B50" s="5" t="s">
+        <v>211</v>
       </c>
       <c r="C50" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B51" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="5">
-        <v>0</v>
+      <c r="B52" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="C52" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D52" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B53" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="5">
-        <v>0</v>
+      <c r="B54" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="C54" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I had forgotten the starting index value with the mappings - now they're included. Not surprisingly, the code fix was easy but the excel file update was a pain. A minor update, but necessary.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="239">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -660,6 +660,81 @@
   </si>
   <si>
     <t>25,25</t>
+  </si>
+  <si>
+    <t>rangeStartingIndex</t>
+  </si>
+  <si>
+    <t>targetedStartingIndex</t>
+  </si>
+  <si>
+    <t>diceDamageStartingIndex</t>
+  </si>
+  <si>
+    <t>diceDamagedurationStartingIndex</t>
+  </si>
+  <si>
+    <t>STRStartingIndex</t>
+  </si>
+  <si>
+    <t>DEXStartingIndex</t>
+  </si>
+  <si>
+    <t>CONStartingIndex</t>
+  </si>
+  <si>
+    <t>WILLStartingIndex</t>
+  </si>
+  <si>
+    <t>INTStartingIndex</t>
+  </si>
+  <si>
+    <t>WISStartingIndex</t>
+  </si>
+  <si>
+    <t>CHRStartingIndex</t>
+  </si>
+  <si>
+    <t>LUCKStartingIndex</t>
+  </si>
+  <si>
+    <t>acStartingIndex</t>
+  </si>
+  <si>
+    <t>damageModStartingIndex</t>
+  </si>
+  <si>
+    <t>hpStartingIndex</t>
+  </si>
+  <si>
+    <t>totalHPStartingIndex</t>
+  </si>
+  <si>
+    <t>totalManaStartingIndex</t>
+  </si>
+  <si>
+    <t>bluntDRStartingIndex</t>
+  </si>
+  <si>
+    <t>chopDRStartingIndex</t>
+  </si>
+  <si>
+    <t>pierceDRStartingIndex</t>
+  </si>
+  <si>
+    <t>slashDRStartingIndex</t>
+  </si>
+  <si>
+    <t>earthDRStartingIndex</t>
+  </si>
+  <si>
+    <t>fireDRStartingIndex</t>
+  </si>
+  <si>
+    <t>waterDRStartingIndex</t>
+  </si>
+  <si>
+    <t>lightningDRStartingIndex</t>
   </si>
 </sst>
 </file>
@@ -724,7 +799,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -733,6 +808,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -4210,10 +4294,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" activeCellId="1" sqref="C11 B11"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4227,7 +4311,7 @@
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="5">
         <v>0</v>
       </c>
       <c r="C1" s="5">
@@ -4279,29 +4363,29 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" s="8" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>162</v>
+        <v>214</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -4309,13 +4393,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -4323,13 +4407,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>163</v>
+        <v>146</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -4337,41 +4421,41 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>148</v>
+        <v>215</v>
       </c>
       <c r="B9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
       </c>
       <c r="C11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -4379,52 +4463,52 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>192</v>
+        <v>216</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
       </c>
       <c r="C12" s="5">
         <v>0</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>164</v>
+      <c r="D12" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
+        <v>149</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>193</v>
+        <v>150</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
       </c>
       <c r="C14" s="5">
         <v>0</v>
       </c>
       <c r="D14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>176</v>
+        <v>217</v>
       </c>
       <c r="B15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="5">
         <v>0</v>
@@ -4435,21 +4519,21 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C16" s="5">
         <v>0</v>
       </c>
-      <c r="D16" s="5">
-        <v>0</v>
+      <c r="D16" s="5" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
@@ -4463,10 +4547,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>195</v>
+        <v>218</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0</v>
       </c>
       <c r="C18" s="5">
         <v>0</v>
@@ -4477,10 +4561,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B19" s="5">
-        <v>1</v>
+        <v>115</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="C19" s="5">
         <v>0</v>
@@ -4491,10 +4575,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>196</v>
+        <v>176</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
       </c>
       <c r="C20" s="5">
         <v>0</v>
@@ -4505,10 +4589,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>173</v>
+        <v>219</v>
       </c>
       <c r="B21" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="5">
         <v>0</v>
@@ -4519,10 +4603,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C22" s="5">
         <v>0</v>
@@ -4533,7 +4617,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
@@ -4547,10 +4631,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>198</v>
+        <v>220</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
       </c>
       <c r="C24" s="5">
         <v>0</v>
@@ -4561,10 +4645,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B25" s="5">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="C25" s="5">
         <v>0</v>
@@ -4575,10 +4659,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>199</v>
+        <v>174</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
       </c>
       <c r="C26" s="5">
         <v>0</v>
@@ -4589,10 +4673,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>170</v>
+        <v>221</v>
       </c>
       <c r="B27" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="5">
         <v>0</v>
@@ -4603,10 +4687,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C28" s="5">
         <v>0</v>
@@ -4617,7 +4701,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
@@ -4631,10 +4715,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>201</v>
+        <v>222</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0</v>
       </c>
       <c r="C30" s="5">
         <v>0</v>
@@ -4645,13 +4729,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B31" s="5">
-        <v>1</v>
+        <v>119</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>197</v>
       </c>
       <c r="C31" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
@@ -4659,13 +4743,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>165</v>
+        <v>172</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0</v>
       </c>
       <c r="D32" s="5">
         <v>0</v>
@@ -4673,10 +4757,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="B33" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="5">
         <v>0</v>
@@ -4687,10 +4771,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C34" s="5">
         <v>0</v>
@@ -4701,7 +4785,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B35" s="5">
         <v>1</v>
@@ -4715,10 +4799,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>204</v>
+        <v>224</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
       </c>
       <c r="C36" s="5">
         <v>0</v>
@@ -4729,10 +4813,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B37" s="5">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="C37" s="5">
         <v>0</v>
@@ -4743,10 +4827,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>205</v>
+        <v>170</v>
+      </c>
+      <c r="B38" s="5">
+        <v>1</v>
       </c>
       <c r="C38" s="5">
         <v>0</v>
@@ -4757,12 +4841,12 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
-        <v>156</v>
+        <v>225</v>
       </c>
       <c r="B39" s="5">
-        <v>1</v>
-      </c>
-      <c r="C39" s="5">
+        <v>0</v>
+      </c>
+      <c r="C39" s="10">
         <v>0</v>
       </c>
       <c r="D39" s="1">
@@ -4771,10 +4855,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C40" s="5">
         <v>0</v>
@@ -4785,7 +4869,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B41" s="5">
         <v>1</v>
@@ -4799,10 +4883,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>207</v>
+        <v>226</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0</v>
       </c>
       <c r="C42" s="5">
         <v>0</v>
@@ -4813,10 +4897,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B43" s="5">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="C43" s="5">
         <v>0</v>
@@ -4827,13 +4911,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>208</v>
+        <v>154</v>
+      </c>
+      <c r="B44" s="5">
+        <v>1</v>
       </c>
       <c r="C44" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="5">
         <v>0</v>
@@ -4841,13 +4925,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
-        <v>159</v>
+        <v>227</v>
       </c>
       <c r="B45" s="5">
-        <v>1</v>
-      </c>
-      <c r="C45" s="5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C45" s="10">
+        <v>1</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
@@ -4855,13 +4939,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C46" s="5">
-        <v>0</v>
+        <v>202</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="D46" s="5">
         <v>0</v>
@@ -4869,7 +4953,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B47" s="5">
         <v>1</v>
@@ -4883,10 +4967,10 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>210</v>
+        <v>228</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0</v>
       </c>
       <c r="C48" s="5">
         <v>0</v>
@@ -4897,10 +4981,10 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B49" s="5">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="C49" s="5">
         <v>0</v>
@@ -4911,10 +4995,10 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>211</v>
+        <v>178</v>
+      </c>
+      <c r="B50" s="5">
+        <v>1</v>
       </c>
       <c r="C50" s="5">
         <v>0</v>
@@ -4925,10 +5009,10 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="B51" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" s="5">
         <v>0</v>
@@ -4939,10 +5023,10 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C52" s="5">
         <v>0</v>
@@ -4953,7 +5037,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B53" s="5">
         <v>1</v>
@@ -4967,10 +5051,10 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>213</v>
+        <v>230</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0</v>
       </c>
       <c r="C54" s="5">
         <v>0</v>
@@ -4981,15 +5065,365 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C55" s="5">
+        <v>0</v>
+      </c>
+      <c r="D55" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" s="5">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0</v>
+      </c>
+      <c r="D56" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B57" s="5">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0</v>
+      </c>
+      <c r="D57" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+      <c r="D58" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="5">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="D59" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" s="5">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0</v>
+      </c>
+      <c r="D60" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="D61" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B62" s="5">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="D62" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B63" s="5">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="D63" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0</v>
+      </c>
+      <c r="D64" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" s="5">
+        <v>1</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="D65" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B66" s="5">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0</v>
+      </c>
+      <c r="D66" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0</v>
+      </c>
+      <c r="D67" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B68" s="5">
+        <v>1</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B69" s="5">
+        <v>0</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0</v>
+      </c>
+      <c r="D69" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0</v>
+      </c>
+      <c r="D70" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B71" s="5">
+        <v>1</v>
+      </c>
+      <c r="C71" s="1">
+        <v>0</v>
+      </c>
+      <c r="D71" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B72" s="5">
+        <v>0</v>
+      </c>
+      <c r="C72" s="1">
+        <v>0</v>
+      </c>
+      <c r="D72" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0</v>
+      </c>
+      <c r="D73" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B74" s="5">
+        <v>1</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0</v>
+      </c>
+      <c r="D74" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" s="5">
+        <v>0</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0</v>
+      </c>
+      <c r="D75" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C76" s="1">
+        <v>0</v>
+      </c>
+      <c r="D76" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B77" s="5">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1">
+        <v>0</v>
+      </c>
+      <c r="D77" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B78" s="5">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0</v>
+      </c>
+      <c r="D78" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0</v>
+      </c>
+      <c r="D79" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B80" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C80" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
So after some soul searching, I've concluded that really, there are only 3 types of effects: permanent, self duration, and target. I've laid down some basic logic for each of the effects, and added a type field to distinguish between them. The basic concept still exists, where the effect will be cloned, however the 'ability' struct is basically obsolete, so I'll eventually rename 'effect' to 'ability'.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -13,12 +13,15 @@
     <sheet name="Events" sheetId="4" r:id="rId4"/>
     <sheet name="Effects" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$84</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="240">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -500,15 +503,9 @@
     <t>slashDREnabled</t>
   </si>
   <si>
-    <t>Fireball</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
-    <t>1,0,10,1,20,2,30,3</t>
-  </si>
-  <si>
     <t>0,-1,1,0</t>
   </si>
   <si>
@@ -518,9 +515,6 @@
     <t>0,0,1,1,2,2,3,3,4,4,5,5,6,6,7,7,8,8,9,9,10,10</t>
   </si>
   <si>
-    <t>Burn</t>
-  </si>
-  <si>
     <t>Duration effect: fire damage over time</t>
   </si>
   <si>
@@ -581,87 +575,9 @@
     <t>totalManaEnabled</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>1,1</t>
-  </si>
-  <si>
     <t>Test Description</t>
   </si>
   <si>
-    <t>2,2</t>
-  </si>
-  <si>
-    <t>3,3</t>
-  </si>
-  <si>
-    <t>4,4</t>
-  </si>
-  <si>
-    <t>5,5</t>
-  </si>
-  <si>
-    <t>6,6</t>
-  </si>
-  <si>
-    <t>7,7</t>
-  </si>
-  <si>
-    <t>8,8</t>
-  </si>
-  <si>
-    <t>9,9</t>
-  </si>
-  <si>
-    <t>10,10</t>
-  </si>
-  <si>
-    <t>11,11</t>
-  </si>
-  <si>
-    <t>12,12</t>
-  </si>
-  <si>
-    <t>13,13</t>
-  </si>
-  <si>
-    <t>14,14</t>
-  </si>
-  <si>
-    <t>15,15</t>
-  </si>
-  <si>
-    <t>16,16</t>
-  </si>
-  <si>
-    <t>17,17</t>
-  </si>
-  <si>
-    <t>18,18</t>
-  </si>
-  <si>
-    <t>19,19</t>
-  </si>
-  <si>
-    <t>20,20</t>
-  </si>
-  <si>
-    <t>21,21</t>
-  </si>
-  <si>
-    <t>22,22</t>
-  </si>
-  <si>
-    <t>23,23</t>
-  </si>
-  <si>
-    <t>24,24</t>
-  </si>
-  <si>
-    <t>25,25</t>
-  </si>
-  <si>
     <t>rangeStartingIndex</t>
   </si>
   <si>
@@ -735,6 +651,96 @@
   </si>
   <si>
     <t>lightningDRStartingIndex</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>perminent</t>
+  </si>
+  <si>
+    <t>self duration</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>range of attack is different for perminent and self (i can attack further) vs. my spell can hit a target x spaces away</t>
+  </si>
+  <si>
+    <t>weather a spell hits or needs to be rolled</t>
+  </si>
+  <si>
+    <t>For a minus, the player could take dice damage, but would have to make sure that they cant cheat health with it</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>1,0,3,1,6,2,9,3</t>
+  </si>
+  <si>
+    <t>0,0,1,1,2,2,3,3</t>
+  </si>
+  <si>
+    <t>-2,-2,-1,-1,0,0,1,1,2,2,3,3</t>
+  </si>
+  <si>
+    <t>-2,-4,-1,-2,0,0,1,2,2,4</t>
+  </si>
+  <si>
+    <t>-3,-3,-2,-2,-1,-1,0,0,1,1,2,2,3,3,4,4,5,5,6,6,7,7,8,8,9,9,10,10</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>-12,-5,-10,-4,-8-3,-6,-2,-4,-1,0,0,4,1,6,2,8,3,10,4,12,5</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0,0,4,1,6,2,8,3,10,4,12,5</t>
+  </si>
+  <si>
+    <t>0,0,2,1,4,2,6,3,8,4,10,5</t>
+  </si>
+  <si>
+    <t>-10,-5,-8,-4,-6,-3,-4,-2,-2,-1,0,0,2,1,4,2,6,3,8,4,10,5</t>
+  </si>
+  <si>
+    <t>0,0,1,2,2,4,3,6,4,8,5,10</t>
+  </si>
+  <si>
+    <t>-5,-10,-4,-8,-3,-6,-2,-4,-1,-2,0,0,1,2,2,4,3,6,4,8,5,10</t>
+  </si>
+  <si>
+    <t>0,0,1,0,2,0,3,0,4,0,5,0</t>
+  </si>
+  <si>
+    <t>mvmtStartingIndex</t>
+  </si>
+  <si>
+    <t>mvmtEnabled</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -758,7 +764,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -768,6 +774,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -799,9 +823,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -810,13 +833,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -4294,1137 +4323,1685 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="5">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5">
+      <c r="B1" s="4">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" s="3" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1">
+      <c r="A4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1">
+      <c r="A6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="B13" s="9">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1">
-      <c r="A3" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B19" s="9">
+        <v>2</v>
+      </c>
+      <c r="C19" s="9">
+        <v>2</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="9">
+        <v>2</v>
+      </c>
+      <c r="C22" s="9">
+        <v>2</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="9">
+        <v>2</v>
+      </c>
+      <c r="C25" s="9">
+        <v>2</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B28" s="9">
+        <v>2</v>
+      </c>
+      <c r="C28" s="9">
+        <v>2</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="9">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B31" s="9">
+        <v>2</v>
+      </c>
+      <c r="C31" s="9">
+        <v>2</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" s="9">
+        <v>1</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" s="9">
+        <v>2</v>
+      </c>
+      <c r="C34" s="9">
+        <v>2</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="9">
+        <v>1</v>
+      </c>
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B37" s="9">
+        <v>2</v>
+      </c>
+      <c r="C37" s="9">
+        <v>2</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="9">
+        <v>1</v>
+      </c>
+      <c r="C39" s="9">
+        <v>1</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" s="9">
+        <v>2</v>
+      </c>
+      <c r="C40" s="9">
+        <v>2</v>
+      </c>
+      <c r="D40" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D41" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="9">
+        <v>1</v>
+      </c>
+      <c r="D42" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B43" s="9">
+        <v>2</v>
+      </c>
+      <c r="C43" s="9">
+        <v>2</v>
+      </c>
+      <c r="D43" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B45" s="9">
+        <v>1</v>
+      </c>
+      <c r="C45" s="9">
+        <v>1</v>
+      </c>
+      <c r="D45" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B51" s="9">
+        <v>0</v>
+      </c>
+      <c r="C51" s="9">
+        <v>1</v>
+      </c>
+      <c r="D51" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52" s="9">
+        <v>0</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D52" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B53" s="9">
+        <v>0</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D53" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B54" s="9">
+        <v>1</v>
+      </c>
+      <c r="C54" s="9">
+        <v>1</v>
+      </c>
+      <c r="D54" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C55" s="9">
+        <v>0</v>
+      </c>
+      <c r="D55" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D56" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" s="9">
+        <v>1</v>
+      </c>
+      <c r="C57" s="9">
+        <v>1</v>
+      </c>
+      <c r="D57" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C58" s="9">
+        <v>0</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D59" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B60" s="9">
+        <v>1</v>
+      </c>
+      <c r="C60" s="9">
+        <v>1</v>
+      </c>
+      <c r="D60" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D61" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D62" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" s="9">
+        <v>1</v>
+      </c>
+      <c r="C63" s="9">
+        <v>1</v>
+      </c>
+      <c r="D63" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D64" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D65" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B66" s="9">
+        <v>1</v>
+      </c>
+      <c r="C66" s="9">
+        <v>1</v>
+      </c>
+      <c r="D66" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D67" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D68" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B69" s="9">
+        <v>1</v>
+      </c>
+      <c r="C69" s="9">
+        <v>1</v>
+      </c>
+      <c r="D69" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D70" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D71" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B72" s="9">
+        <v>1</v>
+      </c>
+      <c r="C72" s="9">
+        <v>1</v>
+      </c>
+      <c r="D72" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D73" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D74" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B75" s="9">
+        <v>1</v>
+      </c>
+      <c r="C75" s="9">
+        <v>1</v>
+      </c>
+      <c r="D75" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D76" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D77" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B78" s="9">
+        <v>1</v>
+      </c>
+      <c r="C78" s="9">
+        <v>1</v>
+      </c>
+      <c r="D78" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D79" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D80" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B81" s="9">
+        <v>1</v>
+      </c>
+      <c r="C81" s="9">
+        <v>1</v>
+      </c>
+      <c r="D81" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D82" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D83" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="B98" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C98" t="s">
+        <v>214</v>
+      </c>
+      <c r="D98" t="s">
+        <v>212</v>
+      </c>
+      <c r="E98" t="s">
+        <v>32</v>
+      </c>
+      <c r="F98" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="15" customHeight="1">
+      <c r="B99" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E99" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="B100" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E100" t="s">
+        <v>26</v>
+      </c>
+      <c r="F100" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="15" customHeight="1">
+      <c r="A101" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="8" customFormat="1">
-      <c r="A5" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
+      <c r="B101" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C101" t="s">
+        <v>215</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E101" t="s">
+        <v>211</v>
+      </c>
+      <c r="F101" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="15" customHeight="1">
+      <c r="A102" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B9" s="5">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
+      <c r="C102" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E102" t="s">
+        <v>27</v>
+      </c>
+      <c r="F102" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="15" customHeight="1">
+      <c r="A103" t="s">
         <v>147</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="3" t="s">
+      <c r="B103" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E103" t="s">
+        <v>27</v>
+      </c>
+      <c r="F103" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" t="s">
         <v>149</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B14" s="5">
-        <v>1</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
+      <c r="B104" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D104" t="s">
+        <v>215</v>
+      </c>
+      <c r="E104" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" t="s">
         <v>151</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B17" s="5">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B18" s="5">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5">
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
+      <c r="B105" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D105" t="s">
+        <v>215</v>
+      </c>
+      <c r="E105" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C19" s="5">
-        <v>0</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B20" s="5">
-        <v>1</v>
-      </c>
-      <c r="C20" s="5">
-        <v>0</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B21" s="5">
-        <v>0</v>
-      </c>
-      <c r="C21" s="5">
-        <v>0</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="3" t="s">
+      <c r="B106" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D106" t="s">
+        <v>215</v>
+      </c>
+      <c r="E106" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C22" s="5">
-        <v>0</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B23" s="5">
-        <v>1</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B24" s="5">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5">
-        <v>0</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="3" t="s">
+      <c r="B107" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D107" t="s">
+        <v>215</v>
+      </c>
+      <c r="E107" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="3" t="s">
+      <c r="B108" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D108" t="s">
+        <v>215</v>
+      </c>
+      <c r="E108" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" t="s">
+        <v>118</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D109" t="s">
+        <v>215</v>
+      </c>
+      <c r="E109" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" t="s">
+        <v>119</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D110" t="s">
+        <v>215</v>
+      </c>
+      <c r="E110" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" t="s">
+        <v>120</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D111" t="s">
+        <v>215</v>
+      </c>
+      <c r="E111" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" t="s">
+        <v>121</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D112" t="s">
+        <v>215</v>
+      </c>
+      <c r="E112" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>122</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D113" t="s">
+        <v>215</v>
+      </c>
+      <c r="E113" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="15" customHeight="1">
+      <c r="A114" t="s">
+        <v>153</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D114" t="s">
+        <v>215</v>
+      </c>
+      <c r="E114" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>155</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D115" t="s">
+        <v>215</v>
+      </c>
+      <c r="E115" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>177</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D116" t="s">
+        <v>215</v>
+      </c>
+      <c r="E116" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
         <v>174</v>
       </c>
-      <c r="B26" s="5">
-        <v>1</v>
-      </c>
-      <c r="C26" s="5">
-        <v>0</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="B27" s="5">
-        <v>0</v>
-      </c>
-      <c r="C27" s="5">
-        <v>0</v>
-      </c>
-      <c r="D27" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C28" s="5">
-        <v>0</v>
-      </c>
-      <c r="D28" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B29" s="5">
-        <v>1</v>
-      </c>
-      <c r="C29" s="5">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B30" s="5">
-        <v>0</v>
-      </c>
-      <c r="C30" s="5">
-        <v>0</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="C31" s="5">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B32" s="5">
-        <v>1</v>
-      </c>
-      <c r="C32" s="5">
-        <v>0</v>
-      </c>
-      <c r="D32" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B33" s="5">
-        <v>0</v>
-      </c>
-      <c r="C33" s="5">
-        <v>0</v>
-      </c>
-      <c r="D33" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C34" s="5">
-        <v>0</v>
-      </c>
-      <c r="D34" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B35" s="5">
-        <v>1</v>
-      </c>
-      <c r="C35" s="5">
-        <v>0</v>
-      </c>
-      <c r="D35" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="B36" s="5">
-        <v>0</v>
-      </c>
-      <c r="C36" s="5">
-        <v>0</v>
-      </c>
-      <c r="D36" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C37" s="5">
-        <v>0</v>
-      </c>
-      <c r="D37" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B38" s="5">
-        <v>1</v>
-      </c>
-      <c r="C38" s="5">
-        <v>0</v>
-      </c>
-      <c r="D38" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B39" s="5">
-        <v>0</v>
-      </c>
-      <c r="C39" s="10">
-        <v>0</v>
-      </c>
-      <c r="D39" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C40" s="5">
-        <v>0</v>
-      </c>
-      <c r="D40" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B41" s="5">
-        <v>1</v>
-      </c>
-      <c r="C41" s="5">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="B42" s="5">
-        <v>0</v>
-      </c>
-      <c r="C42" s="5">
-        <v>0</v>
-      </c>
-      <c r="D42" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C43" s="5">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B44" s="5">
-        <v>1</v>
-      </c>
-      <c r="C44" s="5">
-        <v>1</v>
-      </c>
-      <c r="D44" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B45" s="5">
-        <v>0</v>
-      </c>
-      <c r="C45" s="10">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D46" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47" s="5">
-        <v>1</v>
-      </c>
-      <c r="C47" s="5">
-        <v>0</v>
-      </c>
-      <c r="D47" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B48" s="5">
-        <v>0</v>
-      </c>
-      <c r="C48" s="5">
-        <v>0</v>
-      </c>
-      <c r="D48" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C49" s="5">
-        <v>0</v>
-      </c>
-      <c r="D49" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B50" s="5">
-        <v>1</v>
-      </c>
-      <c r="C50" s="5">
-        <v>0</v>
-      </c>
-      <c r="D50" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B51" s="5">
-        <v>0</v>
-      </c>
-      <c r="C51" s="5">
-        <v>0</v>
-      </c>
-      <c r="D51" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C52" s="5">
-        <v>0</v>
-      </c>
-      <c r="D52" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B53" s="5">
-        <v>1</v>
-      </c>
-      <c r="C53" s="5">
-        <v>0</v>
-      </c>
-      <c r="D53" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B54" s="5">
-        <v>0</v>
-      </c>
-      <c r="C54" s="5">
-        <v>0</v>
-      </c>
-      <c r="D54" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C55" s="5">
-        <v>0</v>
-      </c>
-      <c r="D55" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B56" s="5">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1">
-        <v>0</v>
-      </c>
-      <c r="D56" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="B57" s="5">
-        <v>0</v>
-      </c>
-      <c r="C57" s="1">
-        <v>0</v>
-      </c>
-      <c r="D57" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="3" t="s">
+      <c r="B117" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D117" t="s">
+        <v>215</v>
+      </c>
+      <c r="E117" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>182</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D118" t="s">
+        <v>215</v>
+      </c>
+      <c r="E118" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C58" s="1">
-        <v>0</v>
-      </c>
-      <c r="D58" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B59" s="5">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1">
-        <v>0</v>
-      </c>
-      <c r="D59" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B60" s="5">
-        <v>0</v>
-      </c>
-      <c r="C60" s="1">
-        <v>0</v>
-      </c>
-      <c r="D60" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="3" t="s">
+      <c r="B119" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D119" t="s">
+        <v>215</v>
+      </c>
+      <c r="E119" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C61" s="1">
-        <v>0</v>
-      </c>
-      <c r="D61" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B62" s="5">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1">
-        <v>0</v>
-      </c>
-      <c r="D62" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="B63" s="5">
-        <v>0</v>
-      </c>
-      <c r="C63" s="1">
-        <v>0</v>
-      </c>
-      <c r="D63" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="3" t="s">
+      <c r="B120" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D120" t="s">
+        <v>215</v>
+      </c>
+      <c r="E120" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
         <v>91</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C64" s="1">
-        <v>0</v>
-      </c>
-      <c r="D64" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B65" s="5">
-        <v>1</v>
-      </c>
-      <c r="C65" s="1">
-        <v>0</v>
-      </c>
-      <c r="D65" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B66" s="5">
-        <v>0</v>
-      </c>
-      <c r="C66" s="1">
-        <v>0</v>
-      </c>
-      <c r="D66" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="3" t="s">
+      <c r="B121" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D121" t="s">
+        <v>215</v>
+      </c>
+      <c r="E121" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
         <v>90</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C67" s="1">
-        <v>0</v>
-      </c>
-      <c r="D67" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B68" s="5">
-        <v>1</v>
-      </c>
-      <c r="C68" s="1">
-        <v>0</v>
-      </c>
-      <c r="D68" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B69" s="5">
-        <v>0</v>
-      </c>
-      <c r="C69" s="1">
-        <v>0</v>
-      </c>
-      <c r="D69" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="3" t="s">
+      <c r="B122" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D122" t="s">
+        <v>215</v>
+      </c>
+      <c r="E122" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
         <v>92</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C70" s="1">
-        <v>0</v>
-      </c>
-      <c r="D70" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B71" s="5">
-        <v>1</v>
-      </c>
-      <c r="C71" s="1">
-        <v>0</v>
-      </c>
-      <c r="D71" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B72" s="5">
-        <v>0</v>
-      </c>
-      <c r="C72" s="1">
-        <v>0</v>
-      </c>
-      <c r="D72" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="3" t="s">
+      <c r="B123" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D123" t="s">
+        <v>215</v>
+      </c>
+      <c r="E123" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
         <v>93</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C73" s="1">
-        <v>0</v>
-      </c>
-      <c r="D73" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B74" s="5">
-        <v>1</v>
-      </c>
-      <c r="C74" s="1">
-        <v>0</v>
-      </c>
-      <c r="D74" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B75" s="5">
-        <v>0</v>
-      </c>
-      <c r="C75" s="1">
-        <v>0</v>
-      </c>
-      <c r="D75" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="3" t="s">
+      <c r="B124" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D124" t="s">
+        <v>215</v>
+      </c>
+      <c r="E124" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
         <v>94</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C76" s="1">
-        <v>0</v>
-      </c>
-      <c r="D76" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B77" s="5">
-        <v>1</v>
-      </c>
-      <c r="C77" s="1">
-        <v>0</v>
-      </c>
-      <c r="D77" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B78" s="5">
-        <v>0</v>
-      </c>
-      <c r="C78" s="1">
-        <v>0</v>
-      </c>
-      <c r="D78" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="3" t="s">
+      <c r="B125" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D125" t="s">
+        <v>215</v>
+      </c>
+      <c r="E125" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
         <v>95</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C79" s="1">
-        <v>0</v>
-      </c>
-      <c r="D79" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="3" t="s">
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
         <v>69</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created a function to calculate mana cost - with it, it introduced some more business logic that I hadn't accounted for. Fortunately at this point, I feel that I have a good amount accounted for, and that I can continue on.
At this point, I see the following major tasks ahead of me: 1) create a
view for the user to create an ability, 2) implement the ability logic
in the various locations, 3) allow the user to trigger an ability.
Example cases could be 1) player creates a fireball ability, 2) the
mechanic of the fireball are set up, 3) player uses the fireball on an
enemy.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="17895" windowHeight="1110" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="15375" windowHeight="1110" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,14 @@
     <sheet name="Effects" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$96</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="253">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -509,18 +509,9 @@
     <t>0,-1,1,0</t>
   </si>
   <si>
-    <t>4,1,6,2,8,3,10,4,12,5</t>
-  </si>
-  <si>
     <t>0,0,1,1,2,2,3,3,4,4,5,5,6,6,7,7,8,8,9,9,10,10</t>
   </si>
   <si>
-    <t>Duration effect: fire damage over time</t>
-  </si>
-  <si>
-    <t>Targeted effect: a flying ball of fire</t>
-  </si>
-  <si>
     <t>STREnabled</t>
   </si>
   <si>
@@ -575,9 +566,6 @@
     <t>totalManaEnabled</t>
   </si>
   <si>
-    <t>Test Description</t>
-  </si>
-  <si>
     <t>rangeStartingIndex</t>
   </si>
   <si>
@@ -710,15 +698,9 @@
     <t>3</t>
   </si>
   <si>
-    <t>-12,-5,-10,-4,-8-3,-6,-2,-4,-1,0,0,4,1,6,2,8,3,10,4,12,5</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
-    <t>0,0,4,1,6,2,8,3,10,4,12,5</t>
-  </si>
-  <si>
     <t>0,0,2,1,4,2,6,3,8,4,10,5</t>
   </si>
   <si>
@@ -741,6 +723,63 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>durationEnabled</t>
+  </si>
+  <si>
+    <t>durationStartingIndex</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>Perminent - always affects the player</t>
+  </si>
+  <si>
+    <t>Self - temporarilly affects the player</t>
+  </si>
+  <si>
+    <t>Affects the target individual</t>
+  </si>
+  <si>
+    <t>durationModEnabled</t>
+  </si>
+  <si>
+    <t>durationModStartingIndex</t>
+  </si>
+  <si>
+    <t>durationMod</t>
+  </si>
+  <si>
+    <t>damageEnabled</t>
+  </si>
+  <si>
+    <t>damageStartingIndex</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>0,0,2,-1,4,-2,6,-3,8,-4,10,-5</t>
+  </si>
+  <si>
+    <t>0,0,4,2,6,3,8,4,10,5,12,6</t>
+  </si>
+  <si>
+    <t>diceDamagedurationModEnabled</t>
+  </si>
+  <si>
+    <t>diceDamagedurationModStartingIndex</t>
+  </si>
+  <si>
+    <t>diceDamageDurationMod</t>
+  </si>
+  <si>
+    <t>0,0,4,-2,6,-3,8,-4,10,-5,12,-6</t>
+  </si>
+  <si>
+    <t>-12,-5,-10,-4,-8,-3,-6,-2,-4,-1,0,0,4,1,6,2,8,3,10,4,12,5</t>
   </si>
 </sst>
 </file>
@@ -4323,15 +4362,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -4352,7 +4391,7 @@
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -4361,7 +4400,7 @@
         <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4369,13 +4408,13 @@
         <v>40</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1">
@@ -4422,7 +4461,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B7" s="9">
         <v>0</v>
@@ -4439,13 +4478,13 @@
         <v>86</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4455,8 +4494,8 @@
       <c r="B9" s="9">
         <v>0</v>
       </c>
-      <c r="C9" s="9">
-        <v>0</v>
+      <c r="C9" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
@@ -4464,7 +4503,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B10" s="9">
         <v>0</v>
@@ -4472,8 +4511,8 @@
       <c r="C10" s="9">
         <v>0</v>
       </c>
-      <c r="D10" s="9">
-        <v>0</v>
+      <c r="D10" s="9" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4506,7 +4545,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B13" s="9">
         <v>0</v>
@@ -4526,77 +4565,77 @@
         <v>0</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>162</v>
+        <v>251</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9">
-        <v>1</v>
+        <v>243</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B16" s="9">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
+        <v>244</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="9">
-        <v>0</v>
+        <v>245</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>162</v>
+        <v>246</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B18" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
       </c>
       <c r="D18" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B19" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C19" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19" s="9">
         <v>0</v>
@@ -4604,147 +4643,147 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>224</v>
+        <v>151</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D20" s="9">
-        <v>0</v>
+        <v>247</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>173</v>
+        <v>248</v>
       </c>
       <c r="B21" s="9">
-        <v>1</v>
-      </c>
-      <c r="C21" s="9">
-        <v>1</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>190</v>
+        <v>249</v>
       </c>
       <c r="B22" s="9">
-        <v>2</v>
-      </c>
-      <c r="C22" s="9">
-        <v>2</v>
-      </c>
-      <c r="D22" s="9">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>224</v>
+        <v>250</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0</v>
+        <v>247</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B24" s="9">
-        <v>1</v>
-      </c>
-      <c r="C24" s="9">
-        <v>1</v>
-      </c>
-      <c r="D24" s="9">
-        <v>0</v>
+        <v>234</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B25" s="9">
-        <v>2</v>
-      </c>
-      <c r="C25" s="9">
-        <v>2</v>
-      </c>
-      <c r="D25" s="9">
-        <v>0</v>
+        <v>235</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>117</v>
+        <v>236</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D26" s="9">
-        <v>0</v>
+        <v>247</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B27" s="9">
-        <v>1</v>
-      </c>
-      <c r="C27" s="9">
-        <v>1</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0</v>
+        <v>240</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="9">
-        <v>2</v>
-      </c>
-      <c r="C28" s="9">
-        <v>2</v>
-      </c>
-      <c r="D28" s="9">
-        <v>0</v>
+        <v>241</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>118</v>
+        <v>242</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D29" s="9">
-        <v>0</v>
+        <v>162</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B30" s="9">
         <v>1</v>
@@ -4758,7 +4797,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B31" s="9">
         <v>2</v>
@@ -4772,13 +4811,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D32" s="9">
         <v>0</v>
@@ -4786,7 +4825,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
@@ -4800,7 +4839,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B34" s="9">
         <v>2</v>
@@ -4814,13 +4853,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D35" s="9">
         <v>0</v>
@@ -4828,7 +4867,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
@@ -4842,7 +4881,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B37" s="9">
         <v>2</v>
@@ -4856,13 +4895,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D38" s="9">
         <v>0</v>
@@ -4870,7 +4909,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B39" s="9">
         <v>1</v>
@@ -4884,7 +4923,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B40" s="9">
         <v>2</v>
@@ -4898,13 +4937,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D41" s="9">
         <v>0</v>
@@ -4912,7 +4951,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="B42" s="9">
         <v>1</v>
@@ -4926,7 +4965,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B43" s="9">
         <v>2</v>
@@ -4940,13 +4979,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D44" s="9">
         <v>0</v>
@@ -4954,7 +4993,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B45" s="9">
         <v>1</v>
@@ -4968,13 +5007,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>227</v>
+        <v>190</v>
+      </c>
+      <c r="B46" s="9">
+        <v>2</v>
+      </c>
+      <c r="C46" s="9">
+        <v>2</v>
       </c>
       <c r="D46" s="9">
         <v>0</v>
@@ -4982,13 +5021,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>163</v>
+        <v>220</v>
       </c>
       <c r="D47" s="9">
         <v>0</v>
@@ -4996,52 +5035,52 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>227</v>
+        <v>165</v>
+      </c>
+      <c r="B48" s="9">
+        <v>1</v>
+      </c>
+      <c r="C48" s="9">
+        <v>1</v>
+      </c>
+      <c r="D48" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>227</v>
+        <v>191</v>
+      </c>
+      <c r="B49" s="9">
+        <v>2</v>
+      </c>
+      <c r="C49" s="9">
+        <v>2</v>
+      </c>
+      <c r="D49" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>227</v>
+        <v>220</v>
+      </c>
+      <c r="D50" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B51" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" s="9">
         <v>1</v>
@@ -5052,13 +5091,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B52" s="9">
-        <v>0</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>230</v>
+        <v>2</v>
+      </c>
+      <c r="C52" s="9">
+        <v>2</v>
       </c>
       <c r="D52" s="9">
         <v>0</v>
@@ -5066,13 +5105,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B53" s="9">
-        <v>0</v>
+        <v>122</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>220</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D53" s="9">
         <v>0</v>
@@ -5080,7 +5119,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="B54" s="9">
         <v>1</v>
@@ -5094,13 +5133,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>230</v>
+        <v>193</v>
+      </c>
+      <c r="B55" s="9">
+        <v>2</v>
       </c>
       <c r="C55" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D55" s="9">
         <v>0</v>
@@ -5108,13 +5147,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D56" s="9">
         <v>0</v>
@@ -5122,7 +5161,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="B57" s="9">
         <v>1</v>
@@ -5136,13 +5175,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="C58" s="9">
-        <v>0</v>
+        <v>224</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>223</v>
       </c>
       <c r="D58" s="9">
         <v>0</v>
@@ -5150,13 +5189,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>232</v>
+        <v>162</v>
       </c>
       <c r="D59" s="9">
         <v>0</v>
@@ -5164,52 +5203,52 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B60" s="9">
-        <v>1</v>
-      </c>
-      <c r="C60" s="9">
-        <v>1</v>
-      </c>
-      <c r="D60" s="9">
-        <v>0</v>
+        <v>232</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="D61" s="9">
-        <v>0</v>
+        <v>223</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="D62" s="9">
-        <v>0</v>
+        <v>228</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="B63" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" s="9">
         <v>1</v>
@@ -5220,13 +5259,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>230</v>
+        <v>195</v>
+      </c>
+      <c r="B64" s="9">
+        <v>0</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D64" s="9">
         <v>0</v>
@@ -5234,13 +5273,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>233</v>
+        <v>174</v>
+      </c>
+      <c r="B65" s="9">
+        <v>0</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="D65" s="9">
         <v>0</v>
@@ -5248,7 +5287,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="B66" s="9">
         <v>1</v>
@@ -5262,13 +5301,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+      <c r="C67" s="9">
+        <v>0</v>
       </c>
       <c r="D67" s="9">
         <v>0</v>
@@ -5276,13 +5315,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D68" s="9">
         <v>0</v>
@@ -5290,7 +5329,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="B69" s="9">
         <v>1</v>
@@ -5304,13 +5343,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+      <c r="C70" s="9">
+        <v>0</v>
       </c>
       <c r="D70" s="9">
         <v>0</v>
@@ -5318,13 +5357,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>90</v>
+        <v>179</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D71" s="9">
         <v>0</v>
@@ -5332,7 +5371,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="B72" s="9">
         <v>1</v>
@@ -5346,13 +5385,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D73" s="9">
         <v>0</v>
@@ -5360,13 +5399,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D74" s="9">
         <v>0</v>
@@ -5374,7 +5413,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="B75" s="9">
         <v>1</v>
@@ -5388,13 +5427,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D76" s="9">
         <v>0</v>
@@ -5402,13 +5441,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D77" s="9">
         <v>0</v>
@@ -5416,7 +5455,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="B78" s="9">
         <v>1</v>
@@ -5430,13 +5469,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D79" s="9">
         <v>0</v>
@@ -5444,13 +5483,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D80" s="9">
         <v>0</v>
@@ -5458,7 +5497,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="B81" s="9">
         <v>1</v>
@@ -5472,13 +5511,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D82" s="9">
         <v>0</v>
@@ -5486,13 +5525,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D83" s="9">
         <v>0</v>
@@ -5500,333 +5539,297 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B84" s="9">
+        <v>1</v>
+      </c>
+      <c r="C84" s="9">
+        <v>1</v>
+      </c>
+      <c r="D84" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D85" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D86" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B87" s="9">
+        <v>1</v>
+      </c>
+      <c r="C87" s="9">
+        <v>1</v>
+      </c>
+      <c r="D87" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D88" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D89" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" s="9">
+        <v>1</v>
+      </c>
+      <c r="C90" s="9">
+        <v>1</v>
+      </c>
+      <c r="D90" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D91" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D92" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B93" s="9">
+        <v>1</v>
+      </c>
+      <c r="C93" s="9">
+        <v>1</v>
+      </c>
+      <c r="D93" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D94" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D95" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B84" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="B98" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C98" t="s">
-        <v>214</v>
-      </c>
-      <c r="D98" t="s">
-        <v>212</v>
-      </c>
-      <c r="E98" t="s">
+      <c r="B96" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6">
+      <c r="B110" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C110" t="s">
+        <v>210</v>
+      </c>
+      <c r="D110" t="s">
+        <v>208</v>
+      </c>
+      <c r="E110" t="s">
         <v>32</v>
       </c>
-      <c r="F98" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="15" customHeight="1">
-      <c r="B99" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E99" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="B100" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E100" t="s">
-        <v>26</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="F110" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15" customHeight="1">
-      <c r="A101" t="s">
-        <v>144</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C101" t="s">
-        <v>215</v>
-      </c>
-      <c r="D101" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E101" t="s">
+    <row r="111" spans="2:6" ht="15" customHeight="1">
+      <c r="B111" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="F101" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="15" customHeight="1">
-      <c r="A102" t="s">
-        <v>86</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D102" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E102" t="s">
-        <v>27</v>
-      </c>
-      <c r="F102" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="15" customHeight="1">
-      <c r="A103" t="s">
-        <v>147</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D103" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E103" t="s">
-        <v>27</v>
-      </c>
-      <c r="F103" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104" t="s">
-        <v>149</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D104" t="s">
-        <v>215</v>
-      </c>
-      <c r="E104" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105" t="s">
-        <v>151</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D105" t="s">
-        <v>215</v>
-      </c>
-      <c r="E105" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
-      <c r="A106" t="s">
-        <v>115</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D106" t="s">
-        <v>215</v>
-      </c>
-      <c r="E106" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107" t="s">
-        <v>116</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D107" t="s">
-        <v>215</v>
-      </c>
-      <c r="E107" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108" t="s">
-        <v>117</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D108" t="s">
-        <v>215</v>
-      </c>
-      <c r="E108" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109" t="s">
-        <v>118</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D109" t="s">
-        <v>215</v>
-      </c>
-      <c r="E109" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="A110" t="s">
-        <v>119</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D110" t="s">
-        <v>215</v>
-      </c>
-      <c r="E110" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111" t="s">
-        <v>120</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D111" t="s">
-        <v>215</v>
+      <c r="D111" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="E111" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
-      <c r="A112" t="s">
-        <v>121</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6">
       <c r="B112" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D112" t="s">
-        <v>215</v>
+      <c r="D112" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="E112" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
+        <v>26</v>
+      </c>
+      <c r="F112" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="15" customHeight="1">
       <c r="A113" t="s">
-        <v>122</v>
-      </c>
-      <c r="B113" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C113" t="s">
+        <v>211</v>
+      </c>
+      <c r="D113" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C113" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D113" t="s">
-        <v>215</v>
-      </c>
       <c r="E113" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="15" customHeight="1">
+        <v>207</v>
+      </c>
+      <c r="F113" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="15" customHeight="1">
       <c r="A114" t="s">
-        <v>153</v>
+        <v>86</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D114" t="s">
-        <v>215</v>
+      <c r="D114" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="E114" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5">
+        <v>27</v>
+      </c>
+      <c r="F114" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="15" customHeight="1">
       <c r="A115" t="s">
-        <v>155</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>42</v>
+        <v>147</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E115" t="s">
+        <v>27</v>
+      </c>
+      <c r="F115" t="s">
         <v>215</v>
       </c>
-      <c r="E115" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>42</v>
@@ -5835,15 +5838,15 @@
         <v>42</v>
       </c>
       <c r="D116" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E116" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>42</v>
@@ -5852,15 +5855,15 @@
         <v>42</v>
       </c>
       <c r="D117" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E117" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>182</v>
+        <v>115</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>42</v>
@@ -5869,15 +5872,15 @@
         <v>42</v>
       </c>
       <c r="D118" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E118" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>42</v>
@@ -5886,15 +5889,15 @@
         <v>42</v>
       </c>
       <c r="D119" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E119" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>42</v>
@@ -5903,15 +5906,15 @@
         <v>42</v>
       </c>
       <c r="D120" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E120" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>42</v>
@@ -5920,15 +5923,15 @@
         <v>42</v>
       </c>
       <c r="D121" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E121" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>42</v>
@@ -5937,15 +5940,15 @@
         <v>42</v>
       </c>
       <c r="D122" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E122" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>42</v>
@@ -5954,15 +5957,15 @@
         <v>42</v>
       </c>
       <c r="D123" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E123" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>42</v>
@@ -5971,15 +5974,15 @@
         <v>42</v>
       </c>
       <c r="D124" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E124" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>42</v>
@@ -5988,19 +5991,223 @@
         <v>42</v>
       </c>
       <c r="D125" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E125" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:6" ht="15" customHeight="1">
       <c r="A126" t="s">
+        <v>153</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D126" t="s">
+        <v>211</v>
+      </c>
+      <c r="E126" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" t="s">
+        <v>155</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D127" t="s">
+        <v>211</v>
+      </c>
+      <c r="E127" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" t="s">
+        <v>174</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D128" t="s">
+        <v>211</v>
+      </c>
+      <c r="E128" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>171</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D129" t="s">
+        <v>211</v>
+      </c>
+      <c r="E129" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>179</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D130" t="s">
+        <v>211</v>
+      </c>
+      <c r="E130" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>88</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D131" t="s">
+        <v>211</v>
+      </c>
+      <c r="E131" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>89</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D132" t="s">
+        <v>211</v>
+      </c>
+      <c r="E132" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>91</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D133" t="s">
+        <v>211</v>
+      </c>
+      <c r="E133" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>90</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D134" t="s">
+        <v>211</v>
+      </c>
+      <c r="E134" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>92</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D135" t="s">
+        <v>211</v>
+      </c>
+      <c r="E135" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
+        <v>93</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D136" t="s">
+        <v>211</v>
+      </c>
+      <c r="E136" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
+        <v>94</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D137" t="s">
+        <v>211</v>
+      </c>
+      <c r="E137" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
-      <c r="A127" t="s">
+    <row r="139" spans="1:5">
+      <c r="A139" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added an extraAttack effect, which was added to the self-duration ability template after much deliberation. I also added the area of effect (aoe) to the target ability. Also, I created and tested a clone function for abilities, which will be used when actually creating new abilities. Finally, I added a beautiful 450x450 bmp background for the creation dialog.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -14,14 +14,14 @@
     <sheet name="Effects" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$99</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="257">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -780,6 +780,18 @@
   </si>
   <si>
     <t>-12,-5,-10,-4,-8,-3,-6,-2,-4,-1,0,0,4,1,6,2,8,3,10,4,12,5</t>
+  </si>
+  <si>
+    <t>extraAttackEnabled</t>
+  </si>
+  <si>
+    <t>extraAttackStartingIndex</t>
+  </si>
+  <si>
+    <t>extraAttack</t>
+  </si>
+  <si>
+    <t>0,0,1,2,2,4,3,6</t>
   </si>
 </sst>
 </file>
@@ -4362,10 +4374,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4531,161 +4543,161 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B12" s="3">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9">
-        <v>1</v>
+        <v>253</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>183</v>
+        <v>254</v>
       </c>
       <c r="B13" s="9">
         <v>0</v>
       </c>
-      <c r="C13" s="9">
-        <v>0</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0</v>
+      <c r="C13" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>149</v>
+        <v>255</v>
       </c>
       <c r="B14" s="9">
         <v>0</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>233</v>
+        <v>148</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>223</v>
+        <v>183</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>223</v>
+        <v>149</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B18" s="9">
-        <v>0</v>
-      </c>
-      <c r="C18" s="9">
-        <v>1</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1</v>
+        <v>243</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B19" s="9">
-        <v>0</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0</v>
-      </c>
-      <c r="D19" s="9">
-        <v>0</v>
+        <v>244</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" s="9">
-        <v>0</v>
+        <v>245</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>248</v>
+        <v>150</v>
       </c>
       <c r="B21" s="9">
         <v>0</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>233</v>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>249</v>
+        <v>184</v>
       </c>
       <c r="B22" s="9">
         <v>0</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>223</v>
+      <c r="C22" s="9">
+        <v>0</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>250</v>
+        <v>151</v>
       </c>
       <c r="B23" s="9">
         <v>0</v>
@@ -4699,24 +4711,24 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>223</v>
+        <v>248</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>233</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>223</v>
+        <v>249</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>223</v>
@@ -4727,21 +4739,21 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>223</v>
+        <v>250</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>247</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>223</v>
@@ -4755,7 +4767,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>223</v>
@@ -4769,13 +4781,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>162</v>
+        <v>247</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>223</v>
@@ -4783,49 +4795,49 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B30" s="9">
-        <v>1</v>
-      </c>
-      <c r="C30" s="9">
-        <v>1</v>
-      </c>
-      <c r="D30" s="9">
-        <v>0</v>
+        <v>240</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B31" s="9">
-        <v>2</v>
-      </c>
-      <c r="C31" s="9">
-        <v>2</v>
-      </c>
-      <c r="D31" s="9">
-        <v>0</v>
+        <v>241</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>115</v>
+        <v>242</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="D32" s="9">
-        <v>0</v>
+        <v>162</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
@@ -4839,13 +4851,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B34" s="9">
         <v>2</v>
       </c>
-      <c r="C34" s="9">
-        <v>2</v>
+      <c r="C34" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D34" s="9">
         <v>0</v>
@@ -4853,13 +4865,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>220</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D35" s="9">
         <v>0</v>
@@ -4867,7 +4879,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
@@ -4881,13 +4893,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B37" s="9">
         <v>2</v>
       </c>
-      <c r="C37" s="9">
-        <v>2</v>
+      <c r="C37" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D37" s="9">
         <v>0</v>
@@ -4895,13 +4907,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>220</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D38" s="9">
         <v>0</v>
@@ -4909,7 +4921,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B39" s="9">
         <v>1</v>
@@ -4923,13 +4935,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B40" s="9">
         <v>2</v>
       </c>
-      <c r="C40" s="9">
-        <v>2</v>
+      <c r="C40" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D40" s="9">
         <v>0</v>
@@ -4937,13 +4949,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>220</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D41" s="9">
         <v>0</v>
@@ -4951,7 +4963,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B42" s="9">
         <v>1</v>
@@ -4965,13 +4977,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B43" s="9">
         <v>2</v>
       </c>
-      <c r="C43" s="9">
-        <v>2</v>
+      <c r="C43" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D43" s="9">
         <v>0</v>
@@ -4979,13 +4991,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>220</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D44" s="9">
         <v>0</v>
@@ -4993,7 +5005,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B45" s="9">
         <v>1</v>
@@ -5007,13 +5019,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B46" s="9">
         <v>2</v>
       </c>
-      <c r="C46" s="9">
-        <v>2</v>
+      <c r="C46" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D46" s="9">
         <v>0</v>
@@ -5021,13 +5033,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>220</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D47" s="9">
         <v>0</v>
@@ -5035,7 +5047,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B48" s="9">
         <v>1</v>
@@ -5049,13 +5061,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B49" s="9">
         <v>2</v>
       </c>
-      <c r="C49" s="9">
-        <v>2</v>
+      <c r="C49" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D49" s="9">
         <v>0</v>
@@ -5063,13 +5075,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>220</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D50" s="9">
         <v>0</v>
@@ -5077,7 +5089,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B51" s="9">
         <v>1</v>
@@ -5091,13 +5103,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B52" s="9">
         <v>2</v>
       </c>
-      <c r="C52" s="9">
-        <v>2</v>
+      <c r="C52" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D52" s="9">
         <v>0</v>
@@ -5105,13 +5117,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>220</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D53" s="9">
         <v>0</v>
@@ -5119,7 +5131,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="B54" s="9">
         <v>1</v>
@@ -5133,13 +5145,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B55" s="9">
         <v>2</v>
       </c>
-      <c r="C55" s="9">
-        <v>2</v>
+      <c r="C55" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D55" s="9">
         <v>0</v>
@@ -5147,13 +5159,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D56" s="9">
         <v>0</v>
@@ -5161,7 +5173,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B57" s="9">
         <v>1</v>
@@ -5175,13 +5187,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>223</v>
+        <v>193</v>
+      </c>
+      <c r="B58" s="9">
+        <v>2</v>
+      </c>
+      <c r="C58" s="9">
+        <v>2</v>
       </c>
       <c r="D58" s="9">
         <v>0</v>
@@ -5189,13 +5201,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="D59" s="9">
         <v>0</v>
@@ -5203,94 +5215,94 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>223</v>
+        <v>154</v>
+      </c>
+      <c r="B60" s="9">
+        <v>1</v>
+      </c>
+      <c r="C60" s="9">
+        <v>1</v>
+      </c>
+      <c r="D60" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>231</v>
+        <v>194</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C61" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C61" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="D61" s="9" t="s">
-        <v>223</v>
+      <c r="D61" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>87</v>
+        <v>155</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>223</v>
+        <v>162</v>
+      </c>
+      <c r="D62" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B63" s="9">
-        <v>0</v>
-      </c>
-      <c r="C63" s="9">
-        <v>1</v>
-      </c>
-      <c r="D63" s="9">
-        <v>0</v>
+        <v>232</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B64" s="9">
-        <v>0</v>
+        <v>231</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>225</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="D64" s="9">
-        <v>0</v>
+        <v>223</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B65" s="9">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>229</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="D65" s="9">
-        <v>0</v>
+        <v>228</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B66" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C66" s="9">
         <v>1</v>
@@ -5301,13 +5313,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B67" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B67" s="9">
+        <v>0</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>225</v>
-      </c>
-      <c r="C67" s="9">
-        <v>0</v>
       </c>
       <c r="D67" s="9">
         <v>0</v>
@@ -5315,13 +5327,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>227</v>
+        <v>174</v>
+      </c>
+      <c r="B68" s="9">
+        <v>0</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="D68" s="9">
         <v>0</v>
@@ -5329,7 +5341,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B69" s="9">
         <v>1</v>
@@ -5343,7 +5355,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>225</v>
@@ -5357,7 +5369,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>227</v>
@@ -5371,7 +5383,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="B72" s="9">
         <v>1</v>
@@ -5385,13 +5397,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C73" s="9" t="s">
-        <v>223</v>
+      <c r="C73" s="9">
+        <v>0</v>
       </c>
       <c r="D73" s="9">
         <v>0</v>
@@ -5399,13 +5411,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>227</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D74" s="9">
         <v>0</v>
@@ -5413,7 +5425,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B75" s="9">
         <v>1</v>
@@ -5427,7 +5439,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B76" s="9" t="s">
         <v>225</v>
@@ -5441,7 +5453,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>227</v>
@@ -5455,7 +5467,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B78" s="9">
         <v>1</v>
@@ -5469,7 +5481,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>225</v>
@@ -5483,7 +5495,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>227</v>
@@ -5497,7 +5509,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B81" s="9">
         <v>1</v>
@@ -5511,7 +5523,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>225</v>
@@ -5525,7 +5537,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B83" s="9" t="s">
         <v>227</v>
@@ -5539,7 +5551,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="B84" s="9">
         <v>1</v>
@@ -5553,7 +5565,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B85" s="9" t="s">
         <v>225</v>
@@ -5567,7 +5579,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>227</v>
@@ -5581,7 +5593,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B87" s="9">
         <v>1</v>
@@ -5595,7 +5607,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B88" s="9" t="s">
         <v>225</v>
@@ -5609,7 +5621,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B89" s="9" t="s">
         <v>227</v>
@@ -5623,7 +5635,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B90" s="9">
         <v>1</v>
@@ -5637,7 +5649,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>225</v>
@@ -5651,7 +5663,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>227</v>
@@ -5665,7 +5677,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B93" s="9">
         <v>1</v>
@@ -5679,7 +5691,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B94" s="9" t="s">
         <v>225</v>
@@ -5693,7 +5705,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>227</v>
@@ -5707,90 +5719,78 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B96" s="9">
+        <v>1</v>
+      </c>
+      <c r="C96" s="9">
+        <v>1</v>
+      </c>
+      <c r="D96" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D97" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D98" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B99" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="C99" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="D96" s="9" t="s">
+      <c r="D99" s="9" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="110" spans="2:6">
-      <c r="B110" s="3" t="s">
+    <row r="113" spans="1:6">
+      <c r="B113" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C113" t="s">
         <v>210</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D113" t="s">
         <v>208</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E113" t="s">
         <v>32</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F113" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="111" spans="2:6" ht="15" customHeight="1">
-      <c r="B111" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D111" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E111" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="112" spans="2:6">
-      <c r="B112" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D112" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E112" t="s">
-        <v>26</v>
-      </c>
-      <c r="F112" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="15" customHeight="1">
-      <c r="A113" t="s">
-        <v>144</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C113" t="s">
-        <v>211</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E113" t="s">
-        <v>207</v>
-      </c>
-      <c r="F113" t="s">
-        <v>213</v>
-      </c>
-    </row>
     <row r="114" spans="1:6" ht="15" customHeight="1">
-      <c r="A114" t="s">
-        <v>86</v>
-      </c>
       <c r="B114" s="3" t="s">
         <v>211</v>
       </c>
@@ -5803,16 +5803,10 @@
       <c r="E114" t="s">
         <v>27</v>
       </c>
-      <c r="F114" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="15" customHeight="1">
-      <c r="A115" t="s">
-        <v>147</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>211</v>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="B115" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>42</v>
@@ -5821,66 +5815,75 @@
         <v>42</v>
       </c>
       <c r="E115" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F115" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="15" customHeight="1">
       <c r="A116" t="s">
-        <v>149</v>
-      </c>
-      <c r="B116" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C116" t="s">
+        <v>211</v>
+      </c>
+      <c r="D116" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C116" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D116" t="s">
+      <c r="E116" t="s">
+        <v>207</v>
+      </c>
+      <c r="F116" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="15" customHeight="1">
+      <c r="A117" t="s">
+        <v>86</v>
+      </c>
+      <c r="B117" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="E116" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117" t="s">
-        <v>151</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E117" t="s">
+        <v>27</v>
+      </c>
+      <c r="F117" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="15" customHeight="1">
+      <c r="A118" t="s">
+        <v>147</v>
+      </c>
+      <c r="B118" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="E117" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="A118" t="s">
-        <v>115</v>
-      </c>
-      <c r="B118" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D118" t="s">
-        <v>211</v>
+      <c r="D118" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="E118" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="F118" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>42</v>
@@ -5897,7 +5900,7 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>42</v>
@@ -5914,7 +5917,7 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>42</v>
@@ -5931,7 +5934,7 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>42</v>
@@ -5948,7 +5951,7 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>42</v>
@@ -5965,7 +5968,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>42</v>
@@ -5982,7 +5985,7 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>42</v>
@@ -5997,12 +6000,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="15" customHeight="1">
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>153</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>211</v>
+        <v>120</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C126" s="7" t="s">
         <v>42</v>
@@ -6011,12 +6014,12 @@
         <v>211</v>
       </c>
       <c r="E126" t="s">
-        <v>217</v>
+        <v>38</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>42</v>
@@ -6033,7 +6036,7 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>42</v>
@@ -6048,12 +6051,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" ht="15" customHeight="1">
       <c r="A129" t="s">
-        <v>171</v>
-      </c>
-      <c r="B129" s="6" t="s">
-        <v>42</v>
+        <v>153</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="C129" s="7" t="s">
         <v>42</v>
@@ -6062,12 +6065,12 @@
         <v>211</v>
       </c>
       <c r="E129" t="s">
-        <v>38</v>
+        <v>217</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>42</v>
@@ -6084,7 +6087,7 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>88</v>
+        <v>174</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>42</v>
@@ -6101,7 +6104,7 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" t="s">
-        <v>89</v>
+        <v>171</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>42</v>
@@ -6118,7 +6121,7 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>91</v>
+        <v>179</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>42</v>
@@ -6135,7 +6138,7 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>42</v>
@@ -6152,7 +6155,7 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>42</v>
@@ -6169,7 +6172,7 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>42</v>
@@ -6186,7 +6189,7 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>42</v>
@@ -6203,11 +6206,62 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D138" t="s">
+        <v>211</v>
+      </c>
+      <c r="E138" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
+        <v>93</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D139" t="s">
+        <v>211</v>
+      </c>
+      <c r="E139" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
+        <v>94</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D140" t="s">
+        <v>211</v>
+      </c>
+      <c r="E140" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to the architecture of the project, individual.h now includes abilities, meaning individuals contain abilities (as it should). This did make for some complications dealing with circular dependencies, specifically with checking if the current abilityInstance would work with the player, which I solved by passing in the player parameters I needed to check manually (see interpretLeftAbilityCreation()). While it's not the ideal solution I was striding for, it doesn't break any big rules for me. Aside from that, I implemented the creation functionality - when the user hits 'c' it checks if the current ability is legal (ability type vs. manaCost) - if so, it adds the new ability to the individual and clears the ability form. Also I added a level parameter to the ability struct, which decreases the totalManaCost by its value (times -1) and also I start the calculateManaCost function at -1 to honor the fact that all abilities get 1 free mana
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="15375" windowHeight="1110" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,14 @@
     <sheet name="Effects" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$145</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="263">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -792,6 +792,24 @@
   </si>
   <si>
     <t>0,0,1,2,2,4,3,6</t>
+  </si>
+  <si>
+    <t>aoeEnabled</t>
+  </si>
+  <si>
+    <t>aoeStartingIndex</t>
+  </si>
+  <si>
+    <t>aoe</t>
+  </si>
+  <si>
+    <t>0,0,1,2,2,3,3,4</t>
+  </si>
+  <si>
+    <t>-5,0,-4,0,-3,0,-2,0,-1,0,0,0,1,0,2,0,3,0,4,0,5,0</t>
+  </si>
+  <si>
+    <t>0,0,1,3,2,6,3,9</t>
   </si>
 </sst>
 </file>
@@ -4374,10 +4392,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4490,7 +4508,7 @@
         <v>86</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>219</v>
+        <v>262</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>218</v>
@@ -4520,8 +4538,8 @@
       <c r="B10" s="9">
         <v>0</v>
       </c>
-      <c r="C10" s="9">
-        <v>0</v>
+      <c r="C10" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>233</v>
@@ -4549,10 +4567,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D12" s="9" t="s">
         <v>233</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4565,8 +4583,8 @@
       <c r="C13" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>223</v>
+      <c r="D13" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4577,10 +4595,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D14" s="9" t="s">
         <v>256</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4753,27 +4771,27 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C27" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>233</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>223</v>
+        <v>258</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>223</v>
@@ -4781,21 +4799,21 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>247</v>
+        <v>259</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>223</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>223</v>
@@ -4809,7 +4827,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>223</v>
@@ -4823,13 +4841,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>162</v>
+        <v>247</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>223</v>
@@ -4837,49 +4855,49 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B33" s="9">
-        <v>1</v>
-      </c>
-      <c r="C33" s="9">
-        <v>1</v>
-      </c>
-      <c r="D33" s="9">
-        <v>0</v>
+        <v>240</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B34" s="9">
-        <v>2</v>
+        <v>241</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="D34" s="9">
-        <v>0</v>
+      <c r="D34" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>115</v>
+        <v>242</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D35" s="9">
-        <v>0</v>
+        <v>162</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
@@ -4893,7 +4911,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B37" s="9">
         <v>2</v>
@@ -4907,7 +4925,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>220</v>
@@ -4921,7 +4939,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B39" s="9">
         <v>1</v>
@@ -4935,7 +4953,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B40" s="9">
         <v>2</v>
@@ -4949,7 +4967,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>220</v>
@@ -4963,7 +4981,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B42" s="9">
         <v>1</v>
@@ -4977,7 +4995,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B43" s="9">
         <v>2</v>
@@ -4991,7 +5009,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>220</v>
@@ -5005,7 +5023,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B45" s="9">
         <v>1</v>
@@ -5019,7 +5037,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B46" s="9">
         <v>2</v>
@@ -5033,7 +5051,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>220</v>
@@ -5047,7 +5065,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B48" s="9">
         <v>1</v>
@@ -5061,7 +5079,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B49" s="9">
         <v>2</v>
@@ -5075,7 +5093,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>220</v>
@@ -5089,7 +5107,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B51" s="9">
         <v>1</v>
@@ -5103,7 +5121,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B52" s="9">
         <v>2</v>
@@ -5117,7 +5135,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>220</v>
@@ -5131,7 +5149,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B54" s="9">
         <v>1</v>
@@ -5145,7 +5163,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B55" s="9">
         <v>2</v>
@@ -5159,7 +5177,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>220</v>
@@ -5173,7 +5191,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="B57" s="9">
         <v>1</v>
@@ -5187,13 +5205,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B58" s="9">
         <v>2</v>
       </c>
-      <c r="C58" s="9">
-        <v>2</v>
+      <c r="C58" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D58" s="9">
         <v>0</v>
@@ -5201,13 +5219,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D59" s="9">
         <v>0</v>
@@ -5215,7 +5233,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B60" s="9">
         <v>1</v>
@@ -5229,13 +5247,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>223</v>
+        <v>193</v>
+      </c>
+      <c r="B61" s="9">
+        <v>2</v>
+      </c>
+      <c r="C61" s="9">
+        <v>2</v>
       </c>
       <c r="D61" s="9">
         <v>0</v>
@@ -5243,13 +5261,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="D62" s="9">
         <v>0</v>
@@ -5257,94 +5275,94 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>223</v>
+        <v>154</v>
+      </c>
+      <c r="B63" s="9">
+        <v>1</v>
+      </c>
+      <c r="C63" s="9">
+        <v>1</v>
+      </c>
+      <c r="D63" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>231</v>
+        <v>194</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C64" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C64" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>223</v>
+      <c r="D64" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>87</v>
+        <v>155</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>223</v>
+        <v>162</v>
+      </c>
+      <c r="D65" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B66" s="9">
-        <v>0</v>
-      </c>
-      <c r="C66" s="9">
-        <v>1</v>
-      </c>
-      <c r="D66" s="9">
-        <v>0</v>
+        <v>232</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B67" s="9">
-        <v>0</v>
+        <v>231</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>225</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="D67" s="9">
-        <v>0</v>
+        <v>223</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B68" s="9">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>229</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="D68" s="9">
-        <v>0</v>
+        <v>228</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B69" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69" s="9">
         <v>1</v>
@@ -5355,13 +5373,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B70" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B70" s="9">
+        <v>0</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>225</v>
-      </c>
-      <c r="C70" s="9">
-        <v>0</v>
       </c>
       <c r="D70" s="9">
         <v>0</v>
@@ -5369,13 +5387,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>227</v>
+        <v>174</v>
+      </c>
+      <c r="B71" s="9">
+        <v>0</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="D71" s="9">
         <v>0</v>
@@ -5383,7 +5401,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B72" s="9">
         <v>1</v>
@@ -5397,7 +5415,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>225</v>
@@ -5411,7 +5429,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>227</v>
@@ -5425,7 +5443,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="B75" s="9">
         <v>1</v>
@@ -5439,13 +5457,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B76" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C76" s="9" t="s">
-        <v>223</v>
+      <c r="C76" s="9">
+        <v>0</v>
       </c>
       <c r="D76" s="9">
         <v>0</v>
@@ -5453,13 +5471,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>227</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D77" s="9">
         <v>0</v>
@@ -5467,7 +5485,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B78" s="9">
         <v>1</v>
@@ -5481,7 +5499,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>225</v>
@@ -5495,10 +5513,10 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>230</v>
@@ -5509,7 +5527,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B81" s="9">
         <v>1</v>
@@ -5523,7 +5541,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>225</v>
@@ -5537,10 +5555,10 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>230</v>
@@ -5551,7 +5569,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B84" s="9">
         <v>1</v>
@@ -5565,7 +5583,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B85" s="9" t="s">
         <v>225</v>
@@ -5579,10 +5597,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>230</v>
@@ -5593,7 +5611,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="B87" s="9">
         <v>1</v>
@@ -5607,7 +5625,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B88" s="9" t="s">
         <v>225</v>
@@ -5621,10 +5639,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="C89" s="9" t="s">
         <v>230</v>
@@ -5635,7 +5653,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B90" s="9">
         <v>1</v>
@@ -5649,7 +5667,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>225</v>
@@ -5663,10 +5681,10 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="C92" s="9" t="s">
         <v>230</v>
@@ -5677,7 +5695,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B93" s="9">
         <v>1</v>
@@ -5691,7 +5709,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B94" s="9" t="s">
         <v>225</v>
@@ -5705,10 +5723,10 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="C95" s="9" t="s">
         <v>230</v>
@@ -5719,7 +5737,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B96" s="9">
         <v>1</v>
@@ -5733,7 +5751,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B97" s="9" t="s">
         <v>225</v>
@@ -5747,10 +5765,10 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="C98" s="9" t="s">
         <v>230</v>
@@ -5761,90 +5779,78 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B99" s="9">
+        <v>1</v>
+      </c>
+      <c r="C99" s="9">
+        <v>1</v>
+      </c>
+      <c r="D99" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D100" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D101" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B102" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C99" s="9" t="s">
+      <c r="C102" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="D99" s="9" t="s">
+      <c r="D102" s="9" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
-      <c r="B113" s="3" t="s">
+    <row r="116" spans="1:6">
+      <c r="B116" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C116" t="s">
         <v>210</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D116" t="s">
         <v>208</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E116" t="s">
         <v>32</v>
       </c>
-      <c r="F113" t="s">
+      <c r="F116" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15" customHeight="1">
-      <c r="B114" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E114" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
-      <c r="B115" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C115" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D115" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E115" t="s">
-        <v>26</v>
-      </c>
-      <c r="F115" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="15" customHeight="1">
-      <c r="A116" t="s">
-        <v>144</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C116" t="s">
-        <v>211</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E116" t="s">
-        <v>207</v>
-      </c>
-      <c r="F116" t="s">
-        <v>213</v>
-      </c>
-    </row>
     <row r="117" spans="1:6" ht="15" customHeight="1">
-      <c r="A117" t="s">
-        <v>86</v>
-      </c>
       <c r="B117" s="3" t="s">
         <v>211</v>
       </c>
@@ -5857,16 +5863,10 @@
       <c r="E117" t="s">
         <v>27</v>
       </c>
-      <c r="F117" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1">
-      <c r="A118" t="s">
-        <v>147</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>211</v>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="B118" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>42</v>
@@ -5875,66 +5875,75 @@
         <v>42</v>
       </c>
       <c r="E118" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F118" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="15" customHeight="1">
       <c r="A119" t="s">
-        <v>149</v>
-      </c>
-      <c r="B119" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C119" t="s">
+        <v>211</v>
+      </c>
+      <c r="D119" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C119" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="E119" t="s">
+        <v>207</v>
+      </c>
+      <c r="F119" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="15" customHeight="1">
+      <c r="A120" t="s">
+        <v>86</v>
+      </c>
+      <c r="B120" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="E119" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120" t="s">
-        <v>151</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E120" t="s">
+        <v>27</v>
+      </c>
+      <c r="F120" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="15" customHeight="1">
+      <c r="A121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B121" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="E120" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121" t="s">
-        <v>115</v>
-      </c>
-      <c r="B121" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D121" t="s">
-        <v>211</v>
+      <c r="D121" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="E121" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="F121" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>42</v>
@@ -5951,7 +5960,7 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>42</v>
@@ -5968,7 +5977,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>42</v>
@@ -5985,7 +5994,7 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>42</v>
@@ -6002,7 +6011,7 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>42</v>
@@ -6019,7 +6028,7 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>42</v>
@@ -6036,7 +6045,7 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>42</v>
@@ -6051,12 +6060,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15" customHeight="1">
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>153</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>211</v>
+        <v>120</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C129" s="7" t="s">
         <v>42</v>
@@ -6065,12 +6074,12 @@
         <v>211</v>
       </c>
       <c r="E129" t="s">
-        <v>217</v>
+        <v>38</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>42</v>
@@ -6087,7 +6096,7 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>42</v>
@@ -6102,12 +6111,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" ht="15" customHeight="1">
       <c r="A132" t="s">
-        <v>171</v>
-      </c>
-      <c r="B132" s="6" t="s">
-        <v>42</v>
+        <v>153</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>42</v>
@@ -6116,12 +6125,12 @@
         <v>211</v>
       </c>
       <c r="E132" t="s">
-        <v>38</v>
+        <v>217</v>
       </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>42</v>
@@ -6138,7 +6147,7 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>88</v>
+        <v>174</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>42</v>
@@ -6155,7 +6164,7 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>89</v>
+        <v>171</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>42</v>
@@ -6172,7 +6181,7 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>91</v>
+        <v>179</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>42</v>
@@ -6189,7 +6198,7 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>42</v>
@@ -6206,7 +6215,7 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>42</v>
@@ -6223,7 +6232,7 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>42</v>
@@ -6240,7 +6249,7 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>42</v>
@@ -6257,11 +6266,62 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D141" t="s">
+        <v>211</v>
+      </c>
+      <c r="E141" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" t="s">
+        <v>93</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C142" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D142" t="s">
+        <v>211</v>
+      </c>
+      <c r="E142" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>94</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D143" t="s">
+        <v>211</v>
+      </c>
+      <c r="E143" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tentative commit: I've been working on implementing the ability naming feature - thus far, there's a background image and a loop, as well as some logic attached to the creation instance containing the working string, the selected letter and working string index. Putting it all together, I have a mostly working naming system which can be controlled with up/down/left/right.
As of now, the specific naming functionality is a little buggy and a
little off from what I want, so I'll continue to refine it once I'm back
from this Easter excursion.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -14,14 +14,14 @@
     <sheet name="Effects" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$146</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="264">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -761,9 +761,6 @@
     <t>damage</t>
   </si>
   <si>
-    <t>0,0,2,-1,4,-2,6,-3,8,-4,10,-5</t>
-  </si>
-  <si>
     <t>0,0,4,2,6,3,8,4,10,5,12,6</t>
   </si>
   <si>
@@ -810,6 +807,12 @@
   </si>
   <si>
     <t>0,0,1,3,2,6,3,9</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>0,0,1,-1,2,-2,3,-3,4,-4,5,-5,6,-6,7,-7,8,-8,9,-9,10,-10</t>
   </si>
 </sst>
 </file>
@@ -4392,10 +4395,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4447,93 +4450,93 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1">
+      <c r="A5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="9">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="9">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:4" s="5" customFormat="1">
+      <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="10">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0</v>
+      <c r="B7" s="10">
+        <v>1</v>
       </c>
       <c r="C7" s="9">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>218</v>
+        <v>181</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>261</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
+        <v>219</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
       <c r="B10" s="9">
         <v>0</v>
@@ -4541,47 +4544,47 @@
       <c r="C10" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>233</v>
+      <c r="D10" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="B11" s="9">
         <v>0</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>161</v>
+        <v>233</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>161</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>253</v>
+        <v>147</v>
       </c>
       <c r="B12" s="9">
         <v>0</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
+        <v>161</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B13" s="9">
         <v>0</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="D13" s="9">
         <v>0</v>
@@ -4589,13 +4592,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B14" s="9">
         <v>0</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -4603,189 +4606,189 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" s="3">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>1</v>
+        <v>254</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>255</v>
       </c>
       <c r="D15" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="9">
+        <v>148</v>
+      </c>
+      <c r="B16" s="3">
         <v>0</v>
       </c>
       <c r="C16" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="B17" s="9">
         <v>0</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>247</v>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>223</v>
+        <v>149</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B21" s="9">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9">
-        <v>1</v>
-      </c>
-      <c r="D21" s="9">
-        <v>1</v>
+        <v>245</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="B22" s="9">
         <v>0</v>
       </c>
       <c r="C22" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="B23" s="9">
         <v>0</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>247</v>
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>248</v>
+        <v>151</v>
       </c>
       <c r="B24" s="9">
         <v>0</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B25" s="9">
         <v>0</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B26" s="9">
         <v>0</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B27" s="9">
         <v>0</v>
       </c>
-      <c r="C27" s="9">
-        <v>0</v>
+      <c r="C27" s="9" t="s">
+        <v>246</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B28" s="9">
         <v>0</v>
@@ -4794,12 +4797,12 @@
         <v>0</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B29" s="9">
         <v>0</v>
@@ -4808,32 +4811,32 @@
         <v>0</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>233</v>
+        <v>258</v>
+      </c>
+      <c r="B30" s="9">
+        <v>0</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>223</v>
@@ -4841,13 +4844,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>223</v>
@@ -4855,13 +4858,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>223</v>
@@ -4869,13 +4872,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>223</v>
@@ -4883,13 +4886,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>223</v>
@@ -4897,27 +4900,27 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B36" s="9">
-        <v>1</v>
-      </c>
-      <c r="C36" s="9">
-        <v>1</v>
-      </c>
-      <c r="D36" s="9">
-        <v>0</v>
+        <v>242</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="B37" s="9">
-        <v>2</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>223</v>
+        <v>1</v>
+      </c>
+      <c r="C37" s="9">
+        <v>1</v>
       </c>
       <c r="D37" s="9">
         <v>0</v>
@@ -4925,13 +4928,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>220</v>
+        <v>185</v>
+      </c>
+      <c r="B38" s="9">
+        <v>2</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D38" s="9">
         <v>0</v>
@@ -4939,13 +4942,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B39" s="9">
-        <v>1</v>
-      </c>
-      <c r="C39" s="9">
-        <v>1</v>
+        <v>115</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="D39" s="9">
         <v>0</v>
@@ -4953,13 +4956,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B40" s="9">
-        <v>2</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>223</v>
+        <v>1</v>
+      </c>
+      <c r="C40" s="9">
+        <v>1</v>
       </c>
       <c r="D40" s="9">
         <v>0</v>
@@ -4967,13 +4970,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>220</v>
+        <v>186</v>
+      </c>
+      <c r="B41" s="9">
+        <v>2</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D41" s="9">
         <v>0</v>
@@ -4981,13 +4984,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B42" s="9">
-        <v>1</v>
-      </c>
-      <c r="C42" s="9">
-        <v>1</v>
+        <v>116</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="D42" s="9">
         <v>0</v>
@@ -4995,13 +4998,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="B43" s="9">
-        <v>2</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>223</v>
+        <v>1</v>
+      </c>
+      <c r="C43" s="9">
+        <v>1</v>
       </c>
       <c r="D43" s="9">
         <v>0</v>
@@ -5009,13 +5012,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>220</v>
+        <v>187</v>
+      </c>
+      <c r="B44" s="9">
+        <v>2</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D44" s="9">
         <v>0</v>
@@ -5023,13 +5026,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="9">
-        <v>1</v>
-      </c>
-      <c r="C45" s="9">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="D45" s="9">
         <v>0</v>
@@ -5037,13 +5040,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="B46" s="9">
-        <v>2</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>223</v>
+        <v>1</v>
+      </c>
+      <c r="C46" s="9">
+        <v>1</v>
       </c>
       <c r="D46" s="9">
         <v>0</v>
@@ -5051,13 +5054,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>220</v>
+        <v>188</v>
+      </c>
+      <c r="B47" s="9">
+        <v>2</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D47" s="9">
         <v>0</v>
@@ -5065,13 +5068,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B48" s="9">
-        <v>1</v>
-      </c>
-      <c r="C48" s="9">
-        <v>1</v>
+        <v>118</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="D48" s="9">
         <v>0</v>
@@ -5079,13 +5082,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="B49" s="9">
-        <v>2</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>223</v>
+        <v>1</v>
+      </c>
+      <c r="C49" s="9">
+        <v>1</v>
       </c>
       <c r="D49" s="9">
         <v>0</v>
@@ -5093,13 +5096,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>220</v>
+        <v>189</v>
+      </c>
+      <c r="B50" s="9">
+        <v>2</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D50" s="9">
         <v>0</v>
@@ -5107,13 +5110,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B51" s="9">
-        <v>1</v>
-      </c>
-      <c r="C51" s="9">
-        <v>1</v>
+        <v>119</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="D51" s="9">
         <v>0</v>
@@ -5121,13 +5124,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="B52" s="9">
-        <v>2</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>223</v>
+        <v>1</v>
+      </c>
+      <c r="C52" s="9">
+        <v>1</v>
       </c>
       <c r="D52" s="9">
         <v>0</v>
@@ -5135,13 +5138,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>220</v>
+        <v>190</v>
+      </c>
+      <c r="B53" s="9">
+        <v>2</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D53" s="9">
         <v>0</v>
@@ -5149,13 +5152,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B54" s="9">
-        <v>1</v>
-      </c>
-      <c r="C54" s="9">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="D54" s="9">
         <v>0</v>
@@ -5163,13 +5166,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="B55" s="9">
-        <v>2</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>223</v>
+        <v>1</v>
+      </c>
+      <c r="C55" s="9">
+        <v>1</v>
       </c>
       <c r="D55" s="9">
         <v>0</v>
@@ -5177,13 +5180,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>220</v>
+        <v>191</v>
+      </c>
+      <c r="B56" s="9">
+        <v>2</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D56" s="9">
         <v>0</v>
@@ -5191,13 +5194,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B57" s="9">
-        <v>1</v>
-      </c>
-      <c r="C57" s="9">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="D57" s="9">
         <v>0</v>
@@ -5205,13 +5208,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B58" s="9">
-        <v>2</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>223</v>
+        <v>1</v>
+      </c>
+      <c r="C58" s="9">
+        <v>1</v>
       </c>
       <c r="D58" s="9">
         <v>0</v>
@@ -5219,13 +5222,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>220</v>
+        <v>192</v>
+      </c>
+      <c r="B59" s="9">
+        <v>2</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D59" s="9">
         <v>0</v>
@@ -5233,13 +5236,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B60" s="9">
-        <v>1</v>
-      </c>
-      <c r="C60" s="9">
-        <v>1</v>
+        <v>122</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="D60" s="9">
         <v>0</v>
@@ -5247,13 +5250,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="B61" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="9">
         <v>0</v>
@@ -5261,13 +5264,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>221</v>
+        <v>193</v>
+      </c>
+      <c r="B62" s="9">
+        <v>2</v>
+      </c>
+      <c r="C62" s="9">
+        <v>2</v>
       </c>
       <c r="D62" s="9">
         <v>0</v>
@@ -5275,13 +5278,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B63" s="9">
-        <v>1</v>
-      </c>
-      <c r="C63" s="9">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="D63" s="9">
         <v>0</v>
@@ -5289,13 +5292,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>223</v>
+        <v>154</v>
+      </c>
+      <c r="B64" s="9">
+        <v>1</v>
+      </c>
+      <c r="C64" s="9">
+        <v>1</v>
       </c>
       <c r="D64" s="9">
         <v>0</v>
@@ -5303,13 +5306,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>162</v>
+        <v>224</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>223</v>
       </c>
       <c r="D65" s="9">
         <v>0</v>
@@ -5317,27 +5320,27 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>232</v>
+        <v>155</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>223</v>
+        <v>162</v>
+      </c>
+      <c r="D66" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>223</v>
@@ -5345,13 +5348,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>87</v>
+        <v>231</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>223</v>
@@ -5359,27 +5362,27 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B69" s="9">
-        <v>0</v>
-      </c>
-      <c r="C69" s="9">
-        <v>1</v>
-      </c>
-      <c r="D69" s="9">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="B70" s="9">
         <v>0</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>225</v>
+      <c r="C70" s="9">
+        <v>1</v>
       </c>
       <c r="D70" s="9">
         <v>0</v>
@@ -5387,13 +5390,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="B71" s="9">
         <v>0</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>252</v>
+        <v>225</v>
       </c>
       <c r="D71" s="9">
         <v>0</v>
@@ -5401,13 +5404,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B72" s="9">
-        <v>1</v>
-      </c>
-      <c r="C72" s="9">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>251</v>
       </c>
       <c r="D72" s="9">
         <v>0</v>
@@ -5415,13 +5418,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>225</v>
+        <v>172</v>
+      </c>
+      <c r="B73" s="9">
+        <v>1</v>
       </c>
       <c r="C73" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73" s="9">
         <v>0</v>
@@ -5429,13 +5432,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="C74" s="9">
+        <v>0</v>
       </c>
       <c r="D74" s="9">
         <v>0</v>
@@ -5443,13 +5446,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B75" s="9">
-        <v>1</v>
-      </c>
-      <c r="C75" s="9">
-        <v>1</v>
+        <v>171</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>226</v>
       </c>
       <c r="D75" s="9">
         <v>0</v>
@@ -5457,13 +5460,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>225</v>
+        <v>180</v>
+      </c>
+      <c r="B76" s="9">
+        <v>1</v>
       </c>
       <c r="C76" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76" s="9">
         <v>0</v>
@@ -5471,13 +5474,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="C77" s="9">
+        <v>0</v>
       </c>
       <c r="D77" s="9">
         <v>0</v>
@@ -5485,13 +5488,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B78" s="9">
-        <v>1</v>
-      </c>
-      <c r="C78" s="9">
-        <v>1</v>
+        <v>179</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>226</v>
       </c>
       <c r="D78" s="9">
         <v>0</v>
@@ -5499,13 +5502,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>223</v>
+        <v>156</v>
+      </c>
+      <c r="B79" s="9">
+        <v>1</v>
+      </c>
+      <c r="C79" s="9">
+        <v>1</v>
       </c>
       <c r="D79" s="9">
         <v>0</v>
@@ -5513,13 +5516,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D80" s="9">
         <v>0</v>
@@ -5527,13 +5530,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B81" s="9">
-        <v>1</v>
-      </c>
-      <c r="C81" s="9">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="D81" s="9">
         <v>0</v>
@@ -5541,13 +5544,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>223</v>
+        <v>157</v>
+      </c>
+      <c r="B82" s="9">
+        <v>1</v>
+      </c>
+      <c r="C82" s="9">
+        <v>1</v>
       </c>
       <c r="D82" s="9">
         <v>0</v>
@@ -5555,13 +5558,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>89</v>
+        <v>199</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D83" s="9">
         <v>0</v>
@@ -5569,13 +5572,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B84" s="9">
-        <v>1</v>
-      </c>
-      <c r="C84" s="9">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="D84" s="9">
         <v>0</v>
@@ -5583,13 +5586,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>223</v>
+        <v>158</v>
+      </c>
+      <c r="B85" s="9">
+        <v>1</v>
+      </c>
+      <c r="C85" s="9">
+        <v>1</v>
       </c>
       <c r="D85" s="9">
         <v>0</v>
@@ -5597,13 +5600,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>91</v>
+        <v>200</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D86" s="9">
         <v>0</v>
@@ -5611,13 +5614,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B87" s="9">
-        <v>1</v>
-      </c>
-      <c r="C87" s="9">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="D87" s="9">
         <v>0</v>
@@ -5625,13 +5628,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>223</v>
+        <v>159</v>
+      </c>
+      <c r="B88" s="9">
+        <v>1</v>
+      </c>
+      <c r="C88" s="9">
+        <v>1</v>
       </c>
       <c r="D88" s="9">
         <v>0</v>
@@ -5639,13 +5642,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D89" s="9">
         <v>0</v>
@@ -5653,13 +5656,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B90" s="9">
-        <v>1</v>
-      </c>
-      <c r="C90" s="9">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="D90" s="9">
         <v>0</v>
@@ -5667,13 +5670,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>223</v>
+        <v>175</v>
+      </c>
+      <c r="B91" s="9">
+        <v>1</v>
+      </c>
+      <c r="C91" s="9">
+        <v>1</v>
       </c>
       <c r="D91" s="9">
         <v>0</v>
@@ -5681,13 +5684,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D92" s="9">
         <v>0</v>
@@ -5695,13 +5698,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B93" s="9">
-        <v>1</v>
-      </c>
-      <c r="C93" s="9">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="D93" s="9">
         <v>0</v>
@@ -5709,13 +5712,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>223</v>
+        <v>176</v>
+      </c>
+      <c r="B94" s="9">
+        <v>1</v>
+      </c>
+      <c r="C94" s="9">
+        <v>1</v>
       </c>
       <c r="D94" s="9">
         <v>0</v>
@@ -5723,13 +5726,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
-        <v>93</v>
+        <v>203</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D95" s="9">
         <v>0</v>
@@ -5737,13 +5740,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B96" s="9">
-        <v>1</v>
-      </c>
-      <c r="C96" s="9">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="D96" s="9">
         <v>0</v>
@@ -5751,13 +5754,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>223</v>
+        <v>177</v>
+      </c>
+      <c r="B97" s="9">
+        <v>1</v>
+      </c>
+      <c r="C97" s="9">
+        <v>1</v>
       </c>
       <c r="D97" s="9">
         <v>0</v>
@@ -5765,13 +5768,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
-        <v>94</v>
+        <v>204</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D98" s="9">
         <v>0</v>
@@ -5779,13 +5782,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B99" s="9">
-        <v>1</v>
-      </c>
-      <c r="C99" s="9">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="D99" s="9">
         <v>0</v>
@@ -5793,13 +5796,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B100" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>223</v>
+        <v>178</v>
+      </c>
+      <c r="B100" s="9">
+        <v>1</v>
+      </c>
+      <c r="C100" s="9">
+        <v>1</v>
       </c>
       <c r="D100" s="9">
         <v>0</v>
@@ -5807,13 +5810,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2" t="s">
-        <v>95</v>
+        <v>205</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D101" s="9">
         <v>0</v>
@@ -5821,52 +5824,52 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D102" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B102" s="9" t="s">
+      <c r="B103" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C102" s="9" t="s">
+      <c r="C103" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="D102" s="9" t="s">
+      <c r="D103" s="9" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
-      <c r="B116" s="3" t="s">
+    <row r="117" spans="1:6">
+      <c r="B117" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" t="s">
         <v>210</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D117" t="s">
         <v>208</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E117" t="s">
         <v>32</v>
       </c>
-      <c r="F116" t="s">
+      <c r="F117" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15" customHeight="1">
-      <c r="B117" s="3" t="s">
+    <row r="118" spans="1:6" ht="15" customHeight="1">
+      <c r="B118" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D117" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E117" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="B118" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>42</v>
@@ -5875,55 +5878,49 @@
         <v>42</v>
       </c>
       <c r="E118" t="s">
-        <v>26</v>
-      </c>
-      <c r="F118" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="15" customHeight="1">
-      <c r="A119" t="s">
-        <v>144</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C119" t="s">
-        <v>211</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="B119" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E119" t="s">
-        <v>207</v>
+        <v>26</v>
       </c>
       <c r="F119" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="15" customHeight="1">
       <c r="A120" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C120" s="7" t="s">
-        <v>42</v>
+      <c r="C120" t="s">
+        <v>211</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E120" t="s">
-        <v>27</v>
+        <v>207</v>
       </c>
       <c r="F120" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="15" customHeight="1">
       <c r="A121" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>211</v>
@@ -5938,29 +5935,32 @@
         <v>27</v>
       </c>
       <c r="F121" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="15" customHeight="1">
       <c r="A122" t="s">
-        <v>149</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>42</v>
+        <v>147</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D122" t="s">
-        <v>211</v>
+      <c r="D122" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="E122" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="F122" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>42</v>
@@ -5977,7 +5977,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>42</v>
@@ -5994,7 +5994,7 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>42</v>
@@ -6011,7 +6011,7 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>42</v>
@@ -6028,7 +6028,7 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>42</v>
@@ -6045,7 +6045,7 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>42</v>
@@ -6062,7 +6062,7 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>42</v>
@@ -6079,7 +6079,7 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>42</v>
@@ -6096,7 +6096,7 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>42</v>
@@ -6111,12 +6111,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="15" customHeight="1">
+    <row r="132" spans="1:5">
       <c r="A132" t="s">
-        <v>153</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>211</v>
+        <v>122</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>42</v>
@@ -6125,15 +6125,15 @@
         <v>211</v>
       </c>
       <c r="E132" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="15" customHeight="1">
       <c r="A133" t="s">
-        <v>155</v>
-      </c>
-      <c r="B133" s="6" t="s">
-        <v>42</v>
+        <v>153</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>42</v>
@@ -6142,12 +6142,12 @@
         <v>211</v>
       </c>
       <c r="E133" t="s">
-        <v>38</v>
+        <v>217</v>
       </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>42</v>
@@ -6164,7 +6164,7 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>42</v>
@@ -6181,7 +6181,7 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>42</v>
@@ -6198,7 +6198,7 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>42</v>
@@ -6215,7 +6215,7 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>42</v>
@@ -6232,7 +6232,7 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>42</v>
@@ -6249,7 +6249,7 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>42</v>
@@ -6266,7 +6266,7 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>42</v>
@@ -6283,7 +6283,7 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>42</v>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>42</v>
@@ -6317,11 +6317,28 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D144" t="s">
+        <v>211</v>
+      </c>
+      <c r="E144" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Well, it's about time to get the big ball rollin. I'm starting to implement abilities into the game mechanics, starting with the concept of 'activeAbilities', and a function similar to the existing getAttribute() ones. Also, in doing so, I realized that I've neglected the 'attack' effect from abilities, so I've implemented it in record time. Aside from that, some minor tweaks to the name box.
Also, I've recently made an important decision -- which I'll try not to
read to deeply into so I don't psych myself out -- I made the repository
private, because I have adopted the goal of getting this game in steam.
It'll require a lot of polish, but the bar seems a bit lower than
expected over there - that said, I wont submit it until I feel
comfortable with it.

Now the real quest starts!
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -14,14 +14,14 @@
     <sheet name="Effects" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$149</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="265">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -656,27 +656,6 @@
     <t>self duration</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>range of attack is different for perminent and self (i can attack further) vs. my spell can hit a target x spaces away</t>
-  </si>
-  <si>
-    <t>weather a spell hits or needs to be rolled</t>
-  </si>
-  <si>
-    <t>For a minus, the player could take dice damage, but would have to make sure that they cant cheat health with it</t>
-  </si>
-  <si>
-    <t>Same as above</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>1,0,3,1,6,2,9,3</t>
   </si>
   <si>
@@ -813,6 +792,30 @@
   </si>
   <si>
     <t>0,0,1,-1,2,-2,3,-3,4,-4,5,-5,6,-6,7,-7,8,-8,9,-9,10,-10</t>
+  </si>
+  <si>
+    <t>Earth, Fire, Water, Lightning - the four elements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether the attack </t>
+  </si>
+  <si>
+    <t>The number of spaces that you can us</t>
+  </si>
+  <si>
+    <t>Perminent</t>
+  </si>
+  <si>
+    <t>the number of times you can perform a physical attack per turn</t>
+  </si>
+  <si>
+    <t>attackEnabled</t>
+  </si>
+  <si>
+    <t>attackStartingIndex</t>
+  </si>
+  <si>
+    <t>-3,-6,-2,-4,-1,-2,0,0,1,2,2,4,3,6</t>
   </si>
 </sst>
 </file>
@@ -836,7 +839,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,24 +849,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -895,7 +880,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -906,11 +891,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -919,6 +899,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4395,10 +4381,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F146"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4452,7 +4438,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -4468,13 +4454,13 @@
       <c r="A5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
         <v>1</v>
       </c>
     </row>
@@ -4482,13 +4468,13 @@
       <c r="A6" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4496,13 +4482,13 @@
       <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="10">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
         <v>1</v>
       </c>
     </row>
@@ -4510,13 +4496,13 @@
       <c r="A8" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B8" s="9">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="9">
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
         <v>0</v>
       </c>
     </row>
@@ -4524,27 +4510,27 @@
       <c r="A9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>218</v>
+      <c r="B9" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="9">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D10" s="6">
         <v>1</v>
       </c>
     </row>
@@ -4552,69 +4538,69 @@
       <c r="A11" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B11" s="9">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>233</v>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B12" s="9">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B13" s="9">
-        <v>0</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D13" s="9">
+        <v>245</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B14" s="9">
-        <v>0</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D14" s="9">
+        <v>246</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="D15" s="9">
+        <v>247</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="D15" s="6">
         <v>0</v>
       </c>
     </row>
@@ -4625,10 +4611,10 @@
       <c r="B16" s="3">
         <v>0</v>
       </c>
-      <c r="C16" s="9">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9">
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
         <v>1</v>
       </c>
     </row>
@@ -4636,13 +4622,13 @@
       <c r="A17" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B17" s="9">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9">
-        <v>0</v>
-      </c>
-      <c r="D17" s="9">
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6">
         <v>0</v>
       </c>
     </row>
@@ -4650,55 +4636,55 @@
       <c r="A18" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="9">
-        <v>0</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>246</v>
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>233</v>
+        <v>236</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>223</v>
+        <v>237</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="D21" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>162</v>
       </c>
     </row>
@@ -4706,13 +4692,13 @@
       <c r="A22" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B22" s="9">
-        <v>0</v>
-      </c>
-      <c r="C22" s="9">
-        <v>1</v>
-      </c>
-      <c r="D22" s="9">
+      <c r="B22" s="6">
+        <v>0</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6">
         <v>1</v>
       </c>
     </row>
@@ -4720,13 +4706,13 @@
       <c r="A23" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B23" s="9">
-        <v>0</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0</v>
-      </c>
-      <c r="D23" s="9">
+      <c r="B23" s="6">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6">
         <v>0</v>
       </c>
     </row>
@@ -4734,195 +4720,195 @@
       <c r="A24" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B24" s="9">
-        <v>0</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>246</v>
+      <c r="B24" s="6">
+        <v>0</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B25" s="9">
-        <v>0</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>233</v>
+        <v>240</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="B26" s="9">
-        <v>0</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>223</v>
+        <v>241</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B27" s="9">
-        <v>0</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>246</v>
+        <v>242</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B28" s="9">
-        <v>0</v>
-      </c>
-      <c r="C28" s="9">
-        <v>0</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>233</v>
+        <v>249</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B29" s="9">
-        <v>0</v>
-      </c>
-      <c r="C29" s="9">
-        <v>0</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>223</v>
+        <v>250</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B30" s="9">
-        <v>0</v>
-      </c>
-      <c r="C30" s="9">
-        <v>0</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>259</v>
+        <v>251</v>
+      </c>
+      <c r="B30" s="6">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>223</v>
+        <v>227</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>223</v>
+        <v>228</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>223</v>
+        <v>229</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C34" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>223</v>
+      <c r="B34" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>223</v>
+        <v>234</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C36" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>223</v>
+      <c r="D36" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B37" s="9">
-        <v>1</v>
-      </c>
-      <c r="C37" s="9">
-        <v>1</v>
-      </c>
-      <c r="D37" s="9">
+      <c r="B37" s="6">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6">
+        <v>1</v>
+      </c>
+      <c r="D37" s="6">
         <v>0</v>
       </c>
     </row>
@@ -4930,13 +4916,13 @@
       <c r="A38" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="6">
         <v>2</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D38" s="9">
+      <c r="C38" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D38" s="6">
         <v>0</v>
       </c>
     </row>
@@ -4944,13 +4930,13 @@
       <c r="A39" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D39" s="9">
+      <c r="B39" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D39" s="6">
         <v>0</v>
       </c>
     </row>
@@ -4958,13 +4944,13 @@
       <c r="A40" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B40" s="9">
-        <v>1</v>
-      </c>
-      <c r="C40" s="9">
-        <v>1</v>
-      </c>
-      <c r="D40" s="9">
+      <c r="B40" s="6">
+        <v>1</v>
+      </c>
+      <c r="C40" s="6">
+        <v>1</v>
+      </c>
+      <c r="D40" s="6">
         <v>0</v>
       </c>
     </row>
@@ -4972,13 +4958,13 @@
       <c r="A41" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="6">
         <v>2</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D41" s="9">
+      <c r="C41" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D41" s="6">
         <v>0</v>
       </c>
     </row>
@@ -4986,13 +4972,13 @@
       <c r="A42" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D42" s="9">
+      <c r="B42" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D42" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5000,13 +4986,13 @@
       <c r="A43" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B43" s="9">
-        <v>1</v>
-      </c>
-      <c r="C43" s="9">
-        <v>1</v>
-      </c>
-      <c r="D43" s="9">
+      <c r="B43" s="6">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6">
+        <v>1</v>
+      </c>
+      <c r="D43" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5014,13 +5000,13 @@
       <c r="A44" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="6">
         <v>2</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D44" s="9">
+      <c r="C44" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D44" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5028,13 +5014,13 @@
       <c r="A45" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B45" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D45" s="9">
+      <c r="B45" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D45" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5042,13 +5028,13 @@
       <c r="A46" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B46" s="9">
-        <v>1</v>
-      </c>
-      <c r="C46" s="9">
-        <v>1</v>
-      </c>
-      <c r="D46" s="9">
+      <c r="B46" s="6">
+        <v>1</v>
+      </c>
+      <c r="C46" s="6">
+        <v>1</v>
+      </c>
+      <c r="D46" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5056,13 +5042,13 @@
       <c r="A47" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="6">
         <v>2</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D47" s="9">
+      <c r="C47" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D47" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5070,13 +5056,13 @@
       <c r="A48" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D48" s="9">
+      <c r="B48" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D48" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5084,13 +5070,13 @@
       <c r="A49" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B49" s="9">
-        <v>1</v>
-      </c>
-      <c r="C49" s="9">
-        <v>1</v>
-      </c>
-      <c r="D49" s="9">
+      <c r="B49" s="6">
+        <v>1</v>
+      </c>
+      <c r="C49" s="6">
+        <v>1</v>
+      </c>
+      <c r="D49" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5098,13 +5084,13 @@
       <c r="A50" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B50" s="9">
+      <c r="B50" s="6">
         <v>2</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D50" s="9">
+      <c r="C50" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D50" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5112,13 +5098,13 @@
       <c r="A51" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D51" s="9">
+      <c r="B51" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D51" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5126,13 +5112,13 @@
       <c r="A52" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="9">
-        <v>1</v>
-      </c>
-      <c r="C52" s="9">
-        <v>1</v>
-      </c>
-      <c r="D52" s="9">
+      <c r="B52" s="6">
+        <v>1</v>
+      </c>
+      <c r="C52" s="6">
+        <v>1</v>
+      </c>
+      <c r="D52" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5140,13 +5126,13 @@
       <c r="A53" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B53" s="6">
         <v>2</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D53" s="9">
+      <c r="C53" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D53" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5154,13 +5140,13 @@
       <c r="A54" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D54" s="9">
+      <c r="B54" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D54" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5168,13 +5154,13 @@
       <c r="A55" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B55" s="9">
-        <v>1</v>
-      </c>
-      <c r="C55" s="9">
-        <v>1</v>
-      </c>
-      <c r="D55" s="9">
+      <c r="B55" s="6">
+        <v>1</v>
+      </c>
+      <c r="C55" s="6">
+        <v>1</v>
+      </c>
+      <c r="D55" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5182,13 +5168,13 @@
       <c r="A56" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B56" s="9">
+      <c r="B56" s="6">
         <v>2</v>
       </c>
-      <c r="C56" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D56" s="9">
+      <c r="C56" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D56" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5196,13 +5182,13 @@
       <c r="A57" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D57" s="9">
+      <c r="B57" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D57" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5210,13 +5196,13 @@
       <c r="A58" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B58" s="9">
-        <v>1</v>
-      </c>
-      <c r="C58" s="9">
-        <v>1</v>
-      </c>
-      <c r="D58" s="9">
+      <c r="B58" s="6">
+        <v>1</v>
+      </c>
+      <c r="C58" s="6">
+        <v>1</v>
+      </c>
+      <c r="D58" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5224,13 +5210,13 @@
       <c r="A59" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B59" s="9">
+      <c r="B59" s="6">
         <v>2</v>
       </c>
-      <c r="C59" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D59" s="9">
+      <c r="C59" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D59" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5238,13 +5224,13 @@
       <c r="A60" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B60" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D60" s="9">
+      <c r="B60" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D60" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5252,13 +5238,13 @@
       <c r="A61" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B61" s="9">
-        <v>1</v>
-      </c>
-      <c r="C61" s="9">
-        <v>1</v>
-      </c>
-      <c r="D61" s="9">
+      <c r="B61" s="6">
+        <v>1</v>
+      </c>
+      <c r="C61" s="6">
+        <v>1</v>
+      </c>
+      <c r="D61" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5266,13 +5252,13 @@
       <c r="A62" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B62" s="6">
         <v>2</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="6">
         <v>2</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="6">
         <v>0</v>
       </c>
     </row>
@@ -5280,1069 +5266,1008 @@
       <c r="A63" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="D63" s="9">
+      <c r="B63" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D63" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B64" s="9">
-        <v>1</v>
-      </c>
-      <c r="C64" s="9">
-        <v>1</v>
-      </c>
-      <c r="D64" s="9">
-        <v>0</v>
+        <v>262</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="D65" s="9">
-        <v>0</v>
+        <v>263</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D66" s="9">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>223</v>
+        <v>154</v>
+      </c>
+      <c r="B67" s="6">
+        <v>1</v>
+      </c>
+      <c r="C67" s="6">
+        <v>1</v>
+      </c>
+      <c r="D67" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>223</v>
+        <v>194</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D68" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>223</v>
+        <v>155</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D69" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B70" s="9">
-        <v>0</v>
-      </c>
-      <c r="C70" s="9">
-        <v>1</v>
-      </c>
-      <c r="D70" s="9">
-        <v>0</v>
+        <v>225</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B71" s="9">
-        <v>0</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="D71" s="9">
-        <v>0</v>
+        <v>224</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B72" s="9">
-        <v>0</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="D72" s="9">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B73" s="9">
-        <v>1</v>
-      </c>
-      <c r="C73" s="9">
-        <v>1</v>
-      </c>
-      <c r="D73" s="9">
+        <v>173</v>
+      </c>
+      <c r="B73" s="6">
+        <v>0</v>
+      </c>
+      <c r="C73" s="6">
+        <v>1</v>
+      </c>
+      <c r="D73" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C74" s="9">
-        <v>0</v>
-      </c>
-      <c r="D74" s="9">
+        <v>195</v>
+      </c>
+      <c r="B74" s="6">
+        <v>0</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D74" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="D75" s="9">
+        <v>174</v>
+      </c>
+      <c r="B75" s="6">
+        <v>0</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D75" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B76" s="9">
-        <v>1</v>
-      </c>
-      <c r="C76" s="9">
-        <v>1</v>
-      </c>
-      <c r="D76" s="9">
+        <v>172</v>
+      </c>
+      <c r="B76" s="6">
+        <v>1</v>
+      </c>
+      <c r="C76" s="6">
+        <v>1</v>
+      </c>
+      <c r="D76" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C77" s="9">
-        <v>0</v>
-      </c>
-      <c r="D77" s="9">
+        <v>196</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C77" s="6">
+        <v>0</v>
+      </c>
+      <c r="D77" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="D78" s="9">
+        <v>171</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D78" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B79" s="9">
-        <v>1</v>
-      </c>
-      <c r="C79" s="9">
-        <v>1</v>
-      </c>
-      <c r="D79" s="9">
+        <v>180</v>
+      </c>
+      <c r="B79" s="6">
+        <v>1</v>
+      </c>
+      <c r="C79" s="6">
+        <v>1</v>
+      </c>
+      <c r="D79" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D80" s="9">
+        <v>197</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C80" s="6">
+        <v>0</v>
+      </c>
+      <c r="D80" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D81" s="9">
+        <v>179</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D81" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B82" s="9">
-        <v>1</v>
-      </c>
-      <c r="C82" s="9">
-        <v>1</v>
-      </c>
-      <c r="D82" s="9">
+        <v>156</v>
+      </c>
+      <c r="B82" s="6">
+        <v>1</v>
+      </c>
+      <c r="C82" s="6">
+        <v>1</v>
+      </c>
+      <c r="D82" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D83" s="9">
+        <v>198</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D83" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D84" s="9">
+        <v>88</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D84" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B85" s="9">
-        <v>1</v>
-      </c>
-      <c r="C85" s="9">
-        <v>1</v>
-      </c>
-      <c r="D85" s="9">
+        <v>157</v>
+      </c>
+      <c r="B85" s="6">
+        <v>1</v>
+      </c>
+      <c r="C85" s="6">
+        <v>1</v>
+      </c>
+      <c r="D85" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D86" s="9">
+        <v>199</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D86" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D87" s="9">
+        <v>89</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D87" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B88" s="9">
-        <v>1</v>
-      </c>
-      <c r="C88" s="9">
-        <v>1</v>
-      </c>
-      <c r="D88" s="9">
+        <v>158</v>
+      </c>
+      <c r="B88" s="6">
+        <v>1</v>
+      </c>
+      <c r="C88" s="6">
+        <v>1</v>
+      </c>
+      <c r="D88" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D89" s="9">
+        <v>200</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D89" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D90" s="9">
+        <v>91</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D90" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B91" s="9">
-        <v>1</v>
-      </c>
-      <c r="C91" s="9">
-        <v>1</v>
-      </c>
-      <c r="D91" s="9">
+        <v>159</v>
+      </c>
+      <c r="B91" s="6">
+        <v>1</v>
+      </c>
+      <c r="C91" s="6">
+        <v>1</v>
+      </c>
+      <c r="D91" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D92" s="9">
+        <v>201</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D92" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D93" s="9">
+        <v>90</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D93" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B94" s="9">
-        <v>1</v>
-      </c>
-      <c r="C94" s="9">
-        <v>1</v>
-      </c>
-      <c r="D94" s="9">
+        <v>175</v>
+      </c>
+      <c r="B94" s="6">
+        <v>1</v>
+      </c>
+      <c r="C94" s="6">
+        <v>1</v>
+      </c>
+      <c r="D94" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D95" s="9">
+        <v>202</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D95" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D96" s="9">
+        <v>92</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D96" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B97" s="9">
-        <v>1</v>
-      </c>
-      <c r="C97" s="9">
-        <v>1</v>
-      </c>
-      <c r="D97" s="9">
+        <v>176</v>
+      </c>
+      <c r="B97" s="6">
+        <v>1</v>
+      </c>
+      <c r="C97" s="6">
+        <v>1</v>
+      </c>
+      <c r="D97" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C98" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D98" s="9">
+        <v>203</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D98" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D99" s="9">
+        <v>93</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D99" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B100" s="9">
-        <v>1</v>
-      </c>
-      <c r="C100" s="9">
-        <v>1</v>
-      </c>
-      <c r="D100" s="9">
+        <v>177</v>
+      </c>
+      <c r="B100" s="6">
+        <v>1</v>
+      </c>
+      <c r="C100" s="6">
+        <v>1</v>
+      </c>
+      <c r="D100" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C101" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D101" s="9">
+        <v>204</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D101" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D102" s="9">
+        <v>94</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D102" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" s="6">
+        <v>1</v>
+      </c>
+      <c r="C103" s="6">
+        <v>1</v>
+      </c>
+      <c r="D103" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D104" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D105" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B103" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="D103" s="9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="B117" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C117" t="s">
-        <v>210</v>
-      </c>
-      <c r="D117" t="s">
-        <v>208</v>
-      </c>
-      <c r="E117" t="s">
-        <v>32</v>
-      </c>
-      <c r="F117" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1">
-      <c r="B118" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C118" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E118" t="s">
-        <v>27</v>
+      <c r="B106" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="119" spans="1:6">
-      <c r="B119" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D119" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E119" t="s">
-        <v>26</v>
-      </c>
-      <c r="F119" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="15" customHeight="1">
+      <c r="B119" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>144</v>
       </c>
-      <c r="B120" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C120" t="s">
-        <v>211</v>
-      </c>
-      <c r="D120" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E120" t="s">
-        <v>207</v>
-      </c>
-      <c r="F120" t="s">
-        <v>213</v>
-      </c>
+      <c r="B120" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
     </row>
     <row r="121" spans="1:6" ht="15" customHeight="1">
       <c r="A121" t="s">
         <v>86</v>
       </c>
-      <c r="B121" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C121" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D121" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E121" t="s">
-        <v>27</v>
-      </c>
-      <c r="F121" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="15" customHeight="1">
+      <c r="B121" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="10"/>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>147</v>
       </c>
-      <c r="B122" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D122" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E122" t="s">
-        <v>27</v>
-      </c>
-      <c r="F122" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
+      <c r="B122" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="10"/>
+    </row>
+    <row r="123" spans="1:6" ht="15" customHeight="1">
       <c r="A123" t="s">
+        <v>247</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+    </row>
+    <row r="124" spans="1:6" ht="15" customHeight="1">
+      <c r="A124" t="s">
         <v>149</v>
       </c>
-      <c r="B123" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D123" t="s">
-        <v>211</v>
-      </c>
-      <c r="E123" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" t="s">
-        <v>151</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D124" t="s">
-        <v>211</v>
-      </c>
-      <c r="E124" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="B124" s="10"/>
+      <c r="C124" s="10"/>
+      <c r="D124" s="10"/>
+      <c r="E124" s="10"/>
+      <c r="F124" s="10"/>
+    </row>
+    <row r="125" spans="1:6" ht="15" customHeight="1">
       <c r="A125" t="s">
-        <v>115</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D125" t="s">
-        <v>211</v>
-      </c>
-      <c r="E125" t="s">
-        <v>38</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="B125" s="10"/>
+      <c r="C125" s="10"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="10"/>
+      <c r="F125" s="10"/>
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>116</v>
-      </c>
-      <c r="B126" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C126" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D126" t="s">
-        <v>211</v>
-      </c>
-      <c r="E126" t="s">
-        <v>38</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="B126" s="10"/>
+      <c r="C126" s="10"/>
+      <c r="D126" s="10"/>
+      <c r="E126" s="10"/>
+      <c r="F126" s="10"/>
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>117</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D127" t="s">
-        <v>211</v>
-      </c>
-      <c r="E127" t="s">
-        <v>38</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
+      <c r="F127" s="10"/>
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
+        <v>251</v>
+      </c>
+      <c r="B128" s="10"/>
+      <c r="C128" s="10"/>
+      <c r="D128" s="10"/>
+      <c r="E128" s="10"/>
+      <c r="F128" s="10"/>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" t="s">
+        <v>229</v>
+      </c>
+      <c r="B129" s="10"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
+      <c r="F129" s="10"/>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" t="s">
+        <v>235</v>
+      </c>
+      <c r="B130" s="10"/>
+      <c r="C130" s="10"/>
+      <c r="D130" s="10"/>
+      <c r="E130" s="10"/>
+      <c r="F130" s="10"/>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" t="s">
+        <v>115</v>
+      </c>
+      <c r="B131" s="10"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" t="s">
+        <v>116</v>
+      </c>
+      <c r="B132" s="10"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
+      <c r="F132" s="10"/>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" t="s">
+        <v>117</v>
+      </c>
+      <c r="B133" s="10"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
+      <c r="F133" s="10"/>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" t="s">
         <v>118</v>
       </c>
-      <c r="B128" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C128" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D128" t="s">
-        <v>211</v>
-      </c>
-      <c r="E128" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5">
-      <c r="A129" t="s">
+      <c r="B134" s="10"/>
+      <c r="C134" s="10"/>
+      <c r="D134" s="10"/>
+      <c r="E134" s="10"/>
+      <c r="F134" s="10"/>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" t="s">
         <v>119</v>
       </c>
-      <c r="B129" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D129" t="s">
-        <v>211</v>
-      </c>
-      <c r="E129" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5">
-      <c r="A130" t="s">
+      <c r="B135" s="10"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
+      <c r="F135" s="10"/>
+    </row>
+    <row r="136" spans="1:6" ht="15" customHeight="1">
+      <c r="A136" t="s">
         <v>120</v>
       </c>
-      <c r="B130" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C130" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D130" t="s">
-        <v>211</v>
-      </c>
-      <c r="E130" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5">
-      <c r="A131" t="s">
+      <c r="B136" s="10"/>
+      <c r="C136" s="10"/>
+      <c r="D136" s="10"/>
+      <c r="E136" s="10"/>
+      <c r="F136" s="10"/>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" t="s">
         <v>121</v>
       </c>
-      <c r="B131" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C131" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D131" t="s">
-        <v>211</v>
-      </c>
-      <c r="E131" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5">
-      <c r="A132" t="s">
+      <c r="B137" s="10"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
+      <c r="F137" s="10"/>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" t="s">
         <v>122</v>
       </c>
-      <c r="B132" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C132" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D132" t="s">
-        <v>211</v>
-      </c>
-      <c r="E132" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" ht="15" customHeight="1">
-      <c r="A133" t="s">
+      <c r="B138" s="10"/>
+      <c r="C138" s="10"/>
+      <c r="D138" s="10"/>
+      <c r="E138" s="10"/>
+      <c r="F138" s="10"/>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" t="s">
         <v>153</v>
       </c>
-      <c r="B133" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D133" t="s">
-        <v>211</v>
-      </c>
-      <c r="E133" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
-      <c r="A134" t="s">
+      <c r="B139" s="10"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
+      <c r="F139" s="10"/>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" t="s">
         <v>155</v>
       </c>
-      <c r="B134" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D134" t="s">
-        <v>211</v>
-      </c>
-      <c r="E134" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5">
-      <c r="A135" t="s">
+      <c r="B140" s="10"/>
+      <c r="C140" s="10"/>
+      <c r="D140" s="10"/>
+      <c r="E140" s="10"/>
+      <c r="F140" s="10"/>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" t="s">
+        <v>87</v>
+      </c>
+      <c r="B141" s="10"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+      <c r="F141" s="10"/>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" t="s">
         <v>174</v>
       </c>
-      <c r="B135" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C135" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D135" t="s">
-        <v>211</v>
-      </c>
-      <c r="E135" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5">
-      <c r="A136" t="s">
+      <c r="B142" s="10"/>
+      <c r="C142" s="10"/>
+      <c r="D142" s="10"/>
+      <c r="E142" s="10"/>
+      <c r="F142" s="10"/>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" t="s">
         <v>171</v>
       </c>
-      <c r="B136" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D136" t="s">
-        <v>211</v>
-      </c>
-      <c r="E136" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
-      <c r="A137" t="s">
+      <c r="B143" s="10"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10"/>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" t="s">
         <v>179</v>
       </c>
-      <c r="B137" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D137" t="s">
-        <v>211</v>
-      </c>
-      <c r="E137" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
-      <c r="A138" t="s">
+      <c r="B144" s="10"/>
+      <c r="C144" s="10"/>
+      <c r="D144" s="10"/>
+      <c r="E144" s="10"/>
+      <c r="F144" s="10"/>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" t="s">
         <v>88</v>
       </c>
-      <c r="B138" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C138" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D138" t="s">
-        <v>211</v>
-      </c>
-      <c r="E138" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5">
-      <c r="A139" t="s">
+      <c r="B145" s="10"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
+      <c r="F145" s="10"/>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" t="s">
         <v>89</v>
       </c>
-      <c r="B139" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C139" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D139" t="s">
-        <v>211</v>
-      </c>
-      <c r="E139" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5">
-      <c r="A140" t="s">
+      <c r="B146" s="10"/>
+      <c r="C146" s="10"/>
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
+      <c r="F146" s="10"/>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" t="s">
         <v>91</v>
       </c>
-      <c r="B140" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D140" t="s">
-        <v>211</v>
-      </c>
-      <c r="E140" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5">
-      <c r="A141" t="s">
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
+      <c r="F147" s="10"/>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" t="s">
         <v>90</v>
       </c>
-      <c r="B141" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C141" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D141" t="s">
-        <v>211</v>
-      </c>
-      <c r="E141" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5">
-      <c r="A142" t="s">
+      <c r="B148" s="10"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
+      <c r="E148" s="10"/>
+      <c r="F148" s="10"/>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" t="s">
         <v>92</v>
       </c>
-      <c r="B142" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C142" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D142" t="s">
-        <v>211</v>
-      </c>
-      <c r="E142" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
-      <c r="A143" t="s">
+      <c r="B149" s="9"/>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" t="s">
         <v>93</v>
       </c>
-      <c r="B143" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C143" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D143" t="s">
-        <v>211</v>
-      </c>
-      <c r="E143" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5">
-      <c r="A144" t="s">
+      <c r="B150" s="9"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" t="s">
         <v>94</v>
       </c>
-      <c r="B144" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C144" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D144" t="s">
-        <v>211</v>
-      </c>
-      <c r="E144" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1">
-      <c r="A145" t="s">
+      <c r="B151" s="9"/>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
-      <c r="A146" t="s">
+      <c r="B152" s="9"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" t="s">
         <v>69</v>
       </c>
+      <c r="B153" s="9"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="34">
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Started implementing active abilities - they can now be processed each turn similar to active items. Currently they lack full processing, but they expire and can be used in the attributeSum calls.
Fixed a rather annoying bug which stemmed from a string not being
malloc'd large enough - was causing SIGTRAP errors - pretty interesting.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -11,17 +11,17 @@
     <sheet name="Items" sheetId="2" r:id="rId2"/>
     <sheet name="Individuals" sheetId="3" r:id="rId3"/>
     <sheet name="Events" sheetId="4" r:id="rId4"/>
-    <sheet name="Effects" sheetId="5" r:id="rId5"/>
+    <sheet name="Abilities" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Effects!$A$1:$A$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Abilities!$A$1:$A$153</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="266">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Dagger</t>
   </si>
   <si>
-    <t>A short knife with a pointed tip.&amp;&amp;(+1 Attack, +1 AC, +1 Dam, +1 MinDam, +1 maxDam, Pierce)</t>
-  </si>
-  <si>
     <t>i</t>
   </si>
   <si>
@@ -668,9 +665,6 @@
     <t>-2,-4,-1,-2,0,0,1,2,2,4</t>
   </si>
   <si>
-    <t>-3,-3,-2,-2,-1,-1,0,0,1,1,2,2,3,3,4,4,5,5,6,6,7,7,8,8,9,9,10,10</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -816,6 +810,15 @@
   </si>
   <si>
     <t>-3,-6,-2,-4,-1,-2,0,0,1,2,2,4,3,6</t>
+  </si>
+  <si>
+    <t>A short knife with a pointed tip.&amp;&amp;(+1 Attack, +1 AC, +1 Dam, Pierce)</t>
+  </si>
+  <si>
+    <t>-3,-3,-2,-2,-1,-1,0,0,1,1,2,2,3,3,4,4,5,5</t>
+  </si>
+  <si>
+    <t>0,0,1,1,2,2,3,3,4,4,5,5</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1307,7 @@
         <v>1003</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1324,7 +1327,7 @@
         <v>1006</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1344,7 +1347,7 @@
         <v>1005</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1364,7 +1367,7 @@
         <v>1007</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1406,7 +1409,7 @@
         <v>1003</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13">
         <v>1005</v>
@@ -1417,7 +1420,7 @@
         <v>1003</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C14">
         <v>1006</v>
@@ -1425,7 +1428,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1433,7 +1436,7 @@
         <v>1004</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1457,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AX10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AX10" sqref="AX10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1471,154 +1474,154 @@
   <sheetData>
     <row r="1" spans="1:50">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R1" t="s">
+        <v>128</v>
+      </c>
+      <c r="S1" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" t="s">
+        <v>130</v>
+      </c>
+      <c r="U1" t="s">
+        <v>131</v>
+      </c>
+      <c r="V1" t="s">
+        <v>132</v>
+      </c>
+      <c r="W1" t="s">
+        <v>133</v>
+      </c>
+      <c r="X1" t="s">
         <v>42</v>
       </c>
-      <c r="O1" t="s">
-        <v>135</v>
-      </c>
-      <c r="P1" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>128</v>
-      </c>
-      <c r="R1" t="s">
-        <v>129</v>
-      </c>
-      <c r="S1" t="s">
-        <v>130</v>
-      </c>
-      <c r="T1" t="s">
-        <v>131</v>
-      </c>
-      <c r="U1" t="s">
-        <v>132</v>
-      </c>
-      <c r="V1" t="s">
-        <v>133</v>
-      </c>
-      <c r="W1" t="s">
-        <v>134</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>50</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>51</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>52</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>53</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>54</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>55</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>56</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>57</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>58</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>59</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>60</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>61</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>62</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>63</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>64</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>65</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>66</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>67</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>68</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:50">
@@ -1770,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="AX2" t="s">
-        <v>16</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:50">
@@ -1784,7 +1787,7 @@
         <v>1002</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -1793,7 +1796,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -1808,7 +1811,7 @@
         <v>255</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3">
         <v>3</v>
@@ -1922,7 +1925,7 @@
         <v>0</v>
       </c>
       <c r="AX3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:50">
@@ -1936,7 +1939,7 @@
         <v>1003</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -1960,7 +1963,7 @@
         <v>255</v>
       </c>
       <c r="L4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -2074,7 +2077,7 @@
         <v>0</v>
       </c>
       <c r="AX4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:50">
@@ -2088,7 +2091,7 @@
         <v>1004</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -2112,7 +2115,7 @@
         <v>255</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M5">
         <v>2</v>
@@ -2226,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="AX5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:50">
@@ -2378,7 +2381,7 @@
         <v>1</v>
       </c>
       <c r="AX6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:50">
@@ -2392,13 +2395,13 @@
         <v>1006</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -2416,7 +2419,7 @@
         <v>255</v>
       </c>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -2530,7 +2533,7 @@
         <v>1</v>
       </c>
       <c r="AX7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:50">
@@ -2544,7 +2547,7 @@
         <v>1007</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -2568,7 +2571,7 @@
         <v>255</v>
       </c>
       <c r="L8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -2682,7 +2685,7 @@
         <v>0</v>
       </c>
       <c r="AX8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:50">
@@ -2696,7 +2699,7 @@
         <v>1008</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -2720,7 +2723,7 @@
         <v>255</v>
       </c>
       <c r="L9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -2834,7 +2837,7 @@
         <v>0</v>
       </c>
       <c r="AX9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:50">
@@ -2986,7 +2989,7 @@
         <v>0</v>
       </c>
       <c r="AX10" t="s">
-        <v>16</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -3006,130 +3009,130 @@
   <sheetData>
     <row r="1" spans="1:42">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>121</v>
+      </c>
+      <c r="R1" t="s">
+        <v>122</v>
+      </c>
+      <c r="S1" t="s">
         <v>80</v>
       </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M1" t="s">
-        <v>118</v>
-      </c>
-      <c r="N1" t="s">
-        <v>119</v>
-      </c>
-      <c r="O1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P1" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>122</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>123</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
+        <v>124</v>
+      </c>
+      <c r="V1" t="s">
         <v>81</v>
       </c>
-      <c r="T1" t="s">
-        <v>124</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1" t="s">
         <v>125</v>
       </c>
-      <c r="V1" t="s">
-        <v>82</v>
-      </c>
-      <c r="W1" t="s">
-        <v>83</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>84</v>
       </c>
-      <c r="Y1" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>85</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>86</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>87</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>88</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>90</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>91</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>92</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>93</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>94</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>95</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>96</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>97</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>98</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>99</v>
       </c>
-      <c r="AO1" t="s">
-        <v>100</v>
-      </c>
       <c r="AP1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:42">
@@ -3149,7 +3152,7 @@
         <v>255</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3209,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="Z2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -3277,7 +3280,7 @@
         <v>255</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -3337,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="Z3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -3405,7 +3408,7 @@
         <v>255</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -3465,7 +3468,7 @@
         <v>0</v>
       </c>
       <c r="Z4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -3533,7 +3536,7 @@
         <v>255</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3593,7 +3596,7 @@
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -3661,7 +3664,7 @@
         <v>255</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -3721,7 +3724,7 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA6">
         <v>1</v>
@@ -3789,7 +3792,7 @@
         <v>255</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -3849,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA7">
         <v>1</v>
@@ -3917,7 +3920,7 @@
         <v>255</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -3977,7 +3980,7 @@
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA8">
         <v>1</v>
@@ -4045,7 +4048,7 @@
         <v>255</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -4105,7 +4108,7 @@
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA9">
         <v>1</v>
@@ -4180,46 +4183,46 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" t="s">
         <v>103</v>
       </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>104</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>105</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>106</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>107</v>
-      </c>
-      <c r="S1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -4254,22 +4257,22 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -4301,7 +4304,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M3">
         <v>206</v>
@@ -4371,7 +4374,7 @@
         <v>1005</v>
       </c>
       <c r="J5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4381,10 +4384,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4396,7 +4400,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="4">
         <v>0</v>
@@ -4408,289 +4412,289 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1">
+    <row r="2" spans="1:4" s="3" customFormat="1" hidden="1">
       <c r="A2" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" hidden="1">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="4" spans="1:4" hidden="1">
+      <c r="A4" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" hidden="1">
+      <c r="A5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" hidden="1">
+      <c r="A6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" hidden="1">
+      <c r="A7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" hidden="1">
+      <c r="A8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" hidden="1">
+      <c r="A9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1">
-      <c r="A5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    </row>
+    <row r="10" spans="1:4" hidden="1">
+      <c r="A10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" hidden="1">
+      <c r="A11" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" hidden="1">
+      <c r="A12" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1">
-      <c r="A7" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" s="6" t="s">
+    </row>
+    <row r="13" spans="1:4" hidden="1">
+      <c r="A13" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" hidden="1">
+      <c r="A14" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" hidden="1">
+      <c r="A15" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" hidden="1">
+      <c r="A16" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" hidden="1">
+      <c r="A17" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" hidden="1">
+      <c r="A18" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" hidden="1">
+      <c r="A19" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" hidden="1">
+      <c r="A20" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" hidden="1">
+      <c r="A21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" s="6">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B13" s="6">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B17" s="6">
-        <v>0</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0</v>
-      </c>
-      <c r="D17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18" s="6">
-        <v>0</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B22" s="6">
         <v>0</v>
@@ -4704,7 +4708,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B23" s="6">
         <v>0</v>
@@ -4718,190 +4722,190 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B24" s="6">
         <v>0</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B25" s="6">
         <v>0</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B26" s="6">
         <v>0</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B27" s="6">
         <v>0</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>239</v>
+        <v>265</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" hidden="1">
       <c r="A28" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" hidden="1">
+      <c r="A29" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" hidden="1">
+      <c r="A30" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B28" s="6">
-        <v>0</v>
-      </c>
-      <c r="C28" s="6">
-        <v>0</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="2" t="s">
+      <c r="B30" s="6">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="B29" s="6">
-        <v>0</v>
-      </c>
-      <c r="C29" s="6">
-        <v>0</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0</v>
-      </c>
-      <c r="C30" s="6">
-        <v>0</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C36" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" hidden="1">
+      <c r="A37" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="B37" s="6">
         <v>1</v>
       </c>
@@ -4912,37 +4916,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" hidden="1">
       <c r="A38" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B38" s="6">
         <v>2</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D38" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" hidden="1">
       <c r="A39" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D39" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" hidden="1">
       <c r="A40" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B40" s="6">
         <v>1</v>
@@ -4954,37 +4958,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" hidden="1">
       <c r="A41" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B41" s="6">
         <v>2</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D41" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" hidden="1">
       <c r="A42" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D42" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" hidden="1">
       <c r="A43" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B43" s="6">
         <v>1</v>
@@ -4996,37 +5000,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" hidden="1">
       <c r="A44" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B44" s="6">
         <v>2</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D44" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" hidden="1">
       <c r="A45" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D45" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" hidden="1">
       <c r="A46" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B46" s="6">
         <v>1</v>
@@ -5038,37 +5042,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" hidden="1">
       <c r="A47" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B47" s="6">
         <v>2</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D47" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" hidden="1">
       <c r="A48" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D48" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" hidden="1">
       <c r="A49" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B49" s="6">
         <v>1</v>
@@ -5080,37 +5084,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" hidden="1">
       <c r="A50" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B50" s="6">
         <v>2</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D50" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" hidden="1">
       <c r="A51" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D51" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" hidden="1">
       <c r="A52" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B52" s="6">
         <v>1</v>
@@ -5122,37 +5126,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" hidden="1">
       <c r="A53" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B53" s="6">
         <v>2</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D53" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" hidden="1">
       <c r="A54" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D54" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" hidden="1">
       <c r="A55" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B55" s="6">
         <v>1</v>
@@ -5164,37 +5168,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" hidden="1">
       <c r="A56" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B56" s="6">
         <v>2</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D56" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" hidden="1">
       <c r="A57" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D57" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" hidden="1">
       <c r="A58" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B58" s="6">
         <v>1</v>
@@ -5206,37 +5210,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" hidden="1">
       <c r="A59" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B59" s="6">
         <v>2</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D59" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" hidden="1">
       <c r="A60" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D60" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" hidden="1">
       <c r="A61" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B61" s="6">
         <v>1</v>
@@ -5248,9 +5252,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" hidden="1">
       <c r="A62" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B62" s="6">
         <v>2</v>
@@ -5262,678 +5266,690 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" hidden="1">
       <c r="A63" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D63" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" hidden="1">
+      <c r="A64" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" hidden="1">
+      <c r="A65" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" hidden="1">
+      <c r="A66" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" hidden="1">
+      <c r="A67" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B67" s="6">
+        <v>1</v>
+      </c>
+      <c r="C67" s="6">
+        <v>1</v>
+      </c>
+      <c r="D67" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" hidden="1">
+      <c r="A68" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="D68" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" hidden="1">
+      <c r="A69" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D69" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" hidden="1">
+      <c r="A70" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D70" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D63" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D64" s="6" t="s">
+    </row>
+    <row r="71" spans="1:4" hidden="1">
+      <c r="A71" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B65" s="6" t="s">
+      <c r="C71" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" hidden="1">
+      <c r="A72" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" hidden="1">
+      <c r="A73" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B73" s="6">
+        <v>0</v>
+      </c>
+      <c r="C73" s="6">
+        <v>1</v>
+      </c>
+      <c r="D73" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" hidden="1">
+      <c r="A74" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B74" s="6">
+        <v>0</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D74" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" hidden="1">
+      <c r="A75" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B75" s="6">
+        <v>0</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D75" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" hidden="1">
+      <c r="A76" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B76" s="6">
+        <v>1</v>
+      </c>
+      <c r="C76" s="6">
+        <v>1</v>
+      </c>
+      <c r="D76" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" hidden="1">
+      <c r="A77" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C77" s="6">
+        <v>0</v>
+      </c>
+      <c r="D77" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" hidden="1">
+      <c r="A78" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C78" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="D78" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" hidden="1">
+      <c r="A79" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B79" s="6">
+        <v>1</v>
+      </c>
+      <c r="C79" s="6">
+        <v>1</v>
+      </c>
+      <c r="D79" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" hidden="1">
+      <c r="A80" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C80" s="6">
+        <v>0</v>
+      </c>
+      <c r="D80" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" hidden="1">
+      <c r="A81" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D81" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" hidden="1">
+      <c r="A82" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82" s="6">
+        <v>1</v>
+      </c>
+      <c r="C82" s="6">
+        <v>1</v>
+      </c>
+      <c r="D82" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" hidden="1">
+      <c r="A83" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="D66" s="6" t="s">
+      <c r="C83" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D83" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" hidden="1">
+      <c r="A84" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D84" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" hidden="1">
+      <c r="A85" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B85" s="6">
+        <v>1</v>
+      </c>
+      <c r="C85" s="6">
+        <v>1</v>
+      </c>
+      <c r="D85" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" hidden="1">
+      <c r="A86" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B86" s="6" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B67" s="6">
-        <v>1</v>
-      </c>
-      <c r="C67" s="6">
-        <v>1</v>
-      </c>
-      <c r="D67" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C68" s="8" t="s">
+      <c r="C86" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D86" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" hidden="1">
+      <c r="A87" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D87" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" hidden="1">
+      <c r="A88" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B88" s="6">
+        <v>1</v>
+      </c>
+      <c r="C88" s="6">
+        <v>1</v>
+      </c>
+      <c r="D88" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" hidden="1">
+      <c r="A89" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B89" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="D68" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D69" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D70" s="6" t="s">
+      <c r="C89" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D89" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" hidden="1">
+      <c r="A90" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D90" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" hidden="1">
+      <c r="A91" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B91" s="6">
+        <v>1</v>
+      </c>
+      <c r="C91" s="6">
+        <v>1</v>
+      </c>
+      <c r="D91" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" hidden="1">
+      <c r="A92" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B92" s="6" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C71" s="6" t="s">
+      <c r="C92" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D92" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" hidden="1">
+      <c r="A93" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D93" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" hidden="1">
+      <c r="A94" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B94" s="6">
+        <v>1</v>
+      </c>
+      <c r="C94" s="6">
+        <v>1</v>
+      </c>
+      <c r="D94" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" hidden="1">
+      <c r="A95" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="C95" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D95" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" hidden="1">
+      <c r="A96" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D96" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" hidden="1">
+      <c r="A97" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B97" s="6">
+        <v>1</v>
+      </c>
+      <c r="C97" s="6">
+        <v>1</v>
+      </c>
+      <c r="D97" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" hidden="1">
+      <c r="A98" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C72" s="6" t="s">
+      <c r="C98" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D98" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" hidden="1">
+      <c r="A99" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="D99" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" hidden="1">
+      <c r="A100" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B100" s="6">
+        <v>1</v>
+      </c>
+      <c r="C100" s="6">
+        <v>1</v>
+      </c>
+      <c r="D100" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" hidden="1">
+      <c r="A101" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B101" s="6" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B73" s="6">
-        <v>0</v>
-      </c>
-      <c r="C73" s="6">
-        <v>1</v>
-      </c>
-      <c r="D73" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B74" s="6">
-        <v>0</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D74" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B75" s="6">
-        <v>0</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D75" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B76" s="6">
-        <v>1</v>
-      </c>
-      <c r="C76" s="6">
-        <v>1</v>
-      </c>
-      <c r="D76" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C77" s="6">
-        <v>0</v>
-      </c>
-      <c r="D77" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D78" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B79" s="6">
-        <v>1</v>
-      </c>
-      <c r="C79" s="6">
-        <v>1</v>
-      </c>
-      <c r="D79" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C80" s="6">
-        <v>0</v>
-      </c>
-      <c r="D80" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D81" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B82" s="6">
-        <v>1</v>
-      </c>
-      <c r="C82" s="6">
-        <v>1</v>
-      </c>
-      <c r="D82" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C83" s="6" t="s">
+      <c r="C101" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D101" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" hidden="1">
+      <c r="A102" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D102" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" hidden="1">
+      <c r="A103" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B103" s="6">
+        <v>1</v>
+      </c>
+      <c r="C103" s="6">
+        <v>1</v>
+      </c>
+      <c r="D103" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" hidden="1">
+      <c r="A104" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="D83" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D84" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B85" s="6">
-        <v>1</v>
-      </c>
-      <c r="C85" s="6">
-        <v>1</v>
-      </c>
-      <c r="D85" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D86" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D87" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B88" s="6">
-        <v>1</v>
-      </c>
-      <c r="C88" s="6">
-        <v>1</v>
-      </c>
-      <c r="D88" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D89" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D90" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B91" s="6">
-        <v>1</v>
-      </c>
-      <c r="C91" s="6">
-        <v>1</v>
-      </c>
-      <c r="D91" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D92" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D93" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B94" s="6">
-        <v>1</v>
-      </c>
-      <c r="C94" s="6">
-        <v>1</v>
-      </c>
-      <c r="D94" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D95" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D96" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B97" s="6">
-        <v>1</v>
-      </c>
-      <c r="C97" s="6">
-        <v>1</v>
-      </c>
-      <c r="D97" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D98" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D99" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B100" s="6">
-        <v>1</v>
-      </c>
-      <c r="C100" s="6">
-        <v>1</v>
-      </c>
-      <c r="D100" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D101" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="2" t="s">
+      <c r="C104" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D104" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" hidden="1">
+      <c r="A105" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B102" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D102" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B103" s="6">
-        <v>1</v>
-      </c>
-      <c r="C103" s="6">
-        <v>1</v>
-      </c>
-      <c r="D103" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D104" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="B105" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D105" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" hidden="1">
       <c r="A106" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B106" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D106" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C106" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="D106" s="6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
+    </row>
+    <row r="107" spans="1:4" hidden="1"/>
+    <row r="108" spans="1:4" hidden="1"/>
+    <row r="109" spans="1:4" hidden="1"/>
+    <row r="110" spans="1:4" hidden="1"/>
+    <row r="111" spans="1:4" hidden="1"/>
+    <row r="112" spans="1:4" hidden="1"/>
+    <row r="113" spans="1:6" hidden="1"/>
+    <row r="114" spans="1:6" hidden="1"/>
+    <row r="115" spans="1:6" hidden="1"/>
+    <row r="116" spans="1:6" hidden="1"/>
+    <row r="117" spans="1:6" hidden="1"/>
+    <row r="118" spans="1:6" hidden="1"/>
+    <row r="119" spans="1:6" hidden="1">
       <c r="B119" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" hidden="1">
       <c r="A120" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C120" s="9"/>
       <c r="D120" s="9"/>
       <c r="E120" s="9"/>
       <c r="F120" s="9"/>
     </row>
-    <row r="121" spans="1:6" ht="15" customHeight="1">
+    <row r="121" spans="1:6" ht="15" hidden="1" customHeight="1">
       <c r="A121" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C121" s="10"/>
       <c r="D121" s="10"/>
       <c r="E121" s="10"/>
       <c r="F121" s="10"/>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" hidden="1">
       <c r="A122" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C122" s="10"/>
       <c r="D122" s="10"/>
       <c r="E122" s="10"/>
       <c r="F122" s="10"/>
     </row>
-    <row r="123" spans="1:6" ht="15" customHeight="1">
+    <row r="123" spans="1:6" ht="15" hidden="1" customHeight="1">
       <c r="A123" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C123" s="10"/>
       <c r="D123" s="10"/>
       <c r="E123" s="10"/>
       <c r="F123" s="10"/>
     </row>
-    <row r="124" spans="1:6" ht="15" customHeight="1">
+    <row r="124" spans="1:6" ht="15" hidden="1" customHeight="1">
       <c r="A124" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B124" s="10"/>
       <c r="C124" s="10"/>
@@ -5941,9 +5957,9 @@
       <c r="E124" s="10"/>
       <c r="F124" s="10"/>
     </row>
-    <row r="125" spans="1:6" ht="15" customHeight="1">
+    <row r="125" spans="1:6" ht="15" hidden="1" customHeight="1">
       <c r="A125" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B125" s="10"/>
       <c r="C125" s="10"/>
@@ -5953,7 +5969,7 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
@@ -5963,7 +5979,7 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B127" s="10"/>
       <c r="C127" s="10"/>
@@ -5971,9 +5987,9 @@
       <c r="E127" s="10"/>
       <c r="F127" s="10"/>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" hidden="1">
       <c r="A128" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B128" s="10"/>
       <c r="C128" s="10"/>
@@ -5983,7 +5999,7 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B129" s="10"/>
       <c r="C129" s="10"/>
@@ -5993,7 +6009,7 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B130" s="10"/>
       <c r="C130" s="10"/>
@@ -6001,9 +6017,9 @@
       <c r="E130" s="10"/>
       <c r="F130" s="10"/>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" hidden="1">
       <c r="A131" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B131" s="10"/>
       <c r="C131" s="10"/>
@@ -6011,9 +6027,9 @@
       <c r="E131" s="10"/>
       <c r="F131" s="10"/>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" hidden="1">
       <c r="A132" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B132" s="10"/>
       <c r="C132" s="10"/>
@@ -6021,9 +6037,9 @@
       <c r="E132" s="10"/>
       <c r="F132" s="10"/>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" hidden="1">
       <c r="A133" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B133" s="10"/>
       <c r="C133" s="10"/>
@@ -6031,9 +6047,9 @@
       <c r="E133" s="10"/>
       <c r="F133" s="10"/>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" hidden="1">
       <c r="A134" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B134" s="10"/>
       <c r="C134" s="10"/>
@@ -6041,9 +6057,9 @@
       <c r="E134" s="10"/>
       <c r="F134" s="10"/>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" hidden="1">
       <c r="A135" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B135" s="10"/>
       <c r="C135" s="10"/>
@@ -6051,9 +6067,9 @@
       <c r="E135" s="10"/>
       <c r="F135" s="10"/>
     </row>
-    <row r="136" spans="1:6" ht="15" customHeight="1">
+    <row r="136" spans="1:6" ht="15" hidden="1" customHeight="1">
       <c r="A136" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B136" s="10"/>
       <c r="C136" s="10"/>
@@ -6061,9 +6077,9 @@
       <c r="E136" s="10"/>
       <c r="F136" s="10"/>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" hidden="1">
       <c r="A137" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B137" s="10"/>
       <c r="C137" s="10"/>
@@ -6071,9 +6087,9 @@
       <c r="E137" s="10"/>
       <c r="F137" s="10"/>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" hidden="1">
       <c r="A138" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B138" s="10"/>
       <c r="C138" s="10"/>
@@ -6081,9 +6097,9 @@
       <c r="E138" s="10"/>
       <c r="F138" s="10"/>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" hidden="1">
       <c r="A139" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B139" s="10"/>
       <c r="C139" s="10"/>
@@ -6091,9 +6107,9 @@
       <c r="E139" s="10"/>
       <c r="F139" s="10"/>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" hidden="1">
       <c r="A140" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
@@ -6101,9 +6117,9 @@
       <c r="E140" s="10"/>
       <c r="F140" s="10"/>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" hidden="1">
       <c r="A141" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
@@ -6111,9 +6127,9 @@
       <c r="E141" s="10"/>
       <c r="F141" s="10"/>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" hidden="1">
       <c r="A142" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
@@ -6121,9 +6137,9 @@
       <c r="E142" s="10"/>
       <c r="F142" s="10"/>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" hidden="1">
       <c r="A143" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B143" s="10"/>
       <c r="C143" s="10"/>
@@ -6131,9 +6147,9 @@
       <c r="E143" s="10"/>
       <c r="F143" s="10"/>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" hidden="1">
       <c r="A144" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
@@ -6141,9 +6157,9 @@
       <c r="E144" s="10"/>
       <c r="F144" s="10"/>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" hidden="1">
       <c r="A145" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B145" s="10"/>
       <c r="C145" s="10"/>
@@ -6151,9 +6167,9 @@
       <c r="E145" s="10"/>
       <c r="F145" s="10"/>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" hidden="1">
       <c r="A146" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B146" s="10"/>
       <c r="C146" s="10"/>
@@ -6161,9 +6177,9 @@
       <c r="E146" s="10"/>
       <c r="F146" s="10"/>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" hidden="1">
       <c r="A147" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B147" s="10"/>
       <c r="C147" s="10"/>
@@ -6171,9 +6187,9 @@
       <c r="E147" s="10"/>
       <c r="F147" s="10"/>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" hidden="1">
       <c r="A148" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B148" s="10"/>
       <c r="C148" s="10"/>
@@ -6181,9 +6197,9 @@
       <c r="E148" s="10"/>
       <c r="F148" s="10"/>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" hidden="1">
       <c r="A149" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
@@ -6191,9 +6207,9 @@
       <c r="E149" s="9"/>
       <c r="F149" s="9"/>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" hidden="1">
       <c r="A150" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B150" s="9"/>
       <c r="C150" s="9"/>
@@ -6201,9 +6217,9 @@
       <c r="E150" s="9"/>
       <c r="F150" s="9"/>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" hidden="1">
       <c r="A151" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B151" s="9"/>
       <c r="C151" s="9"/>
@@ -6211,9 +6227,9 @@
       <c r="E151" s="9"/>
       <c r="F151" s="9"/>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" hidden="1">
       <c r="A152" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B152" s="9"/>
       <c r="C152" s="9"/>
@@ -6221,9 +6237,9 @@
       <c r="E152" s="9"/>
       <c r="F152" s="9"/>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" hidden="1">
       <c r="A153" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
@@ -6232,6 +6248,13 @@
       <c r="F153" s="9"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A153">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter val="*duration*"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="34">
     <mergeCell ref="B120:F120"/>
     <mergeCell ref="B148:F148"/>

</xml_diff>

<commit_message>
Tentative Commit: I'm implementing Status and I've made most of the infrastructure changes - this includes creating a new struct to deal with types. It functions very similar to the effectAndManaMapLists, however instead of a numeric effect value it's a string. I have yet to implement the left/right functionality in the ability_creation instance, and I need to update the effect_template. And once I'm finished with that, I'll have to actually implement the status functionality!
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -14,14 +14,14 @@
     <sheet name="Abilities" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Abilities!$A$1:$A$153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Abilities!$A$1:$A$165</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="280">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -470,9 +470,6 @@
     <t>diceDamage</t>
   </si>
   <si>
-    <t>diceDamagedurationEnabled</t>
-  </si>
-  <si>
     <t>diceDamageDuration</t>
   </si>
   <si>
@@ -572,9 +569,6 @@
     <t>diceDamageStartingIndex</t>
   </si>
   <si>
-    <t>diceDamagedurationStartingIndex</t>
-  </si>
-  <si>
     <t>STRStartingIndex</t>
   </si>
   <si>
@@ -737,12 +731,6 @@
     <t>0,0,4,2,6,3,8,4,10,5,12,6</t>
   </si>
   <si>
-    <t>diceDamagedurationModEnabled</t>
-  </si>
-  <si>
-    <t>diceDamagedurationModStartingIndex</t>
-  </si>
-  <si>
     <t>diceDamageDurationMod</t>
   </si>
   <si>
@@ -819,6 +807,60 @@
   </si>
   <si>
     <t>0,0,1,1,2,2,3,3,4,4,5,5</t>
+  </si>
+  <si>
+    <t>statusEnabled</t>
+  </si>
+  <si>
+    <t>statusStartingIndex</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>statusDiceDamageEnabled</t>
+  </si>
+  <si>
+    <t>statusDiceDamageStartingIndex</t>
+  </si>
+  <si>
+    <t>statusDiceDamage</t>
+  </si>
+  <si>
+    <t>statusDamageEnabled</t>
+  </si>
+  <si>
+    <t>statusDamageStartingIndex</t>
+  </si>
+  <si>
+    <t>statusDamage</t>
+  </si>
+  <si>
+    <t>statusDuration</t>
+  </si>
+  <si>
+    <t>statusDurationEnabled</t>
+  </si>
+  <si>
+    <t>statusDurationStartingIndex</t>
+  </si>
+  <si>
+    <t>statusDurationMod</t>
+  </si>
+  <si>
+    <t>statusDurationModStartingIndex</t>
+  </si>
+  <si>
+    <t>statusDurationModEnabled</t>
+  </si>
+  <si>
+    <t>diceHpEnabled</t>
+  </si>
+  <si>
+    <t>diceHpStartingIndex</t>
+  </si>
+  <si>
+    <t>diceHp</t>
   </si>
 </sst>
 </file>
@@ -1773,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="AX2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:50">
@@ -2989,7 +3031,7 @@
         <v>0</v>
       </c>
       <c r="AX10" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3001,8 +3043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP9"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4168,8 +4210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="A2:J5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4177,6 +4219,7 @@
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -4385,10 +4428,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F153"/>
+  <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4412,9 +4455,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" hidden="1">
+    <row r="2" spans="1:4" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -4423,26 +4466,26 @@
         <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" hidden="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" hidden="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -4454,7 +4497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" hidden="1">
+    <row r="5" spans="1:4" s="3" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>142</v>
       </c>
@@ -4468,21 +4511,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" hidden="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>144</v>
       </c>
@@ -4496,9 +4539,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -4510,21 +4553,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" hidden="1">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>145</v>
       </c>
@@ -4532,27 +4575,27 @@
         <v>0</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" s="6">
         <v>0</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" hidden="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>146</v>
       </c>
@@ -4560,55 +4603,55 @@
         <v>0</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" hidden="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B13" s="6">
         <v>0</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D13" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B14" s="6">
         <v>0</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D14" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B15" s="6">
         <v>0</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D15" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>147</v>
       </c>
@@ -4622,9 +4665,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B17" s="6">
         <v>0</v>
@@ -4636,7 +4679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>148</v>
       </c>
@@ -4644,393 +4687,339 @@
         <v>0</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" hidden="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" hidden="1">
-      <c r="A20" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" hidden="1">
-      <c r="A21" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="B21" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B22" s="6">
-        <v>0</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6">
-        <v>1</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B23" s="6">
-        <v>0</v>
-      </c>
-      <c r="C23" s="6">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6">
-        <v>0</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B24" s="6">
-        <v>0</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>237</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="B25" s="6">
         <v>0</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>224</v>
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="B26" s="6">
         <v>0</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>214</v>
+      <c r="C26" s="6">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="B27" s="6">
         <v>0</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" hidden="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>247</v>
+        <v>268</v>
       </c>
       <c r="B28" s="6">
         <v>0</v>
       </c>
-      <c r="C28" s="6">
-        <v>0</v>
+      <c r="C28" s="6" t="s">
+        <v>222</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" hidden="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>248</v>
+        <v>269</v>
       </c>
       <c r="B29" s="6">
         <v>0</v>
       </c>
-      <c r="C29" s="6">
-        <v>0</v>
+      <c r="C29" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" hidden="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>249</v>
+        <v>270</v>
       </c>
       <c r="B30" s="6">
         <v>0</v>
       </c>
-      <c r="C30" s="6">
-        <v>0</v>
+      <c r="C30" s="6" t="s">
+        <v>261</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>214</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>214</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>214</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>214</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>214</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" hidden="1">
+        <v>274</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
       <c r="B37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" s="6">
-        <v>1</v>
-      </c>
-      <c r="D37" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" hidden="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>184</v>
+        <v>244</v>
       </c>
       <c r="B38" s="6">
-        <v>2</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D38" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" hidden="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B39" s="6">
+        <v>0</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D39" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" hidden="1">
-      <c r="A40" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B40" s="6">
-        <v>1</v>
-      </c>
-      <c r="C40" s="6">
-        <v>1</v>
-      </c>
-      <c r="D40" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" hidden="1">
+      <c r="C40" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B41" s="6">
-        <v>2</v>
+        <v>224</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D41" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" hidden="1">
+        <v>212</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>115</v>
+        <v>225</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D42" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" hidden="1">
+        <v>235</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B43" s="6">
-        <v>1</v>
-      </c>
-      <c r="C43" s="6">
-        <v>1</v>
-      </c>
-      <c r="D43" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" hidden="1">
+        <v>229</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B44" s="6">
-        <v>2</v>
+        <v>230</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D44" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" hidden="1">
+        <v>212</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>116</v>
+        <v>231</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D45" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" hidden="1">
+        <v>160</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B46" s="6">
         <v>1</v>
@@ -5042,37 +5031,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1">
+    <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B47" s="6">
         <v>2</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D47" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1">
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D48" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B49" s="6">
         <v>1</v>
@@ -5084,37 +5073,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B50" s="6">
         <v>2</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D50" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1">
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D51" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B52" s="6">
         <v>1</v>
@@ -5126,37 +5115,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B53" s="6">
         <v>2</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D53" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1">
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D54" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1">
+    <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B55" s="6">
         <v>1</v>
@@ -5168,37 +5157,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B56" s="6">
         <v>2</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D56" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D57" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1">
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B58" s="6">
         <v>1</v>
@@ -5210,37 +5199,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1">
+    <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B59" s="6">
         <v>2</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D59" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1">
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D60" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1">
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B61" s="6">
         <v>1</v>
@@ -5252,275 +5241,275 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1">
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B62" s="6">
         <v>2</v>
       </c>
-      <c r="C62" s="6">
+      <c r="C62" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D62" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D63" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" s="6">
+        <v>1</v>
+      </c>
+      <c r="C64" s="6">
+        <v>1</v>
+      </c>
+      <c r="D64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B65" s="6">
         <v>2</v>
       </c>
-      <c r="D62" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" hidden="1">
-      <c r="A63" s="2" t="s">
+      <c r="C65" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D65" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D66" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B67" s="6">
+        <v>1</v>
+      </c>
+      <c r="C67" s="6">
+        <v>1</v>
+      </c>
+      <c r="D67" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B68" s="6">
+        <v>2</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D68" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D69" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B70" s="6">
+        <v>1</v>
+      </c>
+      <c r="C70" s="6">
+        <v>1</v>
+      </c>
+      <c r="D70" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B71" s="6">
+        <v>2</v>
+      </c>
+      <c r="C71" s="6">
+        <v>2</v>
+      </c>
+      <c r="D71" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D72" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B76" s="6">
+        <v>1</v>
+      </c>
+      <c r="C76" s="6">
+        <v>1</v>
+      </c>
+      <c r="D76" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C63" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D63" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" hidden="1">
-      <c r="A64" s="2" t="s">
+      <c r="C77" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D77" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D64" s="6" t="s">
+      <c r="C78" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D78" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" hidden="1">
-      <c r="A65" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" hidden="1">
-      <c r="A66" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" hidden="1">
-      <c r="A67" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B67" s="6">
-        <v>1</v>
-      </c>
-      <c r="C67" s="6">
-        <v>1</v>
-      </c>
-      <c r="D67" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" hidden="1">
-      <c r="A68" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="D68" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" hidden="1">
-      <c r="A69" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="D69" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" hidden="1">
-      <c r="A70" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" hidden="1">
-      <c r="A71" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" hidden="1">
-      <c r="A72" s="2" t="s">
+      <c r="C80" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" hidden="1">
-      <c r="A73" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B73" s="6">
-        <v>0</v>
-      </c>
-      <c r="C73" s="6">
-        <v>1</v>
-      </c>
-      <c r="D73" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" hidden="1">
-      <c r="A74" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B74" s="6">
-        <v>0</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D74" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" hidden="1">
-      <c r="A75" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B75" s="6">
-        <v>0</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D75" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" hidden="1">
-      <c r="A76" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B76" s="6">
-        <v>1</v>
-      </c>
-      <c r="C76" s="6">
-        <v>1</v>
-      </c>
-      <c r="D76" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" hidden="1">
-      <c r="A77" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C77" s="6">
-        <v>0</v>
-      </c>
-      <c r="D77" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" hidden="1">
-      <c r="A78" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D78" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" hidden="1">
-      <c r="A79" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B79" s="6">
-        <v>1</v>
-      </c>
-      <c r="C79" s="6">
-        <v>1</v>
-      </c>
-      <c r="D79" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" hidden="1">
-      <c r="A80" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C80" s="6">
-        <v>0</v>
-      </c>
-      <c r="D80" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" hidden="1">
-      <c r="A81" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>218</v>
@@ -5528,58 +5517,40 @@
       <c r="C81" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="D81" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" hidden="1">
+      <c r="D81" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B82" s="6">
-        <v>1</v>
-      </c>
-      <c r="C82" s="6">
-        <v>1</v>
-      </c>
-      <c r="D82" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" hidden="1">
+        <v>277</v>
+      </c>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D83" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" hidden="1">
+        <v>278</v>
+      </c>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D84" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" hidden="1">
+        <v>279</v>
+      </c>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="B85" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" s="6">
         <v>1</v>
@@ -5588,12 +5559,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1">
+    <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>216</v>
+        <v>192</v>
+      </c>
+      <c r="B86" s="6">
+        <v>0</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>214</v>
@@ -5602,474 +5573,510 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1">
+    <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="6">
+        <v>0</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D87" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B88" s="6">
+        <v>1</v>
+      </c>
+      <c r="C88" s="6">
+        <v>1</v>
+      </c>
+      <c r="D88" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C89" s="6">
+        <v>0</v>
+      </c>
+      <c r="D89" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D90" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B91" s="6">
+        <v>1</v>
+      </c>
+      <c r="C91" s="6">
+        <v>1</v>
+      </c>
+      <c r="D91" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C92" s="6">
+        <v>0</v>
+      </c>
+      <c r="D92" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D93" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B94" s="6">
+        <v>1</v>
+      </c>
+      <c r="C94" s="6">
+        <v>1</v>
+      </c>
+      <c r="D94" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D95" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D96" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B97" s="6">
+        <v>1</v>
+      </c>
+      <c r="C97" s="6">
+        <v>1</v>
+      </c>
+      <c r="D97" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D98" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B99" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D99" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B100" s="6">
+        <v>1</v>
+      </c>
+      <c r="C100" s="6">
+        <v>1</v>
+      </c>
+      <c r="D100" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D101" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D102" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B103" s="6">
+        <v>1</v>
+      </c>
+      <c r="C103" s="6">
+        <v>1</v>
+      </c>
+      <c r="D103" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D104" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D105" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B106" s="6">
+        <v>1</v>
+      </c>
+      <c r="C106" s="6">
+        <v>1</v>
+      </c>
+      <c r="D106" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D107" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D108" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B109" s="6">
+        <v>1</v>
+      </c>
+      <c r="C109" s="6">
+        <v>1</v>
+      </c>
+      <c r="D109" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D110" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D111" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B112" s="6">
+        <v>1</v>
+      </c>
+      <c r="C112" s="6">
+        <v>1</v>
+      </c>
+      <c r="D112" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D113" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D114" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B115" s="6">
+        <v>1</v>
+      </c>
+      <c r="C115" s="6">
+        <v>1</v>
+      </c>
+      <c r="D115" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D116" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D117" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="B131" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" t="s">
+        <v>143</v>
+      </c>
+      <c r="B132" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="C87" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D87" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" hidden="1">
-      <c r="A88" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B88" s="6">
-        <v>1</v>
-      </c>
-      <c r="C88" s="6">
-        <v>1</v>
-      </c>
-      <c r="D88" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" hidden="1">
-      <c r="A89" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D89" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" hidden="1">
-      <c r="A90" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D90" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" hidden="1">
-      <c r="A91" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B91" s="6">
-        <v>1</v>
-      </c>
-      <c r="C91" s="6">
-        <v>1</v>
-      </c>
-      <c r="D91" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" hidden="1">
-      <c r="A92" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D92" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" hidden="1">
-      <c r="A93" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D93" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" hidden="1">
-      <c r="A94" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B94" s="6">
-        <v>1</v>
-      </c>
-      <c r="C94" s="6">
-        <v>1</v>
-      </c>
-      <c r="D94" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" hidden="1">
-      <c r="A95" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D95" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" hidden="1">
-      <c r="A96" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D96" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" hidden="1">
-      <c r="A97" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B97" s="6">
-        <v>1</v>
-      </c>
-      <c r="C97" s="6">
-        <v>1</v>
-      </c>
-      <c r="D97" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" hidden="1">
-      <c r="A98" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D98" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" hidden="1">
-      <c r="A99" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D99" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" hidden="1">
-      <c r="A100" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B100" s="6">
-        <v>1</v>
-      </c>
-      <c r="C100" s="6">
-        <v>1</v>
-      </c>
-      <c r="D100" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" hidden="1">
-      <c r="A101" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D101" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" hidden="1">
-      <c r="A102" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D102" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" hidden="1">
-      <c r="A103" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B103" s="6">
-        <v>1</v>
-      </c>
-      <c r="C103" s="6">
-        <v>1</v>
-      </c>
-      <c r="D103" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" hidden="1">
-      <c r="A104" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D104" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" hidden="1">
-      <c r="A105" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D105" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" hidden="1">
-      <c r="A106" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D106" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" hidden="1"/>
-    <row r="108" spans="1:4" hidden="1"/>
-    <row r="109" spans="1:4" hidden="1"/>
-    <row r="110" spans="1:4" hidden="1"/>
-    <row r="111" spans="1:4" hidden="1"/>
-    <row r="112" spans="1:4" hidden="1"/>
-    <row r="113" spans="1:6" hidden="1"/>
-    <row r="114" spans="1:6" hidden="1"/>
-    <row r="115" spans="1:6" hidden="1"/>
-    <row r="116" spans="1:6" hidden="1"/>
-    <row r="117" spans="1:6" hidden="1"/>
-    <row r="118" spans="1:6" hidden="1"/>
-    <row r="119" spans="1:6" hidden="1">
-      <c r="B119" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" hidden="1">
-      <c r="A120" t="s">
-        <v>143</v>
-      </c>
-      <c r="B120" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
-    </row>
-    <row r="121" spans="1:6" ht="15" hidden="1" customHeight="1">
-      <c r="A121" t="s">
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+    </row>
+    <row r="133" spans="1:6" ht="15" customHeight="1">
+      <c r="A133" t="s">
         <v>85</v>
       </c>
-      <c r="B121" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
-      <c r="E121" s="10"/>
-      <c r="F121" s="10"/>
-    </row>
-    <row r="122" spans="1:6" hidden="1">
-      <c r="A122" t="s">
-        <v>146</v>
-      </c>
-      <c r="B122" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
-      <c r="E122" s="10"/>
-      <c r="F122" s="10"/>
-    </row>
-    <row r="123" spans="1:6" ht="15" hidden="1" customHeight="1">
-      <c r="A123" t="s">
-        <v>245</v>
-      </c>
-      <c r="B123" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="C123" s="10"/>
-      <c r="D123" s="10"/>
-      <c r="E123" s="10"/>
-      <c r="F123" s="10"/>
-    </row>
-    <row r="124" spans="1:6" ht="15" hidden="1" customHeight="1">
-      <c r="A124" t="s">
-        <v>148</v>
-      </c>
-      <c r="B124" s="10"/>
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
-      <c r="E124" s="10"/>
-      <c r="F124" s="10"/>
-    </row>
-    <row r="125" spans="1:6" ht="15" hidden="1" customHeight="1">
-      <c r="A125" t="s">
-        <v>236</v>
-      </c>
-      <c r="B125" s="10"/>
-      <c r="C125" s="10"/>
-      <c r="D125" s="10"/>
-      <c r="E125" s="10"/>
-      <c r="F125" s="10"/>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126" t="s">
-        <v>150</v>
-      </c>
-      <c r="B126" s="10"/>
-      <c r="C126" s="10"/>
-      <c r="D126" s="10"/>
-      <c r="E126" s="10"/>
-      <c r="F126" s="10"/>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127" t="s">
-        <v>240</v>
-      </c>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
-      <c r="E127" s="10"/>
-      <c r="F127" s="10"/>
-    </row>
-    <row r="128" spans="1:6" hidden="1">
-      <c r="A128" t="s">
-        <v>249</v>
-      </c>
-      <c r="B128" s="10"/>
-      <c r="C128" s="10"/>
-      <c r="D128" s="10"/>
-      <c r="E128" s="10"/>
-      <c r="F128" s="10"/>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129" t="s">
-        <v>227</v>
-      </c>
-      <c r="B129" s="10"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="10"/>
-      <c r="F129" s="10"/>
-    </row>
-    <row r="130" spans="1:6">
-      <c r="A130" t="s">
-        <v>233</v>
-      </c>
-      <c r="B130" s="10"/>
-      <c r="C130" s="10"/>
-      <c r="D130" s="10"/>
-      <c r="E130" s="10"/>
-      <c r="F130" s="10"/>
-    </row>
-    <row r="131" spans="1:6" hidden="1">
-      <c r="A131" t="s">
-        <v>114</v>
-      </c>
-      <c r="B131" s="10"/>
-      <c r="C131" s="10"/>
-      <c r="D131" s="10"/>
-      <c r="E131" s="10"/>
-      <c r="F131" s="10"/>
-    </row>
-    <row r="132" spans="1:6" hidden="1">
-      <c r="A132" t="s">
-        <v>115</v>
-      </c>
-      <c r="B132" s="10"/>
-      <c r="C132" s="10"/>
-      <c r="D132" s="10"/>
-      <c r="E132" s="10"/>
-      <c r="F132" s="10"/>
-    </row>
-    <row r="133" spans="1:6" hidden="1">
-      <c r="A133" t="s">
-        <v>116</v>
-      </c>
-      <c r="B133" s="10"/>
+      <c r="B133" s="10" t="s">
+        <v>253</v>
+      </c>
       <c r="C133" s="10"/>
       <c r="D133" s="10"/>
       <c r="E133" s="10"/>
       <c r="F133" s="10"/>
     </row>
-    <row r="134" spans="1:6" hidden="1">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>117</v>
-      </c>
-      <c r="B134" s="10"/>
+        <v>146</v>
+      </c>
+      <c r="B134" s="10" t="s">
+        <v>252</v>
+      </c>
       <c r="C134" s="10"/>
       <c r="D134" s="10"/>
       <c r="E134" s="10"/>
       <c r="F134" s="10"/>
     </row>
-    <row r="135" spans="1:6" hidden="1">
+    <row r="135" spans="1:6" ht="15" customHeight="1">
       <c r="A135" t="s">
-        <v>118</v>
-      </c>
-      <c r="B135" s="10"/>
+        <v>241</v>
+      </c>
+      <c r="B135" s="10" t="s">
+        <v>255</v>
+      </c>
       <c r="C135" s="10"/>
       <c r="D135" s="10"/>
       <c r="E135" s="10"/>
       <c r="F135" s="10"/>
     </row>
-    <row r="136" spans="1:6" ht="15" hidden="1" customHeight="1">
+    <row r="136" spans="1:6" ht="15" customHeight="1">
       <c r="A136" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="B136" s="10"/>
       <c r="C136" s="10"/>
@@ -6077,9 +6084,9 @@
       <c r="E136" s="10"/>
       <c r="F136" s="10"/>
     </row>
-    <row r="137" spans="1:6" hidden="1">
+    <row r="137" spans="1:6" ht="15" customHeight="1">
       <c r="A137" t="s">
-        <v>120</v>
+        <v>234</v>
       </c>
       <c r="B137" s="10"/>
       <c r="C137" s="10"/>
@@ -6087,9 +6094,9 @@
       <c r="E137" s="10"/>
       <c r="F137" s="10"/>
     </row>
-    <row r="138" spans="1:6" hidden="1">
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="B138" s="10"/>
       <c r="C138" s="10"/>
@@ -6097,9 +6104,9 @@
       <c r="E138" s="10"/>
       <c r="F138" s="10"/>
     </row>
-    <row r="139" spans="1:6" hidden="1">
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="B139" s="10"/>
       <c r="C139" s="10"/>
@@ -6107,9 +6114,9 @@
       <c r="E139" s="10"/>
       <c r="F139" s="10"/>
     </row>
-    <row r="140" spans="1:6" hidden="1">
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>154</v>
+        <v>245</v>
       </c>
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
@@ -6117,9 +6124,9 @@
       <c r="E140" s="10"/>
       <c r="F140" s="10"/>
     </row>
-    <row r="141" spans="1:6" hidden="1">
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>86</v>
+        <v>225</v>
       </c>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
@@ -6127,9 +6134,9 @@
       <c r="E141" s="10"/>
       <c r="F141" s="10"/>
     </row>
-    <row r="142" spans="1:6" hidden="1">
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>173</v>
+        <v>231</v>
       </c>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
@@ -6137,9 +6144,9 @@
       <c r="E142" s="10"/>
       <c r="F142" s="10"/>
     </row>
-    <row r="143" spans="1:6" hidden="1">
+    <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="B143" s="10"/>
       <c r="C143" s="10"/>
@@ -6147,9 +6154,9 @@
       <c r="E143" s="10"/>
       <c r="F143" s="10"/>
     </row>
-    <row r="144" spans="1:6" hidden="1">
+    <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>178</v>
+        <v>115</v>
       </c>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
@@ -6157,9 +6164,9 @@
       <c r="E144" s="10"/>
       <c r="F144" s="10"/>
     </row>
-    <row r="145" spans="1:6" hidden="1">
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="B145" s="10"/>
       <c r="C145" s="10"/>
@@ -6167,9 +6174,9 @@
       <c r="E145" s="10"/>
       <c r="F145" s="10"/>
     </row>
-    <row r="146" spans="1:6" hidden="1">
+    <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="B146" s="10"/>
       <c r="C146" s="10"/>
@@ -6177,9 +6184,9 @@
       <c r="E146" s="10"/>
       <c r="F146" s="10"/>
     </row>
-    <row r="147" spans="1:6" hidden="1">
+    <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="B147" s="10"/>
       <c r="C147" s="10"/>
@@ -6187,9 +6194,9 @@
       <c r="E147" s="10"/>
       <c r="F147" s="10"/>
     </row>
-    <row r="148" spans="1:6" hidden="1">
+    <row r="148" spans="1:6" ht="15" customHeight="1">
       <c r="A148" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B148" s="10"/>
       <c r="C148" s="10"/>
@@ -6197,66 +6204,199 @@
       <c r="E148" s="10"/>
       <c r="F148" s="10"/>
     </row>
-    <row r="149" spans="1:6" hidden="1">
+    <row r="149" spans="1:6">
       <c r="A149" t="s">
+        <v>120</v>
+      </c>
+      <c r="B149" s="10"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
+      <c r="F149" s="10"/>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" t="s">
+        <v>121</v>
+      </c>
+      <c r="B150" s="10"/>
+      <c r="C150" s="10"/>
+      <c r="D150" s="10"/>
+      <c r="E150" s="10"/>
+      <c r="F150" s="10"/>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" t="s">
+        <v>151</v>
+      </c>
+      <c r="B151" s="10"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
+      <c r="F151" s="10"/>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" t="s">
+        <v>153</v>
+      </c>
+      <c r="B152" s="10"/>
+      <c r="C152" s="10"/>
+      <c r="D152" s="10"/>
+      <c r="E152" s="10"/>
+      <c r="F152" s="10"/>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" t="s">
+        <v>86</v>
+      </c>
+      <c r="B153" s="10"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
+      <c r="E153" s="10"/>
+      <c r="F153" s="10"/>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" t="s">
+        <v>172</v>
+      </c>
+      <c r="B154" s="10"/>
+      <c r="C154" s="10"/>
+      <c r="D154" s="10"/>
+      <c r="E154" s="10"/>
+      <c r="F154" s="10"/>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" t="s">
+        <v>169</v>
+      </c>
+      <c r="B155" s="10"/>
+      <c r="C155" s="10"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="10"/>
+      <c r="F155" s="10"/>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" t="s">
+        <v>177</v>
+      </c>
+      <c r="B156" s="10"/>
+      <c r="C156" s="10"/>
+      <c r="D156" s="10"/>
+      <c r="E156" s="10"/>
+      <c r="F156" s="10"/>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" t="s">
+        <v>87</v>
+      </c>
+      <c r="B157" s="10"/>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="10"/>
+      <c r="F157" s="10"/>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" t="s">
+        <v>88</v>
+      </c>
+      <c r="B158" s="10"/>
+      <c r="C158" s="10"/>
+      <c r="D158" s="10"/>
+      <c r="E158" s="10"/>
+      <c r="F158" s="10"/>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" t="s">
+        <v>90</v>
+      </c>
+      <c r="B159" s="10"/>
+      <c r="C159" s="10"/>
+      <c r="D159" s="10"/>
+      <c r="E159" s="10"/>
+      <c r="F159" s="10"/>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" t="s">
+        <v>89</v>
+      </c>
+      <c r="B160" s="10"/>
+      <c r="C160" s="10"/>
+      <c r="D160" s="10"/>
+      <c r="E160" s="10"/>
+      <c r="F160" s="10"/>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" t="s">
         <v>91</v>
       </c>
-      <c r="B149" s="9"/>
-      <c r="C149" s="9"/>
-      <c r="D149" s="9"/>
-      <c r="E149" s="9"/>
-      <c r="F149" s="9"/>
-    </row>
-    <row r="150" spans="1:6" hidden="1">
-      <c r="A150" t="s">
+      <c r="B161" s="9"/>
+      <c r="C161" s="9"/>
+      <c r="D161" s="9"/>
+      <c r="E161" s="9"/>
+      <c r="F161" s="9"/>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" t="s">
         <v>92</v>
       </c>
-      <c r="B150" s="9"/>
-      <c r="C150" s="9"/>
-      <c r="D150" s="9"/>
-      <c r="E150" s="9"/>
-      <c r="F150" s="9"/>
-    </row>
-    <row r="151" spans="1:6" hidden="1">
-      <c r="A151" t="s">
+      <c r="B162" s="9"/>
+      <c r="C162" s="9"/>
+      <c r="D162" s="9"/>
+      <c r="E162" s="9"/>
+      <c r="F162" s="9"/>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" t="s">
         <v>93</v>
       </c>
-      <c r="B151" s="9"/>
-      <c r="C151" s="9"/>
-      <c r="D151" s="9"/>
-      <c r="E151" s="9"/>
-      <c r="F151" s="9"/>
-    </row>
-    <row r="152" spans="1:6" hidden="1">
-      <c r="A152" t="s">
+      <c r="B163" s="9"/>
+      <c r="C163" s="9"/>
+      <c r="D163" s="9"/>
+      <c r="E163" s="9"/>
+      <c r="F163" s="9"/>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" t="s">
         <v>94</v>
       </c>
-      <c r="B152" s="9"/>
-      <c r="C152" s="9"/>
-      <c r="D152" s="9"/>
-      <c r="E152" s="9"/>
-      <c r="F152" s="9"/>
-    </row>
-    <row r="153" spans="1:6" hidden="1">
-      <c r="A153" t="s">
+      <c r="B164" s="9"/>
+      <c r="C164" s="9"/>
+      <c r="D164" s="9"/>
+      <c r="E164" s="9"/>
+      <c r="F164" s="9"/>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" t="s">
         <v>68</v>
       </c>
-      <c r="B153" s="9"/>
-      <c r="C153" s="9"/>
-      <c r="D153" s="9"/>
-      <c r="E153" s="9"/>
-      <c r="F153" s="9"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="9"/>
+      <c r="D165" s="9"/>
+      <c r="E165" s="9"/>
+      <c r="F165" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A153">
+  <autoFilter ref="A1:A165">
     <filterColumn colId="0">
       <customFilters>
-        <customFilter val="*duration*"/>
+        <customFilter operator="notEqual" val="*Enabled*"/>
+        <customFilter operator="notEqual" val="*starting*"/>
       </customFilters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="34">
-    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
     <mergeCell ref="B148:F148"/>
     <mergeCell ref="B149:F149"/>
     <mergeCell ref="B150:F150"/>
@@ -6269,27 +6409,15 @@
     <mergeCell ref="B145:F145"/>
     <mergeCell ref="B146:F146"/>
     <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
     <mergeCell ref="B136:F136"/>
     <mergeCell ref="B137:F137"/>
     <mergeCell ref="B138:F138"/>
     <mergeCell ref="B139:F139"/>
     <mergeCell ref="B140:F140"/>
     <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Status has been implemented for abilities! After overcoming the usual bugs, the player can create an ability and a status associated with it. Next comes implementing it in the engine.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -14,14 +14,14 @@
     <sheet name="Abilities" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Abilities!$A$1:$A$165</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Abilities!$A$1:$A$166</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="285">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -497,9 +497,6 @@
     <t>slashDREnabled</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>0,-1,1,0</t>
   </si>
   <si>
@@ -656,6 +653,9 @@
     <t>-2,-2,-1,-1,0,0,1,1,2,2,3,3</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>-2,-4,-1,-2,0,0,1,2,2,4</t>
   </si>
   <si>
@@ -737,9 +737,6 @@
     <t>0,0,4,-2,6,-3,8,-4,10,-5,12,-6</t>
   </si>
   <si>
-    <t>-12,-5,-10,-4,-8,-3,-6,-2,-4,-1,0,0,4,1,6,2,8,3,10,4,12,5</t>
-  </si>
-  <si>
     <t>extraAttackEnabled</t>
   </si>
   <si>
@@ -800,6 +797,9 @@
     <t>-3,-6,-2,-4,-1,-2,0,0,1,2,2,4,3,6</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>A short knife with a pointed tip.&amp;&amp;(+1 Attack, +1 AC, +1 Dam, Pierce)</t>
   </si>
   <si>
@@ -845,15 +845,6 @@
     <t>statusDurationStartingIndex</t>
   </si>
   <si>
-    <t>statusDurationMod</t>
-  </si>
-  <si>
-    <t>statusDurationModStartingIndex</t>
-  </si>
-  <si>
-    <t>statusDurationModEnabled</t>
-  </si>
-  <si>
     <t>diceHpEnabled</t>
   </si>
   <si>
@@ -861,6 +852,30 @@
   </si>
   <si>
     <t>diceHp</t>
+  </si>
+  <si>
+    <t>diceStatusDurationEnabled</t>
+  </si>
+  <si>
+    <t>diceStatusDurationStartingIndex</t>
+  </si>
+  <si>
+    <t>diceStatusDuration</t>
+  </si>
+  <si>
+    <t>damageTypeStartingIndex</t>
+  </si>
+  <si>
+    <t>e,0,f,0,w,0,l,0</t>
+  </si>
+  <si>
+    <t>None,0,Poison,0,Burn,0,Paralysis,0,Confusion,0,Bleed,0,Berzerk,0,Silence,0</t>
+  </si>
+  <si>
+    <t>0,0,1,-1,2,-2,3,-3,4,-4,5,-5</t>
+  </si>
+  <si>
+    <t>-12,-3,-8,-2,-4,-1,0,0,4,1,8,2,12,3</t>
   </si>
 </sst>
 </file>
@@ -4428,10 +4443,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F165"/>
+  <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4457,7 +4472,7 @@
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -4466,7 +4481,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4474,18 +4489,18 @@
         <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>207</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -4511,79 +4526,79 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" s="3" customFormat="1">
+      <c r="A6" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1">
+      <c r="A8" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0</v>
+      <c r="B8" s="7">
+        <v>1</v>
       </c>
       <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>208</v>
+        <v>178</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1</v>
+        <v>208</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B11" s="6">
         <v>0</v>
@@ -4591,47 +4606,47 @@
       <c r="C11" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>222</v>
+      <c r="D11" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="B12" s="6">
         <v>0</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>239</v>
+        <v>146</v>
       </c>
       <c r="B13" s="6">
         <v>0</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0</v>
+        <v>158</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B14" s="6">
         <v>0</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="D14" s="6">
         <v>0</v>
@@ -4639,13 +4654,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B15" s="6">
         <v>0</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="D15" s="6">
         <v>0</v>
@@ -4653,261 +4668,315 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1</v>
+        <v>240</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="D16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B17" s="6">
+        <v>147</v>
+      </c>
+      <c r="B17" s="3">
         <v>0</v>
       </c>
       <c r="C17" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="B18" s="6">
         <v>0</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>235</v>
+      <c r="C18" s="6">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>212</v>
+        <v>148</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>160</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+        <v>234</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+        <v>262</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+        <v>263</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="B25" s="6">
-        <v>0</v>
-      </c>
-      <c r="C25" s="6">
-        <v>1</v>
-      </c>
-      <c r="D25" s="6">
-        <v>1</v>
+        <v>264</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B26" s="6">
         <v>0</v>
       </c>
       <c r="C26" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="B27" s="6">
-        <v>0</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>235</v>
+        <v>266</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B28" s="6">
         <v>0</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B29" s="6">
         <v>0</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0</v>
+        <v>269</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>261</v>
+        <v>212</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>261</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
+        <v>270</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
+        <v>277</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
+        <v>278</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
+        <v>279</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
+        <v>272</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+        <v>273</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B37" s="6">
-        <v>0</v>
-      </c>
-      <c r="C37" s="6">
-        <v>0</v>
+        <v>271</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>222</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B38" s="6">
         <v>0</v>
@@ -4916,12 +4985,12 @@
         <v>0</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B39" s="6">
         <v>0</v>
@@ -4930,32 +4999,32 @@
         <v>0</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>222</v>
+        <v>244</v>
+      </c>
+      <c r="B40" s="6">
+        <v>0</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>212</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>212</v>
@@ -4963,13 +5032,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>212</v>
@@ -4977,13 +5046,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>212</v>
@@ -4991,13 +5060,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>212</v>
@@ -5005,13 +5074,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>160</v>
+        <v>212</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>212</v>
@@ -5019,27 +5088,27 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B46" s="6">
-        <v>1</v>
-      </c>
-      <c r="C46" s="6">
-        <v>1</v>
-      </c>
-      <c r="D46" s="6">
-        <v>0</v>
+        <v>231</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="B47" s="6">
-        <v>2</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="C47" s="6">
+        <v>1</v>
       </c>
       <c r="D47" s="6">
         <v>0</v>
@@ -5047,13 +5116,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>210</v>
+        <v>181</v>
+      </c>
+      <c r="B48" s="6">
+        <v>2</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D48" s="6">
         <v>0</v>
@@ -5061,13 +5130,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B49" s="6">
-        <v>1</v>
-      </c>
-      <c r="C49" s="6">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="D49" s="6">
         <v>0</v>
@@ -5075,13 +5144,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="B50" s="6">
-        <v>2</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="C50" s="6">
+        <v>1</v>
       </c>
       <c r="D50" s="6">
         <v>0</v>
@@ -5089,13 +5158,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>210</v>
+        <v>182</v>
+      </c>
+      <c r="B51" s="6">
+        <v>2</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D51" s="6">
         <v>0</v>
@@ -5103,13 +5172,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B52" s="6">
-        <v>1</v>
-      </c>
-      <c r="C52" s="6">
-        <v>1</v>
+        <v>115</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="D52" s="6">
         <v>0</v>
@@ -5117,13 +5186,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B53" s="6">
-        <v>2</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="C53" s="6">
+        <v>1</v>
       </c>
       <c r="D53" s="6">
         <v>0</v>
@@ -5131,13 +5200,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>210</v>
+        <v>183</v>
+      </c>
+      <c r="B54" s="6">
+        <v>2</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D54" s="6">
         <v>0</v>
@@ -5145,13 +5214,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B55" s="6">
-        <v>1</v>
-      </c>
-      <c r="C55" s="6">
-        <v>1</v>
+        <v>116</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="D55" s="6">
         <v>0</v>
@@ -5159,13 +5228,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="B56" s="6">
-        <v>2</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="C56" s="6">
+        <v>1</v>
       </c>
       <c r="D56" s="6">
         <v>0</v>
@@ -5173,13 +5242,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>210</v>
+        <v>184</v>
+      </c>
+      <c r="B57" s="6">
+        <v>2</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D57" s="6">
         <v>0</v>
@@ -5187,13 +5256,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B58" s="6">
-        <v>1</v>
-      </c>
-      <c r="C58" s="6">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="D58" s="6">
         <v>0</v>
@@ -5201,13 +5270,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="B59" s="6">
-        <v>2</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="C59" s="6">
+        <v>1</v>
       </c>
       <c r="D59" s="6">
         <v>0</v>
@@ -5215,13 +5284,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>210</v>
+        <v>185</v>
+      </c>
+      <c r="B60" s="6">
+        <v>2</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D60" s="6">
         <v>0</v>
@@ -5229,13 +5298,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B61" s="6">
-        <v>1</v>
-      </c>
-      <c r="C61" s="6">
-        <v>1</v>
+        <v>118</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="D61" s="6">
         <v>0</v>
@@ -5243,13 +5312,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="B62" s="6">
-        <v>2</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="C62" s="6">
+        <v>1</v>
       </c>
       <c r="D62" s="6">
         <v>0</v>
@@ -5257,13 +5326,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>210</v>
+        <v>186</v>
+      </c>
+      <c r="B63" s="6">
+        <v>2</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D63" s="6">
         <v>0</v>
@@ -5271,13 +5340,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B64" s="6">
-        <v>1</v>
-      </c>
-      <c r="C64" s="6">
-        <v>1</v>
+        <v>119</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="D64" s="6">
         <v>0</v>
@@ -5285,13 +5354,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="B65" s="6">
-        <v>2</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="C65" s="6">
+        <v>1</v>
       </c>
       <c r="D65" s="6">
         <v>0</v>
@@ -5299,13 +5368,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>210</v>
+        <v>187</v>
+      </c>
+      <c r="B66" s="6">
+        <v>2</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D66" s="6">
         <v>0</v>
@@ -5313,13 +5382,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B67" s="6">
-        <v>1</v>
-      </c>
-      <c r="C67" s="6">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="D67" s="6">
         <v>0</v>
@@ -5327,13 +5396,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="B68" s="6">
-        <v>2</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="C68" s="6">
+        <v>1</v>
       </c>
       <c r="D68" s="6">
         <v>0</v>
@@ -5341,13 +5410,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>210</v>
+        <v>188</v>
+      </c>
+      <c r="B69" s="6">
+        <v>2</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D69" s="6">
         <v>0</v>
@@ -5355,13 +5424,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B70" s="6">
-        <v>1</v>
-      </c>
-      <c r="C70" s="6">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="D70" s="6">
         <v>0</v>
@@ -5369,13 +5438,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="B71" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C71" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D71" s="6">
         <v>0</v>
@@ -5383,13 +5452,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>211</v>
+        <v>189</v>
+      </c>
+      <c r="B72" s="6">
+        <v>2</v>
+      </c>
+      <c r="C72" s="6">
+        <v>2</v>
       </c>
       <c r="D72" s="6">
         <v>0</v>
@@ -5397,27 +5466,27 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>256</v>
+        <v>151</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="D73" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>212</v>
@@ -5425,13 +5494,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>81</v>
+        <v>256</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>212</v>
@@ -5439,27 +5508,27 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B76" s="6">
-        <v>1</v>
-      </c>
-      <c r="C76" s="6">
-        <v>1</v>
-      </c>
-      <c r="D76" s="6">
-        <v>0</v>
+        <v>81</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>212</v>
+        <v>152</v>
+      </c>
+      <c r="B77" s="6">
+        <v>1</v>
+      </c>
+      <c r="C77" s="6">
+        <v>1</v>
       </c>
       <c r="D77" s="6">
         <v>0</v>
@@ -5467,13 +5536,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>261</v>
+        <v>213</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>212</v>
       </c>
       <c r="D78" s="6">
         <v>0</v>
@@ -5481,27 +5550,27 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>221</v>
+        <v>153</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>222</v>
+        <v>260</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>212</v>
+        <v>261</v>
+      </c>
+      <c r="D79" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>212</v>
@@ -5509,13 +5578,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>86</v>
+        <v>220</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>212</v>
@@ -5523,51 +5592,69 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="B83" s="6"/>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
+        <v>274</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C83" s="6">
+        <v>1</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
+        <v>275</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B85" s="6">
-        <v>0</v>
-      </c>
-      <c r="C85" s="6">
-        <v>1</v>
-      </c>
-      <c r="D85" s="6">
-        <v>0</v>
+        <v>276</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="B86" s="6">
         <v>0</v>
       </c>
-      <c r="C86" s="6" t="s">
-        <v>214</v>
+      <c r="C86" s="6">
+        <v>1</v>
       </c>
       <c r="D86" s="6">
         <v>0</v>
@@ -5575,13 +5662,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B87" s="6">
         <v>0</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="D87" s="6">
         <v>0</v>
@@ -5589,13 +5676,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B88" s="6">
-        <v>1</v>
-      </c>
-      <c r="C88" s="6">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="D88" s="6">
         <v>0</v>
@@ -5603,13 +5690,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>214</v>
+        <v>169</v>
+      </c>
+      <c r="B89" s="6">
+        <v>1</v>
       </c>
       <c r="C89" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D89" s="6">
         <v>0</v>
@@ -5617,13 +5704,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
+      </c>
+      <c r="C90" s="6">
+        <v>0</v>
       </c>
       <c r="D90" s="6">
         <v>0</v>
@@ -5631,13 +5718,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B91" s="6">
-        <v>1</v>
-      </c>
-      <c r="C91" s="6">
-        <v>1</v>
+        <v>168</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="D91" s="6">
         <v>0</v>
@@ -5645,13 +5732,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>214</v>
+        <v>177</v>
+      </c>
+      <c r="B92" s="6">
+        <v>1</v>
       </c>
       <c r="C92" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92" s="6">
         <v>0</v>
@@ -5659,13 +5746,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
+      </c>
+      <c r="C93" s="6">
+        <v>0</v>
       </c>
       <c r="D93" s="6">
         <v>0</v>
@@ -5673,13 +5760,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B94" s="6">
-        <v>1</v>
-      </c>
-      <c r="C94" s="6">
-        <v>1</v>
+        <v>176</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="D94" s="6">
         <v>0</v>
@@ -5687,13 +5774,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>212</v>
+        <v>154</v>
+      </c>
+      <c r="B95" s="6">
+        <v>1</v>
+      </c>
+      <c r="C95" s="6">
+        <v>1</v>
       </c>
       <c r="D95" s="6">
         <v>0</v>
@@ -5701,13 +5788,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
-        <v>87</v>
+        <v>194</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D96" s="6">
         <v>0</v>
@@ -5715,13 +5802,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B97" s="6">
-        <v>1</v>
-      </c>
-      <c r="C97" s="6">
-        <v>1</v>
+        <v>87</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="D97" s="6">
         <v>0</v>
@@ -5729,13 +5816,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>212</v>
+        <v>155</v>
+      </c>
+      <c r="B98" s="6">
+        <v>1</v>
+      </c>
+      <c r="C98" s="6">
+        <v>1</v>
       </c>
       <c r="D98" s="6">
         <v>0</v>
@@ -5743,13 +5830,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
-        <v>88</v>
+        <v>195</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D99" s="6">
         <v>0</v>
@@ -5757,13 +5844,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B100" s="6">
-        <v>1</v>
-      </c>
-      <c r="C100" s="6">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="D100" s="6">
         <v>0</v>
@@ -5771,13 +5858,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>212</v>
+        <v>156</v>
+      </c>
+      <c r="B101" s="6">
+        <v>1</v>
+      </c>
+      <c r="C101" s="6">
+        <v>1</v>
       </c>
       <c r="D101" s="6">
         <v>0</v>
@@ -5785,13 +5872,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
-        <v>90</v>
+        <v>196</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D102" s="6">
         <v>0</v>
@@ -5799,13 +5886,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B103" s="6">
-        <v>1</v>
-      </c>
-      <c r="C103" s="6">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="D103" s="6">
         <v>0</v>
@@ -5813,13 +5900,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>212</v>
+        <v>157</v>
+      </c>
+      <c r="B104" s="6">
+        <v>1</v>
+      </c>
+      <c r="C104" s="6">
+        <v>1</v>
       </c>
       <c r="D104" s="6">
         <v>0</v>
@@ -5827,13 +5914,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D105" s="6">
         <v>0</v>
@@ -5841,13 +5928,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B106" s="6">
-        <v>1</v>
-      </c>
-      <c r="C106" s="6">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="D106" s="6">
         <v>0</v>
@@ -5855,13 +5942,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>212</v>
+        <v>172</v>
+      </c>
+      <c r="B107" s="6">
+        <v>1</v>
+      </c>
+      <c r="C107" s="6">
+        <v>1</v>
       </c>
       <c r="D107" s="6">
         <v>0</v>
@@ -5869,13 +5956,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2" t="s">
-        <v>91</v>
+        <v>198</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D108" s="6">
         <v>0</v>
@@ -5883,13 +5970,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B109" s="6">
-        <v>1</v>
-      </c>
-      <c r="C109" s="6">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="D109" s="6">
         <v>0</v>
@@ -5897,13 +5984,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C110" s="6" t="s">
-        <v>212</v>
+        <v>173</v>
+      </c>
+      <c r="B110" s="6">
+        <v>1</v>
+      </c>
+      <c r="C110" s="6">
+        <v>1</v>
       </c>
       <c r="D110" s="6">
         <v>0</v>
@@ -5911,13 +5998,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2" t="s">
-        <v>92</v>
+        <v>199</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D111" s="6">
         <v>0</v>
@@ -5925,13 +6012,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B112" s="6">
-        <v>1</v>
-      </c>
-      <c r="C112" s="6">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="D112" s="6">
         <v>0</v>
@@ -5939,13 +6026,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>212</v>
+        <v>174</v>
+      </c>
+      <c r="B113" s="6">
+        <v>1</v>
+      </c>
+      <c r="C113" s="6">
+        <v>1</v>
       </c>
       <c r="D113" s="6">
         <v>0</v>
@@ -5953,13 +6040,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2" t="s">
-        <v>93</v>
+        <v>200</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D114" s="6">
         <v>0</v>
@@ -5967,13 +6054,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B115" s="6">
-        <v>1</v>
-      </c>
-      <c r="C115" s="6">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="D115" s="6">
         <v>0</v>
@@ -5981,13 +6068,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>212</v>
+        <v>175</v>
+      </c>
+      <c r="B116" s="6">
+        <v>1</v>
+      </c>
+      <c r="C116" s="6">
+        <v>1</v>
       </c>
       <c r="D116" s="6">
         <v>0</v>
@@ -5995,13 +6082,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2" t="s">
-        <v>94</v>
+        <v>201</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D117" s="6">
         <v>0</v>
@@ -6009,50 +6096,52 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D118" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B118" s="6" t="s">
+      <c r="B119" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C119" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="D118" s="6" t="s">
+      <c r="D119" s="6" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
-      <c r="B131" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
     <row r="132" spans="1:6">
-      <c r="A132" t="s">
+      <c r="B132" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" t="s">
         <v>143</v>
       </c>
-      <c r="B132" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="C132" s="9"/>
-      <c r="D132" s="9"/>
-      <c r="E132" s="9"/>
-      <c r="F132" s="9"/>
-    </row>
-    <row r="133" spans="1:6" ht="15" customHeight="1">
-      <c r="A133" t="s">
+      <c r="B133" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+    </row>
+    <row r="134" spans="1:6" ht="15" customHeight="1">
+      <c r="A134" t="s">
         <v>85</v>
-      </c>
-      <c r="B133" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="C133" s="10"/>
-      <c r="D133" s="10"/>
-      <c r="E133" s="10"/>
-      <c r="F133" s="10"/>
-    </row>
-    <row r="134" spans="1:6">
-      <c r="A134" t="s">
-        <v>146</v>
       </c>
       <c r="B134" s="10" t="s">
         <v>252</v>
@@ -6062,12 +6151,12 @@
       <c r="E134" s="10"/>
       <c r="F134" s="10"/>
     </row>
-    <row r="135" spans="1:6" ht="15" customHeight="1">
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>241</v>
+        <v>146</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C135" s="10"/>
       <c r="D135" s="10"/>
@@ -6076,9 +6165,11 @@
     </row>
     <row r="136" spans="1:6" ht="15" customHeight="1">
       <c r="A136" t="s">
-        <v>148</v>
-      </c>
-      <c r="B136" s="10"/>
+        <v>240</v>
+      </c>
+      <c r="B136" s="10" t="s">
+        <v>254</v>
+      </c>
       <c r="C136" s="10"/>
       <c r="D136" s="10"/>
       <c r="E136" s="10"/>
@@ -6086,7 +6177,7 @@
     </row>
     <row r="137" spans="1:6" ht="15" customHeight="1">
       <c r="A137" t="s">
-        <v>234</v>
+        <v>148</v>
       </c>
       <c r="B137" s="10"/>
       <c r="C137" s="10"/>
@@ -6094,9 +6185,9 @@
       <c r="E137" s="10"/>
       <c r="F137" s="10"/>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" ht="15" customHeight="1">
       <c r="A138" t="s">
-        <v>149</v>
+        <v>234</v>
       </c>
       <c r="B138" s="10"/>
       <c r="C138" s="10"/>
@@ -6106,7 +6197,7 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>236</v>
+        <v>149</v>
       </c>
       <c r="B139" s="10"/>
       <c r="C139" s="10"/>
@@ -6116,7 +6207,7 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
@@ -6126,7 +6217,7 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
@@ -6136,7 +6227,7 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
@@ -6146,7 +6237,7 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>114</v>
+        <v>231</v>
       </c>
       <c r="B143" s="10"/>
       <c r="C143" s="10"/>
@@ -6156,7 +6247,7 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
@@ -6166,7 +6257,7 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B145" s="10"/>
       <c r="C145" s="10"/>
@@ -6176,7 +6267,7 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B146" s="10"/>
       <c r="C146" s="10"/>
@@ -6186,7 +6277,7 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B147" s="10"/>
       <c r="C147" s="10"/>
@@ -6194,9 +6285,9 @@
       <c r="E147" s="10"/>
       <c r="F147" s="10"/>
     </row>
-    <row r="148" spans="1:6" ht="15" customHeight="1">
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B148" s="10"/>
       <c r="C148" s="10"/>
@@ -6204,9 +6295,9 @@
       <c r="E148" s="10"/>
       <c r="F148" s="10"/>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" ht="15" customHeight="1">
       <c r="A149" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B149" s="10"/>
       <c r="C149" s="10"/>
@@ -6216,7 +6307,7 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B150" s="10"/>
       <c r="C150" s="10"/>
@@ -6226,7 +6317,7 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="B151" s="10"/>
       <c r="C151" s="10"/>
@@ -6236,7 +6327,7 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B152" s="10"/>
       <c r="C152" s="10"/>
@@ -6246,7 +6337,7 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="B153" s="10"/>
       <c r="C153" s="10"/>
@@ -6256,7 +6347,7 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
@@ -6266,7 +6357,7 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B155" s="10"/>
       <c r="C155" s="10"/>
@@ -6276,7 +6367,7 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B156" s="10"/>
       <c r="C156" s="10"/>
@@ -6286,7 +6377,7 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>87</v>
+        <v>176</v>
       </c>
       <c r="B157" s="10"/>
       <c r="C157" s="10"/>
@@ -6296,7 +6387,7 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B158" s="10"/>
       <c r="C158" s="10"/>
@@ -6306,7 +6397,7 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B159" s="10"/>
       <c r="C159" s="10"/>
@@ -6316,7 +6407,7 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B160" s="10"/>
       <c r="C160" s="10"/>
@@ -6326,17 +6417,17 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>91</v>
-      </c>
-      <c r="B161" s="9"/>
-      <c r="C161" s="9"/>
-      <c r="D161" s="9"/>
-      <c r="E161" s="9"/>
-      <c r="F161" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="B161" s="10"/>
+      <c r="C161" s="10"/>
+      <c r="D161" s="10"/>
+      <c r="E161" s="10"/>
+      <c r="F161" s="10"/>
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
@@ -6346,7 +6437,7 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
@@ -6356,7 +6447,7 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
@@ -6366,7 +6457,7 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
@@ -6374,8 +6465,18 @@
       <c r="E165" s="9"/>
       <c r="F165" s="9"/>
     </row>
+    <row r="166" spans="1:6">
+      <c r="A166" t="s">
+        <v>68</v>
+      </c>
+      <c r="B166" s="9"/>
+      <c r="C166" s="9"/>
+      <c r="D166" s="9"/>
+      <c r="E166" s="9"/>
+      <c r="F166" s="9"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A165">
+  <autoFilter ref="A1:A166">
     <filterColumn colId="0">
       <customFilters>
         <customFilter operator="notEqual" val="*Enabled*"/>
@@ -6384,32 +6485,31 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="34">
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B133:F133"/>
     <mergeCell ref="B161:F161"/>
     <mergeCell ref="B162:F162"/>
     <mergeCell ref="B163:F163"/>
     <mergeCell ref="B164:F164"/>
     <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B166:F166"/>
     <mergeCell ref="B155:F155"/>
     <mergeCell ref="B156:F156"/>
     <mergeCell ref="B157:F157"/>
     <mergeCell ref="B158:F158"/>
     <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B160:F160"/>
     <mergeCell ref="B149:F149"/>
     <mergeCell ref="B150:F150"/>
     <mergeCell ref="B151:F151"/>
     <mergeCell ref="B152:F152"/>
     <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B154:F154"/>
     <mergeCell ref="B143:F143"/>
     <mergeCell ref="B144:F144"/>
     <mergeCell ref="B145:F145"/>
     <mergeCell ref="B146:F146"/>
     <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B148:F148"/>
     <mergeCell ref="B134:F134"/>
     <mergeCell ref="B135:F135"/>
     <mergeCell ref="B136:F136"/>
@@ -6418,6 +6518,7 @@
     <mergeCell ref="B139:F139"/>
     <mergeCell ref="B140:F140"/>
     <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Statuses can be invoked on individuals using the targeted ability type. The 'duration' type will need a bit more work, but as it stands, the general famework is in place. Note that for now it cannot be tested on enemies (just the player) - this is due to the enemy turn not being handled correctly if the enemy dies from the startTurn() call. Will work on that too.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -1517,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AX10"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AX10" sqref="AX10"/>
+    <sheetView topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AX10" sqref="A2:AX10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2065,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AB4">
         <v>0</v>
@@ -2673,7 +2673,7 @@
         <v>0</v>
       </c>
       <c r="AA8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AB8">
         <v>0</v>
@@ -4445,8 +4445,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D119"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5626,7 +5626,7 @@
         <v>212</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>212</v>
@@ -5668,7 +5668,7 @@
         <v>0</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D87" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
Duration abilities can now be used similar to targeted ones. If the ability is considered harmful, the individuals caught within the AOE trigger their onAttack effect. Some enhancements include changing the range of self duration to always be on the casting individual (after all, a self duration ability should always affect the self). Also, NPCs/enemies are not harmed by them yet, and the damages incurred are not calculated. Aside from that, big steps forward in the ability/status process
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="285">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -4445,8 +4445,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4981,8 +4981,8 @@
       <c r="B38" s="6">
         <v>0</v>
       </c>
-      <c r="C38" s="6">
-        <v>0</v>
+      <c r="C38" s="6" t="s">
+        <v>222</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>222</v>
@@ -4995,8 +4995,8 @@
       <c r="B39" s="6">
         <v>0</v>
       </c>
-      <c r="C39" s="6">
-        <v>0</v>
+      <c r="C39" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>212</v>
@@ -5009,8 +5009,8 @@
       <c r="B40" s="6">
         <v>0</v>
       </c>
-      <c r="C40" s="6">
-        <v>0</v>
+      <c r="C40" s="6" t="s">
+        <v>245</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>245</v>

</xml_diff>

<commit_message>
I've started going through the arduous process of implementing all the business logic of the abilities - right now I'm just trying to get everything working just for perminant abilities.
Things are looking good, however it looks like I may need to do some
refactoring: totalHP/Mana doesn't make a lot of since, since it's
composed of multiple attributes, which require getAttribute calls. The
sensible choice would be to compose the totalHP/Mana value every time
it's used, but doing so creates some confusion on what
'totalHP'/'totalMana' really means - I think I may have to do a nasty
name change to 'baseHP/Mana'. Yuck.

Aside from that, I added a new ability effect (actions) and I made the
checking functionality more robust when decreasing CON/WILL w.r.t.
totalMana/totalHP.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="284">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -872,10 +872,7 @@
     <t>None,0,Poison,0,Burn,0,Paralysis,0,Confusion,0,Bleed,0,Berzerk,0,Silence,0</t>
   </si>
   <si>
-    <t>0,0,1,-1,2,-2,3,-3,4,-4,5,-5</t>
-  </si>
-  <si>
-    <t>-12,-3,-8,-2,-4,-1,0,0,4,1,8,2,12,3</t>
+    <t>0,0,4,1,8,2,12,3</t>
   </si>
 </sst>
 </file>
@@ -3058,8 +3055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4445,8 +4442,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:C40"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4842,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>235</v>
@@ -4884,7 +4881,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>261</v>
@@ -5626,7 +5623,7 @@
         <v>212</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>212</v>
@@ -5640,7 +5637,7 @@
         <v>212</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>212</v>

</xml_diff>

<commit_message>
Hallelujah hallelujah I got OpenAL working, Hallelujah. 3 days to figure out WinAPI wouldn't cut it, 7 days to get the OpenAl imports working correctly, 5 days to make it play sounds correctly, 4 days to add it to the codebase. Safe to say I did not anticipate that taking this much effort.
Anyways - I can play sounds, and it's wonderful.

Next step is to update the Global Registry to add a map between sound ID
and filePath - this way the files wont have to be passed around, and if
given an Int ID, music/sound can be played.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Abilities!$A$1:$A$134</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Abilities!$A$1:$A$137</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="288">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -875,6 +875,18 @@
   </si>
   <si>
     <t>0,0,4,-1,8,-2,12,-3,16,-4,20,-5</t>
+  </si>
+  <si>
+    <t>diceDamageMultiplier</t>
+  </si>
+  <si>
+    <t>diceDamageMultiplierEnabled</t>
+  </si>
+  <si>
+    <t>diceDamageMultiplierStartingIndex</t>
+  </si>
+  <si>
+    <t>1,1,2,2,3,3,4,4</t>
   </si>
 </sst>
 </file>
@@ -4490,10 +4502,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F169"/>
+  <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86:E91"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4829,7 +4841,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>231</v>
+        <v>285</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>211</v>
@@ -4846,7 +4858,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>232</v>
+        <v>286</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>211</v>
@@ -4863,24 +4875,24 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>233</v>
+        <v>284</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>211</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>214</v>
+        <v>287</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>211</v>
@@ -4897,10 +4909,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>211</v>
@@ -4914,129 +4926,129 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>211</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>273</v>
+        <v>214</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B26" s="10">
-        <v>0</v>
-      </c>
-      <c r="C26" s="10">
-        <v>1</v>
-      </c>
-      <c r="D26" s="10">
-        <v>1</v>
-      </c>
-      <c r="E26" s="10">
-        <v>1</v>
+        <v>253</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="C27" s="10">
-        <v>0</v>
-      </c>
-      <c r="D27" s="10">
-        <v>0</v>
-      </c>
-      <c r="E27" s="10">
-        <v>0</v>
+        <v>221</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="B28" s="10">
-        <v>0</v>
+        <v>255</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B29" s="10">
         <v>0</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>221</v>
+      <c r="C29" s="10">
+        <v>1</v>
+      </c>
+      <c r="D29" s="10">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
+      </c>
+      <c r="C30" s="10">
+        <v>0</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0</v>
+      </c>
+      <c r="E30" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B31" s="10">
         <v>0</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>211</v>
+        <v>259</v>
+      </c>
+      <c r="B32" s="10">
+        <v>0</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>221</v>
@@ -5050,10 +5062,10 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>249</v>
+        <v>212</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>211</v>
@@ -5067,24 +5079,24 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>211</v>
+        <v>261</v>
+      </c>
+      <c r="B34" s="10">
+        <v>0</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>211</v>
@@ -5101,10 +5113,10 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>213</v>
+        <v>249</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>211</v>
@@ -5118,27 +5130,27 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>211</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>158</v>
+        <v>234</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>158</v>
+        <v>234</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>158</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B38" s="10">
-        <v>0</v>
+        <v>263</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>221</v>
@@ -5147,15 +5159,15 @@
         <v>221</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B39" s="10">
-        <v>0</v>
+        <v>264</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>213</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>211</v>
@@ -5169,33 +5181,33 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B40" s="10">
-        <v>0</v>
+        <v>262</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>242</v>
+        <v>158</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>242</v>
+        <v>158</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>211</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>211</v>
+        <v>239</v>
+      </c>
+      <c r="B41" s="10">
+        <v>0</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>221</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>211</v>
@@ -5203,10 +5215,10 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>211</v>
+        <v>240</v>
+      </c>
+      <c r="B42" s="10">
+        <v>0</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>211</v>
@@ -5220,16 +5232,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>211</v>
+        <v>241</v>
+      </c>
+      <c r="B43" s="10">
+        <v>0</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>211</v>
@@ -5237,7 +5249,7 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>211</v>
@@ -5254,7 +5266,7 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>211</v>
@@ -5271,13 +5283,13 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>211</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>158</v>
+        <v>234</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>211</v>
@@ -5288,7 +5300,7 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>276</v>
+        <v>228</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>211</v>
@@ -5297,15 +5309,15 @@
         <v>221</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>277</v>
+        <v>229</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>211</v>
@@ -5322,50 +5334,50 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>278</v>
+        <v>230</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>211</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>274</v>
+        <v>158</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>274</v>
+        <v>211</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>274</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B50" s="10">
-        <v>1</v>
-      </c>
-      <c r="C50" s="10">
-        <v>1</v>
-      </c>
-      <c r="D50" s="10">
-        <v>0</v>
+        <v>276</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>221</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B51" s="10">
-        <v>2</v>
+        <v>277</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="D51" s="10">
-        <v>0</v>
+      <c r="D51" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>211</v>
@@ -5373,24 +5385,24 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>114</v>
+        <v>278</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D52" s="10">
-        <v>0</v>
+        <v>274</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>274</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>211</v>
+        <v>274</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B53" s="10">
         <v>1</v>
@@ -5401,13 +5413,13 @@
       <c r="D53" s="10">
         <v>0</v>
       </c>
-      <c r="E53" s="10">
-        <v>0</v>
+      <c r="E53" s="10" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B54" s="10">
         <v>2</v>
@@ -5418,13 +5430,13 @@
       <c r="D54" s="10">
         <v>0</v>
       </c>
-      <c r="E54" s="10">
-        <v>0</v>
+      <c r="E54" s="10" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>208</v>
@@ -5435,13 +5447,13 @@
       <c r="D55" s="10">
         <v>0</v>
       </c>
-      <c r="E55" s="10">
-        <v>0</v>
+      <c r="E55" s="10" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B56" s="10">
         <v>1</v>
@@ -5458,7 +5470,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B57" s="10">
         <v>2</v>
@@ -5475,7 +5487,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>208</v>
@@ -5492,7 +5504,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B59" s="10">
         <v>1</v>
@@ -5509,7 +5521,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B60" s="10">
         <v>2</v>
@@ -5526,7 +5538,7 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>208</v>
@@ -5543,7 +5555,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B62" s="10">
         <v>1</v>
@@ -5560,7 +5572,7 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B63" s="10">
         <v>2</v>
@@ -5577,7 +5589,7 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>208</v>
@@ -5594,7 +5606,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B65" s="10">
         <v>1</v>
@@ -5611,7 +5623,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B66" s="10">
         <v>2</v>
@@ -5628,7 +5640,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B67" s="10" t="s">
         <v>208</v>
@@ -5645,7 +5657,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B68" s="10">
         <v>1</v>
@@ -5662,7 +5674,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B69" s="10">
         <v>2</v>
@@ -5679,7 +5691,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B70" s="10" t="s">
         <v>208</v>
@@ -5696,7 +5708,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B71" s="10">
         <v>1</v>
@@ -5713,7 +5725,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B72" s="10">
         <v>2</v>
@@ -5730,7 +5742,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B73" s="10" t="s">
         <v>208</v>
@@ -5747,7 +5759,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B74" s="10">
         <v>1</v>
@@ -5764,13 +5776,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B75" s="10">
         <v>2</v>
       </c>
-      <c r="C75" s="10">
-        <v>2</v>
+      <c r="C75" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="D75" s="10">
         <v>0</v>
@@ -5781,13 +5793,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D76" s="10">
         <v>0</v>
@@ -5798,180 +5810,180 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>221</v>
+        <v>149</v>
+      </c>
+      <c r="B77" s="10">
+        <v>1</v>
+      </c>
+      <c r="C77" s="10">
+        <v>1</v>
+      </c>
+      <c r="D77" s="10">
+        <v>0</v>
+      </c>
+      <c r="E77" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>212</v>
+        <v>188</v>
+      </c>
+      <c r="B78" s="10">
+        <v>2</v>
+      </c>
+      <c r="C78" s="10">
+        <v>2</v>
+      </c>
+      <c r="D78" s="10">
+        <v>0</v>
+      </c>
+      <c r="E78" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>81</v>
+        <v>150</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="D79" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="E79" s="10" t="s">
-        <v>248</v>
+        <v>210</v>
+      </c>
+      <c r="D79" s="10">
+        <v>0</v>
+      </c>
+      <c r="E79" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B80" s="10">
-        <v>1</v>
-      </c>
-      <c r="C80" s="10">
-        <v>1</v>
-      </c>
-      <c r="D80" s="10">
-        <v>0</v>
-      </c>
-      <c r="E80" s="10">
-        <v>1</v>
+        <v>246</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>189</v>
+        <v>247</v>
       </c>
       <c r="B81" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C81" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D81" s="10">
-        <v>0</v>
-      </c>
-      <c r="E81" s="12" t="s">
-        <v>211</v>
+      <c r="C81" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="D82" s="10">
-        <v>0</v>
+        <v>248</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C83" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="D83" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="E83" s="10" t="s">
-        <v>221</v>
+        <v>151</v>
+      </c>
+      <c r="B83" s="10">
+        <v>1</v>
+      </c>
+      <c r="C83" s="10">
+        <v>1</v>
+      </c>
+      <c r="D83" s="10">
+        <v>0</v>
+      </c>
+      <c r="E83" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C84" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D84" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="E84" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D84" s="10">
+        <v>0</v>
+      </c>
+      <c r="E84" s="12" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>217</v>
+        <v>251</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="D85" s="10" t="s">
-        <v>211</v>
+        <v>252</v>
+      </c>
+      <c r="D85" s="10">
+        <v>0</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>216</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C86" s="10">
-        <v>1</v>
+        <v>221</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>221</v>
       </c>
       <c r="D86" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="E86" s="10">
-        <v>1</v>
+      <c r="E86" s="10" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>266</v>
+        <v>219</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>211</v>
@@ -5985,33 +5997,33 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>267</v>
+        <v>86</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>275</v>
+        <v>216</v>
       </c>
       <c r="D88" s="10" t="s">
         <v>211</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>275</v>
+        <v>216</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B89" s="10">
-        <v>0</v>
+        <v>265</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="C89" s="10">
         <v>1</v>
       </c>
-      <c r="D89" s="10">
-        <v>0</v>
+      <c r="D89" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="E89" s="10">
         <v>1</v>
@@ -6019,16 +6031,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B90" s="10">
-        <v>0</v>
+        <v>266</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="D90" s="10">
-        <v>0</v>
+      <c r="D90" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="E90" s="10" t="s">
         <v>211</v>
@@ -6036,27 +6048,27 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B91" s="10">
-        <v>0</v>
+        <v>267</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="D91" s="10">
-        <v>0</v>
+        <v>275</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>214</v>
+        <v>275</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B92" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C92" s="10">
         <v>1</v>
@@ -6065,32 +6077,32 @@
         <v>0</v>
       </c>
       <c r="E92" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C93" s="10">
-        <v>0</v>
+        <v>190</v>
+      </c>
+      <c r="B93" s="10">
+        <v>0</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="D93" s="10">
         <v>0</v>
       </c>
-      <c r="E93" s="10">
-        <v>0</v>
+      <c r="E93" s="10" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B94" s="10" t="s">
-        <v>215</v>
+        <v>170</v>
+      </c>
+      <c r="B94" s="10">
+        <v>0</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>214</v>
@@ -6098,13 +6110,13 @@
       <c r="D94" s="10">
         <v>0</v>
       </c>
-      <c r="E94" s="10">
-        <v>0</v>
+      <c r="E94" s="10" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B95" s="10">
         <v>1</v>
@@ -6121,7 +6133,7 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>213</v>
@@ -6138,7 +6150,7 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>215</v>
@@ -6155,7 +6167,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="B98" s="10">
         <v>1</v>
@@ -6172,13 +6184,13 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B99" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="C99" s="10" t="s">
-        <v>211</v>
+      <c r="C99" s="10">
+        <v>0</v>
       </c>
       <c r="D99" s="10">
         <v>0</v>
@@ -6189,13 +6201,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>87</v>
+        <v>175</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D100" s="10">
         <v>0</v>
@@ -6206,7 +6218,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B101" s="10">
         <v>1</v>
@@ -6223,7 +6235,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B102" s="10" t="s">
         <v>213</v>
@@ -6240,7 +6252,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B103" s="10" t="s">
         <v>243</v>
@@ -6257,7 +6269,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B104" s="10">
         <v>1</v>
@@ -6274,7 +6286,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B105" s="10" t="s">
         <v>213</v>
@@ -6291,7 +6303,7 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B106" s="10" t="s">
         <v>243</v>
@@ -6308,7 +6320,7 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B107" s="10">
         <v>1</v>
@@ -6325,7 +6337,7 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B108" s="10" t="s">
         <v>213</v>
@@ -6342,7 +6354,7 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B109" s="10" t="s">
         <v>243</v>
@@ -6359,7 +6371,7 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B110" s="10">
         <v>1</v>
@@ -6376,7 +6388,7 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B111" s="10" t="s">
         <v>213</v>
@@ -6393,7 +6405,7 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>243</v>
@@ -6410,7 +6422,7 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B113" s="10">
         <v>1</v>
@@ -6427,7 +6439,7 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B114" s="10" t="s">
         <v>213</v>
@@ -6444,7 +6456,7 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B115" s="10" t="s">
         <v>243</v>
@@ -6461,7 +6473,7 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B116" s="10">
         <v>1</v>
@@ -6478,7 +6490,7 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B117" s="10" t="s">
         <v>213</v>
@@ -6495,7 +6507,7 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B118" s="10" t="s">
         <v>243</v>
@@ -6512,7 +6524,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B119" s="10">
         <v>1</v>
@@ -6529,7 +6541,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B120" s="10" t="s">
         <v>213</v>
@@ -6546,7 +6558,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B121" s="10" t="s">
         <v>243</v>
@@ -6563,54 +6575,93 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B122" s="10">
+        <v>1</v>
+      </c>
+      <c r="C122" s="10">
+        <v>1</v>
+      </c>
+      <c r="D122" s="10">
+        <v>0</v>
+      </c>
+      <c r="E122" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C123" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D123" s="10">
+        <v>0</v>
+      </c>
+      <c r="E123" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B124" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C124" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D124" s="10">
+        <v>0</v>
+      </c>
+      <c r="E124" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B122" s="10" t="s">
+      <c r="B125" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="C122" s="10" t="s">
+      <c r="C125" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="D122" s="10" t="s">
+      <c r="D125" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="E122" s="1" t="s">
+      <c r="E125" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="136" spans="5:6">
-      <c r="E136" s="5"/>
-      <c r="F136" s="5"/>
-    </row>
-    <row r="137" spans="5:6" ht="15" customHeight="1">
-      <c r="E137" s="13"/>
-      <c r="F137" s="13"/>
-    </row>
-    <row r="138" spans="5:6">
-      <c r="E138" s="13"/>
-      <c r="F138" s="13"/>
-    </row>
-    <row r="139" spans="5:6" ht="15" customHeight="1">
-      <c r="E139" s="13"/>
-      <c r="F139" s="13"/>
+    <row r="139" spans="5:6">
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
     </row>
     <row r="140" spans="5:6" ht="15" customHeight="1">
       <c r="E140" s="13"/>
       <c r="F140" s="13"/>
     </row>
-    <row r="141" spans="5:6" ht="15" customHeight="1">
+    <row r="141" spans="5:6">
       <c r="E141" s="13"/>
       <c r="F141" s="13"/>
     </row>
-    <row r="142" spans="5:6">
+    <row r="142" spans="5:6" ht="15" customHeight="1">
       <c r="E142" s="13"/>
       <c r="F142" s="13"/>
     </row>
-    <row r="143" spans="5:6">
+    <row r="143" spans="5:6" ht="15" customHeight="1">
       <c r="E143" s="13"/>
       <c r="F143" s="13"/>
     </row>
-    <row r="144" spans="5:6">
+    <row r="144" spans="5:6" ht="15" customHeight="1">
       <c r="E144" s="13"/>
       <c r="F144" s="13"/>
     </row>
@@ -6642,7 +6693,7 @@
       <c r="E151" s="13"/>
       <c r="F151" s="13"/>
     </row>
-    <row r="152" spans="5:6" ht="15" customHeight="1">
+    <row r="152" spans="5:6">
       <c r="E152" s="13"/>
       <c r="F152" s="13"/>
     </row>
@@ -6654,7 +6705,7 @@
       <c r="E154" s="13"/>
       <c r="F154" s="13"/>
     </row>
-    <row r="155" spans="5:6">
+    <row r="155" spans="5:6" ht="15" customHeight="1">
       <c r="E155" s="13"/>
       <c r="F155" s="13"/>
     </row>
@@ -6695,16 +6746,16 @@
       <c r="F164" s="13"/>
     </row>
     <row r="165" spans="5:6">
-      <c r="E165" s="5"/>
-      <c r="F165" s="5"/>
+      <c r="E165" s="13"/>
+      <c r="F165" s="13"/>
     </row>
     <row r="166" spans="5:6">
-      <c r="E166" s="5"/>
-      <c r="F166" s="5"/>
+      <c r="E166" s="13"/>
+      <c r="F166" s="13"/>
     </row>
     <row r="167" spans="5:6">
-      <c r="E167" s="5"/>
-      <c r="F167" s="5"/>
+      <c r="E167" s="13"/>
+      <c r="F167" s="13"/>
     </row>
     <row r="168" spans="5:6">
       <c r="E168" s="5"/>
@@ -6714,8 +6765,20 @@
       <c r="E169" s="5"/>
       <c r="F169" s="5"/>
     </row>
+    <row r="170" spans="5:6">
+      <c r="E170" s="5"/>
+      <c r="F170" s="5"/>
+    </row>
+    <row r="171" spans="5:6">
+      <c r="E171" s="5"/>
+      <c r="F171" s="5"/>
+    </row>
+    <row r="172" spans="5:6">
+      <c r="E172" s="5"/>
+      <c r="F172" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A169">
+  <autoFilter ref="A1:A172">
     <filterColumn colId="0">
       <customFilters>
         <customFilter operator="notEqual" val="*Enabled*"/>

</xml_diff>

<commit_message>
After encountering my little issue again with where to open the audio device, I found a suitable location, namely after wc2 gets registered. Aside form that, I've made good progress, and implemented the globalRegister to contain soundMaps (<id, filepath>), AND I've successfully loaded a local based file path using the registry and played it.
Next up, I'm gonna try throwing in some more sound effects and hooking
them up with an event so that sounds will be played as needed.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -11,19 +11,19 @@
     <sheet name="Items" sheetId="2" r:id="rId2"/>
     <sheet name="Individuals" sheetId="3" r:id="rId3"/>
     <sheet name="Events" sheetId="4" r:id="rId4"/>
-    <sheet name="Abilities" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="Sounds" sheetId="7" r:id="rId5"/>
+    <sheet name="Abilities" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Abilities!$A$1:$A$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Abilities!$A$1:$A$137</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="291">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -887,6 +887,15 @@
   </si>
   <si>
     <t>1,1,2,2,3,3,4,4</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>.\resources\sounds\music\GoTankGo.WAV</t>
+  </si>
+  <si>
+    <t>.\resources\sounds\\soundEffects\smallExplosions2.WAV</t>
   </si>
 </sst>
 </file>
@@ -980,7 +989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1025,6 +1034,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4501,10 +4511,52 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="67.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+    <sheetView topLeftCell="A93" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E125"/>
     </sheetView>
   </sheetViews>
@@ -6791,7 +6843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E40"/>
   <sheetViews>

</xml_diff>

<commit_message>
A lovely enhancement: now when individuals speak, they print out each character and play a short sound. Future enhancements will be to include a 'voice' sound ID so that different individuals produce different sounds.
Note that the sound effect I've included (speak.wav) doesn't appear to
work, my guess is it's too short, I'll tinker with it some more.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="306">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -897,9 +897,6 @@
     <t>.\resources\sounds\music\GoTankGo.WAV</t>
   </si>
   <si>
-    <t>.\resources\sounds\\soundEffects\smallExplosions2.WAV</t>
-  </si>
-  <si>
     <t>[name]</t>
   </si>
   <si>
@@ -922,6 +919,30 @@
   </si>
   <si>
     <t>MissMarker</t>
+  </si>
+  <si>
+    <t>.\resources\sounds\\soundEffects\slash.WAV</t>
+  </si>
+  <si>
+    <t>.\resources\sounds\soundEffects\smallExplosions2.WAV</t>
+  </si>
+  <si>
+    <t>.\resources\sounds\soundEffects\arrow.WAV</t>
+  </si>
+  <si>
+    <t>.\resources\sounds\soundEffects\bash.WAV</t>
+  </si>
+  <si>
+    <t>.\resources\sounds\soundEffects\chop.WAV</t>
+  </si>
+  <si>
+    <t>.\resources\sounds\soundEffects\pierce.WAV</t>
+  </si>
+  <si>
+    <t>.\resources\sounds\soundEffects\slice.WAV</t>
+  </si>
+  <si>
+    <t>.\resources\sounds\soundEffects\speak.WAV</t>
   </si>
 </sst>
 </file>
@@ -4544,10 +4565,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4576,7 +4597,63 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>290</v>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -6880,7 +6957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -6891,30 +6968,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C1" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>295</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B2" s="1">
         <v>4000</v>
@@ -6937,7 +7014,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B3" s="1">
         <v>4001</v>

</xml_diff>

<commit_message>
Fixed the decision arrow issue; it's a complex bit of code with some wierd logic because the text comes from the bottom up, and was essentually fixed by adding an (int) cast and solving an off-by-one error. I tested it, it looks good, now I'm never gonna touch it again.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -441,15 +441,9 @@
     <t>Have at you!</t>
   </si>
   <si>
-    <t>No! I'm mearly trying to infrom you as a friend! (CHR Check)</t>
-  </si>
-  <si>
     <t>(CHR check)</t>
   </si>
   <si>
-    <t>Ah - forgive me for my agression. It takes a stronger man to say the honest thing.</t>
-  </si>
-  <si>
     <t>Map 2</t>
   </si>
   <si>
@@ -943,6 +937,12 @@
   </si>
   <si>
     <t>.\resources\sounds\soundEffects\speak.WAV</t>
+  </si>
+  <si>
+    <t>Ah - forgive me for my aggression. It takes a stronger man to say the honest thing.</t>
+  </si>
+  <si>
+    <t>No! I'm mearly trying to inform you as a friend! (CHR Check)</t>
   </si>
 </sst>
 </file>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1507,7 +1507,7 @@
         <v>1006</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1547,7 +1547,7 @@
         <v>1007</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>304</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1600,7 +1600,7 @@
         <v>1003</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>305</v>
       </c>
       <c r="C14">
         <v>1006</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1953,7 +1953,7 @@
         <v>0</v>
       </c>
       <c r="AX2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:50">
@@ -3169,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="AX10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -4567,8 +4567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4581,7 +4581,7 @@
         <v>78</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4589,7 +4589,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4597,7 +4597,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4605,7 +4605,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4613,7 +4613,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4621,7 +4621,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4629,7 +4629,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4637,7 +4637,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4645,7 +4645,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4653,7 +4653,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>12</v>
@@ -4706,7 +4706,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>16</v>
@@ -4717,21 +4717,21 @@
         <v>39</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -4748,7 +4748,7 @@
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1">
       <c r="A5" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" s="10">
         <v>0</v>
@@ -4765,41 +4765,41 @@
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1">
       <c r="A6" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B8" s="11">
         <v>1</v>
@@ -4816,7 +4816,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B9" s="10">
         <v>0</v>
@@ -4836,13 +4836,13 @@
         <v>85</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E10" s="7">
         <v>0</v>
@@ -4850,13 +4850,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B11" s="10">
         <v>0</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D11" s="10">
         <v>1</v>
@@ -4867,16 +4867,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B12" s="10">
         <v>0</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
@@ -4884,16 +4884,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B13" s="10">
         <v>0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E13" s="7">
         <v>0</v>
@@ -4901,58 +4901,58 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B14" s="10">
         <v>0</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D14" s="10">
         <v>0</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B15" s="10">
         <v>0</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D15" s="10">
         <v>0</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B16" s="10">
         <v>0</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D16" s="10">
         <v>0</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B18" s="10">
         <v>0</v>
@@ -4986,177 +4986,177 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B19" s="10">
         <v>0</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B29" s="10">
         <v>0</v>
@@ -5173,10 +5173,10 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C30" s="10">
         <v>0</v>
@@ -5190,381 +5190,381 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B31" s="10">
         <v>0</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B32" s="10">
         <v>0</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B34" s="10">
         <v>0</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B41" s="10">
         <v>0</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B42" s="10">
         <v>0</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B43" s="10">
         <v>0</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B53" s="10">
         <v>1</v>
@@ -5576,24 +5576,24 @@
         <v>0</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B54" s="10">
         <v>2</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D54" s="10">
         <v>0</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -5601,21 +5601,21 @@
         <v>114</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D55" s="10">
         <v>0</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B56" s="10">
         <v>1</v>
@@ -5632,13 +5632,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B57" s="10">
         <v>2</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D57" s="10">
         <v>0</v>
@@ -5652,10 +5652,10 @@
         <v>115</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D58" s="10">
         <v>0</v>
@@ -5666,7 +5666,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B59" s="10">
         <v>1</v>
@@ -5683,13 +5683,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B60" s="10">
         <v>2</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D60" s="10">
         <v>0</v>
@@ -5703,10 +5703,10 @@
         <v>116</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D61" s="10">
         <v>0</v>
@@ -5717,7 +5717,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B62" s="10">
         <v>1</v>
@@ -5734,13 +5734,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B63" s="10">
         <v>2</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D63" s="10">
         <v>0</v>
@@ -5754,10 +5754,10 @@
         <v>117</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D64" s="10">
         <v>0</v>
@@ -5768,7 +5768,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B65" s="10">
         <v>1</v>
@@ -5785,13 +5785,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B66" s="10">
         <v>2</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D66" s="10">
         <v>0</v>
@@ -5805,10 +5805,10 @@
         <v>118</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D67" s="10">
         <v>0</v>
@@ -5819,7 +5819,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B68" s="10">
         <v>1</v>
@@ -5836,13 +5836,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B69" s="10">
         <v>2</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D69" s="10">
         <v>0</v>
@@ -5856,10 +5856,10 @@
         <v>119</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D70" s="10">
         <v>0</v>
@@ -5870,7 +5870,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B71" s="10">
         <v>1</v>
@@ -5887,13 +5887,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B72" s="10">
         <v>2</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D72" s="10">
         <v>0</v>
@@ -5907,10 +5907,10 @@
         <v>120</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D73" s="10">
         <v>0</v>
@@ -5921,7 +5921,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B74" s="10">
         <v>1</v>
@@ -5938,13 +5938,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B75" s="10">
         <v>2</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D75" s="10">
         <v>0</v>
@@ -5958,10 +5958,10 @@
         <v>121</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D76" s="10">
         <v>0</v>
@@ -5972,7 +5972,7 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B77" s="10">
         <v>1</v>
@@ -5989,7 +5989,7 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B78" s="10">
         <v>2</v>
@@ -6006,13 +6006,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D79" s="10">
         <v>0</v>
@@ -6023,36 +6023,36 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -6060,21 +6060,21 @@
         <v>81</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B83" s="10">
         <v>1</v>
@@ -6091,70 +6091,70 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D84" s="10">
         <v>0</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D85" s="10">
         <v>0</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -6162,30 +6162,30 @@
         <v>86</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C89" s="10">
         <v>1</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E89" s="10">
         <v>1</v>
@@ -6193,41 +6193,41 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B92" s="10">
         <v>0</v>
@@ -6244,41 +6244,41 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B93" s="10">
         <v>0</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D93" s="10">
         <v>0</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B94" s="10">
         <v>0</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D94" s="10">
         <v>0</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B95" s="10">
         <v>1</v>
@@ -6295,10 +6295,10 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C96" s="10">
         <v>0</v>
@@ -6312,13 +6312,13 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D97" s="10">
         <v>0</v>
@@ -6329,7 +6329,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B98" s="10">
         <v>1</v>
@@ -6346,10 +6346,10 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C99" s="10">
         <v>0</v>
@@ -6363,13 +6363,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D100" s="10">
         <v>0</v>
@@ -6380,7 +6380,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B101" s="10">
         <v>1</v>
@@ -6397,13 +6397,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D102" s="10">
         <v>0</v>
@@ -6417,10 +6417,10 @@
         <v>87</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D103" s="10">
         <v>0</v>
@@ -6431,7 +6431,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B104" s="10">
         <v>1</v>
@@ -6448,13 +6448,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D105" s="10">
         <v>0</v>
@@ -6468,10 +6468,10 @@
         <v>88</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D106" s="10">
         <v>0</v>
@@ -6482,7 +6482,7 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B107" s="10">
         <v>1</v>
@@ -6499,13 +6499,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D108" s="10">
         <v>0</v>
@@ -6519,10 +6519,10 @@
         <v>90</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D109" s="10">
         <v>0</v>
@@ -6533,7 +6533,7 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B110" s="10">
         <v>1</v>
@@ -6550,13 +6550,13 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D111" s="10">
         <v>0</v>
@@ -6570,10 +6570,10 @@
         <v>89</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D112" s="10">
         <v>0</v>
@@ -6584,7 +6584,7 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B113" s="10">
         <v>1</v>
@@ -6601,13 +6601,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D114" s="10">
         <v>0</v>
@@ -6621,10 +6621,10 @@
         <v>91</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D115" s="10">
         <v>0</v>
@@ -6635,7 +6635,7 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B116" s="10">
         <v>1</v>
@@ -6652,13 +6652,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D117" s="10">
         <v>0</v>
@@ -6672,10 +6672,10 @@
         <v>92</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D118" s="10">
         <v>0</v>
@@ -6686,7 +6686,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B119" s="10">
         <v>1</v>
@@ -6703,13 +6703,13 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D120" s="10">
         <v>0</v>
@@ -6723,10 +6723,10 @@
         <v>93</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D121" s="10">
         <v>0</v>
@@ -6737,7 +6737,7 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B122" s="10">
         <v>1</v>
@@ -6754,13 +6754,13 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D123" s="10">
         <v>0</v>
@@ -6774,10 +6774,10 @@
         <v>94</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C124" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D124" s="10">
         <v>0</v>
@@ -6791,16 +6791,16 @@
         <v>68</v>
       </c>
       <c r="B125" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="D125" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="C125" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="D125" s="10" t="s">
-        <v>227</v>
-      </c>
       <c r="E125" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="139" spans="5:6">
@@ -6968,30 +6968,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="23" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C1" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>293</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>294</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="22" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B2" s="1">
         <v>4000</v>
@@ -7014,7 +7014,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="22" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B3" s="1">
         <v>4001</v>
@@ -7058,21 +7058,21 @@
     <row r="1" spans="1:5">
       <c r="A1" s="1"/>
       <c r="B1" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="17" t="s">
@@ -7102,7 +7102,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="16"/>
@@ -7113,7 +7113,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -7124,7 +7124,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="17" t="s">
@@ -7139,7 +7139,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="17" t="s">
@@ -7154,7 +7154,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="17" t="s">
@@ -7169,7 +7169,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="17" t="s">
@@ -7184,7 +7184,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="17" t="s">
@@ -7199,7 +7199,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="17" t="s">
@@ -7214,7 +7214,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="17" t="s">
@@ -7229,7 +7229,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="17" t="s">
@@ -7242,7 +7242,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="17" t="s">
@@ -7253,7 +7253,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="17" t="s">
@@ -7264,7 +7264,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="17" t="s">
@@ -7383,7 +7383,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>40</v>
@@ -7411,7 +7411,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>40</v>
@@ -7441,7 +7441,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="17" t="s">
@@ -7452,7 +7452,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="17" t="s">

</xml_diff>

<commit_message>
For the past few weeks, I've been pondering how to implement animations. Today I got the basics of the idea underway - this includes loading, creating, and drawing the animations, as well as creating the animations for individuals and items. So far, only the idle changes have been implemented for individuals, but the genesis of the idea is working.
What comes next is implementing other animation states, and then adding
item animations.

Also, I made a slime.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="326">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -99,9 +99,6 @@
     <t>A potion which restores health.&amp;&amp;(Restores 10 HP)</t>
   </si>
   <si>
-    <t>A short knife with a pointed tip.\n(+1 Attack, +1 AC, +1 Dam, +1 MinDam, +1 maxDam, Pierce)</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>Mountain Plate</t>
   </si>
   <si>
-    <t>A mighty suit of heavy armor.\n(+2 BluntDR, +2 ChopDr, +2 PierceDR, +2 SlashDR)</t>
-  </si>
-  <si>
     <t>IndividualID</t>
   </si>
   <si>
@@ -943,6 +937,72 @@
   </si>
   <si>
     <t>No! I'm mearly trying to inform you as a friend! (CHR Check)</t>
+  </si>
+  <si>
+    <t>ANIMATION_IDLE,</t>
+  </si>
+  <si>
+    <t>ANIMATION_HARM,</t>
+  </si>
+  <si>
+    <t>ANIMATION_DEATH,</t>
+  </si>
+  <si>
+    <t>ANIMATION_CAST,</t>
+  </si>
+  <si>
+    <t>ANIMATION_ATTACK_SLASH,</t>
+  </si>
+  <si>
+    <t>ANIMATION_ATTACK_CHOP,</t>
+  </si>
+  <si>
+    <t>ANIMATION_ATTACK_BLUNT,</t>
+  </si>
+  <si>
+    <t>ANIMATION_ATTACK_PIERCE,</t>
+  </si>
+  <si>
+    <t>ANIMATION_ATTACK_BOW</t>
+  </si>
+  <si>
+    <t>2,200,200,-1</t>
+  </si>
+  <si>
+    <t>1,200-1</t>
+  </si>
+  <si>
+    <t>5,100,100,100,100,100,-1</t>
+  </si>
+  <si>
+    <t>5,100,100,100,100,100,2,7</t>
+  </si>
+  <si>
+    <t>7,100,100,100,100,100,100,100,3,7</t>
+  </si>
+  <si>
+    <t>13,100,100,100,100,100,100,100,100,100,100,100,100,100,-1</t>
+  </si>
+  <si>
+    <t>DefaultAnimation</t>
+  </si>
+  <si>
+    <t>AnimationEnabled?</t>
+  </si>
+  <si>
+    <t>ANIMATION_IDLE_EQUIPT</t>
+  </si>
+  <si>
+    <t>ANIMATION_CONSUME</t>
+  </si>
+  <si>
+    <t>1,100,-1</t>
+  </si>
+  <si>
+    <t>A mighty suit of heavy armor.&amp;&amp;(+2 BluntDR, +2 ChopDr, +2 PierceDR, +2 SlashDR)</t>
+  </si>
+  <si>
+    <t>2,30,30,-1</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1089,6 +1149,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1385,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="B5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1487,7 +1549,7 @@
         <v>1003</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1507,7 +1569,7 @@
         <v>1006</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1527,7 +1589,7 @@
         <v>1005</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1547,7 +1609,7 @@
         <v>1007</v>
       </c>
       <c r="B9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1589,7 +1651,7 @@
         <v>1003</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C13">
         <v>1005</v>
@@ -1600,7 +1662,7 @@
         <v>1003</v>
       </c>
       <c r="B14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C14">
         <v>1006</v>
@@ -1608,7 +1670,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1616,7 +1678,7 @@
         <v>1004</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1638,173 +1700,269 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX10"/>
+  <dimension ref="A1:BK11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="I2:K2"/>
+    <sheetView topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BK2" sqref="BK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="22.7109375" customWidth="1"/>
+    <col min="55" max="55" width="19" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="84.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:63">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>37</v>
       </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
         <v>39</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>132</v>
+      </c>
+      <c r="P1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" t="s">
+        <v>126</v>
+      </c>
+      <c r="S1" t="s">
+        <v>127</v>
+      </c>
+      <c r="T1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V1" t="s">
+        <v>130</v>
+      </c>
+      <c r="W1" t="s">
+        <v>131</v>
+      </c>
+      <c r="X1" t="s">
         <v>40</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Y1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P1" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>127</v>
-      </c>
-      <c r="R1" t="s">
-        <v>128</v>
-      </c>
-      <c r="S1" t="s">
-        <v>129</v>
-      </c>
-      <c r="T1" t="s">
-        <v>130</v>
-      </c>
-      <c r="U1" t="s">
-        <v>131</v>
-      </c>
-      <c r="V1" t="s">
-        <v>132</v>
-      </c>
-      <c r="W1" t="s">
-        <v>133</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>45</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>48</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>49</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>50</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>51</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>52</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>53</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>54</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>55</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>56</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>57</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>58</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>59</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>60</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>61</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>62</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>63</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>64</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>65</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>319</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>304</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>321</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>322</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>305</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>306</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>307</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>308</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>309</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>310</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>311</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>312</v>
+      </c>
+      <c r="BK1" t="s">
         <v>66</v>
       </c>
-      <c r="AW1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50">
+    </row>
+    <row r="2" spans="1:63">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1952,11 +2110,50 @@
       <c r="AW2">
         <v>0</v>
       </c>
-      <c r="AX2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="3" spans="1:50">
+      <c r="AX2">
+        <v>1</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>313</v>
+      </c>
+      <c r="BB2">
+        <v>-1</v>
+      </c>
+      <c r="BC2">
+        <v>-1</v>
+      </c>
+      <c r="BD2" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="BE2">
+        <v>-1</v>
+      </c>
+      <c r="BF2" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="BG2">
+        <v>-1</v>
+      </c>
+      <c r="BH2">
+        <v>-1</v>
+      </c>
+      <c r="BI2">
+        <v>-1</v>
+      </c>
+      <c r="BJ2">
+        <v>-1</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:63">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2104,11 +2301,50 @@
       <c r="AW3">
         <v>0</v>
       </c>
-      <c r="AX3" t="s">
+      <c r="AX3">
+        <v>1</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA3">
+        <v>-1</v>
+      </c>
+      <c r="BB3">
+        <v>-1</v>
+      </c>
+      <c r="BC3">
+        <v>-1</v>
+      </c>
+      <c r="BD3" s="24">
+        <v>-1</v>
+      </c>
+      <c r="BE3">
+        <v>-1</v>
+      </c>
+      <c r="BF3">
+        <v>-1</v>
+      </c>
+      <c r="BG3">
+        <v>-1</v>
+      </c>
+      <c r="BH3">
+        <v>-1</v>
+      </c>
+      <c r="BI3">
+        <v>-1</v>
+      </c>
+      <c r="BJ3">
+        <v>-1</v>
+      </c>
+      <c r="BK3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:63">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2256,11 +2492,50 @@
       <c r="AW4">
         <v>0</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="AX4">
+        <v>1</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA4">
+        <v>-1</v>
+      </c>
+      <c r="BB4">
+        <v>-1</v>
+      </c>
+      <c r="BC4">
+        <v>-1</v>
+      </c>
+      <c r="BD4" s="24">
+        <v>-1</v>
+      </c>
+      <c r="BE4">
+        <v>-1</v>
+      </c>
+      <c r="BF4">
+        <v>-1</v>
+      </c>
+      <c r="BG4">
+        <v>-1</v>
+      </c>
+      <c r="BH4">
+        <v>-1</v>
+      </c>
+      <c r="BI4">
+        <v>-1</v>
+      </c>
+      <c r="BJ4">
+        <v>-1</v>
+      </c>
+      <c r="BK4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:50">
+    <row r="5" spans="1:63">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2408,11 +2683,50 @@
       <c r="AW5">
         <v>0</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="AX5">
+        <v>1</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA5">
+        <v>-1</v>
+      </c>
+      <c r="BB5">
+        <v>-1</v>
+      </c>
+      <c r="BC5">
+        <v>-1</v>
+      </c>
+      <c r="BD5" s="24">
+        <v>-1</v>
+      </c>
+      <c r="BE5">
+        <v>-1</v>
+      </c>
+      <c r="BF5">
+        <v>-1</v>
+      </c>
+      <c r="BG5">
+        <v>-1</v>
+      </c>
+      <c r="BH5">
+        <v>-1</v>
+      </c>
+      <c r="BI5">
+        <v>-1</v>
+      </c>
+      <c r="BJ5">
+        <v>-1</v>
+      </c>
+      <c r="BK5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:63">
       <c r="A6">
         <v>200</v>
       </c>
@@ -2560,11 +2874,50 @@
       <c r="AW6">
         <v>1</v>
       </c>
-      <c r="AX6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:50">
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>313</v>
+      </c>
+      <c r="BB6">
+        <v>-1</v>
+      </c>
+      <c r="BC6">
+        <v>-1</v>
+      </c>
+      <c r="BD6" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="BE6">
+        <v>-1</v>
+      </c>
+      <c r="BF6" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="BG6">
+        <v>-1</v>
+      </c>
+      <c r="BH6">
+        <v>-1</v>
+      </c>
+      <c r="BI6">
+        <v>-1</v>
+      </c>
+      <c r="BJ6">
+        <v>-1</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:63">
       <c r="A7">
         <v>200</v>
       </c>
@@ -2575,13 +2928,13 @@
         <v>1006</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -2599,7 +2952,7 @@
         <v>255</v>
       </c>
       <c r="L7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -2712,11 +3065,50 @@
       <c r="AW7">
         <v>1</v>
       </c>
-      <c r="AX7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:50">
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA7">
+        <v>-1</v>
+      </c>
+      <c r="BB7">
+        <v>-1</v>
+      </c>
+      <c r="BC7">
+        <v>-1</v>
+      </c>
+      <c r="BD7" s="24">
+        <v>-1</v>
+      </c>
+      <c r="BE7">
+        <v>-1</v>
+      </c>
+      <c r="BF7">
+        <v>-1</v>
+      </c>
+      <c r="BG7">
+        <v>-1</v>
+      </c>
+      <c r="BH7">
+        <v>-1</v>
+      </c>
+      <c r="BI7">
+        <v>-1</v>
+      </c>
+      <c r="BJ7">
+        <v>-1</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:63">
       <c r="A8">
         <v>207</v>
       </c>
@@ -2864,11 +3256,50 @@
       <c r="AW8">
         <v>0</v>
       </c>
-      <c r="AX8" t="s">
+      <c r="AX8">
+        <v>0</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA8">
+        <v>-1</v>
+      </c>
+      <c r="BB8">
+        <v>-1</v>
+      </c>
+      <c r="BC8">
+        <v>-1</v>
+      </c>
+      <c r="BD8" s="24">
+        <v>-1</v>
+      </c>
+      <c r="BE8">
+        <v>-1</v>
+      </c>
+      <c r="BF8">
+        <v>-1</v>
+      </c>
+      <c r="BG8">
+        <v>-1</v>
+      </c>
+      <c r="BH8">
+        <v>-1</v>
+      </c>
+      <c r="BI8">
+        <v>-1</v>
+      </c>
+      <c r="BJ8">
+        <v>-1</v>
+      </c>
+      <c r="BK8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:63">
       <c r="A9">
         <v>207</v>
       </c>
@@ -3016,11 +3447,50 @@
       <c r="AW9">
         <v>0</v>
       </c>
-      <c r="AX9" t="s">
+      <c r="AX9">
+        <v>0</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA9">
+        <v>-1</v>
+      </c>
+      <c r="BB9">
+        <v>-1</v>
+      </c>
+      <c r="BC9">
+        <v>-1</v>
+      </c>
+      <c r="BD9" s="24">
+        <v>-1</v>
+      </c>
+      <c r="BE9">
+        <v>-1</v>
+      </c>
+      <c r="BF9">
+        <v>-1</v>
+      </c>
+      <c r="BG9">
+        <v>-1</v>
+      </c>
+      <c r="BH9">
+        <v>-1</v>
+      </c>
+      <c r="BI9">
+        <v>-1</v>
+      </c>
+      <c r="BJ9">
+        <v>-1</v>
+      </c>
+      <c r="BK9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:50">
+    <row r="10" spans="1:63">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3168,154 +3638,281 @@
       <c r="AW10">
         <v>0</v>
       </c>
-      <c r="AX10" t="s">
-        <v>248</v>
-      </c>
+      <c r="AX10">
+        <v>1</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>313</v>
+      </c>
+      <c r="BB10">
+        <v>-1</v>
+      </c>
+      <c r="BC10">
+        <v>-1</v>
+      </c>
+      <c r="BD10" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="BE10">
+        <v>-1</v>
+      </c>
+      <c r="BF10" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="BG10">
+        <v>-1</v>
+      </c>
+      <c r="BH10">
+        <v>-1</v>
+      </c>
+      <c r="BI10">
+        <v>-1</v>
+      </c>
+      <c r="BJ10">
+        <v>-1</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:63">
+      <c r="BD11" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AP9"/>
+  <dimension ref="A1:BA9"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AS3" sqref="AS3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="39.85546875" customWidth="1"/>
+    <col min="48" max="48" width="18" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="30.42578125" customWidth="1"/>
+    <col min="50" max="50" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:53">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>119</v>
+      </c>
+      <c r="R1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="T1" t="s">
+        <v>121</v>
+      </c>
+      <c r="U1" t="s">
+        <v>122</v>
+      </c>
+      <c r="V1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K1" t="s">
-        <v>115</v>
-      </c>
-      <c r="L1" t="s">
-        <v>116</v>
-      </c>
-      <c r="M1" t="s">
-        <v>117</v>
-      </c>
-      <c r="N1" t="s">
-        <v>118</v>
-      </c>
-      <c r="O1" t="s">
-        <v>119</v>
-      </c>
-      <c r="P1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>121</v>
-      </c>
-      <c r="R1" t="s">
-        <v>122</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>80</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y1" t="s">
         <v>123</v>
       </c>
-      <c r="U1" t="s">
-        <v>124</v>
-      </c>
-      <c r="V1" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>82</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>83</v>
       </c>
-      <c r="Y1" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>85</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>86</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>87</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>88</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>89</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>90</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>91</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>92</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>93</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>94</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>95</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>96</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>97</v>
       </c>
-      <c r="AN1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>99</v>
-      </c>
       <c r="AP1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42">
+        <v>109</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>319</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>306</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>307</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>308</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>309</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>311</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -3332,7 +3929,7 @@
         <v>255</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3392,7 +3989,7 @@
         <v>0</v>
       </c>
       <c r="Z2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -3442,8 +4039,41 @@
       <c r="AP2">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:42">
+      <c r="AQ2">
+        <v>1</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>325</v>
+      </c>
+      <c r="AT2">
+        <v>-1</v>
+      </c>
+      <c r="AU2" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="AV2">
+        <v>-1</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>317</v>
+      </c>
+      <c r="AX2">
+        <v>-1</v>
+      </c>
+      <c r="AY2">
+        <v>-1</v>
+      </c>
+      <c r="AZ2">
+        <v>-1</v>
+      </c>
+      <c r="BA2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53">
       <c r="A3">
         <v>2006</v>
       </c>
@@ -3460,7 +4090,7 @@
         <v>255</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -3520,7 +4150,7 @@
         <v>0</v>
       </c>
       <c r="Z3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -3570,8 +4200,41 @@
       <c r="AP3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:42">
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AT3">
+        <v>-1</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>315</v>
+      </c>
+      <c r="AV3">
+        <v>-1</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>316</v>
+      </c>
+      <c r="AX3">
+        <v>-1</v>
+      </c>
+      <c r="AY3">
+        <v>-1</v>
+      </c>
+      <c r="AZ3">
+        <v>-1</v>
+      </c>
+      <c r="BA3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53">
       <c r="A4">
         <v>2007</v>
       </c>
@@ -3588,7 +4251,7 @@
         <v>255</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -3648,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="Z4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -3698,8 +4361,41 @@
       <c r="AP4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:42">
+      <c r="AQ4">
+        <v>1</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>325</v>
+      </c>
+      <c r="AT4">
+        <v>-1</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>315</v>
+      </c>
+      <c r="AV4">
+        <v>-1</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>316</v>
+      </c>
+      <c r="AX4">
+        <v>-1</v>
+      </c>
+      <c r="AY4">
+        <v>-1</v>
+      </c>
+      <c r="AZ4">
+        <v>-1</v>
+      </c>
+      <c r="BA4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53">
       <c r="A5">
         <v>2008</v>
       </c>
@@ -3716,7 +4412,7 @@
         <v>255</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3776,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -3826,8 +4522,41 @@
       <c r="AP5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:42">
+      <c r="AQ5">
+        <v>1</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>325</v>
+      </c>
+      <c r="AT5">
+        <v>-1</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>315</v>
+      </c>
+      <c r="AV5">
+        <v>-1</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>316</v>
+      </c>
+      <c r="AX5">
+        <v>-1</v>
+      </c>
+      <c r="AY5">
+        <v>-1</v>
+      </c>
+      <c r="AZ5">
+        <v>-1</v>
+      </c>
+      <c r="BA5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53">
       <c r="A6">
         <v>2009</v>
       </c>
@@ -3844,7 +4573,7 @@
         <v>255</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -3904,7 +4633,7 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA6">
         <v>1</v>
@@ -3954,8 +4683,41 @@
       <c r="AP6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:42">
+      <c r="AQ6">
+        <v>1</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>325</v>
+      </c>
+      <c r="AT6">
+        <v>-1</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>315</v>
+      </c>
+      <c r="AV6">
+        <v>-1</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>316</v>
+      </c>
+      <c r="AX6">
+        <v>-1</v>
+      </c>
+      <c r="AY6">
+        <v>-1</v>
+      </c>
+      <c r="AZ6">
+        <v>-1</v>
+      </c>
+      <c r="BA6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -3972,7 +4734,7 @@
         <v>255</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -4032,7 +4794,7 @@
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA7">
         <v>1</v>
@@ -4082,8 +4844,41 @@
       <c r="AP7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:42">
+      <c r="AQ7">
+        <v>1</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>325</v>
+      </c>
+      <c r="AT7">
+        <v>-1</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>315</v>
+      </c>
+      <c r="AV7">
+        <v>-1</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>316</v>
+      </c>
+      <c r="AX7">
+        <v>-1</v>
+      </c>
+      <c r="AY7">
+        <v>-1</v>
+      </c>
+      <c r="AZ7">
+        <v>-1</v>
+      </c>
+      <c r="BA7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53">
       <c r="A8">
         <v>2013</v>
       </c>
@@ -4100,7 +4895,7 @@
         <v>255</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -4160,7 +4955,7 @@
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AA8">
         <v>1</v>
@@ -4210,8 +5005,41 @@
       <c r="AP8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:42">
+      <c r="AQ8">
+        <v>1</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>314</v>
+      </c>
+      <c r="AT8">
+        <v>-1</v>
+      </c>
+      <c r="AU8">
+        <v>-1</v>
+      </c>
+      <c r="AV8">
+        <v>-1</v>
+      </c>
+      <c r="AW8">
+        <v>-1</v>
+      </c>
+      <c r="AX8">
+        <v>-1</v>
+      </c>
+      <c r="AY8">
+        <v>-1</v>
+      </c>
+      <c r="AZ8">
+        <v>-1</v>
+      </c>
+      <c r="BA8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -4228,7 +5056,7 @@
         <v>255</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -4288,7 +5116,7 @@
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AA9">
         <v>1</v>
@@ -4337,6 +5165,39 @@
       </c>
       <c r="AP9">
         <v>100</v>
+      </c>
+      <c r="AQ9">
+        <v>1</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>314</v>
+      </c>
+      <c r="AT9">
+        <v>-1</v>
+      </c>
+      <c r="AU9">
+        <v>-1</v>
+      </c>
+      <c r="AV9">
+        <v>-1</v>
+      </c>
+      <c r="AW9">
+        <v>-1</v>
+      </c>
+      <c r="AX9">
+        <v>-1</v>
+      </c>
+      <c r="AY9">
+        <v>-1</v>
+      </c>
+      <c r="AZ9">
+        <v>-1</v>
+      </c>
+      <c r="BA9">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -4364,46 +5225,46 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" t="s">
         <v>102</v>
       </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>103</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>104</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>105</v>
-      </c>
-      <c r="P1" t="s">
-        <v>106</v>
-      </c>
-      <c r="S1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -4438,22 +5299,22 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="T2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -4485,7 +5346,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M3">
         <v>206</v>
@@ -4555,7 +5416,7 @@
         <v>1005</v>
       </c>
       <c r="J5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -4568,7 +5429,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4578,10 +5439,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4589,7 +5450,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4597,7 +5458,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4605,7 +5466,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4613,7 +5474,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4621,7 +5482,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4629,7 +5490,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4637,7 +5498,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4645,7 +5506,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4653,7 +5514,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -4680,7 +5541,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="6">
         <v>0</v>
@@ -4697,7 +5558,7 @@
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>12</v>
@@ -4706,7 +5567,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>16</v>
@@ -4714,24 +5575,24 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -4748,7 +5609,7 @@
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1">
       <c r="A5" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B5" s="10">
         <v>0</v>
@@ -4765,41 +5626,41 @@
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1">
       <c r="A6" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" s="11">
         <v>1</v>
@@ -4816,7 +5677,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B9" s="10">
         <v>0</v>
@@ -4833,16 +5694,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E10" s="7">
         <v>0</v>
@@ -4850,13 +5711,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B11" s="10">
         <v>0</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D11" s="10">
         <v>1</v>
@@ -4867,16 +5728,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B12" s="10">
         <v>0</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
@@ -4884,16 +5745,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B13" s="10">
         <v>0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E13" s="7">
         <v>0</v>
@@ -4901,58 +5762,58 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B14" s="10">
         <v>0</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D14" s="10">
         <v>0</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B15" s="10">
         <v>0</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D15" s="10">
         <v>0</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B16" s="10">
         <v>0</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D16" s="10">
         <v>0</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -4969,7 +5830,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B18" s="10">
         <v>0</v>
@@ -4986,177 +5847,177 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B19" s="10">
         <v>0</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B29" s="10">
         <v>0</v>
@@ -5173,10 +6034,10 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C30" s="10">
         <v>0</v>
@@ -5190,381 +6051,381 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B31" s="10">
         <v>0</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B32" s="10">
         <v>0</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B34" s="10">
         <v>0</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B41" s="10">
         <v>0</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B42" s="10">
         <v>0</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B43" s="10">
         <v>0</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B53" s="10">
         <v>1</v>
@@ -5576,46 +6437,46 @@
         <v>0</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B54" s="10">
         <v>2</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D54" s="10">
         <v>0</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D55" s="10">
         <v>0</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B56" s="10">
         <v>1</v>
@@ -5632,13 +6493,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B57" s="10">
         <v>2</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D57" s="10">
         <v>0</v>
@@ -5649,13 +6510,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D58" s="10">
         <v>0</v>
@@ -5666,7 +6527,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B59" s="10">
         <v>1</v>
@@ -5683,13 +6544,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B60" s="10">
         <v>2</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D60" s="10">
         <v>0</v>
@@ -5700,13 +6561,13 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D61" s="10">
         <v>0</v>
@@ -5717,7 +6578,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B62" s="10">
         <v>1</v>
@@ -5734,13 +6595,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B63" s="10">
         <v>2</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D63" s="10">
         <v>0</v>
@@ -5751,13 +6612,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D64" s="10">
         <v>0</v>
@@ -5768,7 +6629,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B65" s="10">
         <v>1</v>
@@ -5785,13 +6646,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B66" s="10">
         <v>2</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D66" s="10">
         <v>0</v>
@@ -5802,13 +6663,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D67" s="10">
         <v>0</v>
@@ -5819,7 +6680,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B68" s="10">
         <v>1</v>
@@ -5836,13 +6697,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B69" s="10">
         <v>2</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D69" s="10">
         <v>0</v>
@@ -5853,13 +6714,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D70" s="10">
         <v>0</v>
@@ -5870,7 +6731,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B71" s="10">
         <v>1</v>
@@ -5887,13 +6748,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B72" s="10">
         <v>2</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D72" s="10">
         <v>0</v>
@@ -5904,13 +6765,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D73" s="10">
         <v>0</v>
@@ -5921,7 +6782,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B74" s="10">
         <v>1</v>
@@ -5938,13 +6799,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B75" s="10">
         <v>2</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D75" s="10">
         <v>0</v>
@@ -5955,13 +6816,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D76" s="10">
         <v>0</v>
@@ -5972,7 +6833,7 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B77" s="10">
         <v>1</v>
@@ -5989,7 +6850,7 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B78" s="10">
         <v>2</v>
@@ -6006,13 +6867,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D79" s="10">
         <v>0</v>
@@ -6023,58 +6884,58 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B83" s="10">
         <v>1</v>
@@ -6091,101 +6952,101 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D84" s="10">
         <v>0</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D85" s="10">
         <v>0</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C89" s="10">
         <v>1</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E89" s="10">
         <v>1</v>
@@ -6193,41 +7054,41 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B92" s="10">
         <v>0</v>
@@ -6244,41 +7105,41 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B93" s="10">
         <v>0</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D93" s="10">
         <v>0</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B94" s="10">
         <v>0</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D94" s="10">
         <v>0</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B95" s="10">
         <v>1</v>
@@ -6295,10 +7156,10 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C96" s="10">
         <v>0</v>
@@ -6312,13 +7173,13 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D97" s="10">
         <v>0</v>
@@ -6329,7 +7190,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B98" s="10">
         <v>1</v>
@@ -6346,10 +7207,10 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C99" s="10">
         <v>0</v>
@@ -6363,13 +7224,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D100" s="10">
         <v>0</v>
@@ -6380,7 +7241,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B101" s="10">
         <v>1</v>
@@ -6397,13 +7258,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D102" s="10">
         <v>0</v>
@@ -6414,13 +7275,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D103" s="10">
         <v>0</v>
@@ -6431,7 +7292,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B104" s="10">
         <v>1</v>
@@ -6448,13 +7309,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D105" s="10">
         <v>0</v>
@@ -6465,13 +7326,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D106" s="10">
         <v>0</v>
@@ -6482,7 +7343,7 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B107" s="10">
         <v>1</v>
@@ -6499,13 +7360,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D108" s="10">
         <v>0</v>
@@ -6516,13 +7377,13 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D109" s="10">
         <v>0</v>
@@ -6533,7 +7394,7 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B110" s="10">
         <v>1</v>
@@ -6550,13 +7411,13 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D111" s="10">
         <v>0</v>
@@ -6567,13 +7428,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D112" s="10">
         <v>0</v>
@@ -6584,7 +7445,7 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B113" s="10">
         <v>1</v>
@@ -6601,13 +7462,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D114" s="10">
         <v>0</v>
@@ -6618,13 +7479,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D115" s="10">
         <v>0</v>
@@ -6635,7 +7496,7 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B116" s="10">
         <v>1</v>
@@ -6652,13 +7513,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D117" s="10">
         <v>0</v>
@@ -6669,13 +7530,13 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D118" s="10">
         <v>0</v>
@@ -6686,7 +7547,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B119" s="10">
         <v>1</v>
@@ -6703,13 +7564,13 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D120" s="10">
         <v>0</v>
@@ -6720,13 +7581,13 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D121" s="10">
         <v>0</v>
@@ -6737,7 +7598,7 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B122" s="10">
         <v>1</v>
@@ -6754,13 +7615,13 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D123" s="10">
         <v>0</v>
@@ -6771,13 +7632,13 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C124" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D124" s="10">
         <v>0</v>
@@ -6788,19 +7649,19 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B125" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D125" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C125" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="D125" s="10" t="s">
-        <v>225</v>
-      </c>
       <c r="E125" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="139" spans="5:6">
@@ -6968,30 +7829,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>290</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>291</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>292</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="22" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B2" s="1">
         <v>4000</v>
@@ -7014,7 +7875,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="22" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B3" s="1">
         <v>4001</v>
@@ -7058,535 +7919,535 @@
     <row r="1" spans="1:5">
       <c r="A1" s="1"/>
       <c r="B1" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="21"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="21"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="19"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="19"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="19"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="19"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="19"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="19"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="19"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="19"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="19"/>

</xml_diff>

<commit_message>
Implemented delayed animations; some minor things to clean up (such as the delay calculation) however it's working.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="325">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -972,12 +972,6 @@
     <t>1,200-1</t>
   </si>
   <si>
-    <t>5,100,100,100,100,100,-1</t>
-  </si>
-  <si>
-    <t>5,100,100,100,100,100,2,7</t>
-  </si>
-  <si>
     <t>7,100,100,100,100,100,100,100,3,7</t>
   </si>
   <si>
@@ -1003,6 +997,9 @@
   </si>
   <si>
     <t>2,30,30,-1</t>
+  </si>
+  <si>
+    <t>5,5,5,5,5,5,-1</t>
   </si>
 </sst>
 </file>
@@ -1920,19 +1917,19 @@
         <v>65</v>
       </c>
       <c r="AX1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AY1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AZ1" t="s">
         <v>304</v>
       </c>
       <c r="BA1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="BB1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="BC1" t="s">
         <v>305</v>
@@ -2117,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="AZ2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BA2" t="s">
         <v>313</v>
@@ -2129,13 +2126,13 @@
         <v>-1</v>
       </c>
       <c r="BD2" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="BE2">
         <v>-1</v>
       </c>
       <c r="BF2" s="25" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="BG2">
         <v>-1</v>
@@ -2308,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="AZ3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BA3">
         <v>-1</v>
@@ -2499,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="AZ4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BA4">
         <v>-1</v>
@@ -2690,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="AZ5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BA5">
         <v>-1</v>
@@ -2881,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="AZ6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BA6" t="s">
         <v>313</v>
@@ -2893,13 +2890,13 @@
         <v>-1</v>
       </c>
       <c r="BD6" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="BE6">
         <v>-1</v>
       </c>
       <c r="BF6" s="25" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="BG6">
         <v>-1</v>
@@ -3072,7 +3069,7 @@
         <v>0</v>
       </c>
       <c r="AZ7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BA7">
         <v>-1</v>
@@ -3105,7 +3102,7 @@
         <v>-1</v>
       </c>
       <c r="BK7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:63">
@@ -3263,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="AZ8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BA8">
         <v>-1</v>
@@ -3454,7 +3451,7 @@
         <v>0</v>
       </c>
       <c r="AZ9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BA9">
         <v>-1</v>
@@ -3645,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="AZ10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="BA10" t="s">
         <v>313</v>
@@ -3657,13 +3654,13 @@
         <v>-1</v>
       </c>
       <c r="BD10" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="BE10">
         <v>-1</v>
       </c>
       <c r="BF10" s="25" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="BG10">
         <v>-1</v>
@@ -3694,8 +3691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AS3" sqref="AS3"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AT7" sqref="AT7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3879,37 +3876,37 @@
         <v>109</v>
       </c>
       <c r="AQ1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AR1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AS1" t="s">
         <v>304</v>
       </c>
       <c r="AT1" t="s">
+        <v>308</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>309</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>311</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>312</v>
+      </c>
+      <c r="AY1" t="s">
         <v>305</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AZ1" t="s">
         <v>306</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BA1" t="s">
         <v>307</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>308</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>309</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>310</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:53">
@@ -4046,19 +4043,19 @@
         <v>0</v>
       </c>
       <c r="AS2" t="s">
-        <v>325</v>
-      </c>
-      <c r="AT2">
-        <v>-1</v>
-      </c>
-      <c r="AU2" s="24" t="s">
-        <v>318</v>
+        <v>323</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>324</v>
+      </c>
+      <c r="AU2">
+        <v>-1</v>
       </c>
       <c r="AV2">
         <v>-1</v>
       </c>
-      <c r="AW2" t="s">
-        <v>317</v>
+      <c r="AW2">
+        <v>-1</v>
       </c>
       <c r="AX2">
         <v>-1</v>
@@ -4066,8 +4063,8 @@
       <c r="AY2">
         <v>-1</v>
       </c>
-      <c r="AZ2">
-        <v>-1</v>
+      <c r="AZ2" t="s">
+        <v>324</v>
       </c>
       <c r="BA2">
         <v>-1</v>
@@ -4207,19 +4204,19 @@
         <v>0</v>
       </c>
       <c r="AS3" t="s">
-        <v>325</v>
-      </c>
-      <c r="AT3">
-        <v>-1</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>315</v>
+        <v>323</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>324</v>
+      </c>
+      <c r="AU3">
+        <v>-1</v>
       </c>
       <c r="AV3">
         <v>-1</v>
       </c>
-      <c r="AW3" t="s">
-        <v>316</v>
+      <c r="AW3">
+        <v>-1</v>
       </c>
       <c r="AX3">
         <v>-1</v>
@@ -4227,8 +4224,8 @@
       <c r="AY3">
         <v>-1</v>
       </c>
-      <c r="AZ3">
-        <v>-1</v>
+      <c r="AZ3" t="s">
+        <v>324</v>
       </c>
       <c r="BA3">
         <v>-1</v>
@@ -4368,19 +4365,19 @@
         <v>0</v>
       </c>
       <c r="AS4" t="s">
-        <v>325</v>
-      </c>
-      <c r="AT4">
-        <v>-1</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>315</v>
+        <v>323</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>324</v>
+      </c>
+      <c r="AU4">
+        <v>-1</v>
       </c>
       <c r="AV4">
         <v>-1</v>
       </c>
-      <c r="AW4" t="s">
-        <v>316</v>
+      <c r="AW4">
+        <v>-1</v>
       </c>
       <c r="AX4">
         <v>-1</v>
@@ -4388,8 +4385,8 @@
       <c r="AY4">
         <v>-1</v>
       </c>
-      <c r="AZ4">
-        <v>-1</v>
+      <c r="AZ4" t="s">
+        <v>324</v>
       </c>
       <c r="BA4">
         <v>-1</v>
@@ -4529,19 +4526,19 @@
         <v>0</v>
       </c>
       <c r="AS5" t="s">
-        <v>325</v>
-      </c>
-      <c r="AT5">
-        <v>-1</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>315</v>
+        <v>323</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>324</v>
+      </c>
+      <c r="AU5">
+        <v>-1</v>
       </c>
       <c r="AV5">
         <v>-1</v>
       </c>
-      <c r="AW5" t="s">
-        <v>316</v>
+      <c r="AW5">
+        <v>-1</v>
       </c>
       <c r="AX5">
         <v>-1</v>
@@ -4549,8 +4546,8 @@
       <c r="AY5">
         <v>-1</v>
       </c>
-      <c r="AZ5">
-        <v>-1</v>
+      <c r="AZ5" t="s">
+        <v>324</v>
       </c>
       <c r="BA5">
         <v>-1</v>
@@ -4690,19 +4687,19 @@
         <v>0</v>
       </c>
       <c r="AS6" t="s">
-        <v>325</v>
-      </c>
-      <c r="AT6">
-        <v>-1</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>315</v>
+        <v>323</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>324</v>
+      </c>
+      <c r="AU6">
+        <v>-1</v>
       </c>
       <c r="AV6">
         <v>-1</v>
       </c>
-      <c r="AW6" t="s">
-        <v>316</v>
+      <c r="AW6">
+        <v>-1</v>
       </c>
       <c r="AX6">
         <v>-1</v>
@@ -4710,8 +4707,8 @@
       <c r="AY6">
         <v>-1</v>
       </c>
-      <c r="AZ6">
-        <v>-1</v>
+      <c r="AZ6" t="s">
+        <v>324</v>
       </c>
       <c r="BA6">
         <v>-1</v>
@@ -4851,19 +4848,19 @@
         <v>0</v>
       </c>
       <c r="AS7" t="s">
-        <v>325</v>
-      </c>
-      <c r="AT7">
-        <v>-1</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>315</v>
+        <v>323</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>324</v>
+      </c>
+      <c r="AU7">
+        <v>-1</v>
       </c>
       <c r="AV7">
         <v>-1</v>
       </c>
-      <c r="AW7" t="s">
-        <v>316</v>
+      <c r="AW7">
+        <v>-1</v>
       </c>
       <c r="AX7">
         <v>-1</v>
@@ -4871,8 +4868,8 @@
       <c r="AY7">
         <v>-1</v>
       </c>
-      <c r="AZ7">
-        <v>-1</v>
+      <c r="AZ7" t="s">
+        <v>324</v>
       </c>
       <c r="BA7">
         <v>-1</v>

</xml_diff>

<commit_message>
After spending the 4th of July in Chicago, I came back and finished implementing item animations with the individual. Basically, the Items are treated as 'layers' to the individual's 'base' animation-meaning the base animation dictates which frame of the layer to play. this is nice because A) everything is in sync by having one timer and controller for frame changes, and B) the general idea is something that other structs could use. In short, animations are working nicely.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Abilities!$A$1:$A$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Items!$L$1:$L$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="326">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -72,9 +73,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>Dagger</t>
-  </si>
-  <si>
     <t>i</t>
   </si>
   <si>
@@ -105,9 +103,6 @@
     <t>h</t>
   </si>
   <si>
-    <t>Mountain Plate</t>
-  </si>
-  <si>
     <t>IndividualID</t>
   </si>
   <si>
@@ -966,18 +961,9 @@
     <t>ANIMATION_ATTACK_BOW</t>
   </si>
   <si>
-    <t>2,200,200,-1</t>
-  </si>
-  <si>
     <t>1,200-1</t>
   </si>
   <si>
-    <t>7,100,100,100,100,100,100,100,3,7</t>
-  </si>
-  <si>
-    <t>13,100,100,100,100,100,100,100,100,100,100,100,100,100,-1</t>
-  </si>
-  <si>
     <t>DefaultAnimation</t>
   </si>
   <si>
@@ -990,16 +976,34 @@
     <t>ANIMATION_CONSUME</t>
   </si>
   <si>
-    <t>1,100,-1</t>
-  </si>
-  <si>
-    <t>A mighty suit of heavy armor.&amp;&amp;(+2 BluntDR, +2 ChopDr, +2 PierceDR, +2 SlashDR)</t>
-  </si>
-  <si>
     <t>2,30,30,-1</t>
   </si>
   <si>
     <t>5,5,5,5,5,5,-1</t>
+  </si>
+  <si>
+    <t>A sharp long sword.&amp;&amp;(+1 Attack, +1 AC, +2 Dam, Pierce)</t>
+  </si>
+  <si>
+    <t>Long Sword</t>
+  </si>
+  <si>
+    <t>Iron Armor</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>13,10,10,10,10,10,10,10,10,10,10,10,10,100,-1</t>
+  </si>
+  <si>
+    <t>7,5,5,5,5,5,5,5,3,7</t>
+  </si>
+  <si>
+    <t>A sturdy suit of heavy armor.&amp;&amp;(+2 BluntDR, +2 ChopDr, +2 PierceDR, +2 SlashDR)</t>
+  </si>
+  <si>
+    <t>1,10,-1</t>
   </si>
 </sst>
 </file>
@@ -1546,7 +1550,7 @@
         <v>1003</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1566,7 +1570,7 @@
         <v>1006</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1586,7 +1590,7 @@
         <v>1005</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1606,7 +1610,7 @@
         <v>1007</v>
       </c>
       <c r="B9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1648,7 +1652,7 @@
         <v>1003</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13">
         <v>1005</v>
@@ -1659,7 +1663,7 @@
         <v>1003</v>
       </c>
       <c r="B14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C14">
         <v>1006</v>
@@ -1667,7 +1671,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1675,7 +1679,7 @@
         <v>1004</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1697,10 +1701,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BK11"/>
+  <dimension ref="A1:BK10"/>
   <sheetViews>
-    <sheetView topLeftCell="BH1" workbookViewId="0">
-      <selection activeCell="BK2" sqref="BK2"/>
+    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
+      <selection activeCell="BH17" sqref="BH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1770,193 +1774,193 @@
   <sheetData>
     <row r="1" spans="1:63">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>123</v>
+      </c>
+      <c r="R1" t="s">
+        <v>124</v>
+      </c>
+      <c r="S1" t="s">
+        <v>125</v>
+      </c>
+      <c r="T1" t="s">
+        <v>126</v>
+      </c>
+      <c r="U1" t="s">
+        <v>127</v>
+      </c>
+      <c r="V1" t="s">
+        <v>128</v>
+      </c>
+      <c r="W1" t="s">
+        <v>129</v>
+      </c>
+      <c r="X1" t="s">
         <v>38</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Y1" t="s">
         <v>39</v>
       </c>
-      <c r="O1" t="s">
-        <v>132</v>
-      </c>
-      <c r="P1" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>125</v>
-      </c>
-      <c r="R1" t="s">
-        <v>126</v>
-      </c>
-      <c r="S1" t="s">
-        <v>127</v>
-      </c>
-      <c r="T1" t="s">
-        <v>128</v>
-      </c>
-      <c r="U1" t="s">
-        <v>129</v>
-      </c>
-      <c r="V1" t="s">
-        <v>130</v>
-      </c>
-      <c r="W1" t="s">
-        <v>131</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>43</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>45</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>46</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>47</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>49</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>50</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>51</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>52</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>53</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>54</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>55</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>56</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>57</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>58</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>59</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>60</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>61</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>62</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>63</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
+        <v>313</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>312</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>302</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>314</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>306</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>307</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>308</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>309</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>310</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>305</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>315</v>
+      </c>
+      <c r="BK1" t="s">
         <v>64</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>318</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>317</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>304</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>319</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>320</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>305</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>306</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>307</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>308</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>309</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>310</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>312</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:63">
@@ -1973,7 +1977,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>321</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -1994,7 +1998,7 @@
         <v>255</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>319</v>
       </c>
       <c r="M2">
         <v>3</v>
@@ -2051,7 +2055,7 @@
         <v>1</v>
       </c>
       <c r="AE2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AF2">
         <v>1</v>
@@ -2114,31 +2118,31 @@
         <v>0</v>
       </c>
       <c r="AZ2" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="BA2" t="s">
-        <v>313</v>
-      </c>
-      <c r="BB2">
-        <v>-1</v>
+        <v>316</v>
+      </c>
+      <c r="BB2" s="25" t="s">
+        <v>323</v>
       </c>
       <c r="BC2">
         <v>-1</v>
       </c>
-      <c r="BD2" s="24" t="s">
-        <v>316</v>
+      <c r="BD2">
+        <v>-1</v>
       </c>
       <c r="BE2">
         <v>-1</v>
       </c>
-      <c r="BF2" s="25" t="s">
-        <v>315</v>
+      <c r="BF2">
+        <v>-1</v>
       </c>
       <c r="BG2">
         <v>-1</v>
       </c>
-      <c r="BH2">
-        <v>-1</v>
+      <c r="BH2" s="24" t="s">
+        <v>322</v>
       </c>
       <c r="BI2">
         <v>-1</v>
@@ -2147,7 +2151,7 @@
         <v>-1</v>
       </c>
       <c r="BK2" t="s">
-        <v>246</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:63">
@@ -2161,7 +2165,7 @@
         <v>1002</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -2170,7 +2174,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -2185,7 +2189,7 @@
         <v>255</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M3">
         <v>3</v>
@@ -2305,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="AZ3" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="BA3">
         <v>-1</v>
@@ -2316,7 +2320,7 @@
       <c r="BC3">
         <v>-1</v>
       </c>
-      <c r="BD3" s="24">
+      <c r="BD3">
         <v>-1</v>
       </c>
       <c r="BE3">
@@ -2328,7 +2332,7 @@
       <c r="BG3">
         <v>-1</v>
       </c>
-      <c r="BH3">
+      <c r="BH3" s="24">
         <v>-1</v>
       </c>
       <c r="BI3">
@@ -2338,7 +2342,7 @@
         <v>-1</v>
       </c>
       <c r="BK3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:63">
@@ -2352,7 +2356,7 @@
         <v>1003</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -2376,7 +2380,7 @@
         <v>255</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -2496,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="AZ4" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="BA4">
         <v>-1</v>
@@ -2507,7 +2511,7 @@
       <c r="BC4">
         <v>-1</v>
       </c>
-      <c r="BD4" s="24">
+      <c r="BD4">
         <v>-1</v>
       </c>
       <c r="BE4">
@@ -2519,7 +2523,7 @@
       <c r="BG4">
         <v>-1</v>
       </c>
-      <c r="BH4">
+      <c r="BH4" s="24">
         <v>-1</v>
       </c>
       <c r="BI4">
@@ -2529,7 +2533,7 @@
         <v>-1</v>
       </c>
       <c r="BK4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:63">
@@ -2543,7 +2547,7 @@
         <v>1004</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -2567,7 +2571,7 @@
         <v>255</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M5">
         <v>2</v>
@@ -2687,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="AZ5" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="BA5">
         <v>-1</v>
@@ -2698,7 +2702,7 @@
       <c r="BC5">
         <v>-1</v>
       </c>
-      <c r="BD5" s="24">
+      <c r="BD5">
         <v>-1</v>
       </c>
       <c r="BE5">
@@ -2710,7 +2714,7 @@
       <c r="BG5">
         <v>-1</v>
       </c>
-      <c r="BH5">
+      <c r="BH5" s="24">
         <v>-1</v>
       </c>
       <c r="BI5">
@@ -2720,7 +2724,7 @@
         <v>-1</v>
       </c>
       <c r="BK5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:63">
@@ -2737,7 +2741,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>321</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -2758,7 +2762,7 @@
         <v>255</v>
       </c>
       <c r="L6" t="s">
-        <v>15</v>
+        <v>319</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -2815,7 +2819,7 @@
         <v>1</v>
       </c>
       <c r="AE6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AF6">
         <v>1</v>
@@ -2878,31 +2882,31 @@
         <v>0</v>
       </c>
       <c r="AZ6" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="BA6" t="s">
-        <v>313</v>
-      </c>
-      <c r="BB6">
-        <v>-1</v>
+        <v>316</v>
+      </c>
+      <c r="BB6" s="25" t="s">
+        <v>323</v>
       </c>
       <c r="BC6">
         <v>-1</v>
       </c>
-      <c r="BD6" s="24" t="s">
-        <v>316</v>
+      <c r="BD6">
+        <v>-1</v>
       </c>
       <c r="BE6">
         <v>-1</v>
       </c>
-      <c r="BF6" s="25" t="s">
-        <v>315</v>
+      <c r="BF6">
+        <v>-1</v>
       </c>
       <c r="BG6">
         <v>-1</v>
       </c>
-      <c r="BH6">
-        <v>-1</v>
+      <c r="BH6" s="24" t="s">
+        <v>322</v>
       </c>
       <c r="BI6">
         <v>-1</v>
@@ -2911,7 +2915,7 @@
         <v>-1</v>
       </c>
       <c r="BK6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:63">
@@ -2919,19 +2923,19 @@
         <v>200</v>
       </c>
       <c r="B7">
-        <v>3020</v>
+        <v>3024</v>
       </c>
       <c r="C7">
         <v>1006</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -2949,7 +2953,7 @@
         <v>255</v>
       </c>
       <c r="L7" t="s">
-        <v>26</v>
+        <v>320</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -3069,18 +3073,18 @@
         <v>0</v>
       </c>
       <c r="AZ7" t="s">
-        <v>321</v>
-      </c>
-      <c r="BA7">
-        <v>-1</v>
-      </c>
-      <c r="BB7">
-        <v>-1</v>
+        <v>325</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>316</v>
+      </c>
+      <c r="BB7" s="25" t="s">
+        <v>323</v>
       </c>
       <c r="BC7">
         <v>-1</v>
       </c>
-      <c r="BD7" s="24">
+      <c r="BD7">
         <v>-1</v>
       </c>
       <c r="BE7">
@@ -3092,8 +3096,8 @@
       <c r="BG7">
         <v>-1</v>
       </c>
-      <c r="BH7">
-        <v>-1</v>
+      <c r="BH7" s="24" t="s">
+        <v>322</v>
       </c>
       <c r="BI7">
         <v>-1</v>
@@ -3102,7 +3106,7 @@
         <v>-1</v>
       </c>
       <c r="BK7" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:63">
@@ -3116,7 +3120,7 @@
         <v>1007</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -3140,7 +3144,7 @@
         <v>255</v>
       </c>
       <c r="L8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -3260,7 +3264,7 @@
         <v>0</v>
       </c>
       <c r="AZ8" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="BA8">
         <v>-1</v>
@@ -3271,7 +3275,7 @@
       <c r="BC8">
         <v>-1</v>
       </c>
-      <c r="BD8" s="24">
+      <c r="BD8">
         <v>-1</v>
       </c>
       <c r="BE8">
@@ -3283,7 +3287,7 @@
       <c r="BG8">
         <v>-1</v>
       </c>
-      <c r="BH8">
+      <c r="BH8" s="24">
         <v>-1</v>
       </c>
       <c r="BI8">
@@ -3293,7 +3297,7 @@
         <v>-1</v>
       </c>
       <c r="BK8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:63">
@@ -3307,7 +3311,7 @@
         <v>1008</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -3331,7 +3335,7 @@
         <v>255</v>
       </c>
       <c r="L9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -3451,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="AZ9" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="BA9">
         <v>-1</v>
@@ -3462,7 +3466,7 @@
       <c r="BC9">
         <v>-1</v>
       </c>
-      <c r="BD9" s="24">
+      <c r="BD9">
         <v>-1</v>
       </c>
       <c r="BE9">
@@ -3474,7 +3478,7 @@
       <c r="BG9">
         <v>-1</v>
       </c>
-      <c r="BH9">
+      <c r="BH9" s="24">
         <v>-1</v>
       </c>
       <c r="BI9">
@@ -3484,7 +3488,7 @@
         <v>-1</v>
       </c>
       <c r="BK9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:63">
@@ -3501,7 +3505,7 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>321</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
@@ -3522,7 +3526,7 @@
         <v>255</v>
       </c>
       <c r="L10" t="s">
-        <v>15</v>
+        <v>319</v>
       </c>
       <c r="M10">
         <v>2</v>
@@ -3579,7 +3583,7 @@
         <v>1</v>
       </c>
       <c r="AE10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AF10">
         <v>1</v>
@@ -3642,31 +3646,31 @@
         <v>0</v>
       </c>
       <c r="AZ10" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="BA10" t="s">
-        <v>313</v>
-      </c>
-      <c r="BB10">
-        <v>-1</v>
+        <v>316</v>
+      </c>
+      <c r="BB10" s="25" t="s">
+        <v>323</v>
       </c>
       <c r="BC10">
         <v>-1</v>
       </c>
-      <c r="BD10" s="24" t="s">
-        <v>316</v>
+      <c r="BD10">
+        <v>-1</v>
       </c>
       <c r="BE10">
         <v>-1</v>
       </c>
-      <c r="BF10" s="25" t="s">
-        <v>315</v>
+      <c r="BF10">
+        <v>-1</v>
       </c>
       <c r="BG10">
         <v>-1</v>
       </c>
-      <c r="BH10">
-        <v>-1</v>
+      <c r="BH10" s="24" t="s">
+        <v>322</v>
       </c>
       <c r="BI10">
         <v>-1</v>
@@ -3675,11 +3679,8 @@
         <v>-1</v>
       </c>
       <c r="BK10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="11" spans="1:63">
-      <c r="BD11" s="24"/>
+        <v>244</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3691,8 +3692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AT7" sqref="AT7"/>
+    <sheetView topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3750,163 +3751,163 @@
   <sheetData>
     <row r="1" spans="1:53">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R1" t="s">
+        <v>118</v>
+      </c>
+      <c r="S1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="T1" t="s">
+        <v>119</v>
+      </c>
+      <c r="U1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V1" t="s">
         <v>77</v>
       </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" t="s">
-        <v>115</v>
-      </c>
-      <c r="N1" t="s">
-        <v>116</v>
-      </c>
-      <c r="O1" t="s">
-        <v>117</v>
-      </c>
-      <c r="P1" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>119</v>
-      </c>
-      <c r="R1" t="s">
-        <v>120</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>78</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" t="s">
         <v>121</v>
       </c>
-      <c r="U1" t="s">
-        <v>122</v>
-      </c>
-      <c r="V1" t="s">
-        <v>79</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>80</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>81</v>
       </c>
-      <c r="Y1" t="s">
-        <v>123</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>82</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>83</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>84</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>85</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>86</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>87</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>88</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>89</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>90</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>91</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>92</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>93</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>94</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>95</v>
       </c>
-      <c r="AN1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>97</v>
-      </c>
       <c r="AP1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AQ1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="AR1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="AS1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>306</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>307</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>308</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>309</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>304</v>
       </c>
-      <c r="AT1" t="s">
-        <v>308</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>309</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>310</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>311</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>312</v>
-      </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>305</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>306</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:53">
@@ -3926,7 +3927,7 @@
         <v>255</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3986,7 +3987,7 @@
         <v>0</v>
       </c>
       <c r="Z2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -4043,10 +4044,10 @@
         <v>0</v>
       </c>
       <c r="AS2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="AT2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="AU2">
         <v>-1</v>
@@ -4064,7 +4065,7 @@
         <v>-1</v>
       </c>
       <c r="AZ2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="BA2">
         <v>-1</v>
@@ -4087,7 +4088,7 @@
         <v>255</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -4147,7 +4148,7 @@
         <v>0</v>
       </c>
       <c r="Z3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -4204,10 +4205,10 @@
         <v>0</v>
       </c>
       <c r="AS3" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="AT3" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="AU3">
         <v>-1</v>
@@ -4225,7 +4226,7 @@
         <v>-1</v>
       </c>
       <c r="AZ3" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="BA3">
         <v>-1</v>
@@ -4248,7 +4249,7 @@
         <v>255</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -4308,7 +4309,7 @@
         <v>0</v>
       </c>
       <c r="Z4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -4365,10 +4366,10 @@
         <v>0</v>
       </c>
       <c r="AS4" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="AT4" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="AU4">
         <v>-1</v>
@@ -4386,7 +4387,7 @@
         <v>-1</v>
       </c>
       <c r="AZ4" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="BA4">
         <v>-1</v>
@@ -4409,7 +4410,7 @@
         <v>255</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -4469,7 +4470,7 @@
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -4526,10 +4527,10 @@
         <v>0</v>
       </c>
       <c r="AS5" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="AT5" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="AU5">
         <v>-1</v>
@@ -4547,7 +4548,7 @@
         <v>-1</v>
       </c>
       <c r="AZ5" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="BA5">
         <v>-1</v>
@@ -4570,7 +4571,7 @@
         <v>255</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -4630,7 +4631,7 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AA6">
         <v>1</v>
@@ -4687,10 +4688,10 @@
         <v>0</v>
       </c>
       <c r="AS6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="AT6" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="AU6">
         <v>-1</v>
@@ -4708,7 +4709,7 @@
         <v>-1</v>
       </c>
       <c r="AZ6" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="BA6">
         <v>-1</v>
@@ -4731,7 +4732,7 @@
         <v>255</v>
       </c>
       <c r="F7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -4791,7 +4792,7 @@
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AA7">
         <v>1</v>
@@ -4848,10 +4849,10 @@
         <v>0</v>
       </c>
       <c r="AS7" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="AT7" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="AU7">
         <v>-1</v>
@@ -4869,7 +4870,7 @@
         <v>-1</v>
       </c>
       <c r="AZ7" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="BA7">
         <v>-1</v>
@@ -4892,7 +4893,7 @@
         <v>255</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -4952,7 +4953,7 @@
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AA8">
         <v>1</v>
@@ -5009,7 +5010,7 @@
         <v>0</v>
       </c>
       <c r="AS8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="AT8">
         <v>-1</v>
@@ -5053,7 +5054,7 @@
         <v>255</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -5113,7 +5114,7 @@
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AA9">
         <v>1</v>
@@ -5170,7 +5171,7 @@
         <v>0</v>
       </c>
       <c r="AS9" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="AT9">
         <v>-1</v>
@@ -5222,46 +5223,46 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" t="s">
         <v>100</v>
       </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I1" t="s">
-        <v>111</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>101</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>102</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>103</v>
-      </c>
-      <c r="P1" t="s">
-        <v>104</v>
-      </c>
-      <c r="S1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -5296,22 +5297,22 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="S2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="T2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -5343,7 +5344,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M3">
         <v>206</v>
@@ -5413,7 +5414,7 @@
         <v>1005</v>
       </c>
       <c r="J5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -5436,10 +5437,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5447,7 +5448,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5455,7 +5456,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5463,7 +5464,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5471,7 +5472,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5479,7 +5480,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5487,7 +5488,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5495,7 +5496,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5503,7 +5504,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5511,7 +5512,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -5538,7 +5539,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="6">
         <v>0</v>
@@ -5555,41 +5556,41 @@
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -5606,7 +5607,7 @@
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1">
       <c r="A5" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B5" s="10">
         <v>0</v>
@@ -5623,41 +5624,41 @@
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1">
       <c r="A6" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B8" s="11">
         <v>1</v>
@@ -5674,7 +5675,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B9" s="10">
         <v>0</v>
@@ -5691,16 +5692,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E10" s="7">
         <v>0</v>
@@ -5708,13 +5709,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B11" s="10">
         <v>0</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D11" s="10">
         <v>1</v>
@@ -5725,16 +5726,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B12" s="10">
         <v>0</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
@@ -5742,16 +5743,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B13" s="10">
         <v>0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E13" s="7">
         <v>0</v>
@@ -5759,58 +5760,58 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B14" s="10">
         <v>0</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D14" s="10">
         <v>0</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B15" s="10">
         <v>0</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D15" s="10">
         <v>0</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B16" s="10">
         <v>0</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D16" s="10">
         <v>0</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -5827,7 +5828,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B18" s="10">
         <v>0</v>
@@ -5844,177 +5845,177 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B19" s="10">
         <v>0</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B29" s="10">
         <v>0</v>
@@ -6031,10 +6032,10 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C30" s="10">
         <v>0</v>
@@ -6048,381 +6049,381 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B31" s="10">
         <v>0</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B32" s="10">
         <v>0</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B34" s="10">
         <v>0</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B41" s="10">
         <v>0</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B42" s="10">
         <v>0</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B43" s="10">
         <v>0</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B53" s="10">
         <v>1</v>
@@ -6434,46 +6435,46 @@
         <v>0</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B54" s="10">
         <v>2</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D54" s="10">
         <v>0</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D55" s="10">
         <v>0</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B56" s="10">
         <v>1</v>
@@ -6490,13 +6491,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B57" s="10">
         <v>2</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D57" s="10">
         <v>0</v>
@@ -6507,13 +6508,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D58" s="10">
         <v>0</v>
@@ -6524,7 +6525,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B59" s="10">
         <v>1</v>
@@ -6541,13 +6542,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B60" s="10">
         <v>2</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D60" s="10">
         <v>0</v>
@@ -6558,13 +6559,13 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D61" s="10">
         <v>0</v>
@@ -6575,7 +6576,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B62" s="10">
         <v>1</v>
@@ -6592,13 +6593,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B63" s="10">
         <v>2</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D63" s="10">
         <v>0</v>
@@ -6609,13 +6610,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D64" s="10">
         <v>0</v>
@@ -6626,7 +6627,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B65" s="10">
         <v>1</v>
@@ -6643,13 +6644,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B66" s="10">
         <v>2</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D66" s="10">
         <v>0</v>
@@ -6660,13 +6661,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D67" s="10">
         <v>0</v>
@@ -6677,7 +6678,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B68" s="10">
         <v>1</v>
@@ -6694,13 +6695,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B69" s="10">
         <v>2</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D69" s="10">
         <v>0</v>
@@ -6711,13 +6712,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D70" s="10">
         <v>0</v>
@@ -6728,7 +6729,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B71" s="10">
         <v>1</v>
@@ -6745,13 +6746,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B72" s="10">
         <v>2</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D72" s="10">
         <v>0</v>
@@ -6762,13 +6763,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D73" s="10">
         <v>0</v>
@@ -6779,7 +6780,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B74" s="10">
         <v>1</v>
@@ -6796,13 +6797,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B75" s="10">
         <v>2</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D75" s="10">
         <v>0</v>
@@ -6813,13 +6814,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D76" s="10">
         <v>0</v>
@@ -6830,7 +6831,7 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B77" s="10">
         <v>1</v>
@@ -6847,7 +6848,7 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B78" s="10">
         <v>2</v>
@@ -6864,13 +6865,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D79" s="10">
         <v>0</v>
@@ -6881,58 +6882,58 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B83" s="10">
         <v>1</v>
@@ -6949,101 +6950,101 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D84" s="10">
         <v>0</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D85" s="10">
         <v>0</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C89" s="10">
         <v>1</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E89" s="10">
         <v>1</v>
@@ -7051,41 +7052,41 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B92" s="10">
         <v>0</v>
@@ -7102,41 +7103,41 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B93" s="10">
         <v>0</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D93" s="10">
         <v>0</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B94" s="10">
         <v>0</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D94" s="10">
         <v>0</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B95" s="10">
         <v>1</v>
@@ -7153,10 +7154,10 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C96" s="10">
         <v>0</v>
@@ -7170,13 +7171,13 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D97" s="10">
         <v>0</v>
@@ -7187,7 +7188,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B98" s="10">
         <v>1</v>
@@ -7204,10 +7205,10 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C99" s="10">
         <v>0</v>
@@ -7221,13 +7222,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D100" s="10">
         <v>0</v>
@@ -7238,7 +7239,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B101" s="10">
         <v>1</v>
@@ -7255,13 +7256,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D102" s="10">
         <v>0</v>
@@ -7272,13 +7273,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D103" s="10">
         <v>0</v>
@@ -7289,7 +7290,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B104" s="10">
         <v>1</v>
@@ -7306,13 +7307,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D105" s="10">
         <v>0</v>
@@ -7323,13 +7324,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D106" s="10">
         <v>0</v>
@@ -7340,7 +7341,7 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B107" s="10">
         <v>1</v>
@@ -7357,13 +7358,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D108" s="10">
         <v>0</v>
@@ -7374,13 +7375,13 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D109" s="10">
         <v>0</v>
@@ -7391,7 +7392,7 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B110" s="10">
         <v>1</v>
@@ -7408,13 +7409,13 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D111" s="10">
         <v>0</v>
@@ -7425,13 +7426,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D112" s="10">
         <v>0</v>
@@ -7442,7 +7443,7 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B113" s="10">
         <v>1</v>
@@ -7459,13 +7460,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D114" s="10">
         <v>0</v>
@@ -7476,13 +7477,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D115" s="10">
         <v>0</v>
@@ -7493,7 +7494,7 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B116" s="10">
         <v>1</v>
@@ -7510,13 +7511,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D117" s="10">
         <v>0</v>
@@ -7527,13 +7528,13 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D118" s="10">
         <v>0</v>
@@ -7544,7 +7545,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B119" s="10">
         <v>1</v>
@@ -7561,13 +7562,13 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D120" s="10">
         <v>0</v>
@@ -7578,13 +7579,13 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D121" s="10">
         <v>0</v>
@@ -7595,7 +7596,7 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B122" s="10">
         <v>1</v>
@@ -7612,13 +7613,13 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D123" s="10">
         <v>0</v>
@@ -7629,13 +7630,13 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C124" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D124" s="10">
         <v>0</v>
@@ -7646,19 +7647,19 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B125" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D125" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="C125" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D125" s="10" t="s">
-        <v>223</v>
-      </c>
       <c r="E125" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="139" spans="5:6">
@@ -7826,30 +7827,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>289</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>290</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B2" s="1">
         <v>4000</v>
@@ -7872,7 +7873,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="22" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B3" s="1">
         <v>4001</v>
@@ -7916,535 +7917,535 @@
     <row r="1" spans="1:5">
       <c r="A1" s="1"/>
       <c r="B1" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="21"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="21"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="19"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="19"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="19"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="19"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="19"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="19"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="19"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="19"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="19"/>

</xml_diff>

<commit_message>
I sketched out the logic flow for the enemy A.I. If I'm particularly inspired, I may upload it. So far, I implemented the 'survival' phase, which checks for mana/hp levels, and if the enemy has the intellect to do something about it. If they are low on mana (<35%) they use an item. If low on hp (<35%) they use an Item or an ability if they have one. I've not yet tested the use ability functionality (that'll require a bit of mocking), however items (both consumable and duration) have been used successfully.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -21,12 +21,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Items!$L$1:$L$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="326">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -1701,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BK10"/>
+  <dimension ref="A1:BK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
-      <selection activeCell="BH17" sqref="BH17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3682,6 +3681,770 @@
         <v>244</v>
       </c>
     </row>
+    <row r="11" spans="1:63">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>3024</v>
+      </c>
+      <c r="C11">
+        <v>1010</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>50</v>
+      </c>
+      <c r="I11">
+        <v>255</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>255</v>
+      </c>
+      <c r="L11" t="s">
+        <v>320</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>2</v>
+      </c>
+      <c r="AL11">
+        <v>2</v>
+      </c>
+      <c r="AM11">
+        <v>2</v>
+      </c>
+      <c r="AN11">
+        <v>2</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11">
+        <v>0</v>
+      </c>
+      <c r="AX11">
+        <v>1</v>
+      </c>
+      <c r="AY11">
+        <v>0</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>325</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>316</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>323</v>
+      </c>
+      <c r="BC11">
+        <v>-1</v>
+      </c>
+      <c r="BD11">
+        <v>-1</v>
+      </c>
+      <c r="BE11">
+        <v>-1</v>
+      </c>
+      <c r="BF11">
+        <v>-1</v>
+      </c>
+      <c r="BG11">
+        <v>-1</v>
+      </c>
+      <c r="BH11" t="s">
+        <v>322</v>
+      </c>
+      <c r="BI11">
+        <v>-1</v>
+      </c>
+      <c r="BJ11">
+        <v>-1</v>
+      </c>
+      <c r="BK11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:63">
+      <c r="A12">
+        <v>200</v>
+      </c>
+      <c r="B12">
+        <v>3021</v>
+      </c>
+      <c r="C12">
+        <v>1011</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>255</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>255</v>
+      </c>
+      <c r="L12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>2</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>2</v>
+      </c>
+      <c r="AH12">
+        <v>5</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>0</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>0</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
+      <c r="AR12">
+        <v>0</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12">
+        <v>0</v>
+      </c>
+      <c r="AU12">
+        <v>0</v>
+      </c>
+      <c r="AV12">
+        <v>0</v>
+      </c>
+      <c r="AW12">
+        <v>0</v>
+      </c>
+      <c r="AX12">
+        <v>1</v>
+      </c>
+      <c r="AY12">
+        <v>0</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>325</v>
+      </c>
+      <c r="BA12">
+        <v>-1</v>
+      </c>
+      <c r="BB12">
+        <v>-1</v>
+      </c>
+      <c r="BC12">
+        <v>-1</v>
+      </c>
+      <c r="BD12">
+        <v>-1</v>
+      </c>
+      <c r="BE12">
+        <v>-1</v>
+      </c>
+      <c r="BF12">
+        <v>-1</v>
+      </c>
+      <c r="BG12">
+        <v>-1</v>
+      </c>
+      <c r="BH12" s="24">
+        <v>-1</v>
+      </c>
+      <c r="BI12">
+        <v>-1</v>
+      </c>
+      <c r="BJ12">
+        <v>-1</v>
+      </c>
+      <c r="BK12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:63">
+      <c r="A13">
+        <v>200</v>
+      </c>
+      <c r="B13">
+        <v>3023</v>
+      </c>
+      <c r="C13">
+        <v>1012</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <v>20</v>
+      </c>
+      <c r="I13">
+        <v>255</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>255</v>
+      </c>
+      <c r="L13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>6</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13">
+        <v>0</v>
+      </c>
+      <c r="AS13">
+        <v>0</v>
+      </c>
+      <c r="AT13">
+        <v>0</v>
+      </c>
+      <c r="AU13">
+        <v>0</v>
+      </c>
+      <c r="AV13">
+        <v>0</v>
+      </c>
+      <c r="AW13">
+        <v>0</v>
+      </c>
+      <c r="AX13">
+        <v>1</v>
+      </c>
+      <c r="AY13">
+        <v>0</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>325</v>
+      </c>
+      <c r="BA13">
+        <v>-1</v>
+      </c>
+      <c r="BB13">
+        <v>-1</v>
+      </c>
+      <c r="BC13">
+        <v>-1</v>
+      </c>
+      <c r="BD13">
+        <v>-1</v>
+      </c>
+      <c r="BE13">
+        <v>-1</v>
+      </c>
+      <c r="BF13">
+        <v>-1</v>
+      </c>
+      <c r="BG13">
+        <v>-1</v>
+      </c>
+      <c r="BH13" s="24">
+        <v>-1</v>
+      </c>
+      <c r="BI13">
+        <v>-1</v>
+      </c>
+      <c r="BJ13">
+        <v>-1</v>
+      </c>
+      <c r="BK13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:63">
+      <c r="A14">
+        <v>200</v>
+      </c>
+      <c r="B14">
+        <v>3022</v>
+      </c>
+      <c r="C14">
+        <v>1013</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>15</v>
+      </c>
+      <c r="I14">
+        <v>255</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>255</v>
+      </c>
+      <c r="L14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>10</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
+      <c r="AR14">
+        <v>0</v>
+      </c>
+      <c r="AS14">
+        <v>0</v>
+      </c>
+      <c r="AT14">
+        <v>0</v>
+      </c>
+      <c r="AU14">
+        <v>0</v>
+      </c>
+      <c r="AV14">
+        <v>0</v>
+      </c>
+      <c r="AW14">
+        <v>0</v>
+      </c>
+      <c r="AX14">
+        <v>1</v>
+      </c>
+      <c r="AY14">
+        <v>0</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>325</v>
+      </c>
+      <c r="BA14">
+        <v>-1</v>
+      </c>
+      <c r="BB14">
+        <v>-1</v>
+      </c>
+      <c r="BC14">
+        <v>-1</v>
+      </c>
+      <c r="BD14">
+        <v>-1</v>
+      </c>
+      <c r="BE14">
+        <v>-1</v>
+      </c>
+      <c r="BF14">
+        <v>-1</v>
+      </c>
+      <c r="BG14">
+        <v>-1</v>
+      </c>
+      <c r="BH14" s="24">
+        <v>-1</v>
+      </c>
+      <c r="BI14">
+        <v>-1</v>
+      </c>
+      <c r="BJ14">
+        <v>-1</v>
+      </c>
+      <c r="BK14" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Couldn't sleep on account of the jetlag, so I've implemented ability loading. I can make a prepared targeted ability from a txt file and load it into the registry - I'll work on implementing the other ability forms with some basic abilities as well.
Also, template abilities are now included in the Global Registry and are
added from the create_ability source, so the templates exist in two
(separate) forms. Not a totally stellar design, but better than what was
there before.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Abilities" sheetId="5" r:id="rId6"/>
     <sheet name="Images" sheetId="8" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId8"/>
+    <sheet name="TargetedAbilities" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Abilities!$A$1:$A$137</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="334">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -1003,6 +1004,30 @@
   </si>
   <si>
     <t>1,10,-1</t>
+  </si>
+  <si>
+    <t>faction</t>
+  </si>
+  <si>
+    <t>LoS</t>
+  </si>
+  <si>
+    <t>isSneaking</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>fireball</t>
+  </si>
+  <si>
+    <t>diceDamageMult</t>
+  </si>
+  <si>
+    <t>burn</t>
+  </si>
+  <si>
+    <t>mana Cost override</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1151,6 +1176,17 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1702,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1:AX1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4453,10 +4489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA9"/>
+  <dimension ref="A1:BD9"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="AX6" sqref="AX6"/>
+    <sheetView topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="AX12" sqref="AX12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4485,34 +4521,36 @@
     <col min="26" max="26" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="17" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="39.85546875" customWidth="1"/>
-    <col min="48" max="48" width="18" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="30.42578125" customWidth="1"/>
-    <col min="50" max="50" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="6.140625" customWidth="1"/>
+    <col min="31" max="31" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="19" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="39.85546875" customWidth="1"/>
+    <col min="51" max="51" width="18" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="30.42578125" customWidth="1"/>
+    <col min="53" max="53" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:56">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -4598,82 +4636,91 @@
         <v>82</v>
       </c>
       <c r="AC1" t="s">
+        <v>327</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>328</v>
+      </c>
+      <c r="AE1" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>84</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>85</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>86</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>87</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>88</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>89</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>90</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>91</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>92</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>93</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>94</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>95</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>107</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
+        <v>326</v>
+      </c>
+      <c r="AT1" t="s">
         <v>313</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>312</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>302</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>306</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>307</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>308</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>309</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>310</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>303</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>304</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:56">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -4759,7 +4806,7 @@
         <v>3</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -4798,43 +4845,52 @@
         <v>0</v>
       </c>
       <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
         <v>15</v>
       </c>
-      <c r="AQ2">
-        <v>1</v>
-      </c>
-      <c r="AR2">
-        <v>0</v>
-      </c>
-      <c r="AS2" t="s">
+      <c r="AS2">
+        <v>1</v>
+      </c>
+      <c r="AT2">
+        <v>1</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="s">
         <v>316</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AW2" t="s">
         <v>317</v>
       </c>
-      <c r="AU2">
-        <v>-1</v>
-      </c>
-      <c r="AV2">
-        <v>-1</v>
-      </c>
-      <c r="AW2">
-        <v>-1</v>
-      </c>
       <c r="AX2">
         <v>-1</v>
       </c>
       <c r="AY2">
         <v>-1</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="AZ2">
+        <v>-1</v>
+      </c>
+      <c r="BA2">
+        <v>-1</v>
+      </c>
+      <c r="BB2">
+        <v>-1</v>
+      </c>
+      <c r="BC2" t="s">
         <v>317</v>
       </c>
-      <c r="BA2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53">
+      <c r="BD2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56">
       <c r="A3">
         <v>2006</v>
       </c>
@@ -4920,7 +4976,7 @@
         <v>3</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD3">
         <v>0</v>
@@ -4959,43 +5015,52 @@
         <v>0</v>
       </c>
       <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
         <v>5</v>
       </c>
-      <c r="AQ3">
-        <v>1</v>
-      </c>
-      <c r="AR3">
-        <v>0</v>
-      </c>
-      <c r="AS3" t="s">
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>1</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3" t="s">
         <v>316</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AW3" t="s">
         <v>317</v>
       </c>
-      <c r="AU3">
-        <v>-1</v>
-      </c>
-      <c r="AV3">
-        <v>-1</v>
-      </c>
-      <c r="AW3">
-        <v>-1</v>
-      </c>
       <c r="AX3">
         <v>-1</v>
       </c>
       <c r="AY3">
         <v>-1</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="AZ3">
+        <v>-1</v>
+      </c>
+      <c r="BA3">
+        <v>-1</v>
+      </c>
+      <c r="BB3">
+        <v>-1</v>
+      </c>
+      <c r="BC3" t="s">
         <v>317</v>
       </c>
-      <c r="BA3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53">
+      <c r="BD3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56">
       <c r="A4">
         <v>2007</v>
       </c>
@@ -5081,7 +5146,7 @@
         <v>3</v>
       </c>
       <c r="AC4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -5120,43 +5185,52 @@
         <v>0</v>
       </c>
       <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
         <v>5</v>
       </c>
-      <c r="AQ4">
-        <v>1</v>
-      </c>
-      <c r="AR4">
-        <v>0</v>
-      </c>
-      <c r="AS4" t="s">
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>1</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4" t="s">
         <v>316</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AW4" t="s">
         <v>317</v>
       </c>
-      <c r="AU4">
-        <v>-1</v>
-      </c>
-      <c r="AV4">
-        <v>-1</v>
-      </c>
-      <c r="AW4">
-        <v>-1</v>
-      </c>
       <c r="AX4">
         <v>-1</v>
       </c>
       <c r="AY4">
         <v>-1</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="AZ4">
+        <v>-1</v>
+      </c>
+      <c r="BA4">
+        <v>-1</v>
+      </c>
+      <c r="BB4">
+        <v>-1</v>
+      </c>
+      <c r="BC4" t="s">
         <v>317</v>
       </c>
-      <c r="BA4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53">
+      <c r="BD4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56">
       <c r="A5">
         <v>2008</v>
       </c>
@@ -5242,7 +5316,7 @@
         <v>3</v>
       </c>
       <c r="AC5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -5281,43 +5355,52 @@
         <v>0</v>
       </c>
       <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
         <v>5</v>
       </c>
-      <c r="AQ5">
-        <v>1</v>
-      </c>
-      <c r="AR5">
-        <v>0</v>
-      </c>
-      <c r="AS5" t="s">
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>1</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5" t="s">
         <v>316</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AW5" t="s">
         <v>317</v>
       </c>
-      <c r="AU5">
-        <v>-1</v>
-      </c>
-      <c r="AV5">
-        <v>-1</v>
-      </c>
-      <c r="AW5">
-        <v>-1</v>
-      </c>
       <c r="AX5">
         <v>-1</v>
       </c>
       <c r="AY5">
         <v>-1</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="AZ5">
+        <v>-1</v>
+      </c>
+      <c r="BA5">
+        <v>-1</v>
+      </c>
+      <c r="BB5">
+        <v>-1</v>
+      </c>
+      <c r="BC5" t="s">
         <v>317</v>
       </c>
-      <c r="BA5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53">
+      <c r="BD5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56">
       <c r="A6">
         <v>2009</v>
       </c>
@@ -5403,7 +5486,7 @@
         <v>3</v>
       </c>
       <c r="AC6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -5442,43 +5525,52 @@
         <v>0</v>
       </c>
       <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
         <v>5</v>
       </c>
-      <c r="AQ6">
-        <v>1</v>
-      </c>
-      <c r="AR6">
-        <v>0</v>
-      </c>
-      <c r="AS6" t="s">
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>1</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6" t="s">
         <v>316</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AW6" t="s">
         <v>317</v>
       </c>
-      <c r="AU6">
-        <v>-1</v>
-      </c>
-      <c r="AV6">
-        <v>-1</v>
-      </c>
-      <c r="AW6">
-        <v>-1</v>
-      </c>
       <c r="AX6">
         <v>-1</v>
       </c>
       <c r="AY6">
         <v>-1</v>
       </c>
-      <c r="AZ6" t="s">
+      <c r="AZ6">
+        <v>-1</v>
+      </c>
+      <c r="BA6">
+        <v>-1</v>
+      </c>
+      <c r="BB6">
+        <v>-1</v>
+      </c>
+      <c r="BC6" t="s">
         <v>317</v>
       </c>
-      <c r="BA6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:53">
+      <c r="BD6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -5564,7 +5656,7 @@
         <v>3</v>
       </c>
       <c r="AC7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD7">
         <v>0</v>
@@ -5603,43 +5695,52 @@
         <v>0</v>
       </c>
       <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
         <v>5</v>
       </c>
-      <c r="AQ7">
-        <v>1</v>
-      </c>
-      <c r="AR7">
-        <v>0</v>
-      </c>
-      <c r="AS7" t="s">
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>1</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7" t="s">
         <v>316</v>
       </c>
-      <c r="AT7" t="s">
+      <c r="AW7" t="s">
         <v>317</v>
       </c>
-      <c r="AU7">
-        <v>-1</v>
-      </c>
-      <c r="AV7">
-        <v>-1</v>
-      </c>
-      <c r="AW7">
-        <v>-1</v>
-      </c>
       <c r="AX7">
         <v>-1</v>
       </c>
       <c r="AY7">
         <v>-1</v>
       </c>
-      <c r="AZ7" t="s">
+      <c r="AZ7">
+        <v>-1</v>
+      </c>
+      <c r="BA7">
+        <v>-1</v>
+      </c>
+      <c r="BB7">
+        <v>-1</v>
+      </c>
+      <c r="BC7" t="s">
         <v>317</v>
       </c>
-      <c r="BA7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53">
+      <c r="BD7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:56">
       <c r="A8">
         <v>2013</v>
       </c>
@@ -5725,7 +5826,7 @@
         <v>3</v>
       </c>
       <c r="AC8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD8">
         <v>0</v>
@@ -5761,29 +5862,29 @@
         <v>0</v>
       </c>
       <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
         <v>1000</v>
       </c>
-      <c r="AP8">
+      <c r="AR8">
         <v>30</v>
       </c>
-      <c r="AQ8">
-        <v>1</v>
-      </c>
-      <c r="AR8">
-        <v>0</v>
-      </c>
-      <c r="AS8" t="s">
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>1</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8" t="s">
         <v>311</v>
       </c>
-      <c r="AT8">
-        <v>-1</v>
-      </c>
-      <c r="AU8">
-        <v>-1</v>
-      </c>
-      <c r="AV8">
-        <v>-1</v>
-      </c>
       <c r="AW8">
         <v>-1</v>
       </c>
@@ -5799,8 +5900,17 @@
       <c r="BA8">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:53">
+      <c r="BB8">
+        <v>-1</v>
+      </c>
+      <c r="BC8">
+        <v>-1</v>
+      </c>
+      <c r="BD8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -5886,7 +5996,7 @@
         <v>3</v>
       </c>
       <c r="AC9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD9">
         <v>0</v>
@@ -5922,29 +6032,29 @@
         <v>0</v>
       </c>
       <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
         <v>1004</v>
       </c>
-      <c r="AP9">
+      <c r="AR9">
         <v>100</v>
       </c>
-      <c r="AQ9">
-        <v>1</v>
-      </c>
-      <c r="AR9">
-        <v>0</v>
-      </c>
-      <c r="AS9" t="s">
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>1</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9" t="s">
         <v>311</v>
       </c>
-      <c r="AT9">
-        <v>-1</v>
-      </c>
-      <c r="AU9">
-        <v>-1</v>
-      </c>
-      <c r="AV9">
-        <v>-1</v>
-      </c>
       <c r="AW9">
         <v>-1</v>
       </c>
@@ -5958,6 +6068,15 @@
         <v>-1</v>
       </c>
       <c r="BA9">
+        <v>-1</v>
+      </c>
+      <c r="BB9">
+        <v>-1</v>
+      </c>
+      <c r="BC9">
+        <v>-1</v>
+      </c>
+      <c r="BD9">
         <v>-1</v>
       </c>
     </row>
@@ -6288,8 +6407,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E125"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6531,8 +6650,8 @@
       <c r="C14" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D14" s="10">
-        <v>0</v>
+      <c r="D14" s="10" t="s">
+        <v>205</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>215</v>
@@ -8668,7 +8787,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D1" sqref="A1:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9216,4 +9335,281 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="28">
+        <v>100</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="29">
+        <v>1</v>
+      </c>
+      <c r="D2" s="29">
+        <v>1</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="29">
+        <v>1</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="28">
+        <v>101</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" s="29">
+        <v>1</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="29">
+        <v>1</v>
+      </c>
+      <c r="K3" s="29">
+        <v>1</v>
+      </c>
+      <c r="L3" s="29">
+        <v>1</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Made a way to load abilities to indiviudals. It's slightly annoying because in the 'createIndividualFromLine' function just passed parameters to the defineIndividual function, so I have to make a abilityList and pass it through. End result is correct however, and the foundation is laid for the other ability types.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="339">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -1028,6 +1028,21 @@
   </si>
   <si>
     <t>mana Cost override</t>
+  </si>
+  <si>
+    <t>permenantAbilityIDs</t>
+  </si>
+  <si>
+    <t>durationAbilityIDs</t>
+  </si>
+  <si>
+    <t>targetedAbilityIDs</t>
+  </si>
+  <si>
+    <t>InstantAbilityIDs</t>
+  </si>
+  <si>
+    <t>2,100,101</t>
   </si>
 </sst>
 </file>
@@ -4489,10 +4504,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD9"/>
+  <dimension ref="A1:BH9"/>
   <sheetViews>
-    <sheetView topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="AX12" sqref="AX12"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="AW6" sqref="AW6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4537,20 +4552,23 @@
     <col min="43" max="43" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="19" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="39.85546875" customWidth="1"/>
-    <col min="51" max="51" width="18" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="30.42578125" customWidth="1"/>
-    <col min="53" max="53" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="17" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="19" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="39.85546875" customWidth="1"/>
+    <col min="55" max="55" width="18" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="30.42578125" customWidth="1"/>
+    <col min="57" max="57" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56">
+    <row r="1" spans="1:60">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -4687,40 +4705,52 @@
         <v>326</v>
       </c>
       <c r="AT1" t="s">
+        <v>334</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AX1" t="s">
         <v>313</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AY1" t="s">
         <v>312</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AZ1" t="s">
         <v>302</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BA1" t="s">
         <v>306</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BB1" t="s">
         <v>307</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BC1" t="s">
         <v>308</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BD1" t="s">
         <v>309</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BE1" t="s">
         <v>310</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BF1" t="s">
         <v>303</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BG1" t="s">
         <v>304</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BH1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:56">
+    <row r="2" spans="1:60">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -4857,40 +4887,52 @@
         <v>1</v>
       </c>
       <c r="AT2">
-        <v>1</v>
-      </c>
-      <c r="AU2">
-        <v>0</v>
-      </c>
-      <c r="AV2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="AU2" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AV2" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="AW2" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AX2" s="25">
+        <v>1</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>316</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="BA2" t="s">
         <v>317</v>
       </c>
-      <c r="AX2">
-        <v>-1</v>
-      </c>
-      <c r="AY2">
-        <v>-1</v>
-      </c>
-      <c r="AZ2">
-        <v>-1</v>
-      </c>
-      <c r="BA2">
-        <v>-1</v>
-      </c>
       <c r="BB2">
         <v>-1</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BC2">
+        <v>-1</v>
+      </c>
+      <c r="BD2">
+        <v>-1</v>
+      </c>
+      <c r="BE2">
+        <v>-1</v>
+      </c>
+      <c r="BF2">
+        <v>-1</v>
+      </c>
+      <c r="BG2" t="s">
         <v>317</v>
       </c>
-      <c r="BD2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:56">
+      <c r="BH2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:60">
       <c r="A3">
         <v>2006</v>
       </c>
@@ -5027,40 +5069,52 @@
         <v>0</v>
       </c>
       <c r="AT3">
-        <v>1</v>
-      </c>
-      <c r="AU3">
-        <v>0</v>
-      </c>
-      <c r="AV3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="AU3" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AV3" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AW3" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AX3" s="25">
+        <v>1</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3" t="s">
         <v>316</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="BA3" t="s">
         <v>317</v>
       </c>
-      <c r="AX3">
-        <v>-1</v>
-      </c>
-      <c r="AY3">
-        <v>-1</v>
-      </c>
-      <c r="AZ3">
-        <v>-1</v>
-      </c>
-      <c r="BA3">
-        <v>-1</v>
-      </c>
       <c r="BB3">
         <v>-1</v>
       </c>
-      <c r="BC3" t="s">
+      <c r="BC3">
+        <v>-1</v>
+      </c>
+      <c r="BD3">
+        <v>-1</v>
+      </c>
+      <c r="BE3">
+        <v>-1</v>
+      </c>
+      <c r="BF3">
+        <v>-1</v>
+      </c>
+      <c r="BG3" t="s">
         <v>317</v>
       </c>
-      <c r="BD3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:56">
+      <c r="BH3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:60">
       <c r="A4">
         <v>2007</v>
       </c>
@@ -5197,40 +5251,52 @@
         <v>0</v>
       </c>
       <c r="AT4">
-        <v>1</v>
-      </c>
-      <c r="AU4">
-        <v>0</v>
-      </c>
-      <c r="AV4" t="s">
+        <v>-1</v>
+      </c>
+      <c r="AU4" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AV4" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AW4" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AX4" s="25">
+        <v>1</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>316</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="BA4" t="s">
         <v>317</v>
       </c>
-      <c r="AX4">
-        <v>-1</v>
-      </c>
-      <c r="AY4">
-        <v>-1</v>
-      </c>
-      <c r="AZ4">
-        <v>-1</v>
-      </c>
-      <c r="BA4">
-        <v>-1</v>
-      </c>
       <c r="BB4">
         <v>-1</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BC4">
+        <v>-1</v>
+      </c>
+      <c r="BD4">
+        <v>-1</v>
+      </c>
+      <c r="BE4">
+        <v>-1</v>
+      </c>
+      <c r="BF4">
+        <v>-1</v>
+      </c>
+      <c r="BG4" t="s">
         <v>317</v>
       </c>
-      <c r="BD4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:56">
+      <c r="BH4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:60">
       <c r="A5">
         <v>2008</v>
       </c>
@@ -5367,40 +5433,52 @@
         <v>0</v>
       </c>
       <c r="AT5">
-        <v>1</v>
-      </c>
-      <c r="AU5">
-        <v>0</v>
-      </c>
-      <c r="AV5" t="s">
+        <v>-1</v>
+      </c>
+      <c r="AU5" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AV5" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AW5" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AX5" s="25">
+        <v>1</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5" t="s">
         <v>316</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="BA5" t="s">
         <v>317</v>
       </c>
-      <c r="AX5">
-        <v>-1</v>
-      </c>
-      <c r="AY5">
-        <v>-1</v>
-      </c>
-      <c r="AZ5">
-        <v>-1</v>
-      </c>
-      <c r="BA5">
-        <v>-1</v>
-      </c>
       <c r="BB5">
         <v>-1</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BC5">
+        <v>-1</v>
+      </c>
+      <c r="BD5">
+        <v>-1</v>
+      </c>
+      <c r="BE5">
+        <v>-1</v>
+      </c>
+      <c r="BF5">
+        <v>-1</v>
+      </c>
+      <c r="BG5" t="s">
         <v>317</v>
       </c>
-      <c r="BD5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:56">
+      <c r="BH5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:60">
       <c r="A6">
         <v>2009</v>
       </c>
@@ -5537,40 +5615,52 @@
         <v>0</v>
       </c>
       <c r="AT6">
-        <v>1</v>
-      </c>
-      <c r="AU6">
-        <v>0</v>
-      </c>
-      <c r="AV6" t="s">
+        <v>-1</v>
+      </c>
+      <c r="AU6" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AV6" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AW6" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AX6" s="25">
+        <v>1</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="AZ6" t="s">
         <v>316</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="BA6" t="s">
         <v>317</v>
       </c>
-      <c r="AX6">
-        <v>-1</v>
-      </c>
-      <c r="AY6">
-        <v>-1</v>
-      </c>
-      <c r="AZ6">
-        <v>-1</v>
-      </c>
-      <c r="BA6">
-        <v>-1</v>
-      </c>
       <c r="BB6">
         <v>-1</v>
       </c>
-      <c r="BC6" t="s">
+      <c r="BC6">
+        <v>-1</v>
+      </c>
+      <c r="BD6">
+        <v>-1</v>
+      </c>
+      <c r="BE6">
+        <v>-1</v>
+      </c>
+      <c r="BF6">
+        <v>-1</v>
+      </c>
+      <c r="BG6" t="s">
         <v>317</v>
       </c>
-      <c r="BD6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:56">
+      <c r="BH6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:60">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -5707,40 +5797,52 @@
         <v>0</v>
       </c>
       <c r="AT7">
-        <v>1</v>
-      </c>
-      <c r="AU7">
-        <v>0</v>
-      </c>
-      <c r="AV7" t="s">
+        <v>-1</v>
+      </c>
+      <c r="AU7" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AV7" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AW7" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AX7" s="25">
+        <v>1</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7" t="s">
         <v>316</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="BA7" t="s">
         <v>317</v>
       </c>
-      <c r="AX7">
-        <v>-1</v>
-      </c>
-      <c r="AY7">
-        <v>-1</v>
-      </c>
-      <c r="AZ7">
-        <v>-1</v>
-      </c>
-      <c r="BA7">
-        <v>-1</v>
-      </c>
       <c r="BB7">
         <v>-1</v>
       </c>
-      <c r="BC7" t="s">
+      <c r="BC7">
+        <v>-1</v>
+      </c>
+      <c r="BD7">
+        <v>-1</v>
+      </c>
+      <c r="BE7">
+        <v>-1</v>
+      </c>
+      <c r="BF7">
+        <v>-1</v>
+      </c>
+      <c r="BG7" t="s">
         <v>317</v>
       </c>
-      <c r="BD7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:56">
+      <c r="BH7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:60">
       <c r="A8">
         <v>2013</v>
       </c>
@@ -5877,26 +5979,26 @@
         <v>0</v>
       </c>
       <c r="AT8">
-        <v>1</v>
-      </c>
-      <c r="AU8">
-        <v>0</v>
-      </c>
-      <c r="AV8" t="s">
+        <v>-1</v>
+      </c>
+      <c r="AU8" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AV8" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="AW8" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AX8" s="25">
+        <v>1</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
+      </c>
+      <c r="AZ8" t="s">
         <v>311</v>
       </c>
-      <c r="AW8">
-        <v>-1</v>
-      </c>
-      <c r="AX8">
-        <v>-1</v>
-      </c>
-      <c r="AY8">
-        <v>-1</v>
-      </c>
-      <c r="AZ8">
-        <v>-1</v>
-      </c>
       <c r="BA8">
         <v>-1</v>
       </c>
@@ -5909,8 +6011,20 @@
       <c r="BD8">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:56">
+      <c r="BE8">
+        <v>-1</v>
+      </c>
+      <c r="BF8">
+        <v>-1</v>
+      </c>
+      <c r="BG8">
+        <v>-1</v>
+      </c>
+      <c r="BH8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:60">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -6047,26 +6161,26 @@
         <v>0</v>
       </c>
       <c r="AT9">
-        <v>1</v>
-      </c>
-      <c r="AU9">
-        <v>0</v>
-      </c>
-      <c r="AV9" t="s">
+        <v>-1</v>
+      </c>
+      <c r="AU9" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AV9" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="AW9" s="25">
+        <v>-1</v>
+      </c>
+      <c r="AX9" s="25">
+        <v>1</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="AZ9" t="s">
         <v>311</v>
       </c>
-      <c r="AW9">
-        <v>-1</v>
-      </c>
-      <c r="AX9">
-        <v>-1</v>
-      </c>
-      <c r="AY9">
-        <v>-1</v>
-      </c>
-      <c r="AZ9">
-        <v>-1</v>
-      </c>
       <c r="BA9">
         <v>-1</v>
       </c>
@@ -6077,6 +6191,18 @@
         <v>-1</v>
       </c>
       <c r="BD9">
+        <v>-1</v>
+      </c>
+      <c r="BE9">
+        <v>-1</v>
+      </c>
+      <c r="BF9">
+        <v>-1</v>
+      </c>
+      <c r="BG9">
+        <v>-1</v>
+      </c>
+      <c r="BH9">
         <v>-1</v>
       </c>
     </row>
@@ -9341,8 +9467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
I changed some of the Fundamentals of how a targeted ability works; since it's now treated as both a helping and offensive ability, many more attributes were added to it. Moreover, those attributes are absolute - meaning that the cost of -5 DR Chop is the same as 5 DR Chop. Also, a new method was added to determine if the ability is offensive. For example, if an ability heals d4 but causes -1 to DR Earth, it would be classified as harmful, and then be used as an 'attack' as well as how a duration ability would.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,12 @@
     <sheet name="Events" sheetId="4" r:id="rId4"/>
     <sheet name="Sounds" sheetId="7" r:id="rId5"/>
     <sheet name="Abilities" sheetId="5" r:id="rId6"/>
-    <sheet name="Images" sheetId="8" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId8"/>
-    <sheet name="TargetedAbilities" sheetId="9" r:id="rId9"/>
+    <sheet name="AbilityFeatureChart" sheetId="6" r:id="rId7"/>
+    <sheet name="Images" sheetId="8" r:id="rId8"/>
+    <sheet name="PermenantAbilities" sheetId="10" r:id="rId9"/>
+    <sheet name="DurationAbilities" sheetId="11" r:id="rId10"/>
+    <sheet name="TargetedAbilities" sheetId="9" r:id="rId11"/>
+    <sheet name="InstantAbilities" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Abilities!$A$1:$A$137</definedName>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="345">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -1043,6 +1046,24 @@
   </si>
   <si>
     <t>2,100,101</t>
+  </si>
+  <si>
+    <t>-2,2,-1,1,0,0,1,1,2,2,3,3</t>
+  </si>
+  <si>
+    <t>-2,2,-1,1,0,0,1,2,2,4</t>
+  </si>
+  <si>
+    <t>-3,6,-2,4,-1,2,0,0,1,2,2,4,3,6</t>
+  </si>
+  <si>
+    <t>-3,3,-2,2,-1,1,0,0,1,1,2,2,3,3,4,4,5,5</t>
+  </si>
+  <si>
+    <t>-5,10,-4,8,-3,6,-2,4,-1,2,0,0,1,2,2,4,3,6,4,8,5,10</t>
+  </si>
+  <si>
+    <t>-10,5,-8,4,-6,3,-4,2,-2,1,0,0,2,1,4,2,6,3,8,4,10,5</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1087,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1100,6 +1121,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1142,7 +1169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1200,6 +1227,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1749,6 +1779,307 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="28">
+        <v>100</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="29">
+        <v>1</v>
+      </c>
+      <c r="D2" s="29">
+        <v>1</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="29">
+        <v>1</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="28">
+        <v>101</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" s="29">
+        <v>1</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="29">
+        <v>1</v>
+      </c>
+      <c r="K3" s="29">
+        <v>1</v>
+      </c>
+      <c r="L3" s="29">
+        <v>1</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BK14"/>
@@ -4506,8 +4837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="AW6" sqref="AW6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6208,6 +6539,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="AV2 AV8:AV9" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -6533,8 +6867,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7287,7 +7621,7 @@
         <v>215</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>205</v>
@@ -7321,7 +7655,7 @@
         <v>228</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>205</v>
@@ -7338,7 +7672,7 @@
         <v>215</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>205</v>
@@ -7372,7 +7706,7 @@
         <v>152</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>205</v>
+        <v>152</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>205</v>
@@ -7440,7 +7774,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>205</v>
@@ -7456,8 +7790,8 @@
       <c r="C54" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D54" s="10">
-        <v>0</v>
+      <c r="D54" s="10" t="s">
+        <v>205</v>
       </c>
       <c r="E54" s="10" t="s">
         <v>205</v>
@@ -7473,8 +7807,8 @@
       <c r="C55" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D55" s="10">
-        <v>0</v>
+      <c r="D55" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="E55" s="10" t="s">
         <v>205</v>
@@ -7491,7 +7825,7 @@
         <v>1</v>
       </c>
       <c r="D56" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" s="10">
         <v>0</v>
@@ -7508,7 +7842,7 @@
         <v>205</v>
       </c>
       <c r="D57" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E57" s="10">
         <v>0</v>
@@ -7524,8 +7858,8 @@
       <c r="C58" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D58" s="10">
-        <v>0</v>
+      <c r="D58" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="E58" s="10">
         <v>0</v>
@@ -7542,7 +7876,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" s="10">
         <v>0</v>
@@ -7559,7 +7893,7 @@
         <v>205</v>
       </c>
       <c r="D60" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E60" s="10">
         <v>0</v>
@@ -7575,8 +7909,8 @@
       <c r="C61" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D61" s="10">
-        <v>0</v>
+      <c r="D61" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="E61" s="10">
         <v>0</v>
@@ -7593,7 +7927,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" s="10">
         <v>0</v>
@@ -7610,7 +7944,7 @@
         <v>205</v>
       </c>
       <c r="D63" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E63" s="10">
         <v>0</v>
@@ -7626,8 +7960,8 @@
       <c r="C64" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D64" s="10">
-        <v>0</v>
+      <c r="D64" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="E64" s="10">
         <v>0</v>
@@ -7644,7 +7978,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" s="10">
         <v>0</v>
@@ -7661,7 +7995,7 @@
         <v>205</v>
       </c>
       <c r="D66" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E66" s="10">
         <v>0</v>
@@ -7677,8 +8011,8 @@
       <c r="C67" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D67" s="10">
-        <v>0</v>
+      <c r="D67" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="E67" s="10">
         <v>0</v>
@@ -7695,7 +8029,7 @@
         <v>1</v>
       </c>
       <c r="D68" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" s="10">
         <v>0</v>
@@ -7712,7 +8046,7 @@
         <v>205</v>
       </c>
       <c r="D69" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E69" s="10">
         <v>0</v>
@@ -7728,8 +8062,8 @@
       <c r="C70" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D70" s="10">
-        <v>0</v>
+      <c r="D70" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="E70" s="10">
         <v>0</v>
@@ -7746,7 +8080,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="10">
         <v>0</v>
@@ -7763,7 +8097,7 @@
         <v>205</v>
       </c>
       <c r="D72" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E72" s="10">
         <v>0</v>
@@ -7779,8 +8113,8 @@
       <c r="C73" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D73" s="10">
-        <v>0</v>
+      <c r="D73" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="E73" s="10">
         <v>0</v>
@@ -7797,7 +8131,7 @@
         <v>1</v>
       </c>
       <c r="D74" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" s="10">
         <v>0</v>
@@ -7814,7 +8148,7 @@
         <v>205</v>
       </c>
       <c r="D75" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E75" s="10">
         <v>0</v>
@@ -7830,8 +8164,8 @@
       <c r="C76" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D76" s="10">
-        <v>0</v>
+      <c r="D76" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="E76" s="10">
         <v>0</v>
@@ -7848,7 +8182,7 @@
         <v>1</v>
       </c>
       <c r="D77" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" s="10">
         <v>0</v>
@@ -7865,7 +8199,7 @@
         <v>2</v>
       </c>
       <c r="D78" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E78" s="10">
         <v>0</v>
@@ -7881,8 +8215,8 @@
       <c r="C79" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D79" s="10">
-        <v>0</v>
+      <c r="D79" s="10" t="s">
+        <v>340</v>
       </c>
       <c r="E79" s="10">
         <v>0</v>
@@ -7899,7 +8233,7 @@
         <v>215</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E80" s="10" t="s">
         <v>215</v>
@@ -7916,7 +8250,7 @@
         <v>206</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E81" s="10" t="s">
         <v>206</v>
@@ -7933,7 +8267,7 @@
         <v>242</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>205</v>
+        <v>341</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>242</v>
@@ -7950,7 +8284,7 @@
         <v>1</v>
       </c>
       <c r="D83" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" s="10">
         <v>1</v>
@@ -7966,8 +8300,8 @@
       <c r="C84" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="D84" s="10">
-        <v>0</v>
+      <c r="D84" s="10" t="s">
+        <v>206</v>
       </c>
       <c r="E84" s="12" t="s">
         <v>205</v>
@@ -7983,8 +8317,8 @@
       <c r="C85" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="D85" s="10">
-        <v>0</v>
+      <c r="D85" s="10" t="s">
+        <v>342</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>246</v>
@@ -8001,7 +8335,7 @@
         <v>215</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="E86" s="10" t="s">
         <v>215</v>
@@ -8018,7 +8352,7 @@
         <v>205</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>205</v>
@@ -8035,7 +8369,7 @@
         <v>210</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>205</v>
+        <v>343</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>210</v>
@@ -8051,8 +8385,8 @@
       <c r="C89" s="10">
         <v>1</v>
       </c>
-      <c r="D89" s="10" t="s">
-        <v>205</v>
+      <c r="D89" s="10">
+        <v>1</v>
       </c>
       <c r="E89" s="10">
         <v>1</v>
@@ -8086,7 +8420,7 @@
         <v>269</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>205</v>
+        <v>269</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>269</v>
@@ -8103,7 +8437,7 @@
         <v>1</v>
       </c>
       <c r="D92" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" s="10">
         <v>1</v>
@@ -8119,8 +8453,8 @@
       <c r="C93" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D93" s="10">
-        <v>0</v>
+      <c r="D93" s="10" t="s">
+        <v>205</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>205</v>
@@ -8136,8 +8470,8 @@
       <c r="C94" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="D94" s="10">
-        <v>0</v>
+      <c r="D94" s="10" t="s">
+        <v>208</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>208</v>
@@ -8154,7 +8488,7 @@
         <v>1</v>
       </c>
       <c r="D95" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" s="10">
         <v>0</v>
@@ -8170,8 +8504,8 @@
       <c r="C96" s="10">
         <v>0</v>
       </c>
-      <c r="D96" s="10">
-        <v>0</v>
+      <c r="D96" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="E96" s="10">
         <v>0</v>
@@ -8187,8 +8521,8 @@
       <c r="C97" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="D97" s="10">
-        <v>0</v>
+      <c r="D97" s="10" t="s">
+        <v>344</v>
       </c>
       <c r="E97" s="10">
         <v>0</v>
@@ -8205,7 +8539,7 @@
         <v>1</v>
       </c>
       <c r="D98" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98" s="10">
         <v>0</v>
@@ -8221,8 +8555,8 @@
       <c r="C99" s="10">
         <v>0</v>
       </c>
-      <c r="D99" s="10">
-        <v>0</v>
+      <c r="D99" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="E99" s="10">
         <v>0</v>
@@ -8238,8 +8572,8 @@
       <c r="C100" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="D100" s="10">
-        <v>0</v>
+      <c r="D100" s="10" t="s">
+        <v>344</v>
       </c>
       <c r="E100" s="10">
         <v>0</v>
@@ -8256,7 +8590,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101" s="10">
         <v>0</v>
@@ -8272,8 +8606,8 @@
       <c r="C102" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D102" s="10">
-        <v>0</v>
+      <c r="D102" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="E102" s="10">
         <v>0</v>
@@ -8289,8 +8623,8 @@
       <c r="C103" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D103" s="10">
-        <v>0</v>
+      <c r="D103" s="10" t="s">
+        <v>237</v>
       </c>
       <c r="E103" s="10">
         <v>0</v>
@@ -8307,7 +8641,7 @@
         <v>1</v>
       </c>
       <c r="D104" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E104" s="10">
         <v>0</v>
@@ -8323,8 +8657,8 @@
       <c r="C105" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D105" s="10">
-        <v>0</v>
+      <c r="D105" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="E105" s="10">
         <v>0</v>
@@ -8340,8 +8674,8 @@
       <c r="C106" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D106" s="10">
-        <v>0</v>
+      <c r="D106" s="10" t="s">
+        <v>237</v>
       </c>
       <c r="E106" s="10">
         <v>0</v>
@@ -8358,7 +8692,7 @@
         <v>1</v>
       </c>
       <c r="D107" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" s="10">
         <v>0</v>
@@ -8374,8 +8708,8 @@
       <c r="C108" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D108" s="10">
-        <v>0</v>
+      <c r="D108" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="E108" s="10">
         <v>0</v>
@@ -8391,8 +8725,8 @@
       <c r="C109" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D109" s="10">
-        <v>0</v>
+      <c r="D109" s="10" t="s">
+        <v>237</v>
       </c>
       <c r="E109" s="10">
         <v>0</v>
@@ -8409,7 +8743,7 @@
         <v>1</v>
       </c>
       <c r="D110" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" s="10">
         <v>0</v>
@@ -8425,8 +8759,8 @@
       <c r="C111" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D111" s="10">
-        <v>0</v>
+      <c r="D111" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="E111" s="10">
         <v>0</v>
@@ -8442,8 +8776,8 @@
       <c r="C112" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D112" s="10">
-        <v>0</v>
+      <c r="D112" s="10" t="s">
+        <v>237</v>
       </c>
       <c r="E112" s="10">
         <v>0</v>
@@ -8460,7 +8794,7 @@
         <v>1</v>
       </c>
       <c r="D113" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" s="10">
         <v>0</v>
@@ -8476,8 +8810,8 @@
       <c r="C114" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D114" s="10">
-        <v>0</v>
+      <c r="D114" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="E114" s="10">
         <v>0</v>
@@ -8493,8 +8827,8 @@
       <c r="C115" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D115" s="10">
-        <v>0</v>
+      <c r="D115" s="10" t="s">
+        <v>237</v>
       </c>
       <c r="E115" s="10">
         <v>0</v>
@@ -8511,7 +8845,7 @@
         <v>1</v>
       </c>
       <c r="D116" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E116" s="10">
         <v>0</v>
@@ -8527,8 +8861,8 @@
       <c r="C117" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D117" s="10">
-        <v>0</v>
+      <c r="D117" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="E117" s="10">
         <v>0</v>
@@ -8544,8 +8878,8 @@
       <c r="C118" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D118" s="10">
-        <v>0</v>
+      <c r="D118" s="10" t="s">
+        <v>237</v>
       </c>
       <c r="E118" s="10">
         <v>0</v>
@@ -8562,7 +8896,7 @@
         <v>1</v>
       </c>
       <c r="D119" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119" s="10">
         <v>0</v>
@@ -8578,8 +8912,8 @@
       <c r="C120" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D120" s="10">
-        <v>0</v>
+      <c r="D120" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="E120" s="10">
         <v>0</v>
@@ -8595,8 +8929,8 @@
       <c r="C121" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D121" s="10">
-        <v>0</v>
+      <c r="D121" s="10" t="s">
+        <v>237</v>
       </c>
       <c r="E121" s="10">
         <v>0</v>
@@ -8613,7 +8947,7 @@
         <v>1</v>
       </c>
       <c r="D122" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E122" s="10">
         <v>0</v>
@@ -8629,8 +8963,8 @@
       <c r="C123" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D123" s="10">
-        <v>0</v>
+      <c r="D123" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="E123" s="10">
         <v>0</v>
@@ -8646,8 +8980,8 @@
       <c r="C124" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D124" s="10">
-        <v>0</v>
+      <c r="D124" s="10" t="s">
+        <v>237</v>
       </c>
       <c r="E124" s="10">
         <v>0</v>
@@ -8822,6 +9156,561 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1"/>
+      <c r="B1" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="19"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="19"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="19"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="19"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="19"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="19"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="31"/>
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="19"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="31"/>
+      <c r="E24" s="19"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="31"/>
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="31"/>
+      <c r="E26" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="31"/>
+      <c r="E27" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="31"/>
+      <c r="E28" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="31"/>
+      <c r="E29" s="21"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="31"/>
+      <c r="E30" s="21"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="31"/>
+      <c r="E31" s="19"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="31"/>
+      <c r="E32" s="19"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="31"/>
+      <c r="E33" s="19"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="31"/>
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="31"/>
+      <c r="E35" s="19"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="31"/>
+      <c r="E36" s="19"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="31"/>
+      <c r="E37" s="19"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="31"/>
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="31"/>
+      <c r="E39" s="19"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="31"/>
+      <c r="E40" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8908,834 +9797,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1"/>
-      <c r="B1" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="19"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="19"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="19"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="19"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="19"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="19"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="19"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="19"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="19"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="19"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="19"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="21"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="21"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="19"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="19"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="19"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="19"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="19"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="19"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="19"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="19"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="19"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="19"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:P3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="30" t="s">
-        <v>329</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="28">
-        <v>100</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>330</v>
-      </c>
-      <c r="C2" s="29">
-        <v>1</v>
-      </c>
-      <c r="D2" s="29">
-        <v>1</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="29">
-        <v>1</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="28">
-        <v>101</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>332</v>
-      </c>
-      <c r="C3" s="29">
-        <v>1</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1">
-        <v>2</v>
-      </c>
-      <c r="J3" s="29">
-        <v>1</v>
-      </c>
-      <c r="K3" s="29">
-        <v>1</v>
-      </c>
-      <c r="L3" s="29">
-        <v>1</v>
-      </c>
-      <c r="M3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
hooookay - So all the steps in the enemy AI have more or less been implemented, including some minor refactorings (e.g. attack/tactical modules, spot selection for movement, etc.). There's still a bit of tweaking required for how behavior works, perhaps changing how offensiveness/supportiveness works, however the rough sketch is complete. Still several more things to test and bugs to find.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="354">
   <si>
     <t>Hello, adventurer.</t>
   </si>
@@ -1043,9 +1043,6 @@
     <t>InstantAbilityIDs</t>
   </si>
   <si>
-    <t>2,100,101</t>
-  </si>
-  <si>
     <t>-2,2,-1,1,0,0,1,1,2,2,3,3</t>
   </si>
   <si>
@@ -1070,7 +1067,31 @@
     <t>Heal Target</t>
   </si>
   <si>
-    <t>3,100,101,102</t>
+    <t>offensiveness</t>
+  </si>
+  <si>
+    <t>abilityAffinity</t>
+  </si>
+  <si>
+    <t>cowardness</t>
+  </si>
+  <si>
+    <t>tacticalness</t>
+  </si>
+  <si>
+    <t>Muscle Time</t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t>1,100</t>
+  </si>
+  <si>
+    <t>4,100,101,102,103</t>
+  </si>
+  <si>
+    <t>2,102,103</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1230,6 +1251,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1779,12 +1801,307 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AO2" sqref="A2:AO2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41">
+      <c r="A1" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1793,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1975,7 +2292,7 @@
         <v>100</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C2" s="29">
         <v>1</v>
@@ -2231,7 +2548,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C4" s="29">
         <v>1</v>
@@ -2355,11 +2672,132 @@
       </c>
     </row>
     <row r="5" spans="1:42">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="A5" s="26">
+        <v>103</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>350</v>
+      </c>
+      <c r="C5" s="27">
+        <v>1</v>
+      </c>
+      <c r="D5" s="27">
+        <v>1</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA5">
+        <v>4</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:42">
       <c r="A6" s="26"/>
@@ -2460,9 +2898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BK14"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1:AX1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5211,10 +5647,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BH9"/>
+  <dimension ref="A1:BL9"/>
   <sheetViews>
-    <sheetView topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="AW18" sqref="AW18"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BL2" sqref="BL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5259,23 +5695,27 @@
     <col min="43" max="43" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="19" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="39.85546875" customWidth="1"/>
-    <col min="55" max="55" width="18" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="30.42578125" customWidth="1"/>
-    <col min="57" max="57" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="17" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="39.85546875" customWidth="1"/>
+    <col min="59" max="59" width="18" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="30.42578125" customWidth="1"/>
+    <col min="61" max="61" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60">
+    <row r="1" spans="1:64">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -5412,52 +5852,64 @@
         <v>326</v>
       </c>
       <c r="AT1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>348</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>347</v>
+      </c>
+      <c r="AX1" t="s">
         <v>333</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AY1" t="s">
         <v>334</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AZ1" t="s">
         <v>335</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BA1" t="s">
         <v>336</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BB1" t="s">
         <v>313</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BC1" t="s">
         <v>312</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BD1" t="s">
         <v>302</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BE1" t="s">
         <v>306</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BF1" t="s">
         <v>307</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BG1" t="s">
         <v>308</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BH1" t="s">
         <v>309</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BI1" t="s">
         <v>310</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BJ1" t="s">
         <v>303</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BK1" t="s">
         <v>304</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BL1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:60">
+    <row r="2" spans="1:64">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -5537,7 +5989,7 @@
         <v>66</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB2">
         <v>3</v>
@@ -5594,52 +6046,64 @@
         <v>1</v>
       </c>
       <c r="AT2">
-        <v>-1</v>
-      </c>
-      <c r="AU2" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AV2" s="25" t="s">
-        <v>346</v>
-      </c>
-      <c r="AW2" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AX2" s="25">
-        <v>1</v>
-      </c>
-      <c r="AY2">
-        <v>0</v>
-      </c>
-      <c r="AZ2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU2">
+        <v>50</v>
+      </c>
+      <c r="AV2">
+        <v>25</v>
+      </c>
+      <c r="AW2">
+        <v>5</v>
+      </c>
+      <c r="AX2">
+        <v>-1</v>
+      </c>
+      <c r="AY2" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="AZ2" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="BA2" s="25">
+        <v>-1</v>
+      </c>
+      <c r="BB2" s="25">
+        <v>1</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="s">
         <v>316</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BE2" t="s">
         <v>317</v>
       </c>
-      <c r="BB2">
-        <v>-1</v>
-      </c>
-      <c r="BC2">
-        <v>-1</v>
-      </c>
-      <c r="BD2">
-        <v>-1</v>
-      </c>
-      <c r="BE2">
-        <v>-1</v>
-      </c>
       <c r="BF2">
         <v>-1</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BG2">
+        <v>-1</v>
+      </c>
+      <c r="BH2">
+        <v>-1</v>
+      </c>
+      <c r="BI2">
+        <v>-1</v>
+      </c>
+      <c r="BJ2">
+        <v>-1</v>
+      </c>
+      <c r="BK2" t="s">
         <v>317</v>
       </c>
-      <c r="BH2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:60">
+      <c r="BL2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64">
       <c r="A3">
         <v>2006</v>
       </c>
@@ -5776,52 +6240,64 @@
         <v>0</v>
       </c>
       <c r="AT3">
-        <v>-1</v>
-      </c>
-      <c r="AU3" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AV3" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AW3" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AX3" s="25">
-        <v>1</v>
-      </c>
-      <c r="AY3">
-        <v>0</v>
-      </c>
-      <c r="AZ3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU3">
+        <v>50</v>
+      </c>
+      <c r="AV3">
+        <v>25</v>
+      </c>
+      <c r="AW3">
+        <v>15</v>
+      </c>
+      <c r="AX3">
+        <v>-1</v>
+      </c>
+      <c r="AY3" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="AZ3" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="BA3" s="25">
+        <v>-1</v>
+      </c>
+      <c r="BB3" s="25">
+        <v>1</v>
+      </c>
+      <c r="BC3">
+        <v>0</v>
+      </c>
+      <c r="BD3" t="s">
         <v>316</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BE3" t="s">
         <v>317</v>
       </c>
-      <c r="BB3">
-        <v>-1</v>
-      </c>
-      <c r="BC3">
-        <v>-1</v>
-      </c>
-      <c r="BD3">
-        <v>-1</v>
-      </c>
-      <c r="BE3">
-        <v>-1</v>
-      </c>
       <c r="BF3">
         <v>-1</v>
       </c>
-      <c r="BG3" t="s">
+      <c r="BG3">
+        <v>-1</v>
+      </c>
+      <c r="BH3">
+        <v>-1</v>
+      </c>
+      <c r="BI3">
+        <v>-1</v>
+      </c>
+      <c r="BJ3">
+        <v>-1</v>
+      </c>
+      <c r="BK3" t="s">
         <v>317</v>
       </c>
-      <c r="BH3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:60">
+      <c r="BL3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64">
       <c r="A4">
         <v>2007</v>
       </c>
@@ -5958,52 +6434,64 @@
         <v>0</v>
       </c>
       <c r="AT4">
-        <v>-1</v>
-      </c>
-      <c r="AU4" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AV4" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AW4" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AX4" s="25">
-        <v>1</v>
-      </c>
-      <c r="AY4">
-        <v>0</v>
-      </c>
-      <c r="AZ4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU4">
+        <v>50</v>
+      </c>
+      <c r="AV4">
+        <v>25</v>
+      </c>
+      <c r="AW4">
+        <v>15</v>
+      </c>
+      <c r="AX4">
+        <v>-1</v>
+      </c>
+      <c r="AY4" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="AZ4" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="BA4" s="25">
+        <v>-1</v>
+      </c>
+      <c r="BB4" s="25">
+        <v>1</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BD4" t="s">
         <v>316</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BE4" t="s">
         <v>317</v>
       </c>
-      <c r="BB4">
-        <v>-1</v>
-      </c>
-      <c r="BC4">
-        <v>-1</v>
-      </c>
-      <c r="BD4">
-        <v>-1</v>
-      </c>
-      <c r="BE4">
-        <v>-1</v>
-      </c>
       <c r="BF4">
         <v>-1</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BG4">
+        <v>-1</v>
+      </c>
+      <c r="BH4">
+        <v>-1</v>
+      </c>
+      <c r="BI4">
+        <v>-1</v>
+      </c>
+      <c r="BJ4">
+        <v>-1</v>
+      </c>
+      <c r="BK4" t="s">
         <v>317</v>
       </c>
-      <c r="BH4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:60">
+      <c r="BL4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64">
       <c r="A5">
         <v>2008</v>
       </c>
@@ -6140,52 +6628,64 @@
         <v>0</v>
       </c>
       <c r="AT5">
-        <v>-1</v>
-      </c>
-      <c r="AU5" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AV5" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AW5" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AX5" s="25">
-        <v>1</v>
-      </c>
-      <c r="AY5">
-        <v>0</v>
-      </c>
-      <c r="AZ5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU5">
+        <v>50</v>
+      </c>
+      <c r="AV5">
+        <v>25</v>
+      </c>
+      <c r="AW5">
+        <v>15</v>
+      </c>
+      <c r="AX5">
+        <v>-1</v>
+      </c>
+      <c r="AY5" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="AZ5" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="BA5" s="25">
+        <v>-1</v>
+      </c>
+      <c r="BB5" s="25">
+        <v>1</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
+      </c>
+      <c r="BD5" t="s">
         <v>316</v>
       </c>
-      <c r="BA5" t="s">
+      <c r="BE5" t="s">
         <v>317</v>
       </c>
-      <c r="BB5">
-        <v>-1</v>
-      </c>
-      <c r="BC5">
-        <v>-1</v>
-      </c>
-      <c r="BD5">
-        <v>-1</v>
-      </c>
-      <c r="BE5">
-        <v>-1</v>
-      </c>
       <c r="BF5">
         <v>-1</v>
       </c>
-      <c r="BG5" t="s">
+      <c r="BG5">
+        <v>-1</v>
+      </c>
+      <c r="BH5">
+        <v>-1</v>
+      </c>
+      <c r="BI5">
+        <v>-1</v>
+      </c>
+      <c r="BJ5">
+        <v>-1</v>
+      </c>
+      <c r="BK5" t="s">
         <v>317</v>
       </c>
-      <c r="BH5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:60">
+      <c r="BL5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64">
       <c r="A6">
         <v>2009</v>
       </c>
@@ -6322,52 +6822,64 @@
         <v>0</v>
       </c>
       <c r="AT6">
-        <v>-1</v>
-      </c>
-      <c r="AU6" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AV6" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AW6" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AX6" s="25">
-        <v>1</v>
-      </c>
-      <c r="AY6">
-        <v>0</v>
-      </c>
-      <c r="AZ6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU6">
+        <v>50</v>
+      </c>
+      <c r="AV6">
+        <v>25</v>
+      </c>
+      <c r="AW6">
+        <v>15</v>
+      </c>
+      <c r="AX6">
+        <v>-1</v>
+      </c>
+      <c r="AY6" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="AZ6" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="BA6" s="25">
+        <v>-1</v>
+      </c>
+      <c r="BB6" s="25">
+        <v>1</v>
+      </c>
+      <c r="BC6">
+        <v>0</v>
+      </c>
+      <c r="BD6" t="s">
         <v>316</v>
       </c>
-      <c r="BA6" t="s">
+      <c r="BE6" t="s">
         <v>317</v>
       </c>
-      <c r="BB6">
-        <v>-1</v>
-      </c>
-      <c r="BC6">
-        <v>-1</v>
-      </c>
-      <c r="BD6">
-        <v>-1</v>
-      </c>
-      <c r="BE6">
-        <v>-1</v>
-      </c>
       <c r="BF6">
         <v>-1</v>
       </c>
-      <c r="BG6" t="s">
+      <c r="BG6">
+        <v>-1</v>
+      </c>
+      <c r="BH6">
+        <v>-1</v>
+      </c>
+      <c r="BI6">
+        <v>-1</v>
+      </c>
+      <c r="BJ6">
+        <v>-1</v>
+      </c>
+      <c r="BK6" t="s">
         <v>317</v>
       </c>
-      <c r="BH6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:60">
+      <c r="BL6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -6504,52 +7016,64 @@
         <v>0</v>
       </c>
       <c r="AT7">
-        <v>-1</v>
-      </c>
-      <c r="AU7" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AV7" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AW7" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AX7" s="25">
-        <v>1</v>
-      </c>
-      <c r="AY7">
-        <v>0</v>
-      </c>
-      <c r="AZ7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU7">
+        <v>50</v>
+      </c>
+      <c r="AV7">
+        <v>25</v>
+      </c>
+      <c r="AW7">
+        <v>15</v>
+      </c>
+      <c r="AX7">
+        <v>-1</v>
+      </c>
+      <c r="AY7" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="AZ7" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="BA7" s="25">
+        <v>-1</v>
+      </c>
+      <c r="BB7" s="25">
+        <v>1</v>
+      </c>
+      <c r="BC7">
+        <v>0</v>
+      </c>
+      <c r="BD7" t="s">
         <v>316</v>
       </c>
-      <c r="BA7" t="s">
+      <c r="BE7" t="s">
         <v>317</v>
       </c>
-      <c r="BB7">
-        <v>-1</v>
-      </c>
-      <c r="BC7">
-        <v>-1</v>
-      </c>
-      <c r="BD7">
-        <v>-1</v>
-      </c>
-      <c r="BE7">
-        <v>-1</v>
-      </c>
       <c r="BF7">
         <v>-1</v>
       </c>
-      <c r="BG7" t="s">
+      <c r="BG7">
+        <v>-1</v>
+      </c>
+      <c r="BH7">
+        <v>-1</v>
+      </c>
+      <c r="BI7">
+        <v>-1</v>
+      </c>
+      <c r="BJ7">
+        <v>-1</v>
+      </c>
+      <c r="BK7" t="s">
         <v>317</v>
       </c>
-      <c r="BH7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:60">
+      <c r="BL7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64">
       <c r="A8">
         <v>2013</v>
       </c>
@@ -6686,38 +7210,38 @@
         <v>0</v>
       </c>
       <c r="AT8">
-        <v>-1</v>
-      </c>
-      <c r="AU8" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AV8" s="25" t="s">
-        <v>337</v>
-      </c>
-      <c r="AW8" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AX8" s="25">
-        <v>1</v>
-      </c>
-      <c r="AY8">
-        <v>0</v>
-      </c>
-      <c r="AZ8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU8">
+        <v>50</v>
+      </c>
+      <c r="AV8">
+        <v>25</v>
+      </c>
+      <c r="AW8">
+        <v>25</v>
+      </c>
+      <c r="AX8">
+        <v>-1</v>
+      </c>
+      <c r="AY8" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="AZ8" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="BA8" s="25">
+        <v>-1</v>
+      </c>
+      <c r="BB8" s="25">
+        <v>1</v>
+      </c>
+      <c r="BC8">
+        <v>0</v>
+      </c>
+      <c r="BD8" t="s">
         <v>311</v>
       </c>
-      <c r="BA8">
-        <v>-1</v>
-      </c>
-      <c r="BB8">
-        <v>-1</v>
-      </c>
-      <c r="BC8">
-        <v>-1</v>
-      </c>
-      <c r="BD8">
-        <v>-1</v>
-      </c>
       <c r="BE8">
         <v>-1</v>
       </c>
@@ -6730,8 +7254,20 @@
       <c r="BH8">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:60">
+      <c r="BI8">
+        <v>-1</v>
+      </c>
+      <c r="BJ8">
+        <v>-1</v>
+      </c>
+      <c r="BK8">
+        <v>-1</v>
+      </c>
+      <c r="BL8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -6868,38 +7404,38 @@
         <v>0</v>
       </c>
       <c r="AT9">
-        <v>-1</v>
-      </c>
-      <c r="AU9" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AV9" s="25" t="s">
-        <v>337</v>
-      </c>
-      <c r="AW9" s="25">
-        <v>-1</v>
-      </c>
-      <c r="AX9" s="25">
-        <v>1</v>
-      </c>
-      <c r="AY9">
-        <v>0</v>
-      </c>
-      <c r="AZ9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU9">
+        <v>50</v>
+      </c>
+      <c r="AV9">
+        <v>25</v>
+      </c>
+      <c r="AW9">
+        <v>25</v>
+      </c>
+      <c r="AX9">
+        <v>-1</v>
+      </c>
+      <c r="AY9" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="AZ9" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="BA9" s="25">
+        <v>-1</v>
+      </c>
+      <c r="BB9" s="25">
+        <v>1</v>
+      </c>
+      <c r="BC9">
+        <v>0</v>
+      </c>
+      <c r="BD9" t="s">
         <v>311</v>
       </c>
-      <c r="BA9">
-        <v>-1</v>
-      </c>
-      <c r="BB9">
-        <v>-1</v>
-      </c>
-      <c r="BC9">
-        <v>-1</v>
-      </c>
-      <c r="BD9">
-        <v>-1</v>
-      </c>
       <c r="BE9">
         <v>-1</v>
       </c>
@@ -6910,14 +7446,23 @@
         <v>-1</v>
       </c>
       <c r="BH9">
+        <v>-1</v>
+      </c>
+      <c r="BI9">
+        <v>-1</v>
+      </c>
+      <c r="BJ9">
+        <v>-1</v>
+      </c>
+      <c r="BK9">
+        <v>-1</v>
+      </c>
+      <c r="BL9">
         <v>-1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="AV8:AV9" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -7243,8 +7788,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8184,7 +8729,7 @@
         <v>201</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E55" s="10" t="s">
         <v>205</v>
@@ -8235,7 +8780,7 @@
         <v>201</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E58" s="10">
         <v>0</v>
@@ -8286,7 +8831,7 @@
         <v>201</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E61" s="10">
         <v>0</v>
@@ -8337,7 +8882,7 @@
         <v>201</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E64" s="10">
         <v>0</v>
@@ -8388,7 +8933,7 @@
         <v>201</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E67" s="10">
         <v>0</v>
@@ -8439,7 +8984,7 @@
         <v>201</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E70" s="10">
         <v>0</v>
@@ -8490,7 +9035,7 @@
         <v>201</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E73" s="10">
         <v>0</v>
@@ -8541,7 +9086,7 @@
         <v>201</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E76" s="10">
         <v>0</v>
@@ -8592,7 +9137,7 @@
         <v>204</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E79" s="10">
         <v>0</v>
@@ -8643,7 +9188,7 @@
         <v>242</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>242</v>
@@ -8694,7 +9239,7 @@
         <v>246</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>246</v>
@@ -8745,7 +9290,7 @@
         <v>210</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>210</v>
@@ -8898,7 +9443,7 @@
         <v>208</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E97" s="10">
         <v>0</v>
@@ -8949,7 +9494,7 @@
         <v>208</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E100" s="10">
         <v>0</v>
@@ -9534,8 +10079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated images for the big graphics overhaul; started the change - The commit message I wrote for this was a lot longer the first time, but the commit failed so here's the highlights:
-Gonna change image default size to 50x50, can be as big as 100x100, and
-No longer using one image for all sprites, rather their individual
sprite sheets.

It's gonna be a pain.
</commit_message>
<xml_diff>
--- a/GameData.xlsx
+++ b/GameData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="2700" windowHeight="1110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -2111,7 +2111,7 @@
   <dimension ref="A1:AP16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2898,7 +2898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BK14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5649,8 +5651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BL9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
-      <selection activeCell="BL2" sqref="BL2"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:BL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6052,7 +6054,7 @@
         <v>50</v>
       </c>
       <c r="AV2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="AW2">
         <v>5</v>
@@ -7096,10 +7098,10 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8">
         <v>0</v>

</xml_diff>